<commit_message>
Fixed bug in fb.py driver_fb_search had the wrong url name. Added random waits in ebs.py.
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +58,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,8 +466,8 @@
           <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT Details 11 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 753 View Street (2nd floor, Hermmans Jazz Club) Date: Saturday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>45810.89125604976</v>
+      <c r="C2" s="3" t="n">
+        <v>45810.89125605324</v>
       </c>
     </row>
     <row r="3">
@@ -480,8 +481,8 @@
           <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY The Coda About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY Details 81 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 751 View Street (2nd floor, Hermmans Jazz Club) Date: Friday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>45810.89125604976</v>
+      <c r="C3" s="3" t="n">
+        <v>45810.89125605324</v>
       </c>
     </row>
     <row r="4">
@@ -495,8 +496,1538 @@
           <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com or 15$ cash/e-transfer at the door. Formed in the heart of Chinatown, Rosebuds is a dynamic ensemble that brings the vibrant sounds of jazz, blues &amp; swing to life.  The group plays a mixture of originals and jazz standards, and is influenced by artists like Louis Armstrong, Billie Holiday, Lester Young, and Lionel Hampton. Featuring Rebecca Wells (vocals/guitar), Alex Moore (guitar/keys) Bryden Amos (guitar/keys), Matisse Gubby-Hurtig (bass), Owen Chow (trumpet), and Andrew Greenwood (tenor saxophone). Samba e Sol is a newly formed Brazilian bossa nova jazz trio featuring Andrew Greenwood (flute), Alex Moore (guitar), and Matisse Gubby-Hurtig (bass), playing music by artists like Antonio Carlos Jobim, Marcos Valle, Luiz Bonfa, and more. Instagram: https://www.instagram.com/rosebudsband/ See less Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria Guests See All</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>45810.89125604976</v>
+      <c r="C4" s="3" t="n">
+        <v>45810.89125605324</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/667083456006099/</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT Details 11 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 753 View Street (2nd floor, Hermmans Jazz Club) Date: Saturday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>45810.92020050926</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1910904133047825/</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY The Coda About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY Details 81 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 751 View Street (2nd floor, Hermmans Jazz Club) Date: Friday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>45810.92020050926</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1132427048350776/</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com or 15$ cash/e-transfer at the door. Formed in the heart of Chinatown, Rosebuds is a dynamic ensemble that brings the vibrant sounds of jazz, blues &amp; swing to life.  The group plays a mixture of originals and jazz standards, and is influenced by artists like Louis Armstrong, Billie Holiday, Lester Young, and Lionel Hampton. Featuring Rebecca Wells (vocals/guitar), Alex Moore (guitar/keys) Bryden Amos (guitar/keys), Matisse Gubby-Hurtig (bass), Owen Chow (trumpet), and Andrew Greenwood (tenor saxophone). Samba e Sol is a newly formed Brazilian bossa nova jazz trio featuring Andrew Greenwood (flute), Alex Moore (guitar), and Matisse Gubby-Hurtig (bass), playing music by artists like Antonio Carlos Jobim, Marcos Valle, Luiz Bonfa, and more. Instagram: https://www.instagram.com/rosebudsband/ See less Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>45810.92020050926</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1179097320623502/</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 37 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1029869435768837/</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Saturday 22 March 2025 at 20:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC This event has been cancelled. You cannot share this event, but you can still post. About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 14 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3006474846197996/</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 21 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 27, 2025 | Lesson:  Intro class TBD Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro class TBD • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/960236445839425/</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Saturday 22 June 2024 from 18:00-21:00 Kizomba/UrbanKiz at Clover Clover Pt, Victoria, BC V8S, Canada About Discussion More About Discussion Kizomba/UrbanKiz at Clover Interested Details 56 people responded Event by Becky Mowat Clover Pt, Victoria, BC V8S, Canada Duration: 3 hr Public · Anyone on or off Facebook Come join us for our first time dancing at Clover Point! There will be no lesson beforehand and this is super casual. Just a bunch of friends hanging out and dancing. Bring snacks, something to drink, blankets, warm clothes (as it is typically cooler by the ocean). There isn't a lot of parking at Clover Point but you can park along Dallas Rd and just walk down. Feel free to invite friends and family. Hope to see you all there! See less Victoria, British Columbia Clover Pt, Victoria, BC V8S, Canada 1301 Clover Pt, Victoria, BC V8S, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1079226067560481/</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 41 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 6, 2025 | Lesson:  Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/372311028526699/</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Saturday 9 December 2023 from 20:30-23:30 Victoria Kizomba Social: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Social: Fall Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1060779176049104/</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Thursday 3 October 2024 from 19:30-22:30 Kizomba Practica Thursdays: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Kizomba Practica Thursdays: Fall Series Details 20 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Join us every Thursday for Kizomba/Urbankiz classes. Intermediate 7:30PM-8:15pm Beginner 8:15pm-9:00pm Practica until 10:30pm Class only: $10 Class &amp; Practica: $15 or $10 for university students w/ID Practice only $10 Classes will be provided by your local Instructor (David Lamine) and assistants (Robyn, Becky) and occasionally by some out of town and International Instructors. Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/758501768607647/</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 6 6 Apr 2023 at 20:00 – 10 Apr 2023 at 10:00 Victoria International Kizomba Festival 4th Edition Victoria Conference Centre About Discussion More About Discussion Victoria International Kizomba Festival 4th Edition Going Details 702 people responded Event by Island Afro Latin Events Victoria Conference Centre Duration: 4 days Public · Anyone on or off Facebook Welcome to the Victoria International Kizomba Festival, APOCALYPSE EDITION!! What to expect?? Locally and Internationally renowned instructors, teaching Semba, Kizomba, Urban Kiz, Tarraxinha, Tarraxo, Douceur, Afro Beat, Afro House, Kuduro and More! ALL IN ONE: - Over 27.000 square feet of space - 3 ROOMS: Kizomba room, Urban Kiz room, Social room - After party room go until 6-7am with (Douceur, Tarraxinha and Sweet Kiz) VIKF 4rd Edition is offering you: *4 days of workshops *3 day-time socials *4 nights of dancing, *3 afterparties until 6-7am *15Hours + of workshops *40H + of dancing * 2 educational sessions of Cultural Aspect of African dances * 1 Gala Night of celebration of Multiculturalism, Diversity, the Arts including performances and fashion shows by African Designers IMPORTANT NOTICE: This 4 Day Festival has some free components offered to the general public as well as some activities with a minimal cost (to be announced at a later date) ARTISTS CONFIRMED - JP &amp; STEPHY (PARIS - FRANCE) - BONIFACIO (LISBON - PORTUGAL) - STEPHANE (PARIS - FRANCE) - SAMY (MONTREAL - CANADA) - LENA (VANCOUVER - CANADA) - ELVIS (OTTAWA - CANADA) - DJ PARAISO (PARIS - FRANCE) - DJ SINK (MONTREAL - CANADA) - DJ GUELAS (MIAMI - USA) - DJ MADARA (PARIS - FRANCE) AND MORE TO COME ... JP and STEPHY 10h Training program starts on Thursday April 6, 2023 in the afternoon DJ Training by DJ paraiso by Individual or Group of 4 (Friday - Saturday and Sunday) 10+ Taxi dancers 20+ International Special Guests HOTEL DEALS: WE HAVE 4 PREMIUMS HOTELS TO HOST YOU. A) FAIRMONT EMPRESS HOTEL is adjacent to the Convention Centre (all in one): TO BOOK YOUR ROOM: call the Reservations Department at 250 384 8111 or the Global Reservations Centre at 1 800-441-1414. Please identify yourself as being with the Victoria International Kizomba Festival group. TWO DOUBLE BEDS: $279 Rates will be available 3 days prior to the event and 3 days post B) MARRIOTT VICTORIA INNER HARBOUR, (just across the street, 1min walking distance) Book your accommodation by calling reservations toll-free at 1-888-236-2427 and asking for the "Victoria International Kizomba Festival group" to book online: https://www.marriott.com/event.../reservation-link.mi... 1 KING BED: $CAD199 2 QUEEN BEDS: $CAD199 C) DOUBLE TREE BY HILTON Reservations can be make by calling Central Reservations at 1-800-222-TREE and referencing KIZOMBA FEST 2023. or by using the HiltonLink: https://www.hilton.com/en/book/reservation/rooms/... - STANDARD ROOM: 2 QUEEN BEDS $CAD219 - SUITE WITH 2 QUEEN BEDS + SOFA BED, $CAD249 ALL rooms have all amenities (Fridge, kettle, Microwave, Iron, etc...) IMPORTANT NOTE: - If you are no longer able to join, you can transfer your pass to another participant without any fee; transfer your pass to the next edition; or ask for a refund within 15 days after the event. - Must be 18+ to attend this event - Click on the *Going* tab on facebook to receive notifications about line up updates and any useful information regarding this event. - By purchasing the pass, you grant the photographer, videographer, the Organization and its partners/sponsors  the permission to use your image  in any and all forms of media for commercial purposes, advertising, promotion... - COVID-19 clause: This event may be postponed or cancelled by the Organizer due to the Covid19 pandemic or any other resulting event related to the instructions of the federal government of Canada and the BC provincial government. In such case, the buyer can ask for a full refund. See less Dance Victoria, British Columbia Victoria Conference Centre 720 Douglas Street, Victoria The VCC is a boutique facility.  We’re small enough to be intimate yet able to handle conferences as Guests See All</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1861230087752141/</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 3 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 31, 2025 | Lesson:  Intro to Salsa with Adam &amp; Alicia Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1337760257449745/</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 4 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 10, 2025 | Lesson:   Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2637194793152555/</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 81 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 29, 2025 | Lesson:  Intro to Salsa Rueda with Sam and Katie Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa Rueda • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1293301738436581/</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Sunday 6 April 2025 at 17:00 Kizomba Sundown Party: Free of charge Method Studio - Victoria BC David Lamine Victoria invited you About Discussion More About Discussion Kizomba Sundown Party: Free of charge Details 58 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Method Studio - Victoria BC Public · Anyone on or off Facebook Free Pre-VIKFest party. Bring snack and drink. Expect great music, great energy, great atmosphere. "Dance with your heart. your feet will follow" Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1743571267040445/</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 20 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 8, 2025 | Lesson: Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/947213690692385/</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3185065321631809/</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Saturday 15 March 2025 from 20:00-00:00 Urban Kiz Workshop with Mannie Method Studio - Victoria BC Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 48 people responded Event by Becky Mowat and David Lamine Victoria Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1184791909680061/</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Thursday 13 March 2025 from 19:30-23:00 Urban Kiz Workshop with Mannie Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 50 people responded Event by Becky Mowat and David Lamine Victoria Ukrainian Cultural Centre Duration: 3 hr 30 min Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1152065639712042/</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 20 20 Feb at 19:30 – 23 Feb at 23:00 Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Details 49 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 days Public · Anyone on or off Facebook Join us for our special edition Urbankiz &amp; Tarraxo workshops with Mike Ahombi Mike has been a big supporter of our VIKF and bringing his talent and low key vibe to the west coast. He is based out of Ottawa but you will find him at many different festivals and cities teaching Kizomba, Urbakiz and Tarraxo. We cannot wait for you all to have the opportunity to learn from such an incredible person and instructor. Details: Feb 20th Urbankiz Workshop 7:30pm-9:30pm Practica 9:30pm-11:00pm Feb 22nd Tarraxo Workshop 8:00pm-10:00pm Practica 10:00-11:30pm Price $90 Workshops only $70 Practica only $20 *** please e transfer to becksmith@hotmail.com *** Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>45810.92591060185</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1813229489279716/</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Thursday 29 May 2025 from 19:55-21:00 Sensual Bachata 4 Week Series Method Studio - Victoria BC Thu, 15 May Thu, 22 May Thu, 29 May +1 About Discussion More About Discussion Sensual Bachata 4 Week Series Details 6 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 1 hr 5 min Public · Anyone on or off Facebook Ready to level up your Sensual Bachata? May 8, 15, 22, 29 Method Studio | 7:55–9:00 PM | $80 for all 4 classes Join us for an exciting and dynamic Bachata Sensual class designed for experienced beginners and intermediate dancers! We’re blending solid fundamentals with fresh, fun, and sensual combos to help you grow, challenge yourself, and have an amazing time on the dance floor. No partner needed — just bring yourself and your love for dance! Spots are limited — don’t miss out! Register by e-transferring $80 to maximumotion@gmail.com and mentioning “Bachata Sensual” in the notes. Get ready to connect, move, and elevate your dancing! P.S. All fees are non-refundable as they go directly toward securing the studio space and running the class. See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1350929566137538/</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 4 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation August 10, 2025 | Lesson: Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/9677364319006080/</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 49 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation July 20, 2025 | Lesson:  Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1069894401564900/</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Monday Nights! 111 Superior St, Victoria, BC V8V 1T2, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion Sensual Bachata Series – Monday Nights! Details 15 people responded Event by Victoria Latin Dance Association 111 Superior St, Victoria, BC V8V 1T2, Canada Duration: 3 hr Public · Anyone on or off Facebook Sensual Bachata Series – Monday Nights! Mondays – April 7th, 14th, 21st &amp; 28th at 111 Superior Street Foundation Class (6:30–7:35 PM) Perfect for absolute beginners or dancers looking to strengthen their foundation! In this class, we’ll break down the essential steps, body movement, and partner connection in a fun environment. You’ll learn the basics with proper technique while also adding styling to make your dancing look and feel smooth on the dance floor. No experience or partner needed—just bring your curiosity and energy! Intermediate Class (7:35–8:40 PM) Ready to level up? This class is designed for dancers who already feel comfortable with the basics and want to challenge themselves. We’ll dive into more fun patterns while also exploring musicality—how to connect those movements to the music in a more expressive way. Get ready to build confidence, fluidity, and your own unique style! To Register: Send your e-transfer to maximumotion@gmail.com and include in the memo: Foundation, Intermediate, or Both + Lead or Follow Class Cancellation &amp; Refunds We understand that plans can change. However, due to limited spots, renting space in advance, and the preparation required for each class, we’re unable to offer refunds for cancellations. Please make sure you’re committed before signing up. We truly appreciate your understanding and support! See less Victoria, British Columbia 111 Superior St, Victoria, BC V8V 1T2, Canada 111 Superior St, Victoria, BC V8V 1T2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1300938064467261/</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Thursday 20 March 2025 from 20:00-22:00 Intermediate Sensual Bachata Workshop Method Studio - Victoria BC About Discussion More About Discussion Intermediate Sensual Bachata Workshop Details 24 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 2 hr Public · Anyone on or off Facebook Sensual Bachata Workshop in March! Intermediate workshop - March 20 Time: 8:00-9:30 PM + Practice 9:30-10:00 PM Location: Method Studio, 841 Fisgard St. Cost: $30 per workshop (includes 2 hours!) Intermediate workshop: Take your skills to a higher level! Master the advanced variations of the Madrid pass, smooth transitions and musicality. No partner needed, just bring your energy and comfortable shoes! Register at: maximumotion@gmail.com #BachataWorkshop #VictoriaBC #LearnToDance #BachataLovers See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3975145332748137/</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Friday 13 June 2025 from 20:00-00:00 Bachata Night Method Studio - Victoria BC About Discussion More About Discussion Bachata Night Interested Going Invite Details 32 people responded Event by Bachata Nights Victoria BC , Sebastian Carmona and Alysha Kopala Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights June 13 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342233713680795/</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Thursday 1 May 2025 at 21:00 Bachata &amp; Merengue- All Levels- May Series Studio 4 Athletics About Discussion More About Discussion Bachata &amp; Merengue- All Levels- May Series Details 3 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Bachata &amp; Merengue are both dances from the Dominican Republic. Bachata can be anywhere from slow and romantic with lots of dips, sway and body movement to more upbeat and percussive with lots of musical footwork. Merengue is carefree, flirtatious and fun! Classes are registered on a monthly basis and take place every Thursday from 8:00- 9:00pm, May 1, 8, 15, 22, 29. No experience required.  No partner is necessary as we rotate partners throughout the lesson.  Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1057471579628015/</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Friday 16 May 2025 at 17:00 Bachata Nights Victoria Bc Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Victoria Bc Details 9 people responded Event by Bachata Nights Victoria BC and Sebastian Carmona Method Studio - Victoria BC Public · Anyone on or off Facebook Join us on our next Bachata Nights May 23 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1901245437276872/</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Friday 9 May 2025 from 20:00-00:00 Bachata Nights Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Details 40 people responded Event by Bachata Nights Victoria BC , Alysha Kopala and Sebastian Carmona Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights May 09 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @yourgirlalysha  and @davidch_78  will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person The evening starts with an Open-level Bachata lesson from 8:15 PM to 9:00 PM—great for all skill levels! Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/717475250956404/</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Friday 30 May 2025 at 18:00 FREE Beginner Bachata Class 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 About Discussion More About Discussion FREE Beginner Bachata Class Details 65 people responded Event by Mayfair Shopping Centre and Victoria Latin Dance Association 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 Public · Anyone on or off Facebook Ready to get your groove on? We’re teaming up with the Victoria Latin Dance Association  for a FREE Beginner Bachata Class right here at Centre Court! Join us on Friday, May 30 at 6:00 PM for an evening of fun and dancing. FREE Beginner Bachata Class May 30th, Friday at 6PM NO partner or experience necessary! Bachata is a beautiful and easy-to-learn dance that’s great for meeting new people, getting active, and connecting with an amazing community. See less Dance Victoria, British Columbia 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 3147 Douglas St, Victoria, BC V8Z 3K3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C34" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/692165093260868/</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 13:00-16:00 Salsa &amp; Bachata Masterclass with Adam &amp; Ghada Solwood Studio About Discussion More About Discussion Salsa &amp; Bachata Masterclass with Adam &amp; Ghada🔥 Details 60 people responded Event by Dancing Time Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook Hello everyone! Spring is here, and many things are happening, but I can’t but dance with you one last time before leaving for the entire summer!! To make things spicy, I am extremely happy to collaborate with Adam on a Salsa &amp; Bachata Masterclass! Get ready to learn details that will help you with creating flow – both as leads and follows – in addition to some socials-friendly tricks! Date: Saturday, May 10 Time: 1:00-2:30 | Salsa, 2:30-4:00 | Bachata Price: 25$ for one class, 35$ for two classes Location: Solwood studio, 1303 Broad st To register, please fill in this quick form and send an e-transfer to ghadacyoussef@gmail.com. https://forms.gle/4QThxT6yByd3h5KH8 Note: kindly understand that no-shows and cancellations made in less than 1 week from the workshop cannot be refunded. I will be happy to fully refund for earlier cancellations if need be. See less Victoria, British Columbia Solwood Studio Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1388695712154512/</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 65 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation June 22, 2025 | Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342792743590871/</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Monday 7 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- April series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, April 7, 14, 28. Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/966455485665576/</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Thursday 3 April 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- April series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Apr 1, 8, 15, 22, 29 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/10048344358532607/</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- May series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. May 6, 13, 20, 27 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/669591372187091/</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 10:00-11:00 Salsa &amp; ChaCha Solo Westshore Dance Studios Sat, 17 May Sat, 24 May Sat, 31 May +7 About Discussion More About Discussion Salsa &amp; ChaCha Solo Details 2 people responded Event by Dance Praktika Westshore Dance Studios Duration: 1 hr Public · Anyone on or off Facebook Elevate your dance journey with our Ladies Solo Class. Join our exciting series and learn the basics of Salsa and Cha Cha. Perfect for beginners looking to spice up their dance skills! Class Highlights: - Learn exciting dance moves tailored for solo dancers; - Fun and welcoming environment; - Suitable for absolute beginners. Come dance with us and let the rhythm guide you! To register to April classes please use links at "Tickets". See less Langford, British Columbia Westshore Dance Studios 109-2675 Wilfert Road, Victoria www.westshoredance.com 2years+ Competitive&amp;Production a space for everyone with a love of dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2214494908966327/</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Monday 5 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Int/ Adv- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- May series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, May 5, 12, 26 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/679241811720932/</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Fundamentals- May Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- May Series Details 7 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, May 6, 13, 20, 27 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C42" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1298465587898458/</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Tuesday 4 March 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- March series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- March series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Mar 4, 11, 18, 25 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1382188962971661/</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Tuesday 1 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Fundamentals- April Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- April Series Details 9 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, Apr 1, 8, 15, 22, 29 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2233725973712106/</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Monday 3 March 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- March series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- March series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, Mar 3, 10, 17, 24, 31 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/884101187183426/</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 July 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in June. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Veronica, Ali and 5 friends are interested 940 people interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends 33 people interested Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 7 friends 199 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/909522138040202/</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Friday 28 November 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 7 friends 199 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 41 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 65 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1239163193996279/</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 14 Saturday 14 June 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Tickets · CA$17.31 www.eventbrite.com/e/caliente-salsa-saturdays-tickets-1390062838369 Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in May. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Tickets Find Tickets Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 49 people interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Veronica, Ali and 5 friends are interested 940 people interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends 33 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1636237610432412/</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Saturday 16 August 2025 from 20:00-23:59 Salsa Sunset Latin Party – August 16th! Latin Dance Canada About Discussion More About Discussion 🌅🔥 Salsa Sunset Latin Party – August 16th! 🔥🌅 Interested Going Invite Details 29 people responded Event by Latin Dance Canada Latin Dance Canada Duration: 3 hr 59 min Public · Anyone on or off Facebook Salsa Sunset Latin Party – August 16th! Get ready for a magical summer night filled with Latin rhythms, sunset vibes, and non-stop dancing! Join us for the Salsa Sunset Latin Party, where the Salsa, Bachata, and Merengue beats will keep you moving all night long under the stunning sunset sky! Dress Code: Wear your best sunset-inspired outfit – think bright, tropical colors, and beach party vibes! Dance to the best Salsa, Bachata, Merengue &amp; Latin hits all night! No partner? No problem! Join our fun intro class at 8:00 PM! Location: Ukrainian Cultural Centre, 3277 Douglas St., Victoria, BC Date: Saturday, August 16, 2025 Intro Class: 8:00 PM | Social Dance: 8:30 PM - Late Entry: $15 at the door – Bring cash, please! What to Expect: Vibrant salsa rhythms &amp; tropical vibes! Tropical-themed decorations &amp; stunning sunset views! A welcoming dance community &amp; unforgettable fun! Let’s dance as the sun sets and make it a night to remember! Tag your friends and let’s create memories under the summer sky! #SalsaSunsetLatinParty #SalsaBachata #LatinDanceParty #VictoriaBC #LatinDanceCanada See less Dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C49" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1059622278965884/</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 8 Saturday 8 November 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in October. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 175 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 65 people interested Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 5 friends 149 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/624858640069610/</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 Friday 22 August 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 7 friends 199 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 41 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 65 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3899920353641309/</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 9 Saturday 9 August 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in July. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 175 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 49 people interested Interested Mon, 30 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne and Ali 15 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C52" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1624603351798270/</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 April 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 175 people interested Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 7 friends 199 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 65 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C53" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2251848171850840/</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 Saturday 10 May 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in April. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 175 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 49 people interested Interested Mon, 4 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Ali 3 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C54" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/939376108286434/</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Friday 27 June 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 7 friends 199 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 65 people interested Interested This Saturday at 21:00 Goth Nite: UNDERGROUND Victoria, BC, Canada, British Columbia 172 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C55" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/530862806349067/</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Sunday 30 March 2025 from 13:00-17:00 Salsa Gonzales tasting! 🍋‍🟩 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia About Discussion More About Discussion Salsa Gonzales tasting! 🍋‍🟩 Details 6 people responded Event by THE ROOT CELLAR | village green grocer 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia Duration: 4 hr Public · Anyone on or off Facebook Hey friends! It's time to get those tastebuds tingling - you're invited to come and join us for a Salsa Gonzales tasting at our McKenzie Corner store! Salsa Gonzales is a little condiment company with a big personality! Nestled on Gonzales Beach in Victoria, they craft salsas, hot sauces, pickles, preserves, and more – all with a generous splash of love and a fiery kick. When: Sunday March 30th, 1pm-5pm Where: Our McKenzie Corner location We're looking forward to seeing you there! XO See less Victoria, British Columbia 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia 1286 McKenzie Ave, Saanich, BC V8P 5P2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C56" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1618420955545842/</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 30 Friday 30 May 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing at an all ages venue with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 7 friends 199 people interested Interested Mon, 14 Jul at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Ali is going 2 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 41 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C57" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1106484714432492/</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Wednesday from 18:30-21:00 Zouk practica and social White Eagle Hall, 90 Dock St, Victoria BC Wed, 21 May Wed, 28 May Wed, 4 Jun Wed, 11 Jun +29 About Discussion More About Discussion Zouk practica and social Interested Going Invite Details 2 people responded Event by Victoria Zouk Collective and Victoria Zouk Collective Group White Eagle Hall, 90 Dock St, Victoria BC Duration: 2 hr 30 min Public · Anyone on or off Facebook Drop-in zouk practica by donation - everyone welcome! White Eagle Polish Hall every Wednesday 6:30-9 pm Shared warm up, free dance time, review material from lessons and congresses, connect and share knowledge! Help is always available. Minimum $5 donation. Cash at the door, or etransfer to oceanzouk@gmail.com Enter the lower hall by the side door on Niagara Street just beside the Polka food truck. Also available in Victoria are zouk lessons with Javi, an amazing instructor from Vancouver! More info at https://www.facebook.com/Sabor.Asi.Dance.Salsa.Victoria or email danceinflow@gmail.com See you there! See less Victoria, British Columbia White Eagle Hall, 90 Dock St, Victoria BC 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C58" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1411005319893067/</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Monday 28 April 2025 from 18:30-22:30 Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion 🔥Bachata &amp; Brazilian Zouk 🌊 dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard Details 7 people responded Event by Bachata and Zouk with Javi in Victoria 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 4 hr Public · Anyone on or off Facebook Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard street | Victoria Join us for a 4 week course exploring the joy and magic of Brazilian Zouk &amp; Bachata dancing! Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on enhancing body awareness, building confidence in dance vocabulary with lead and follow techniques, exploring musicality, and loving yourself deeper with styling! Be prepared to have lots of fun dancing with new friends! Register today! Schedule: Monday April 7 - 28th 6:30-7:25pm | Brazilian Zouk - Level 2 (ask Javi for permission) 7:30-8:25pm | Brazilian Zouk - Level 1 8:30-9:25pm | Sensual Bachata - Beginner Foundations 9:30-10:30pm | Sensual Bachata - Intermediate "Trending Moves" Tuition: $20 | 1 Class $35 | 2 Classes (Brazilian Zouk 1&amp;2, or Brazilian Zouk 1 &amp; Bachata, Bachata 1&amp;2) $50| 3 Classes (3 classes, BEST value) 1709 Blanshard St, Victoria, BC Registration: E-transfer to: danceinflow@gmail.com or send us a message on Whatsapp: 7785877665 (Also accepting credit card/cash at the door) Please add a note if you're registering as a "Leader", "Follower", or "Open to both" Space is limited. Register in advance to reserve your spot! Looking fwd to dancing and flowing with you, Warmly, Javi See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C59" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1356293392177099/</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Monday 3 March 2025 from 18:30-21:30 Open House | FREE Classes - Bachata Sensual &amp; Brazilian Zouk 1709 Blanshard St, Victoria, BC V8W 2J8, Canada About Discussion More About Discussion Open House | FREE Classes - Bachata Sensual &amp; Brazilian Zouk Details 28 people responded Event by Bachata and Zouk with Javi in Victoria and Javi Zouker 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 3 hr Public · Anyone on or off Facebook Join us for our Open House / Free classes on Monday March 3rd with Javi Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on body awareness, lead and follow techniques, musicality, styling, and how to have lots of fun dancing with new friends!  Learn with Javi, with over ten Years of teaching experience.  Learn dance with clear, fun, and inspiring teachings open to all levels! Schedule: Monday March 3rd 6:30-6:45pm | Meet &amp; Greet 6:45-7:30pm | Traditional Bachata - Beginner 7:40-8:25pm | Sensual Bachata - Intermediate 8:35-9:20pm | Brazilian Zouk - Beginner 9:20-9:30pm | Sharing circle Tuition = FREE Space is Limited:  Please email us to register your spot and please share if you are leading or following or open to either. email:  danceinflow@gmail.com 4 week session on Monday March 10-31st Phillippine Bayanihan Community Centre - 1709 Blanshard st, Victoria, BC See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C60" s="3" t="n">
+        <v>45810.93691175926</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/544121845403419/</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 13:00-23:55 Swing Session: Balboa with Yoshi and Etsuko Solwood Studio About Discussion More About Discussion Swing Session: Balboa with Yoshi and Etsuko Details 108 people responded Event by Swing Dance Association of Victoria , Dave Henderson and 2 others Solwood Studio Duration: 10 hr 55 min Public · Anyone on or off Facebook Lace up your shoes on May 31, 2025 for an afternoon of Balboa Classes and an evening of Social Dancing with Yoshi and Etsuko Uemura. 4 Classes for everyone &amp; 1 Social Dance! Passes go on sale April 19 at noon at our SDAV Square Shop! You must know and be comfortable with Balboa basics for all of these classes - they won't be covered at this workshop. All the specifics are available at swingvictoria.net , but here are the notes: May 31st, at Solwood Studio, with doors at 12:30pm . Bring indoor shoes, please! 4 classes for everyone and there's a dance from 9-12am. Passes go on sale April 19th at noon. See less Victoria, British Columbia Solwood Studio 1303 Broad St, Victoria, BC V8W 2A8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C61" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/634773653668605/</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Saturday Night West Coast Swing BC Swing Dance Club Victoria 15 Jun 2019 22 Jun 2019 29 Jun 2019 +2 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night West Coast Swing Details 9 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook June means summertime and sunny days! Along with the weather, things for BC Swing Dance Cub Victoria will be changing too. Here's what is happening this month: 7 - 8pm 1st Saturday of the Month: Lesson with Meaghan, plus an assistant from our dance community 7 - 8pm Remaining Saturdays each month: TBD (stay tuned for workshops, activities or practices - updates will be posted on each event page) Note:  The 7 - 8pm weekly timeslot is included in the dance entrance price. -------------------------------------------------- Come join us every Saturday all year long for a fabulous WCS social dance from 8 - 11pm. Just $10 for the ($5 for students). Meaghan Efford and Bob Gebbie 's lesson on June 1st (starting PROMPTLY at 7pm) will be the only lesson in June, and it will be a great way to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity.  The lesson is included in the dance entrance price.  No experience or partner is required. -------------------------------------------------- • 6:45 pm - Doors open • 7:00 pm - TBD each week* • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *lesson with Meaghan and Bob on June 1st Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C62" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1035925295253912/</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Friday 18 April 2025 at 18:30 Swing out with the ATOMIC COCKTAILS 751 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Swing out with the ATOMIC COCKTAILS Details 64 people responded Event by Peter Sandmark 751 View St, Victoria, BC V8W 1J9, Canada Public · Anyone on or off Facebook Join the ATOMIC COCKTAILS as they swing out for their pre-Japan Tour dance party on April 18 at the Coda, 751 View Street.  Doors open 6 pn, show from 6:30-8:30 pm!  Tickets $20.  With songs from their new album BLUE LIGHT BOOGIE! See less Victoria, British Columbia 751 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C63" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1776457206589544/</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Friday 21 March 2025 from 18:30-20:30 Slim Sandy's Atomic Cocktails swing speakeasy party! The Coda About Discussion More About Discussion Slim Sandy's Atomic Cocktails swing speakeasy party! Details 72 people responded Event by Peter Sandmark and Trace Nelson The Coda Duration: 2 hr Public · Anyone on or off Facebook Join Slim Sandy's Atomic Cocktails and dance as they play 2 sets of swing jazz, jive and rhythm and blues from the 20’s to the 40’s. Slim, on guitar and harmonica, is joined by Willa Mae on vocals, “Big Daddy Bo” on bass, and Bryn Bad on trumpet.  Slim Sandy has been playing music for over 40 years with acts such as Ray Condo and the Crazy Rhythm Daddies.  In 2012, he and Willa Mae co-created the Slim Sandy band in Victoria!  They have played music festivals in Canada, France, Spain, Germany, Belgium, and the Netherlands.  In May they will be touring in Japan! See less Victoria, British Columbia The Coda 749 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C64" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/302778660295534/</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Sunday 19 August 2018 from 18:00-21:00 West Coast Swing in the Park! Cameron Bandshell @ Beacon Hill Park Carolyn Gebbie invited you About Discussion More About Discussion West Coast Swing in the Park! Details 58 people responded Event by Carolyn Gebbie Cameron Bandshell @ Beacon Hill Park Duration: 3 hr Public · Anyone on or off Facebook Come join us for another evening of fun and WCS dancing in Beacon Hill Park! WCS music will be provided by DJ Carolyn. For those who are familiar with the routine, the 2018 WCS Rally Song will be played at 6:30, 7:30 and 8:30pm. Sam Jackson and Meaghan Efford, from wcsmovementmethods.com will be on hand to answer questions about WCS or how to improve your WCS dancing. They will also demo some incredible WCS dancing at 7pm. Please invite your WCS dance friends by sharing this event! See less Victoria, British Columbia Cameron Bandshell @ Beacon Hill Park Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C65" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/373500473108499/</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Sunday Swing at Logan's Logan's Pub 10 Dec 2017 Debi Wong invited you About Discussion More About Discussion Sunday Swing at Logan's Details Event by Swing X Logan's Pub Duration: 3 hr 30 min Public · Anyone on or off Facebook Sunday Swing at Logan's is BACK! Come join us for some great tunes and we'll party like it's 1939. Bring your dancing shoes, sweet moves, and a few dollars for our fabulous DJ (and gracious bartenders). Feel free to come early to hang out and grab a bite to eat. 19+. NEW: Crash course 15min swing lesson at 8:30pm! This is intended to be the bare minimum for someone to show up and know the basics of swing dancing, nothing fancy! DETAILS: * 8:30pm Quickie 15min beginner lesson! * 8:45pm social dancing until as late as midnight (maybe!) * Usually gets bluesy after 11pm See less Victoria, British Columbia Logan's Pub 1821 Cook Street, Victoria Original - Authentic - Unique Guests See All</t>
+        </is>
+      </c>
+      <c r="C66" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663756533046485/</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Friday 11 April 2025 at 21:30 Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. Details 36 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Public · Anyone on or off Facebook Miguelito Valdes presents Contodo What happens when you bring together three Cuban and two Canadian musicians, with a deep love of all music and a wide range of musical experiences?  A joyful mix of party and deep groove, that's what! Guaranteed to make you want to dance, these brothers from other mothers bring it all. Con Todo! Featuring: Miguelito Valdes – brass/vocals/percussion Jose Sanchez – drumset/timbales Hector Ramos – congas/percussion Peter Dowse - bass Brooke Maxwell – keys/vocals See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C67" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663135653237580/</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Method Studio - Victoria BC Canice Ma invited you Interested Going About Discussion More About Discussion WACK! Another West Coast Swing Social Dance Invite Details 36 people responded Event by Canice Ma and Wyatt Ritchie Method Studio - Victoria BC Duration: 3 hr 30 min Public · Anyone on or off Facebook Guess who's back, it's WACK! (please ignore the fact that it's been 2 years...) The schmucks are back with another spontaneous west coast swing social dance, featuring music by DJs Topknot and Amandance from Vancouver! DETAILS: • Friday, June 20th, 2025 • Method Studio, 841 Fisgard St, Victoria, BC • 7:30-11 pm: social dancing with 100% west coast swing (sorry, no lesson!) • Admission: $10 • Water and AC on us (and maybe some bonus chocolate) • Please keep in mind that parking is limited at the venue GENERAL SOCIAL DANCE ETIQUETTE: • Consent is cool- don't be creepy. • Shake off any shyness and get out there! Ask people to dance regardless if you’re a lead or follow, dancing for 10 years or started yesterday- it's more fun that way! • No teaching or unsolicited feedback on the dance floor. Good vibes only! • If you would like to partake in a steal dance, try to remain with that group for the whole song. • Bring a water bottle! The studio is known to get warm with more bodies in the space so we want you to stay healthy and hydrated. • Personal hygiene is important! Consider bringing a towel and/or a spare shirt to change into if you sweat easily. Our studio has a bathroom and change rooms available for all to use. • We recommend wearing clothes that are easy to move in, especially pants given the nature of the dance. • Clean, comfortable shoes (ideally dance shoes) on the dance floor only! See less Victoria, British Columbia Method Studio - Victoria BC 833 Fisgard St, Victoria, BC V8W 1R9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C68" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1692156731689650/</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 3 Tomorrow from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 Tue, 20 May Tue, 27 May Tue, 3 Jun Tue, 17 Jun +22 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Interested Going Invite Details 2 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Saanich, BC V8Z 3S3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C69" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/417338985546213/</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Thursday 29 August 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - August 29! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - August 29! Details 109 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for a fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C70" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2441697862726705/</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Sunday 30 June 2019 at 19:00 Journey’s 50th Birthday!!  A West Coast Swing dance party!! Eastern Star Hall Chapters No 5 &amp; No 17 Journeey Song invited you About Discussion More About Discussion Journey’s 50th Birthday!!  A West Coast Swing dance party!! Details 13 people responded Event by Journeey Song Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook 3281 Harriet Road, Victoria,BC Bring your own alcohol-free beverage... Bring a gluten-free appie if you’d like. Dance West Coast Swing until 10 pm to Blues, Pop, RnB, Swing, and a wee bit of Ballroom Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C71" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/402729737034904/</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Thursday 5 September 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Details 123 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for our second fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C72" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1594011994641933/</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Tuesday 22 April 2025 from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Details 9 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. No street shoes. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C73" s="3" t="n">
+        <v>45810.94217068287</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1766891834185825/</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Interested Going Invite Details 34 people responded Event by Jeannie Kam and Alive Tango Victoria Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends SAVE THE DATE! The next Sunday afternoon Milonga is on 8 June 2025 1-4pm. The Coda Club (formerly Hermanns Upstairs) is a beautiful newly renovated venue with awesome ambience, nice wood floor and great sound system. Come join us for a wonderful afternoon of warm hugs and close embrace. Sunday 8June 2025 1-4pm The Coda, 751 View Street, Victoria Admission: $15 (plus tax) Special Guest DJ: Francis Nowaczynski (from Vancouver) Free parking at View Street Parkade (next door) or Broughton Parkade. Cash bar is open for drinks. See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C74" s="3" t="n">
+        <v>45810.94507917824</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/713923214640962/</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Sunday 4 May 2025 from 13:00-16:00 May 4th Afternoon Milonga Solwood Studio About Discussion More About Discussion May 4th Afternoon Milonga Details 45 people responded Event by Ingrid Love and Kathryn Stone Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook A one-time special afternoon milonga! Join us in celebrating the warmth of Spring and return to sunshine. Or, star wars, if you like. Featuring special guests Kimberly and Khang performing live music (violin/guitar) DJ Ingrid Hosts: Kathryn &amp; Ingrid $15 entry (cash only) 1:00pm-4:00pm Solwood Studio 1303 Broad St Victoria, BC See less Victoria, British Columbia Solwood Studio Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C75" s="3" t="n">
+        <v>45810.94507917824</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/644050564927019/</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends! A NEW SUNDAY AFTERNOON MILONGA! This is the first of a regular monthly milonga at a beautiful new venue…The Coda Club (formerly Hermann’s Upstairs) at 751 View Street, Victoria. Great ambience, nice wood floor, good sound system. So come join us for the warm hugs and close embrace and dance to the beautiful music of our very own DJ John Dewhirst. Sunday, 6 April 2025 2.00pm-5.00pm The Coda Club, 751 View Street, Victoria Admission $15 DJ: John Dewhirst Cash Bar is open for drinks Free Parking at View Street Parkade just next door Come celebrate this exciting day with us! See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C76" s="3" t="n">
+        <v>45810.94507917824</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1318668532737609/</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 16 16 Apr at 18:30 – 18 Apr at 21:00 Tango week with Lya Alive Tango Victoria About Discussion More About Discussion Tango week with Lya Details 36 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 3 days Public · Anyone on or off Facebook Ignite Your Tango 16th of April, Wednesday 6:30-8:00 On &amp; Off Acis for social dance 18th of April, Friday 6:00 - 7:30 Follower technique 7:45 - 9:00 Switch role / connection Search - Grow &amp; Transform! Seminar series for Tango Dancers that want to transform their way of moving and connecting! We will travel through the Essentials of Tango in order to look for new answers and deeper understanding. What makes tango truly captivating? It’s the embrace, the connection, and the walk. These three fundamental elements are the heartbeat of tango, and mastering them is essential for creating an unforgettable dance experience. You will learn how to condition your body to move with control, fluidity, and elegance. You’ll discover how to find and perfect your axis, which is essential for maintaining balance and stability in every step. We will also explore dissociation, a technique that allows you to move the upper and lower body independently but associated. This workshop series will show you how to apply these principles in both the leader and follower roles, improving connection and response in every moment of the dance. We will apply all this to: The secrets to generating power for boleos effortlessly off and on axis special follower technique class Pro tips to dance with ease and confidence 90 min class - $30 All 3 classes - $80 To register email grazs@shaw.ca or pm me, or talk to me . See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C77" s="3" t="n">
+        <v>45810.94507917824</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1864555154338100/</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 21 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Alive Tango Victoria About Discussion More About Discussion Weekend with Tango Interested Going Invite Details 8 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 21st 5pm-6pm solo technique all levels. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) We will continue from May with the musicality for phrase change but this time we will add “double time” to help us with it, using examples of different orchestras. We will work with a “rebound” and half giros to change the direction within the phrase. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 22nd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are September 20th &amp; 21st. Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C78" s="3" t="n">
+        <v>45810.94507917824</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1838888640215250/</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Friday 28 February 2025 at 19:00 Argentine Tango for Beginner - level 2 1303 Broad St, Victoria, BC V8W 2A8, Canada About Discussion More About Discussion Argentine Tango for Beginner - level 2 Details 19 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria 1303 Broad St, Victoria, BC V8W 2A8, Canada Public · Anyone on or off Facebook We are happy to announce that we continue with Argentinian Tango for Beginners - level 2. This 6 weeks session is progressive and requires preregistration. It is designed for students who have completed Beginner - level 1 or would like to deepen their skills. If not sure where you are with your tango contact us To register email us : grazs@shaw.ca or PM Grazyna Feb 28th - April 4th Fridays 7-8pm Price per person : $80 series (6 weeks) See less Victoria, British Columbia 1303 Broad St, Victoria, BC V8W 2A8, Canada 1303 Broad St, Victoria, BC V8W 2A8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C79" s="3" t="n">
+        <v>45810.94507917824</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1146571100253242/</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 22 Feb at 17:00 – 23 Feb at 13:30 Weekend with Tango Alive Tango Victoria About Discussion More About Discussion Weekend with Tango Details 27 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 22nd 5pm-6pm solo technique all levels. Balance and weight transfer while walking, change of dynamics to create a better connection with your body. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) Fundamentals of giros! We will look for the right moments for sacadas, barridas and adornos without affecting the partner's axis in elastic hugs of closed embrace. 8pm milonga !!! .. and Jorge’s BIRTHDAY !! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 23rd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons are full. March workshop dates are the 22nd&amp;23th Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C80" s="3" t="n">
+        <v>45810.94507917824</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3637725693193744/</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 22 Mar at 17:00 – 23 Mar at 13:30 Weekend with Tango with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Weekend with Tango with Jorge Olguín Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 22nd 5pm-6pm solo technique all levels. Balance and weight transfer while walking, change of dynamics to create a better connection with your body. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) Marathon is just around the corner so this month we continue with comfortable close embrace! We continue with dancing in small spaces!! Let’s move gracefully without affecting the partner's axis in elastic hugs of closed embrace. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 23rd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available only on Saturday. Sunday - sold out Next workshop dates are the May 17th &amp;18th Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C81" s="3" t="n">
+        <v>45810.94507917824</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1009684807956058/</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 17 17 May at 17:00 – 18 May at 13:30 Tango weekend with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Tango weekend with Jorge Olguín Details 28 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 17th 5pm-6pm solo technique all levels. ( no partner required) Please bring elastic bands!! 6.30pm-7.30pm for couples only ( need some experience) Sacadas, barridas and colgadas in an elastic embrace in order to create a circular movement. We will work with different orchestras to study the changes we need to do to introduce different tempos and rhythms. Get ready for a workout with musicality! 8pm milonga !!! Join us even if you didn’t take the classes. DJ Ingrid !! Free for people registered for the workshops. $10 for drop-ins. Sunday, 18th 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are June 21st &amp; 22nd Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C82" s="3" t="n">
+        <v>45810.94507917824</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1225266505917189/</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Saturday Beginner Lesson and Social Dancing Dance Victoria Sat, 7 Jun Sat, 14 Jun Sat, 21 Jun +4 About Discussion More About Discussion Victoria WCS Collective hosts Saturday Beginner Lesson and Social Dancing Interested Going Invite Details 1 person responded Event by Donna Forsyth Dance Victoria Duration: 3 hr 30 min Public · Anyone on or off Facebook Back to AIR CONDITIONED comfort at Dance Victoria Studios Beginner lesson from 7 to 8 pm Social dancing  from 8 to 10:15 pm Cost $15/$12 for students No need to register and no need for previous dance experience or a partner. Please bring scuff-free inside low-heeled dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C83" s="3" t="n">
+        <v>45810.94752665509</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2162855673833831/</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 11 May 2019 18 May 2019 25 May 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 8 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook Wow! April went by so quickly, which means it must've been super fun, which it definitely was.  Everyone at BC Swing Dance Club Victoria is so pleased with the way the first month of social dances went, and we hope to generate the same amount of enthusiasm in May. Let's make this month just as much fun! Come join us on May 4th for the first intro lesson and social dance of the month (plus every Saturday night after that). Just $10 for the lesson and/or social dance ($5 for students). No experience or partner required. • 6:45 pm - Doors open • 7:00 pm - Intro lesson with Sam Jackson and Meaghan Efford * • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *PLEASE NOTE that the weekly lessons will start PROMPTLY at 7pm.  It is disruptive to the flow of the lesson if participants arrive late. For anyone who's interested in building their West Coast Swing fundamentals quickly, note that May will be the last month we'll be offering weekly classes with both Sam and Meaghan. With summer approaching it's a great time to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity. Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C84" s="3" t="n">
+        <v>45810.94752665509</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/641769172035949/</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Saturday April 12 Beginner lesson and social dance at Dance Victoria Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 12 Beginner lesson and social dance at Dance Victoria Details 5 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginners lesson by Donna from 7 to 8 pm Social dancing from 8 to 10:15 pm DJs Andre and Nel Cost $15 /$12 for Students No need to register and no partner required. Please bring scuff-free inside dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C85" s="3" t="n">
+        <v>45810.94752665509</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/516994561244886/</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:45 Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING White Eagle Polish Association About Discussion More About Discussion Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING Details 15 people responded Event by Donna Forsyth , Andre Russo and Victoria West Coast Swing Collective White Eagle Polish Association Public · Anyone on or off Facebook Doors open at 6:45pm at this fabulous new venue! Advanced beginner/intermediate lesson by Chantelle Pianetta from 7 to 8 pm Social dancing for 3 HOURS from 8 to 11 pm DJs Donna and Andre Cost $15 /$12 for students ALL at the spacious White Eagle Hall No need to register and you do not need a dance partner. Please bring scuff-free dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia White Eagle Polish Association 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C86" s="3" t="n">
+        <v>45810.94752665509</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1024182725709172/</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Saturday April 19th Lesson and Social Dance Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 19th Lesson and Social Dance Details 4 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginner plus lesson with Pamela Podmoroff from 8 to 10:15 pm Social dancing from 8 to 10:15 pm DJs Donna and Amanda Cost $15/ $12 for students No need to register and no partner required. Please bring scuff-free indoor dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C87" s="3" t="n">
+        <v>45810.94752665509</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2238975779474166/</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 13 Apr 2019 20 Apr 2019 27 Apr 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 23 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook A new month, a new social! Come and join in on the fun at our inaugural Saturday night dance and intro lesson on April 6 (and every Saturday night after that)! Just $10 for the Lesson and/or Social ($5 for Students). No experience or partner required. • 6:45 pm – Doors open • 7:00 pm – Beginner Lesson with Sam and Meaghan (this is perfect as a refresher class too!) • 8:00 – 11:00 pm Social Dancing featuring DJ Carolyn Please note the NEW START TIMES for the BC Swing Victoria Saturday night dances. See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C88" s="3" t="n">
+        <v>45810.94752665509</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1366072544640156/</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Saturday 17 May 2025 at 18:45 Victoria WCS Collective Beginner Lesson and Social Dancing Dance Victoria About Discussion More About Discussion Victoria WCS Collective Beginner Lesson and Social Dancing Details 9 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson from 7 to 8 pm by John de Pfyffer Social dancing from 8 to 10:15pm DJg by Donna and Nel Cost $15/ $12 for students No need to register and no need for dance experience.. Also, no partner necessary, we got you! Please bring indoor scuff-free dance shoes or socks to dance in. See less Victoria, British Columbia Dance Victoria 2750 Quadra St # 111, Victoria Dance Victoria brings the "World's Best Dance" to the Royal Theatre and supports new dance creation for the international stage from its studios. Guests See All</t>
+        </is>
+      </c>
+      <c r="C89" s="3" t="n">
+        <v>45810.94752665509</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/967438905456066/</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Wednesday 26 March 2025 at 10:00 Victoria WCS Lesson and Dance at Eastern Star Hall Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria WCS Lesson and Dance at Eastern Star Hall Details 1 person responded Event by Donna Forsyth Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson by John de Pyffer from 7 to 8 pm Social dancing from 8 to 10:15pm Djs Amanda and Nel Cost $12 No need to register and no partner required. Please bring scuff-free indoor shoes or socks to dance in  and a water bottle. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C90" s="3" t="n">
+        <v>45810.94752665509</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1142760357225336/</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 26 26 Jul at 10:00 – 27 Jul at 17:00 ArtisTREE Festival 1401 rockland ave, Victoria, BC, Canada About Discussion More About Discussion ArtisTREE Festival Interested Going Invite Details 982 people responded Event by Artistree Festival , MORENA CLOTHING and Cory Judge 1401 rockland ave, Victoria, BC, Canada Duration: 2 days Public · Anyone on or off Facebook Saturday July 26 10-7pm Sunday July 27 10-5pm Government House of BC 1402 Rockland Ave Celebration of Creativity profiling 130 Juried Artisans, Live Music, Installation and Performance Art, Indigenous Makers and Traditions, Kids section, Live Painters, Delicious Food and Ice cream. See less Shopping Victoria, British Columbia 1401 rockland ave, Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C91" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1399479741193649/</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Saxe Point Public House About Discussion More About Discussion TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Details 4 people responded Event by Tom Watson Saxe Point Public House Public · Anyone on or off Facebook Join Vinyl Wave at the lovely Saxe Point Pub for a couple of hours of smooth tunes that'll help ease you into the week! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C92" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1217747446718881/</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 18:00-22:00 Maifest - Evening of Live Music Edelweiss Club About Discussion More About Discussion Maifest - Evening of Live Music Details 36 people responded Event by Cindy Kent and Victoria Edelweiss Club Edelweiss Club Duration: 4 hr Public · Anyone on or off Facebook Join the Edelweiss Club for a lively evening of music and dance with Bijoux du Bayou and The Helen Davies Band. Let the infectious Zydeco beats and soulful rhythms set the tone for a night of fun, complete with delicious German snacks from the kitchen. Don’t miss out on this high-energy event! Get your tickets online or call 250-383-4823. www.victoriaedelweiss.ca/events See less Victoria, British Columbia Edelweiss Club 108 Niagara Street, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C93" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/651664851189740/</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 12:00-18:00 Music in the Orchard (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Music in the Orchard (RAIN OR SHINE) Interested Going Invite Details 137 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Come enjoy the start of the summer in the orchard. We have two amazing artists for you, some delicious fun summer ciders for you to try and amazing food to enjoy to complete the experience. Delicious Cider Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀ Beautiful location ⠀⠀⠀⠀ Dog Friendly ⠀⠀ ⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your WELL BEHAVED two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C94" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/979769967649565/</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 15:00-18:00 Live Music at the Legion 102-622 Admirals Rd, V9A 2N7 Sat, 17 May Sat, 24 May Sat, 31 May +2 About Discussion More About Discussion Live Music at the Legion Details 8 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Come enjoy live music on Saturdays 3-6 p. Dancing encouraged! Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C95" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/4223643791110348/</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Sunday 22 June 2025 at 13:00 Victoria Italian Day 195 Bay St, Victoria, BC V9A 3K4, Canada About Discussion More About Discussion Victoria Italian Day Interested Going Invite Details 3 people responded Event by Calabrisella 195 Bay St, Victoria, BC V9A 3K4, Canada Public · Anyone on or off Facebook Join us for live music, food, gelato, games, cars, cultural exhibits, vendors, bike valets and much more - Free admission !! Victoria, British Columbia 195 Bay St, Victoria, BC V9A 3K4, Canada 195 Bay St, Victoria, BC V9A 3K4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C96" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3513597908934465/</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Saturday 12 April 2025 from 12:00-20:00 Live Music Benefit Event for Veteran's House 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion Live Music Benefit Event for Veteran's House Details 34 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 8 hr Public · Anyone on or off Facebook Admission by Donation (Non-Perishable Food Items, Charitable Donations, Gift Cards, accepted). Enjoy live music throughout the day by Bryce Allan, Love Cats, OTR, Donny Peterson &amp; the Tone Rangers, Helen Davies, and David Carl Trio. See less Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C97" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/686146924271113/</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>(20+) Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 2 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 5 Thursday from 19:00-22:00 Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz 753 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz Interested Going Invite Details Event by Adonis Puentes and Brent Jarvis 753 View St, Victoria, BC V8W 1J9, Canada Tickets hermannsjazz.com/reservations&amp;event_id=741898 Public · Anyone on or off Facebook An evening of Jazzy Cuban Fusion Music; traditional, contemporary, romance and dance. Juno &amp; Grammy Nominated vocalist, Adonis Puentes, will be joined by the Jazz Bohemians, featuring Brent Jarvis (piano), Ken Lister (bass), Nicholas Marquez (percussion) and Brooke Maxwell (Sax). Adonis Puentes opens up the marvelous world of Cuban music to his audience the second they hear his rich voice. When the other players kick in with their tight, multi-layered arrangements, it becomes clear that Adonis is a powerful bandleader. Fronting an acoustic band, Adonis' vocals are surrounded by piano, bass, strings, and percussion. Music reflects the present and Adonis Puentes is a Cuban Sonero for our times. Adonis thrives on the growth and acclaim for his original sonero sound. As he puts it, "I feel like a messenger of my roots and tradition, blessed that with me I have taken my music and heritage to many different places in the world; from Cuba, to Canada, USA, Mexico, Europe and Asia. My mission is to make you dance and enjoy my melodies and rhythms." Musician Line-Up: Adonis Puentes - Vocals Brent Jarvis - Piano Ken Lister - Bass Nicolas Marquez - Percussion Brooke Maxwell - Sax See less Music and audio Victoria, British Columbia Tickets Find Tickets 753 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Meet your hosts Adonis Puentes 33 past events · Page · Musician/band Adonis Puentes is a great singer and an elegant composer and lyricist grounded and nourished by his Cuban roots and worldly experience. Message Brent Jarvis 37 past events · Profile · Musician Message Suggested events Wed, 18 Jun at 16:00 Victoria Ska &amp; Reggae Fest Kickoff: Waahli, The Resignators, Hezron, Gun Street Ghouls &amp; Cabin Fever Victoria, BC, Canada, British Columbia 483 people interested Interested This Saturday at 21:00 Goth Nite: UNDERGROUND Victoria, BC, Canada, British Columbia 172 people interested Interested Thu, 19 Jun at 16:00 Victoria Ska &amp; Reggae Fest: Turbulence, La Severa Matacera, Spiritual Warriors, Sonic Alley &amp; Ari DL Victoria, BC, Canada, British Columbia 226 people interested Interested Popular with friends This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested Sat, 21 Jun-22 Jun Weekend with Tango Alive Tango Victoria Dalie is interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C98" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1975172826621817/</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>(20+) Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Today from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Roy and 3 friends Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 2 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Thursday 12 June 2025 from 19:00-20:30 Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Little Fernwood Gallery. About Discussion More About Discussion Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Interested Going Invite Details Event by Anna Bigland-Pritchard Little Fernwood Gallery. Tickets www.annabiglandpritchard.com/event-details/rest-resonate-restorative-yoga-ft-cozy-live-music Public · Anyone on or off Facebook Do you need some R&amp;R? Join Anna &amp; Roxie for a dreamy candlelit evening of restorative yoga, live music, and guided journalling. Facilitated by Roxie Fehr of Across the Water | Yoga Anna Bigland-Pritchard of ABP Music Studio | Music As experienced, intuitive space-holders, our goal to support your Nervous System and capacity for hope with a feast of restful offerings. We know life is stressful and we want to help you feel more connected to your intuition so you can not only survive, but also have the capacity to take the next right step in your life in a way that positively impacts the world. The space will be dreamy, there will be tea, guided journalling, poetry, restorative yoga shapes that can be adapted for any body, and LIVE MUSIC! Anna will be playing guitar, creating dreamy sound worlds with vocal looping, and singing you lullabies all evening. What to bring Yoga mat (We'll have a few available to borrow) Journal &amp; pen/pencil (We'll also have some spare paper and writing/drawing utensils) Yourself in your comfy cozies Details June 12, 7-8:30pm at Little Fernwood $42 Accessibility This event is on the ground floor There is a unisex/non-gendered bathroom on the same level We care about making this event accessible, so please let us know if you have any questions or accessibility needs. This will be a VERY gentle practice, and modifications will be offered. Happy pride! As members of and allies of the 2SLGBTQIA community, we (Anna &amp; Roxie) will create a supportive, inclusive, affirming environment and expect all participants to do the same. If cost is a barrier, please contact us directly as we have a limited number of discount codes available This is our first time offering this class, and we hope it will be a hit so we can make it a regular thing. Come as you are, leave nourished by your dreams See less Victoria, British Columbia Tickets Find Tickets Little Fernwood Gallery. 1923 Fernwood Ave., Victoria Meet your host Anna Bigland-Pritchard 5 past events · Page · Musician/band Based in Lekwungen territory (Victoria, BC), Anna Bigland-Pritchard is a: -Soprano -Voice teacher… Follow Suggested events Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends 34 people interested Interested Sun, 29 Jun at 10:00 Victor / Victoria Switch Practica Solwood Studio Adam and Dalie are interested 22 people interested Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested 1395 people interested Interested Popular with friends This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested Sat, 21 Jun-22 Jun Weekend with Tango Alive Tango Victoria Dalie is interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C99" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/665127126496204/</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Tuesday 27 May 2025 at 19:30 Live Music at the Saxe Point Public House Saxe Point Public House About Discussion More About Discussion Live Music at the Saxe Point Public House Details 9 people responded Event by VINYL WAVE Saxe Point Public House Public · Anyone on or off Facebook Live Music every other Tuesday starting May 27th! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C100" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/986310396630042/</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SATURDAY SONG-A-THON 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada About Discussion More About Discussion THE SATURDAY SONG-A-THON Details 9 people responded Event by Bucket Crab Johnny and CRAB BUCKET STUFF 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada Duration: 5 hr Public · Anyone on or off Facebook an INDOOR PICNIC PARTY with FREE LIVE MUSIC Click on the Photo at the top to see the whole poster and zoom in on the details. Victoria, British Columbia 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada THE SATURDAY SONG-A-THON 1 member active Open chat Guests See All</t>
+        </is>
+      </c>
+      <c r="C101" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1414577976223422/</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 19:00-23:00 Solstice Slammer 3 - Moon Under Water, Victoria The Moon Under Water Brewpub About Discussion More About Discussion Solstice Slammer 3 - Moon Under Water, Victoria Interested Going Invite Details 27 people responded Event by Electric Druids and Gate Theory The Moon Under Water Brewpub Tickets · CA$10 www.eventbrite.com/e/solstice-slammer-3-tickets-1389012316229 Public · Anyone on or off Facebook Come join us for Solstice Slammer III at Moon Under Water Brewpub and Distillery! Get ready to celebrate with Electric Druids, Gate Theory and Insulam, hefty drinks and good vibes. Whether you're a craft beer enthusiast or just an enthusiast, there's something for everyone at this epic night of live music. Don't miss out - mark your calendars! See less Music and audio Victoria, British Columbia Tickets Find Tickets The Moon Under Water Brewpub 5435 Fowler Rd, Saanich, BC V8Y 1Y4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C102" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1198411931645258/</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Saturday 26 April 2025 from 15:00-18:00 LIVE MUSIC - The City Slickers 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion LIVE MUSIC - The City Slickers Details 21 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Members $5, Guests $10 Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C103" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2579625309035667/</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Sunday 18 May 2025 from 12:00-18:00 Live Music @ Junction (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Live Music @ Junction (RAIN OR SHINE) Details 125 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Here we go again, its a long weekend so let's get our Sunday Funday on. First Live Music of the year at Junction Up first is-  Emergency Exit  are playing from 1230-230pm To take us home is - An &amp; Ben are playing from 3-5pm Tasting Room and Picnic Area are open 12-6pm Oh and if you haven't heard me say it before ITS RAIN OR SHINE. Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Cider ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Mini Market and a Beautiful location ⠀⠀⠀⠀⠀⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your well behaved two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C104" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/639017139056190/</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Saturday 19 April 2025 from 15:00-18:00 Live Music - Love Cats 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion Live Music - Love Cats Details 22 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Members $5, Guests $10 Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C105" s="3" t="n">
+        <v>45810.95421294607</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1050242777151793/</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 2 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 10 Jun at 09:00 – 15 Jun at 19:00 KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Victoria ,BC About Discussion More About Discussion KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Interested Going Invite Details 40 people responded Event by Congregation Emanu-El, Victoria, British Columbia Victoria ,BC Duration: 6 days Public · Anyone on or off Facebook Registration required for both in person and virtual attendance. https://klezcadia.org https://congregationemanuelnews.wordpress.com/.../klezca.../ Locations of performances and workshops provided upon registration. See less Victoria, British Columbia Victoria ,BC 528 Broughton St, Victoria, BC V8W 1C6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C106" s="3" t="n">
+        <v>45810.95421294607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some json parsing errors in llm.py in extract_and_parse_json.
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1802,7 +1802,7 @@
         </is>
       </c>
       <c r="C91" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="92">
@@ -1817,7 +1817,7 @@
         </is>
       </c>
       <c r="C92" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="93">
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="C93" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="94">
@@ -1847,7 +1847,7 @@
         </is>
       </c>
       <c r="C94" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="95">
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="C95" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="96">
@@ -1877,7 +1877,7 @@
         </is>
       </c>
       <c r="C96" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="97">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="C97" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="98">
@@ -1907,7 +1907,7 @@
         </is>
       </c>
       <c r="C98" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="99">
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="C99" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="100">
@@ -1937,7 +1937,7 @@
         </is>
       </c>
       <c r="C100" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="101">
@@ -1952,7 +1952,7 @@
         </is>
       </c>
       <c r="C101" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="102">
@@ -1967,7 +1967,7 @@
         </is>
       </c>
       <c r="C102" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="103">
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="C103" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="104">
@@ -1997,7 +1997,7 @@
         </is>
       </c>
       <c r="C104" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="105">
@@ -2012,7 +2012,7 @@
         </is>
       </c>
       <c r="C105" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
       </c>
     </row>
     <row r="106">
@@ -2027,7 +2027,1522 @@
         </is>
       </c>
       <c r="C106" s="3" t="n">
-        <v>45810.95421294607</v>
+        <v>45810.95421295139</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/667083456006099/</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT Details 11 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 753 View Street (2nd floor, Hermmans Jazz Club) Date: Saturday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C107" s="3" t="n">
+        <v>45811.56311059028</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1910904133047825/</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY The Coda About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY Details 81 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 751 View Street (2nd floor, Hermmans Jazz Club) Date: Friday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C108" s="3" t="n">
+        <v>45811.56311059028</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1132427048350776/</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com or 15$ cash/e-transfer at the door. Formed in the heart of Chinatown, Rosebuds is a dynamic ensemble that brings the vibrant sounds of jazz, blues &amp; swing to life.  The group plays a mixture of originals and jazz standards, and is influenced by artists like Louis Armstrong, Billie Holiday, Lester Young, and Lionel Hampton. Featuring Rebecca Wells (vocals/guitar), Alex Moore (guitar/keys) Bryden Amos (guitar/keys), Matisse Gubby-Hurtig (bass), Owen Chow (trumpet), and Andrew Greenwood (tenor saxophone). Samba e Sol is a newly formed Brazilian bossa nova jazz trio featuring Andrew Greenwood (flute), Alex Moore (guitar), and Matisse Gubby-Hurtig (bass), playing music by artists like Antonio Carlos Jobim, Marcos Valle, Luiz Bonfa, and more. Instagram: https://www.instagram.com/rosebudsband/ See less Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C109" s="3" t="n">
+        <v>45811.56311059028</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1079226067560481/</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 41 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 6, 2025 | Lesson:  Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C110" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1060779176049104/</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Thursday 3 October 2024 from 19:30-22:30 Kizomba Practica Thursdays: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Kizomba Practica Thursdays: Fall Series Details 20 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Join us every Thursday for Kizomba/Urbankiz classes. Intermediate 7:30PM-8:15pm Beginner 8:15pm-9:00pm Practica until 10:30pm Class only: $10 Class &amp; Practica: $15 or $10 for university students w/ID Practice only $10 Classes will be provided by your local Instructor (David Lamine) and assistants (Robyn, Becky) and occasionally by some out of town and International Instructors. Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C111" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/960236445839425/</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Saturday 22 June 2024 from 18:00-21:00 Kizomba/UrbanKiz at Clover Clover Pt, Victoria, BC V8S, Canada About Discussion More About Discussion Kizomba/UrbanKiz at Clover Interested Details 56 people responded Event by Becky Mowat Clover Pt, Victoria, BC V8S, Canada Duration: 3 hr Public · Anyone on or off Facebook Come join us for our first time dancing at Clover Point! There will be no lesson beforehand and this is super casual. Just a bunch of friends hanging out and dancing. Bring snacks, something to drink, blankets, warm clothes (as it is typically cooler by the ocean). There isn't a lot of parking at Clover Point but you can park along Dallas Rd and just walk down. Feel free to invite friends and family. Hope to see you all there! See less Victoria, British Columbia Clover Pt, Victoria, BC V8S, Canada 1301 Clover Pt, Victoria, BC V8S, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C112" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1861230087752141/</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 3 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 31, 2025 | Lesson:  Intro to Salsa with Adam &amp; Alicia Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C113" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/947213690692385/</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C114" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3006474846197996/</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 25 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 27, 2025 | Lesson:  Intro class TBD Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro class TBD • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C115" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1743571267040445/</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 20 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 8, 2025 | Lesson: Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C116" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1293301738436581/</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Sunday 6 April 2025 at 17:00 Kizomba Sundown Party: Free of charge Method Studio - Victoria BC David Lamine Victoria invited you About Discussion More About Discussion Kizomba Sundown Party: Free of charge Details 58 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Method Studio - Victoria BC Public · Anyone on or off Facebook Free Pre-VIKFest party. Bring snack and drink. Expect great music, great energy, great atmosphere. "Dance with your heart. your feet will follow" Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C117" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1029869435768837/</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Saturday 22 March 2025 at 20:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC This event has been cancelled. You cannot share this event, but you can still post. About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 14 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C118" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/758501768607647/</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 6 6 Apr 2023 at 20:00 – 10 Apr 2023 at 10:00 Victoria International Kizomba Festival 4th Edition Victoria Conference Centre About Discussion More About Discussion Victoria International Kizomba Festival 4th Edition Going Details 702 people responded Event by Island Afro Latin Events Victoria Conference Centre Duration: 4 days Public · Anyone on or off Facebook Welcome to the Victoria International Kizomba Festival, APOCALYPSE EDITION!! What to expect?? Locally and Internationally renowned instructors, teaching Semba, Kizomba, Urban Kiz, Tarraxinha, Tarraxo, Douceur, Afro Beat, Afro House, Kuduro and More! ALL IN ONE: - Over 27.000 square feet of space - 3 ROOMS: Kizomba room, Urban Kiz room, Social room - After party room go until 6-7am with (Douceur, Tarraxinha and Sweet Kiz) VIKF 4rd Edition is offering you: *4 days of workshops *3 day-time socials *4 nights of dancing, *3 afterparties until 6-7am *15Hours + of workshops *40H + of dancing * 2 educational sessions of Cultural Aspect of African dances * 1 Gala Night of celebration of Multiculturalism, Diversity, the Arts including performances and fashion shows by African Designers IMPORTANT NOTICE: This 4 Day Festival has some free components offered to the general public as well as some activities with a minimal cost (to be announced at a later date) ARTISTS CONFIRMED - JP &amp; STEPHY (PARIS - FRANCE) - BONIFACIO (LISBON - PORTUGAL) - STEPHANE (PARIS - FRANCE) - SAMY (MONTREAL - CANADA) - LENA (VANCOUVER - CANADA) - ELVIS (OTTAWA - CANADA) - DJ PARAISO (PARIS - FRANCE) - DJ SINK (MONTREAL - CANADA) - DJ GUELAS (MIAMI - USA) - DJ MADARA (PARIS - FRANCE) AND MORE TO COME ... JP and STEPHY 10h Training program starts on Thursday April 6, 2023 in the afternoon DJ Training by DJ paraiso by Individual or Group of 4 (Friday - Saturday and Sunday) 10+ Taxi dancers 20+ International Special Guests HOTEL DEALS: WE HAVE 4 PREMIUMS HOTELS TO HOST YOU. A) FAIRMONT EMPRESS HOTEL is adjacent to the Convention Centre (all in one): TO BOOK YOUR ROOM: call the Reservations Department at 250 384 8111 or the Global Reservations Centre at 1 800-441-1414. Please identify yourself as being with the Victoria International Kizomba Festival group. TWO DOUBLE BEDS: $279 Rates will be available 3 days prior to the event and 3 days post B) MARRIOTT VICTORIA INNER HARBOUR, (just across the street, 1min walking distance) Book your accommodation by calling reservations toll-free at 1-888-236-2427 and asking for the "Victoria International Kizomba Festival group" to book online: https://www.marriott.com/event.../reservation-link.mi... 1 KING BED: $CAD199 2 QUEEN BEDS: $CAD199 C) DOUBLE TREE BY HILTON Reservations can be make by calling Central Reservations at 1-800-222-TREE and referencing KIZOMBA FEST 2023. or by using the HiltonLink: https://www.hilton.com/en/book/reservation/rooms/... - STANDARD ROOM: 2 QUEEN BEDS $CAD219 - SUITE WITH 2 QUEEN BEDS + SOFA BED, $CAD249 ALL rooms have all amenities (Fridge, kettle, Microwave, Iron, etc...) IMPORTANT NOTE: - If you are no longer able to join, you can transfer your pass to another participant without any fee; transfer your pass to the next edition; or ask for a refund within 15 days after the event. - Must be 18+ to attend this event - Click on the *Going* tab on facebook to receive notifications about line up updates and any useful information regarding this event. - By purchasing the pass, you grant the photographer, videographer, the Organization and its partners/sponsors  the permission to use your image  in any and all forms of media for commercial purposes, advertising, promotion... - COVID-19 clause: This event may be postponed or cancelled by the Organizer due to the Covid19 pandemic or any other resulting event related to the instructions of the federal government of Canada and the BC provincial government. In such case, the buyer can ask for a full refund. See less Dance Victoria, British Columbia Victoria Conference Centre 720 Douglas Street, Victoria The VCC is a boutique facility.  We’re small enough to be intimate yet able to handle conferences as Guests See All</t>
+        </is>
+      </c>
+      <c r="C119" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2637194793152555/</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 81 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 29, 2025 | Lesson:  Intro to Salsa Rueda with Sam and Katie Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa Rueda • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C120" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/372311028526699/</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Saturday 9 December 2023 from 20:30-23:30 Victoria Kizomba Social: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Social: Fall Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C121" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1337760257449745/</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 4 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 10, 2025 | Lesson:   Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C122" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1179097320623502/</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 37 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C123" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1184791909680061/</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Thursday 13 March 2025 from 19:30-23:00 Urban Kiz Workshop with Mannie Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 50 people responded Event by Becky Mowat and David Lamine Victoria Ukrainian Cultural Centre Duration: 3 hr 30 min Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C124" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1152065639712042/</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 20 20 Feb at 19:30 – 23 Feb at 23:00 Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Details 49 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 days Public · Anyone on or off Facebook Join us for our special edition Urbankiz &amp; Tarraxo workshops with Mike Ahombi Mike has been a big supporter of our VIKF and bringing his talent and low key vibe to the west coast. He is based out of Ottawa but you will find him at many different festivals and cities teaching Kizomba, Urbakiz and Tarraxo. We cannot wait for you all to have the opportunity to learn from such an incredible person and instructor. Details: Feb 20th Urbankiz Workshop 7:30pm-9:30pm Practica 9:30pm-11:00pm Feb 22nd Tarraxo Workshop 8:00pm-10:00pm Practica 10:00-11:30pm Price $90 Workshops only $70 Practica only $20 *** please e transfer to becksmith@hotmail.com *** Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C125" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3185065321631809/</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Saturday 15 March 2025 from 20:00-00:00 Urban Kiz Workshop with Mannie Method Studio - Victoria BC Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 48 people responded Event by Becky Mowat and David Lamine Victoria Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C126" s="3" t="n">
+        <v>45811.56868980324</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1388695712154512/</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 66 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation June 22, 2025 | Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C127" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/9677364319006080/</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 49 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation July 20, 2025 | Lesson:  Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C128" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342233713680795/</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Thursday 1 May 2025 at 21:00 Bachata &amp; Merengue- All Levels- May Series Studio 4 Athletics About Discussion More About Discussion Bachata &amp; Merengue- All Levels- May Series Details 3 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Bachata &amp; Merengue are both dances from the Dominican Republic. Bachata can be anywhere from slow and romantic with lots of dips, sway and body movement to more upbeat and percussive with lots of musical footwork. Merengue is carefree, flirtatious and fun! Classes are registered on a monthly basis and take place every Thursday from 8:00- 9:00pm, May 1, 8, 15, 22, 29. No experience required.  No partner is necessary as we rotate partners throughout the lesson.  Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C129" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1069894401564900/</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Monday Nights! 111 Superior St, Victoria, BC V8V 1T2, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion Sensual Bachata Series – Monday Nights! Details 15 people responded Event by Victoria Latin Dance Association 111 Superior St, Victoria, BC V8V 1T2, Canada Duration: 3 hr Public · Anyone on or off Facebook Sensual Bachata Series – Monday Nights! Mondays – April 7th, 14th, 21st &amp; 28th at 111 Superior Street Foundation Class (6:30–7:35 PM) Perfect for absolute beginners or dancers looking to strengthen their foundation! In this class, we’ll break down the essential steps, body movement, and partner connection in a fun environment. You’ll learn the basics with proper technique while also adding styling to make your dancing look and feel smooth on the dance floor. No experience or partner needed—just bring your curiosity and energy! Intermediate Class (7:35–8:40 PM) Ready to level up? This class is designed for dancers who already feel comfortable with the basics and want to challenge themselves. We’ll dive into more fun patterns while also exploring musicality—how to connect those movements to the music in a more expressive way. Get ready to build confidence, fluidity, and your own unique style! To Register: Send your e-transfer to maximumotion@gmail.com and include in the memo: Foundation, Intermediate, or Both + Lead or Follow Class Cancellation &amp; Refunds We understand that plans can change. However, due to limited spots, renting space in advance, and the preparation required for each class, we’re unable to offer refunds for cancellations. Please make sure you’re committed before signing up. We truly appreciate your understanding and support! See less Victoria, British Columbia 111 Superior St, Victoria, BC V8V 1T2, Canada 111 Superior St, Victoria, BC V8V 1T2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C130" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/692165093260868/</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 13:00-16:00 Salsa &amp; Bachata Masterclass with Adam &amp; Ghada Solwood Studio About Discussion More About Discussion Salsa &amp; Bachata Masterclass with Adam &amp; Ghada🔥 Details 60 people responded Event by Dancing Time Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook Hello everyone! Spring is here, and many things are happening, but I can’t but dance with you one last time before leaving for the entire summer!! To make things spicy, I am extremely happy to collaborate with Adam on a Salsa &amp; Bachata Masterclass! Get ready to learn details that will help you with creating flow – both as leads and follows – in addition to some socials-friendly tricks! Date: Saturday, May 10 Time: 1:00-2:30 | Salsa, 2:30-4:00 | Bachata Price: 25$ for one class, 35$ for two classes Location: Solwood studio, 1303 Broad st To register, please fill in this quick form and send an e-transfer to ghadacyoussef@gmail.com. https://forms.gle/4QThxT6yByd3h5KH8 Note: kindly understand that no-shows and cancellations made in less than 1 week from the workshop cannot be refunded. I will be happy to fully refund for earlier cancellations if need be. See less Victoria, British Columbia Solwood Studio Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C131" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1813229489279716/</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Thursday 29 May 2025 from 19:55-21:00 Sensual Bachata 4 Week Series Method Studio - Victoria BC Thu, 15 May Thu, 22 May Thu, 29 May +1 About Discussion More About Discussion Sensual Bachata 4 Week Series Details 6 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 1 hr 5 min Public · Anyone on or off Facebook Ready to level up your Sensual Bachata? May 8, 15, 22, 29 Method Studio | 7:55–9:00 PM | $80 for all 4 classes Join us for an exciting and dynamic Bachata Sensual class designed for experienced beginners and intermediate dancers! We’re blending solid fundamentals with fresh, fun, and sensual combos to help you grow, challenge yourself, and have an amazing time on the dance floor. No partner needed — just bring yourself and your love for dance! Spots are limited — don’t miss out! Register by e-transferring $80 to maximumotion@gmail.com and mentioning “Bachata Sensual” in the notes. Get ready to connect, move, and elevate your dancing! P.S. All fees are non-refundable as they go directly toward securing the studio space and running the class. See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C132" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/717475250956404/</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Friday 30 May 2025 at 18:00 FREE Beginner Bachata Class 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 About Discussion More About Discussion FREE Beginner Bachata Class Details 65 people responded Event by Mayfair Shopping Centre and Victoria Latin Dance Association 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 Public · Anyone on or off Facebook Ready to get your groove on? We’re teaming up with the Victoria Latin Dance Association  for a FREE Beginner Bachata Class right here at Centre Court! Join us on Friday, May 30 at 6:00 PM for an evening of fun and dancing. FREE Beginner Bachata Class May 30th, Friday at 6PM NO partner or experience necessary! Bachata is a beautiful and easy-to-learn dance that’s great for meeting new people, getting active, and connecting with an amazing community. See less Dance Victoria, British Columbia 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 3147 Douglas St, Victoria, BC V8Z 3K3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C133" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1901245437276872/</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Friday 9 May 2025 from 20:00-00:00 Bachata Nights Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Details 40 people responded Event by Bachata Nights Victoria BC , Alysha Kopala and Sebastian Carmona Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights May 09 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @yourgirlalysha  and @davidch_78  will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person The evening starts with an Open-level Bachata lesson from 8:15 PM to 9:00 PM—great for all skill levels! Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C134" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3975145332748137/</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Friday 13 June 2025 from 20:00-00:00 Bachata Night Method Studio - Victoria BC About Discussion More About Discussion Bachata Night Interested Going Invite Details 40 people responded Event by Bachata Nights Victoria BC , Sebastian Carmona and Alysha Kopala Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights June 13 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C135" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1057471579628015/</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Friday 16 May 2025 at 17:00 Bachata Nights Victoria Bc Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Victoria Bc Details 9 people responded Event by Bachata Nights Victoria BC and Sebastian Carmona Method Studio - Victoria BC Public · Anyone on or off Facebook Join us on our next Bachata Nights May 23 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C136" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1300938064467261/</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Thursday 20 March 2025 from 20:00-22:00 Intermediate Sensual Bachata Workshop Method Studio - Victoria BC About Discussion More About Discussion Intermediate Sensual Bachata Workshop Details 24 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 2 hr Public · Anyone on or off Facebook Sensual Bachata Workshop in March! Intermediate workshop - March 20 Time: 8:00-9:30 PM + Practice 9:30-10:00 PM Location: Method Studio, 841 Fisgard St. Cost: $30 per workshop (includes 2 hours!) Intermediate workshop: Take your skills to a higher level! Master the advanced variations of the Madrid pass, smooth transitions and musicality. No partner needed, just bring your energy and comfortable shoes! Register at: maximumotion@gmail.com #BachataWorkshop #VictoriaBC #LearnToDance #BachataLovers See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C137" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1350929566137538/</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 4 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation August 10, 2025 | Lesson: Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C138" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/679241811720932/</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Fundamentals- May Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- May Series Details 7 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, May 6, 13, 20, 27 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C139" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1298465587898458/</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Tuesday 4 March 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- March series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- March series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Mar 4, 11, 18, 25 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C140" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1382188962971661/</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Tuesday 1 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Fundamentals- April Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- April Series Details 9 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, Apr 1, 8, 15, 22, 29 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C141" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2233725973712106/</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Monday 3 March 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- March series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- March series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, Mar 3, 10, 17, 24, 31 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C142" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342792743590871/</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Monday 7 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- April series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, April 7, 14, 28. Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C143" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/966455485665576/</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Thursday 3 April 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- April series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Apr 1, 8, 15, 22, 29 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C144" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/10048344358532607/</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- May series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. May 6, 13, 20, 27 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C145" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/669591372187091/</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 10:00-11:00 Salsa &amp; ChaCha Solo Westshore Dance Studios Sat, 17 May Sat, 24 May Sat, 31 May +7 About Discussion More About Discussion Salsa &amp; ChaCha Solo Details 2 people responded Event by Dance Praktika Westshore Dance Studios Duration: 1 hr Public · Anyone on or off Facebook Elevate your dance journey with our Ladies Solo Class. Join our exciting series and learn the basics of Salsa and Cha Cha. Perfect for beginners looking to spice up their dance skills! Class Highlights: - Learn exciting dance moves tailored for solo dancers; - Fun and welcoming environment; - Suitable for absolute beginners. Come dance with us and let the rhythm guide you! To register to April classes please use links at "Tickets". See less Langford, British Columbia Westshore Dance Studios 109-2675 Wilfert Road, Victoria www.westshoredance.com 2years+ Competitive&amp;Production a space for everyone with a love of dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C146" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2214494908966327/</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Monday 5 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Int/ Adv- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- May series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, May 5, 12, 26 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C147" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/909522138040202/</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Friday 28 November 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 41 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 66 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 20 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C148" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1059622278965884/</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 8 Saturday 8 November 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in October. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 177 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 66 people interested Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 5 friends 149 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C149" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/530862806349067/</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Sunday 30 March 2025 from 13:00-17:00 Salsa Gonzales tasting! 🍋‍🟩 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia About Discussion More About Discussion Salsa Gonzales tasting! 🍋‍🟩 Details 6 people responded Event by THE ROOT CELLAR | village green grocer 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia Duration: 4 hr Public · Anyone on or off Facebook Hey friends! It's time to get those tastebuds tingling - you're invited to come and join us for a Salsa Gonzales tasting at our McKenzie Corner store! Salsa Gonzales is a little condiment company with a big personality! Nestled on Gonzales Beach in Victoria, they craft salsas, hot sauces, pickles, preserves, and more – all with a generous splash of love and a fiery kick. When: Sunday March 30th, 1pm-5pm Where: Our McKenzie Corner location We're looking forward to seeing you there! XO See less Victoria, British Columbia 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia 1286 McKenzie Ave, Saanich, BC V8P 5P2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C150" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2251848171850840/</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 Saturday 10 May 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in April. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 177 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 49 people interested Interested Mon, 4 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Ali 3 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C151" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/884101187183426/</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 July 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in June. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 29 Jun at 10:00 Victor / Victoria Switch Practica Solwood Studio Adam and Dalie are interested 23 people interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Veronica, Ali and 5 friends are interested 943 people interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends 40 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C152" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3899920353641309/</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 9 Saturday 9 August 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in July. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 177 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 49 people interested Interested Mon, 30 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne and Ali 15 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C153" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1624603351798270/</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 April 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 177 people interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends 40 people interested Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 7 friends 201 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C154" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1239163193996279/</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 14 Saturday 14 June 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Tickets · CA$17.31 www.eventbrite.com/e/caliente-salsa-saturdays-tickets-1390062838369 Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in May. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Tickets Find Tickets Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 29 Jun at 10:00 Victor / Victoria Switch Practica Solwood Studio Adam and Dalie are interested 23 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 49 people interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Veronica, Ali and 5 friends are interested 943 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C155" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1618420955545842/</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 30 Friday 30 May 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing at an all ages venue with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 4 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Ali 3 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 41 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 66 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C156" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/624858640069610/</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 Friday 22 August 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 41 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 66 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 20 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C157" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/939376108286434/</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Friday 27 June 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 16 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Ali and Dalie 34 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 66 people interested Interested This Saturday at 21:00 Goth Nite: UNDERGROUND Victoria, BC, Canada, British Columbia 173 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 13:00 Sunday Afternoon Milonga Downtown Victoria, Victoria Dalie is going Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C158" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1636237610432412/</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Saturday 16 August 2025 from 20:00-23:59 Salsa Sunset Latin Party – August 16th! Latin Dance Canada About Discussion More About Discussion 🌅🔥 Salsa Sunset Latin Party – August 16th! 🔥🌅 Interested Going Invite Details 29 people responded Event by Latin Dance Canada Latin Dance Canada Duration: 3 hr 59 min Public · Anyone on or off Facebook Salsa Sunset Latin Party – August 16th! Get ready for a magical summer night filled with Latin rhythms, sunset vibes, and non-stop dancing! Join us for the Salsa Sunset Latin Party, where the Salsa, Bachata, and Merengue beats will keep you moving all night long under the stunning sunset sky! Dress Code: Wear your best sunset-inspired outfit – think bright, tropical colors, and beach party vibes! Dance to the best Salsa, Bachata, Merengue &amp; Latin hits all night! No partner? No problem! Join our fun intro class at 8:00 PM! Location: Ukrainian Cultural Centre, 3277 Douglas St., Victoria, BC Date: Saturday, August 16, 2025 Intro Class: 8:00 PM | Social Dance: 8:30 PM - Late Entry: $15 at the door – Bring cash, please! What to Expect: Vibrant salsa rhythms &amp; tropical vibes! Tropical-themed decorations &amp; stunning sunset views! A welcoming dance community &amp; unforgettable fun! Let’s dance as the sun sets and make it a night to remember! Tag your friends and let’s create memories under the summer sky! #SalsaSunsetLatinParty #SalsaBachata #LatinDanceParty #VictoriaBC #LatinDanceCanada See less Dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C159" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1356293392177099/</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Monday 3 March 2025 from 18:30-21:30 Open House | FREE Classes - Bachata Sensual &amp; Brazilian Zouk 1709 Blanshard St, Victoria, BC V8W 2J8, Canada About Discussion More About Discussion Open House | FREE Classes - Bachata Sensual &amp; Brazilian Zouk Details 28 people responded Event by Bachata and Zouk with Javi in Victoria and Javi Zouker 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 3 hr Public · Anyone on or off Facebook Join us for our Open House / Free classes on Monday March 3rd with Javi Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on body awareness, lead and follow techniques, musicality, styling, and how to have lots of fun dancing with new friends!  Learn with Javi, with over ten Years of teaching experience.  Learn dance with clear, fun, and inspiring teachings open to all levels! Schedule: Monday March 3rd 6:30-6:45pm | Meet &amp; Greet 6:45-7:30pm | Traditional Bachata - Beginner 7:40-8:25pm | Sensual Bachata - Intermediate 8:35-9:20pm | Brazilian Zouk - Beginner 9:20-9:30pm | Sharing circle Tuition = FREE Space is Limited:  Please email us to register your spot and please share if you are leading or following or open to either. email:  danceinflow@gmail.com 4 week session on Monday March 10-31st Phillippine Bayanihan Community Centre - 1709 Blanshard st, Victoria, BC See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C160" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1106484714432492/</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 4 Tomorrow from 18:30-21:00 Zouk practica and social White Eagle Hall, 90 Dock St, Victoria BC Wed, 21 May Wed, 28 May Wed, 4 Jun Wed, 11 Jun +29 About Discussion More About Discussion Zouk practica and social Interested Going Invite Details 2 people responded Event by Victoria Zouk Collective and Victoria Zouk Collective Group White Eagle Hall, 90 Dock St, Victoria BC Duration: 2 hr 30 min Public · Anyone on or off Facebook Drop-in zouk practica by donation - everyone welcome! White Eagle Polish Hall every Wednesday 6:30-9 pm Shared warm up, free dance time, review material from lessons and congresses, connect and share knowledge! Help is always available. Minimum $5 donation. Cash at the door, or etransfer to oceanzouk@gmail.com Enter the lower hall by the side door on Niagara Street just beside the Polka food truck. Also available in Victoria are zouk lessons with Javi, an amazing instructor from Vancouver! More info at https://www.facebook.com/Sabor.Asi.Dance.Salsa.Victoria or email danceinflow@gmail.com See you there! See less Victoria, British Columbia White Eagle Hall, 90 Dock St, Victoria BC 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C161" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1411005319893067/</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Monday 28 April 2025 from 18:30-22:30 Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion 🔥Bachata &amp; Brazilian Zouk 🌊 dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard Details 7 people responded Event by Bachata and Zouk with Javi in Victoria 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 4 hr Public · Anyone on or off Facebook Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard street | Victoria Join us for a 4 week course exploring the joy and magic of Brazilian Zouk &amp; Bachata dancing! Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on enhancing body awareness, building confidence in dance vocabulary with lead and follow techniques, exploring musicality, and loving yourself deeper with styling! Be prepared to have lots of fun dancing with new friends! Register today! Schedule: Monday April 7 - 28th 6:30-7:25pm | Brazilian Zouk - Level 2 (ask Javi for permission) 7:30-8:25pm | Brazilian Zouk - Level 1 8:30-9:25pm | Sensual Bachata - Beginner Foundations 9:30-10:30pm | Sensual Bachata - Intermediate "Trending Moves" Tuition: $20 | 1 Class $35 | 2 Classes (Brazilian Zouk 1&amp;2, or Brazilian Zouk 1 &amp; Bachata, Bachata 1&amp;2) $50| 3 Classes (3 classes, BEST value) 1709 Blanshard St, Victoria, BC Registration: E-transfer to: danceinflow@gmail.com or send us a message on Whatsapp: 7785877665 (Also accepting credit card/cash at the door) Please add a note if you're registering as a "Leader", "Follower", or "Open to both" Space is limited. Register in advance to reserve your spot! Looking fwd to dancing and flowing with you, Warmly, Javi See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C162" s="3" t="n">
+        <v>45811.57870013889</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/544121845403419/</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 13:00-23:55 Swing Session: Balboa with Yoshi and Etsuko Solwood Studio About Discussion More About Discussion Swing Session: Balboa with Yoshi and Etsuko Details 108 people responded Event by Swing Dance Association of Victoria , Dave Henderson and 2 others Solwood Studio Duration: 10 hr 55 min Public · Anyone on or off Facebook Lace up your shoes on May 31, 2025 for an afternoon of Balboa Classes and an evening of Social Dancing with Yoshi and Etsuko Uemura. 4 Classes for everyone &amp; 1 Social Dance! Passes go on sale April 19 at noon at our SDAV Square Shop! You must know and be comfortable with Balboa basics for all of these classes - they won't be covered at this workshop. All the specifics are available at swingvictoria.net , but here are the notes: May 31st, at Solwood Studio, with doors at 12:30pm . Bring indoor shoes, please! 4 classes for everyone and there's a dance from 9-12am. Passes go on sale April 19th at noon. See less Victoria, British Columbia Solwood Studio 1303 Broad St, Victoria, BC V8W 2A8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C163" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1035925295253912/</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Friday 18 April 2025 at 18:30 Swing out with the ATOMIC COCKTAILS 751 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Swing out with the ATOMIC COCKTAILS Details 64 people responded Event by Peter Sandmark 751 View St, Victoria, BC V8W 1J9, Canada Public · Anyone on or off Facebook Join the ATOMIC COCKTAILS as they swing out for their pre-Japan Tour dance party on April 18 at the Coda, 751 View Street.  Doors open 6 pn, show from 6:30-8:30 pm!  Tickets $20.  With songs from their new album BLUE LIGHT BOOGIE! See less Victoria, British Columbia 751 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C164" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663135653237580/</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Method Studio - Victoria BC Canice Ma invited you Interested Going About Discussion More About Discussion WACK! Another West Coast Swing Social Dance Invite Details 36 people responded Event by Canice Ma and Wyatt Ritchie Method Studio - Victoria BC Duration: 3 hr 30 min Public · Anyone on or off Facebook Guess who's back, it's WACK! (please ignore the fact that it's been 2 years...) The schmucks are back with another spontaneous west coast swing social dance, featuring music by DJs Topknot and Amandance from Vancouver! DETAILS: • Friday, June 20th, 2025 • Method Studio, 841 Fisgard St, Victoria, BC • 7:30-11 pm: social dancing with 100% west coast swing (sorry, no lesson!) • Admission: $10 • Water and AC on us (and maybe some bonus chocolate) • Please keep in mind that parking is limited at the venue GENERAL SOCIAL DANCE ETIQUETTE: • Consent is cool- don't be creepy. • Shake off any shyness and get out there! Ask people to dance regardless if you’re a lead or follow, dancing for 10 years or started yesterday- it's more fun that way! • No teaching or unsolicited feedback on the dance floor. Good vibes only! • If you would like to partake in a steal dance, try to remain with that group for the whole song. • Bring a water bottle! The studio is known to get warm with more bodies in the space so we want you to stay healthy and hydrated. • Personal hygiene is important! Consider bringing a towel and/or a spare shirt to change into if you sweat easily. Our studio has a bathroom and change rooms available for all to use. • We recommend wearing clothes that are easy to move in, especially pants given the nature of the dance. • Clean, comfortable shoes (ideally dance shoes) on the dance floor only! See less Victoria, British Columbia Method Studio - Victoria BC 833 Fisgard St, Victoria, BC V8W 1R9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C165" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663756533046485/</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Friday 11 April 2025 at 21:30 Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. Details 36 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Public · Anyone on or off Facebook Miguelito Valdes presents Contodo What happens when you bring together three Cuban and two Canadian musicians, with a deep love of all music and a wide range of musical experiences?  A joyful mix of party and deep groove, that's what! Guaranteed to make you want to dance, these brothers from other mothers bring it all. Con Todo! Featuring: Miguelito Valdes – brass/vocals/percussion Jose Sanchez – drumset/timbales Hector Ramos – congas/percussion Peter Dowse - bass Brooke Maxwell – keys/vocals See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C166" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2441697862726705/</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Sunday 30 June 2019 at 19:00 Journey’s 50th Birthday!!  A West Coast Swing dance party!! Eastern Star Hall Chapters No 5 &amp; No 17 Journeey Song invited you About Discussion More About Discussion Journey’s 50th Birthday!!  A West Coast Swing dance party!! Details 13 people responded Event by Journeey Song Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook 3281 Harriet Road, Victoria,BC Bring your own alcohol-free beverage... Bring a gluten-free appie if you’d like. Dance West Coast Swing until 10 pm to Blues, Pop, RnB, Swing, and a wee bit of Ballroom Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C167" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1776457206589544/</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Friday 21 March 2025 from 18:30-20:30 Slim Sandy's Atomic Cocktails swing speakeasy party! The Coda About Discussion More About Discussion Slim Sandy's Atomic Cocktails swing speakeasy party! Details 72 people responded Event by Peter Sandmark and Trace Nelson The Coda Duration: 2 hr Public · Anyone on or off Facebook Join Slim Sandy's Atomic Cocktails and dance as they play 2 sets of swing jazz, jive and rhythm and blues from the 20’s to the 40’s. Slim, on guitar and harmonica, is joined by Willa Mae on vocals, “Big Daddy Bo” on bass, and Bryn Bad on trumpet.  Slim Sandy has been playing music for over 40 years with acts such as Ray Condo and the Crazy Rhythm Daddies.  In 2012, he and Willa Mae co-created the Slim Sandy band in Victoria!  They have played music festivals in Canada, France, Spain, Germany, Belgium, and the Netherlands.  In May they will be touring in Japan! See less Victoria, British Columbia The Coda 749 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C168" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/373500473108499/</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Sunday Swing at Logan's Logan's Pub 10 Dec 2017 Debi Wong invited you About Discussion More About Discussion Sunday Swing at Logan's Details Event by Swing X Logan's Pub Duration: 3 hr 30 min Public · Anyone on or off Facebook Sunday Swing at Logan's is BACK! Come join us for some great tunes and we'll party like it's 1939. Bring your dancing shoes, sweet moves, and a few dollars for our fabulous DJ (and gracious bartenders). Feel free to come early to hang out and grab a bite to eat. 19+. NEW: Crash course 15min swing lesson at 8:30pm! This is intended to be the bare minimum for someone to show up and know the basics of swing dancing, nothing fancy! DETAILS: * 8:30pm Quickie 15min beginner lesson! * 8:45pm social dancing until as late as midnight (maybe!) * Usually gets bluesy after 11pm See less Victoria, British Columbia Logan's Pub 1821 Cook Street, Victoria Original - Authentic - Unique Guests See All</t>
+        </is>
+      </c>
+      <c r="C169" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/302778660295534/</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Sunday 19 August 2018 from 18:00-21:00 West Coast Swing in the Park! Cameron Bandshell @ Beacon Hill Park Carolyn Gebbie invited you About Discussion More About Discussion West Coast Swing in the Park! Details 58 people responded Event by Carolyn Gebbie Cameron Bandshell @ Beacon Hill Park Duration: 3 hr Public · Anyone on or off Facebook Come join us for another evening of fun and WCS dancing in Beacon Hill Park! WCS music will be provided by DJ Carolyn. For those who are familiar with the routine, the 2018 WCS Rally Song will be played at 6:30, 7:30 and 8:30pm. Sam Jackson and Meaghan Efford, from wcsmovementmethods.com will be on hand to answer questions about WCS or how to improve your WCS dancing. They will also demo some incredible WCS dancing at 7pm. Please invite your WCS dance friends by sharing this event! See less Victoria, British Columbia Cameron Bandshell @ Beacon Hill Park Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C170" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/417338985546213/</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Thursday 29 August 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - August 29! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - August 29! Details 109 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for a fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C171" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1594011994641933/</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Tuesday 22 April 2025 from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Details 9 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. No street shoes. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C172" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1692156731689650/</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 2 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 3 Today from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 Tue, 20 May Tue, 27 May Tue, 3 Jun Tue, 17 Jun +22 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Interested Going Invite Details 2 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Saanich, BC V8Z 3S3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C173" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/634773653668605/</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Saturday Night West Coast Swing BC Swing Dance Club Victoria 15 Jun 2019 22 Jun 2019 29 Jun 2019 +2 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night West Coast Swing Details 9 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook June means summertime and sunny days! Along with the weather, things for BC Swing Dance Cub Victoria will be changing too. Here's what is happening this month: 7 - 8pm 1st Saturday of the Month: Lesson with Meaghan, plus an assistant from our dance community 7 - 8pm Remaining Saturdays each month: TBD (stay tuned for workshops, activities or practices - updates will be posted on each event page) Note:  The 7 - 8pm weekly timeslot is included in the dance entrance price. -------------------------------------------------- Come join us every Saturday all year long for a fabulous WCS social dance from 8 - 11pm. Just $10 for the ($5 for students). Meaghan Efford and Bob Gebbie 's lesson on June 1st (starting PROMPTLY at 7pm) will be the only lesson in June, and it will be a great way to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity.  The lesson is included in the dance entrance price.  No experience or partner is required. -------------------------------------------------- • 6:45 pm - Doors open • 7:00 pm - TBD each week* • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *lesson with Meaghan and Bob on June 1st Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C174" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/402729737034904/</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Thursday 5 September 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Details 123 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for our second fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C175" s="3" t="n">
+        <v>45811.58401604167</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1766891834185825/</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Interested Going Invite Details 35 people responded Event by Jeannie Kam and Alive Tango Victoria Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends SAVE THE DATE! The next Sunday afternoon Milonga is on 8 June 2025 1-4pm. The Coda Club (formerly Hermanns Upstairs) is a beautiful newly renovated venue with awesome ambience, nice wood floor and great sound system. Come join us for a wonderful afternoon of warm hugs and close embrace. Sunday 8June 2025 1-4pm The Coda, 751 View Street, Victoria Admission: $15 (plus tax) Special Guest DJ: Francis Nowaczynski (from Vancouver) Free parking at View Street Parkade (next door) or Broughton Parkade. Cash bar is open for drinks. See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C176" s="3" t="n">
+        <v>45811.58705930556</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/713923214640962/</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Sunday 4 May 2025 from 13:00-16:00 May 4th Afternoon Milonga Solwood Studio About Discussion More About Discussion May 4th Afternoon Milonga Details 45 people responded Event by Ingrid Love and Kathryn Stone Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook A one-time special afternoon milonga! Join us in celebrating the warmth of Spring and return to sunshine. Or, star wars, if you like. Featuring special guests Kimberly and Khang performing live music (violin/guitar) DJ Ingrid Hosts: Kathryn &amp; Ingrid $15 entry (cash only) 1:00pm-4:00pm Solwood Studio 1303 Broad St Victoria, BC See less Victoria, British Columbia Solwood Studio Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C177" s="3" t="n">
+        <v>45811.58705930556</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/644050564927019/</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends! A NEW SUNDAY AFTERNOON MILONGA! This is the first of a regular monthly milonga at a beautiful new venue…The Coda Club (formerly Hermann’s Upstairs) at 751 View Street, Victoria. Great ambience, nice wood floor, good sound system. So come join us for the warm hugs and close embrace and dance to the beautiful music of our very own DJ John Dewhirst. Sunday, 6 April 2025 2.00pm-5.00pm The Coda Club, 751 View Street, Victoria Admission $15 DJ: John Dewhirst Cash Bar is open for drinks Free Parking at View Street Parkade just next door Come celebrate this exciting day with us! See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C178" s="3" t="n">
+        <v>45811.58705930556</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1146571100253242/</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 22 Feb at 17:00 – 23 Feb at 13:30 Weekend with Tango Alive Tango Victoria About Discussion More About Discussion Weekend with Tango Details 27 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 22nd 5pm-6pm solo technique all levels. Balance and weight transfer while walking, change of dynamics to create a better connection with your body. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) Fundamentals of giros! We will look for the right moments for sacadas, barridas and adornos without affecting the partner's axis in elastic hugs of closed embrace. 8pm milonga !!! .. and Jorge’s BIRTHDAY !! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 23rd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons are full. March workshop dates are the 22nd&amp;23th Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C179" s="3" t="n">
+        <v>45811.58705930556</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1009684807956058/</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 17 17 May at 17:00 – 18 May at 13:30 Tango weekend with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Tango weekend with Jorge Olguín Details 28 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 17th 5pm-6pm solo technique all levels. ( no partner required) Please bring elastic bands!! 6.30pm-7.30pm for couples only ( need some experience) Sacadas, barridas and colgadas in an elastic embrace in order to create a circular movement. We will work with different orchestras to study the changes we need to do to introduce different tempos and rhythms. Get ready for a workout with musicality! 8pm milonga !!! Join us even if you didn’t take the classes. DJ Ingrid !! Free for people registered for the workshops. $10 for drop-ins. Sunday, 18th 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are June 21st &amp; 22nd Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C180" s="3" t="n">
+        <v>45811.58705930556</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1864555154338100/</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 21 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Alive Tango Victoria About Discussion More About Discussion Weekend with Tango Interested Going Invite Details 9 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 21st 5pm-6pm solo technique all levels. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) We will continue from May with the musicality for phrase change but this time we will add “double time” to help us with it, using examples of different orchestras. We will work with a “rebound” and half giros to change the direction within the phrase. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 22nd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are September 20th &amp; 21st. Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C181" s="3" t="n">
+        <v>45811.58705930556</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3637725693193744/</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 22 Mar at 17:00 – 23 Mar at 13:30 Weekend with Tango with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Weekend with Tango with Jorge Olguín Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 22nd 5pm-6pm solo technique all levels. Balance and weight transfer while walking, change of dynamics to create a better connection with your body. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) Marathon is just around the corner so this month we continue with comfortable close embrace! We continue with dancing in small spaces!! Let’s move gracefully without affecting the partner's axis in elastic hugs of closed embrace. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 23rd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available only on Saturday. Sunday - sold out Next workshop dates are the May 17th &amp;18th Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C182" s="3" t="n">
+        <v>45811.58705930556</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1318668532737609/</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 16 16 Apr at 18:30 – 18 Apr at 21:00 Tango week with Lya Alive Tango Victoria About Discussion More About Discussion Tango week with Lya Details 36 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 3 days Public · Anyone on or off Facebook Ignite Your Tango 16th of April, Wednesday 6:30-8:00 On &amp; Off Acis for social dance 18th of April, Friday 6:00 - 7:30 Follower technique 7:45 - 9:00 Switch role / connection Search - Grow &amp; Transform! Seminar series for Tango Dancers that want to transform their way of moving and connecting! We will travel through the Essentials of Tango in order to look for new answers and deeper understanding. What makes tango truly captivating? It’s the embrace, the connection, and the walk. These three fundamental elements are the heartbeat of tango, and mastering them is essential for creating an unforgettable dance experience. You will learn how to condition your body to move with control, fluidity, and elegance. You’ll discover how to find and perfect your axis, which is essential for maintaining balance and stability in every step. We will also explore dissociation, a technique that allows you to move the upper and lower body independently but associated. This workshop series will show you how to apply these principles in both the leader and follower roles, improving connection and response in every moment of the dance. We will apply all this to: The secrets to generating power for boleos effortlessly off and on axis special follower technique class Pro tips to dance with ease and confidence 90 min class - $30 All 3 classes - $80 To register email grazs@shaw.ca or pm me, or talk to me . See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C183" s="3" t="n">
+        <v>45811.58705930556</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1838888640215250/</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Friday 28 February 2025 at 19:00 Argentine Tango for Beginner - level 2 1303 Broad St, Victoria, BC V8W 2A8, Canada About Discussion More About Discussion Argentine Tango for Beginner - level 2 Details 19 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria 1303 Broad St, Victoria, BC V8W 2A8, Canada Public · Anyone on or off Facebook We are happy to announce that we continue with Argentinian Tango for Beginners - level 2. This 6 weeks session is progressive and requires preregistration. It is designed for students who have completed Beginner - level 1 or would like to deepen their skills. If not sure where you are with your tango contact us To register email us : grazs@shaw.ca or PM Grazyna Feb 28th - April 4th Fridays 7-8pm Price per person : $80 series (6 weeks) See less Victoria, British Columbia 1303 Broad St, Victoria, BC V8W 2A8, Canada 1303 Broad St, Victoria, BC V8W 2A8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C184" s="3" t="n">
+        <v>45811.58705930556</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1225266505917189/</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Saturday Beginner Lesson and Social Dancing Dance Victoria Sat, 7 Jun Sat, 14 Jun Sat, 21 Jun +4 About Discussion More About Discussion Victoria WCS Collective hosts Saturday Beginner Lesson and Social Dancing Interested Going Invite Details 1 person responded Event by Donna Forsyth Dance Victoria Duration: 3 hr 30 min Public · Anyone on or off Facebook Back to AIR CONDITIONED comfort at Dance Victoria Studios Beginner lesson from 7 to 8 pm Social dancing  from 8 to 10:15 pm Cost $15/$12 for students No need to register and no need for previous dance experience or a partner. Please bring scuff-free inside low-heeled dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C185" s="3" t="n">
+        <v>45811.58969681713</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/516994561244886/</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:45 Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING White Eagle Polish Association About Discussion More About Discussion Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING Details 15 people responded Event by Donna Forsyth , Andre Russo and Victoria West Coast Swing Collective White Eagle Polish Association Public · Anyone on or off Facebook Doors open at 6:45pm at this fabulous new venue! Advanced beginner/intermediate lesson by Chantelle Pianetta from 7 to 8 pm Social dancing for 3 HOURS from 8 to 11 pm DJs Donna and Andre Cost $15 /$12 for students ALL at the spacious White Eagle Hall No need to register and you do not need a dance partner. Please bring scuff-free dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia White Eagle Polish Association 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C186" s="3" t="n">
+        <v>45811.58969681713</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/967438905456066/</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Wednesday 26 March 2025 at 10:00 Victoria WCS Lesson and Dance at Eastern Star Hall Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria WCS Lesson and Dance at Eastern Star Hall Details 1 person responded Event by Donna Forsyth Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson by John de Pyffer from 7 to 8 pm Social dancing from 8 to 10:15pm Djs Amanda and Nel Cost $12 No need to register and no partner required. Please bring scuff-free indoor shoes or socks to dance in  and a water bottle. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C187" s="3" t="n">
+        <v>45811.58969681713</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/641769172035949/</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Saturday April 12 Beginner lesson and social dance at Dance Victoria Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 12 Beginner lesson and social dance at Dance Victoria Details 5 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginners lesson by Donna from 7 to 8 pm Social dancing from 8 to 10:15 pm DJs Andre and Nel Cost $15 /$12 for Students No need to register and no partner required. Please bring scuff-free inside dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C188" s="3" t="n">
+        <v>45811.58969681713</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2162855673833831/</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 11 May 2019 18 May 2019 25 May 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 8 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook Wow! April went by so quickly, which means it must've been super fun, which it definitely was.  Everyone at BC Swing Dance Club Victoria is so pleased with the way the first month of social dances went, and we hope to generate the same amount of enthusiasm in May. Let's make this month just as much fun! Come join us on May 4th for the first intro lesson and social dance of the month (plus every Saturday night after that). Just $10 for the lesson and/or social dance ($5 for students). No experience or partner required. • 6:45 pm - Doors open • 7:00 pm - Intro lesson with Sam Jackson and Meaghan Efford * • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *PLEASE NOTE that the weekly lessons will start PROMPTLY at 7pm.  It is disruptive to the flow of the lesson if participants arrive late. For anyone who's interested in building their West Coast Swing fundamentals quickly, note that May will be the last month we'll be offering weekly classes with both Sam and Meaghan. With summer approaching it's a great time to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity. Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C189" s="3" t="n">
+        <v>45811.58969681713</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1024182725709172/</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Saturday April 19th Lesson and Social Dance Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 19th Lesson and Social Dance Details 4 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginner plus lesson with Pamela Podmoroff from 8 to 10:15 pm Social dancing from 8 to 10:15 pm DJs Donna and Amanda Cost $15/ $12 for students No need to register and no partner required. Please bring scuff-free indoor dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C190" s="3" t="n">
+        <v>45811.58969681713</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2238975779474166/</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 13 Apr 2019 20 Apr 2019 27 Apr 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 23 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook A new month, a new social! Come and join in on the fun at our inaugural Saturday night dance and intro lesson on April 6 (and every Saturday night after that)! Just $10 for the Lesson and/or Social ($5 for Students). No experience or partner required. • 6:45 pm – Doors open • 7:00 pm – Beginner Lesson with Sam and Meaghan (this is perfect as a refresher class too!) • 8:00 – 11:00 pm Social Dancing featuring DJ Carolyn Please note the NEW START TIMES for the BC Swing Victoria Saturday night dances. See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C191" s="3" t="n">
+        <v>45811.58969681713</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1366072544640156/</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Saturday 17 May 2025 at 18:45 Victoria WCS Collective Beginner Lesson and Social Dancing Dance Victoria About Discussion More About Discussion Victoria WCS Collective Beginner Lesson and Social Dancing Details 9 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson from 7 to 8 pm by John de Pfyffer Social dancing from 8 to 10:15pm DJg by Donna and Nel Cost $15/ $12 for students No need to register and no need for dance experience.. Also, no partner necessary, we got you! Please bring indoor scuff-free dance shoes or socks to dance in. See less Victoria, British Columbia Dance Victoria 2750 Quadra St # 111, Victoria Dance Victoria brings the "World's Best Dance" to the Royal Theatre and supports new dance creation for the international stage from its studios. Guests See All</t>
+        </is>
+      </c>
+      <c r="C192" s="3" t="n">
+        <v>45811.58969681713</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1142760357225336/</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 26 26 Jul at 10:00 – 27 Jul at 17:00 ArtisTREE Festival 1401 rockland ave, Victoria, BC, Canada About Discussion More About Discussion ArtisTREE Festival Interested Going Invite Details 988 people responded Event by Artistree Festival , MORENA CLOTHING and Cory Judge 1401 rockland ave, Victoria, BC, Canada Duration: 2 days Public · Anyone on or off Facebook Saturday July 26 10-7pm Sunday July 27 10-5pm Government House of BC 1402 Rockland Ave Celebration of Creativity profiling 130 Juried Artisans, Live Music, Installation and Performance Art, Indigenous Makers and Traditions, Kids section, Live Painters, Delicious Food and Ice cream. See less Shopping Victoria, British Columbia 1401 rockland ave, Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C193" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/651664851189740/</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 12:00-18:00 Music in the Orchard (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Music in the Orchard (RAIN OR SHINE) Interested Going Invite Details 140 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Come enjoy the start of the summer in the orchard. We have two amazing artists for you, some delicious fun summer ciders for you to try and amazing food to enjoy to complete the experience. Delicious Cider Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀ Beautiful location ⠀⠀⠀⠀ Dog Friendly ⠀⠀ ⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your WELL BEHAVED two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C194" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1399479741193649/</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Saxe Point Public House About Discussion More About Discussion TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Details 4 people responded Event by Tom Watson Saxe Point Public House Public · Anyone on or off Facebook Join Vinyl Wave at the lovely Saxe Point Pub for a couple of hours of smooth tunes that'll help ease you into the week! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C195" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/4223643791110348/</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Sunday 22 June 2025 at 13:00 Victoria Italian Day 195 Bay St, Victoria, BC V9A 3K4, Canada About Discussion More About Discussion Victoria Italian Day Interested Going Invite Details 3 people responded Event by Calabrisella 195 Bay St, Victoria, BC V9A 3K4, Canada Public · Anyone on or off Facebook Join us for live music, food, gelato, games, cars, cultural exhibits, vendors, bike valets and much more - Free admission !! Victoria, British Columbia 195 Bay St, Victoria, BC V9A 3K4, Canada 195 Bay St, Victoria, BC V9A 3K4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C196" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1198411931645258/</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Saturday 26 April 2025 from 15:00-18:00 LIVE MUSIC - The City Slickers 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion LIVE MUSIC - The City Slickers Details 21 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Members $5, Guests $10 Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C197" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/639017139056190/</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Saturday 19 April 2025 from 15:00-18:00 Live Music - Love Cats 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion Live Music - Love Cats Details 22 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Members $5, Guests $10 Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C198" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2579625309035667/</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Sunday 18 May 2025 from 12:00-18:00 Live Music @ Junction (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Live Music @ Junction (RAIN OR SHINE) Details 125 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Here we go again, its a long weekend so let's get our Sunday Funday on. First Live Music of the year at Junction Up first is-  Emergency Exit  are playing from 1230-230pm To take us home is - An &amp; Ben are playing from 3-5pm Tasting Room and Picnic Area are open 12-6pm Oh and if you haven't heard me say it before ITS RAIN OR SHINE. Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Cider ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Mini Market and a Beautiful location ⠀⠀⠀⠀⠀⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your well behaved two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C199" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3513597908934465/</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Saturday 12 April 2025 from 12:00-20:00 Live Music Benefit Event for Veteran's House 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion Live Music Benefit Event for Veteran's House Details 34 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 8 hr Public · Anyone on or off Facebook Admission by Donation (Non-Perishable Food Items, Charitable Donations, Gift Cards, accepted). Enjoy live music throughout the day by Bryce Allan, Love Cats, OTR, Donny Peterson &amp; the Tone Rangers, Helen Davies, and David Carl Trio. See less Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C200" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/979769967649565/</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 15:00-18:00 Live Music at the Legion 102-622 Admirals Rd, V9A 2N7 Sat, 17 May Sat, 24 May Sat, 31 May +2 About Discussion More About Discussion Live Music at the Legion Details 8 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Come enjoy live music on Saturdays 3-6 p. Dancing encouraged! Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C201" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1217747446718881/</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 18:00-22:00 Maifest - Evening of Live Music Edelweiss Club About Discussion More About Discussion Maifest - Evening of Live Music Details 36 people responded Event by Cindy Kent and Victoria Edelweiss Club Edelweiss Club Duration: 4 hr Public · Anyone on or off Facebook Join the Edelweiss Club for a lively evening of music and dance with Bijoux du Bayou and The Helen Davies Band. Let the infectious Zydeco beats and soulful rhythms set the tone for a night of fun, complete with delicious German snacks from the kitchen. Don’t miss out on this high-energy event! Get your tickets online or call 250-383-4823. www.victoriaedelweiss.ca/events See less Victoria, British Columbia Edelweiss Club 108 Niagara Street, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C202" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/986310396630042/</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>SATURDAY SONG-A-THON 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada About Discussion More About Discussion THE SATURDAY SONG-A-THON Details 9 people responded Event by Bucket Crab Johnny and CRAB BUCKET STUFF 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada Duration: 5 hr Public · Anyone on or off Facebook an INDOOR PICNIC PARTY with FREE LIVE MUSIC Click on the Photo at the top to see the whole poster and zoom in on the details. Victoria, British Columbia 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada THE SATURDAY SONG-A-THON 1 member active Open chat Guests See All</t>
+        </is>
+      </c>
+      <c r="C203" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1975172826621817/</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>(20+) Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Thursday 12 June 2025 from 19:00-20:30 Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Little Fernwood Gallery. About Discussion More About Discussion Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Interested Going Invite Details Event by Anna Bigland-Pritchard Little Fernwood Gallery. Tickets www.annabiglandpritchard.com/event-details/rest-resonate-restorative-yoga-ft-cozy-live-music Public · Anyone on or off Facebook Do you need some R&amp;R? Join Anna &amp; Roxie for a dreamy candlelit evening of restorative yoga, live music, and guided journalling. Facilitated by Roxie Fehr of Across the Water | Yoga Anna Bigland-Pritchard of ABP Music Studio | Music As experienced, intuitive space-holders, our goal to support your Nervous System and capacity for hope with a feast of restful offerings. We know life is stressful and we want to help you feel more connected to your intuition so you can not only survive, but also have the capacity to take the next right step in your life in a way that positively impacts the world. The space will be dreamy, there will be tea, guided journalling, poetry, restorative yoga shapes that can be adapted for any body, and LIVE MUSIC! Anna will be playing guitar, creating dreamy sound worlds with vocal looping, and singing you lullabies all evening. What to bring Yoga mat (We'll have a few available to borrow) Journal &amp; pen/pencil (We'll also have some spare paper and writing/drawing utensils) Yourself in your comfy cozies Details June 12, 7-8:30pm at Little Fernwood $42 Accessibility This event is on the ground floor There is a unisex/non-gendered bathroom on the same level We care about making this event accessible, so please let us know if you have any questions or accessibility needs. This will be a VERY gentle practice, and modifications will be offered. Happy pride! As members of and allies of the 2SLGBTQIA community, we (Anna &amp; Roxie) will create a supportive, inclusive, affirming environment and expect all participants to do the same. If cost is a barrier, please contact us directly as we have a limited number of discount codes available This is our first time offering this class, and we hope it will be a hit so we can make it a regular thing. Come as you are, leave nourished by your dreams See less Victoria, British Columbia Tickets Find Tickets Little Fernwood Gallery. 1923 Fernwood Ave., Victoria Meet your host Anna Bigland-Pritchard 5 past events · Page · Musician/band Based in Lekwungen territory (Victoria, BC), Anna Bigland-Pritchard is a: -Soprano -Voice teacher… Follow Suggested events Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested 6029 people interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends 40 people interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Veronica, Ali and 5 friends are interested 943 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Veronica, Ali and 5 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C204" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/665127126496204/</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Tuesday 27 May 2025 at 19:30 Live Music at the Saxe Point Public House Saxe Point Public House About Discussion More About Discussion Live Music at the Saxe Point Public House Details 9 people responded Event by VINYL WAVE Saxe Point Public House Public · Anyone on or off Facebook Live Music every other Tuesday starting May 27th! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C205" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1414577976223422/</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 19:00-23:00 Solstice Slammer 3 - Moon Under Water, Victoria The Moon Under Water Brewpub About Discussion More About Discussion Solstice Slammer 3 - Moon Under Water, Victoria Interested Going Invite Details 29 people responded Event by Electric Druids and Gate Theory The Moon Under Water Brewpub Tickets · CA$10 www.eventbrite.com/e/solstice-slammer-3-tickets-1389012316229 Public · Anyone on or off Facebook Come join us for Solstice Slammer III at Moon Under Water Brewpub and Distillery! Get ready to celebrate with Electric Druids, Gate Theory and Insulam, hefty drinks and good vibes. Whether you're a craft beer enthusiast or just an enthusiast, there's something for everyone at this epic night of live music. Don't miss out - mark your calendars! See less Music and audio Victoria, British Columbia Tickets Find Tickets The Moon Under Water Brewpub 5435 Fowler Rd, Saanich, BC V8Y 1Y4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C206" s="3" t="n">
+        <v>45811.59506936924</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/686146924271113/</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>(20+) Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Recommended events See all Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Friday from 16:00-22:00 Oak Bay Tea Party Roy and 6 friends Sunday from 10:00-18:00 Cook Street Village Block Party! Sophia and 5 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 5 Thursday from 19:00-22:00 Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz 753 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz Interested Going Invite Details Event by Adonis Puentes and Brent Jarvis 753 View St, Victoria, BC V8W 1J9, Canada Tickets hermannsjazz.com/reservations&amp;event_id=741898 Public · Anyone on or off Facebook An evening of Jazzy Cuban Fusion Music; traditional, contemporary, romance and dance. Juno &amp; Grammy Nominated vocalist, Adonis Puentes, will be joined by the Jazz Bohemians, featuring Brent Jarvis (piano), Ken Lister (bass), Nicholas Marquez (percussion) and Brooke Maxwell (Sax). Adonis Puentes opens up the marvelous world of Cuban music to his audience the second they hear his rich voice. When the other players kick in with their tight, multi-layered arrangements, it becomes clear that Adonis is a powerful bandleader. Fronting an acoustic band, Adonis' vocals are surrounded by piano, bass, strings, and percussion. Music reflects the present and Adonis Puentes is a Cuban Sonero for our times. Adonis thrives on the growth and acclaim for his original sonero sound. As he puts it, "I feel like a messenger of my roots and tradition, blessed that with me I have taken my music and heritage to many different places in the world; from Cuba, to Canada, USA, Mexico, Europe and Asia. My mission is to make you dance and enjoy my melodies and rhythms." Musician Line-Up: Adonis Puentes - Vocals Brent Jarvis - Piano Ken Lister - Bass Nicolas Marquez - Percussion Brooke Maxwell - Sax See less Music and audio Victoria, British Columbia Tickets Find Tickets 753 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Meet your hosts Adonis Puentes 33 past events · Page · Musician/band Adonis Puentes is a great singer and an elegant composer and lyricist grounded and nourished by his Cuban roots and worldly experience. Message Brent Jarvis 37 past events · Profile · Musician Message Suggested events Wed, 18 Jun at 16:00 Victoria Ska &amp; Reggae Fest Kickoff: Waahli, The Resignators, Hezron, Gun Street Ghouls &amp; Cabin Fever Victoria, BC, Canada, British Columbia 486 people interested Interested This Saturday at 21:00 Goth Nite: UNDERGROUND Victoria, BC, Canada, British Columbia 173 people interested Interested Thu, 19 Jun at 16:00 Victoria Ska &amp; Reggae Fest: Turbulence, La Severa Matacera, Spiritual Warriors, Sonic Alley &amp; Ari DL Victoria, BC, Canada, British Columbia 228 people interested Interested Popular with friends This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Friday at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 5 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Veronica, Ali and 5 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C207" s="3" t="n">
+        <v>45811.59506936924</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added an url relevancy check in ebs.py in eventbrite_search.
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C207"/>
+  <dimension ref="A1:C307"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3332,7 +3332,7 @@
         </is>
       </c>
       <c r="C193" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="194">
@@ -3347,7 +3347,7 @@
         </is>
       </c>
       <c r="C194" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="195">
@@ -3362,7 +3362,7 @@
         </is>
       </c>
       <c r="C195" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="196">
@@ -3377,7 +3377,7 @@
         </is>
       </c>
       <c r="C196" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="197">
@@ -3392,7 +3392,7 @@
         </is>
       </c>
       <c r="C197" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="198">
@@ -3407,7 +3407,7 @@
         </is>
       </c>
       <c r="C198" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="199">
@@ -3422,7 +3422,7 @@
         </is>
       </c>
       <c r="C199" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="200">
@@ -3437,7 +3437,7 @@
         </is>
       </c>
       <c r="C200" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="201">
@@ -3452,7 +3452,7 @@
         </is>
       </c>
       <c r="C201" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="202">
@@ -3467,7 +3467,7 @@
         </is>
       </c>
       <c r="C202" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="203">
@@ -3482,7 +3482,7 @@
         </is>
       </c>
       <c r="C203" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="204">
@@ -3497,7 +3497,7 @@
         </is>
       </c>
       <c r="C204" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="205">
@@ -3512,7 +3512,7 @@
         </is>
       </c>
       <c r="C205" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="206">
@@ -3527,7 +3527,7 @@
         </is>
       </c>
       <c r="C206" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
       </c>
     </row>
     <row r="207">
@@ -3542,7 +3542,1507 @@
         </is>
       </c>
       <c r="C207" s="3" t="n">
-        <v>45811.59506936924</v>
+        <v>45811.595069375</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/667083456006099/</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT Details 11 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 753 View Street (2nd floor, Hermmans Jazz Club) Date: Saturday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C208" s="3" t="n">
+        <v>45813.16284033565</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1910904133047825/</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY The Coda About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY Details 81 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 751 View Street (2nd floor, Hermmans Jazz Club) Date: Friday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C209" s="3" t="n">
+        <v>45813.16284033565</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1132427048350776/</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com or 15$ cash/e-transfer at the door. Formed in the heart of Chinatown, Rosebuds is a dynamic ensemble that brings the vibrant sounds of jazz, blues &amp; swing to life.  The group plays a mixture of originals and jazz standards, and is influenced by artists like Louis Armstrong, Billie Holiday, Lester Young, and Lionel Hampton. Featuring Rebecca Wells (vocals/guitar), Alex Moore (guitar/keys) Bryden Amos (guitar/keys), Matisse Gubby-Hurtig (bass), Owen Chow (trumpet), and Andrew Greenwood (tenor saxophone). Samba e Sol is a newly formed Brazilian bossa nova jazz trio featuring Andrew Greenwood (flute), Alex Moore (guitar), and Matisse Gubby-Hurtig (bass), playing music by artists like Antonio Carlos Jobim, Marcos Valle, Luiz Bonfa, and more. Instagram: https://www.instagram.com/rosebudsband/ See less Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C210" s="3" t="n">
+        <v>45813.16284033565</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1337760257449745/</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 5 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 10, 2025 | Lesson:   Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C211" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1861230087752141/</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 3 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 31, 2025 | Lesson:  Intro to Salsa with Adam &amp; Alicia Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C212" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/960236445839425/</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Saturday 22 June 2024 from 18:00-21:00 Kizomba/UrbanKiz at Clover Clover Pt, Victoria, BC V8S, Canada About Discussion More About Discussion Kizomba/UrbanKiz at Clover Interested Details 56 people responded Event by Becky Mowat Clover Pt, Victoria, BC V8S, Canada Duration: 3 hr Public · Anyone on or off Facebook Come join us for our first time dancing at Clover Point! There will be no lesson beforehand and this is super casual. Just a bunch of friends hanging out and dancing. Bring snacks, something to drink, blankets, warm clothes (as it is typically cooler by the ocean). There isn't a lot of parking at Clover Point but you can park along Dallas Rd and just walk down. Feel free to invite friends and family. Hope to see you all there! See less Victoria, British Columbia Clover Pt, Victoria, BC V8S, Canada 1301 Clover Pt, Victoria, BC V8S, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C213" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1293301738436581/</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Sunday 6 April 2025 at 17:00 Kizomba Sundown Party: Free of charge Method Studio - Victoria BC David Lamine Victoria invited you About Discussion More About Discussion Kizomba Sundown Party: Free of charge Details 58 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Method Studio - Victoria BC Public · Anyone on or off Facebook Free Pre-VIKFest party. Bring snack and drink. Expect great music, great energy, great atmosphere. "Dance with your heart. your feet will follow" Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C214" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1079226067560481/</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 41 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 6, 2025 | Lesson:  Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C215" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/372311028526699/</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Saturday 9 December 2023 from 20:30-23:30 Victoria Kizomba Social: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Social: Fall Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C216" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/947213690692385/</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C217" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1029869435768837/</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Saturday 22 March 2025 at 20:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC This event has been cancelled. You cannot share this event, but you can still post. About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 14 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C218" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1743571267040445/</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Ali Jorgensen invited you Interested Going About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Invite Details 37 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 8, 2025 | Lesson: Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C219" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/758501768607647/</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 6 6 Apr 2023 at 20:00 – 10 Apr 2023 at 10:00 Victoria International Kizomba Festival 4th Edition Victoria Conference Centre About Discussion More About Discussion Victoria International Kizomba Festival 4th Edition Going Details 702 people responded Event by Island Afro Latin Events Victoria Conference Centre Duration: 4 days Public · Anyone on or off Facebook Welcome to the Victoria International Kizomba Festival, APOCALYPSE EDITION!! What to expect?? Locally and Internationally renowned instructors, teaching Semba, Kizomba, Urban Kiz, Tarraxinha, Tarraxo, Douceur, Afro Beat, Afro House, Kuduro and More! ALL IN ONE: - Over 27.000 square feet of space - 3 ROOMS: Kizomba room, Urban Kiz room, Social room - After party room go until 6-7am with (Douceur, Tarraxinha and Sweet Kiz) VIKF 4rd Edition is offering you: *4 days of workshops *3 day-time socials *4 nights of dancing, *3 afterparties until 6-7am *15Hours + of workshops *40H + of dancing * 2 educational sessions of Cultural Aspect of African dances * 1 Gala Night of celebration of Multiculturalism, Diversity, the Arts including performances and fashion shows by African Designers IMPORTANT NOTICE: This 4 Day Festival has some free components offered to the general public as well as some activities with a minimal cost (to be announced at a later date) ARTISTS CONFIRMED - JP &amp; STEPHY (PARIS - FRANCE) - BONIFACIO (LISBON - PORTUGAL) - STEPHANE (PARIS - FRANCE) - SAMY (MONTREAL - CANADA) - LENA (VANCOUVER - CANADA) - ELVIS (OTTAWA - CANADA) - DJ PARAISO (PARIS - FRANCE) - DJ SINK (MONTREAL - CANADA) - DJ GUELAS (MIAMI - USA) - DJ MADARA (PARIS - FRANCE) AND MORE TO COME ... JP and STEPHY 10h Training program starts on Thursday April 6, 2023 in the afternoon DJ Training by DJ paraiso by Individual or Group of 4 (Friday - Saturday and Sunday) 10+ Taxi dancers 20+ International Special Guests HOTEL DEALS: WE HAVE 4 PREMIUMS HOTELS TO HOST YOU. A) FAIRMONT EMPRESS HOTEL is adjacent to the Convention Centre (all in one): TO BOOK YOUR ROOM: call the Reservations Department at 250 384 8111 or the Global Reservations Centre at 1 800-441-1414. Please identify yourself as being with the Victoria International Kizomba Festival group. TWO DOUBLE BEDS: $279 Rates will be available 3 days prior to the event and 3 days post B) MARRIOTT VICTORIA INNER HARBOUR, (just across the street, 1min walking distance) Book your accommodation by calling reservations toll-free at 1-888-236-2427 and asking for the "Victoria International Kizomba Festival group" to book online: https://www.marriott.com/event.../reservation-link.mi... 1 KING BED: $CAD199 2 QUEEN BEDS: $CAD199 C) DOUBLE TREE BY HILTON Reservations can be make by calling Central Reservations at 1-800-222-TREE and referencing KIZOMBA FEST 2023. or by using the HiltonLink: https://www.hilton.com/en/book/reservation/rooms/... - STANDARD ROOM: 2 QUEEN BEDS $CAD219 - SUITE WITH 2 QUEEN BEDS + SOFA BED, $CAD249 ALL rooms have all amenities (Fridge, kettle, Microwave, Iron, etc...) IMPORTANT NOTE: - If you are no longer able to join, you can transfer your pass to another participant without any fee; transfer your pass to the next edition; or ask for a refund within 15 days after the event. - Must be 18+ to attend this event - Click on the *Going* tab on facebook to receive notifications about line up updates and any useful information regarding this event. - By purchasing the pass, you grant the photographer, videographer, the Organization and its partners/sponsors  the permission to use your image  in any and all forms of media for commercial purposes, advertising, promotion... - COVID-19 clause: This event may be postponed or cancelled by the Organizer due to the Covid19 pandemic or any other resulting event related to the instructions of the federal government of Canada and the BC provincial government. In such case, the buyer can ask for a full refund. See less Dance Victoria, British Columbia Victoria Conference Centre 720 Douglas Street, Victoria The VCC is a boutique facility.  We’re small enough to be intimate yet able to handle conferences as Guests See All</t>
+        </is>
+      </c>
+      <c r="C220" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1179097320623502/</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 37 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C221" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1060779176049104/</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Thursday 3 October 2024 from 19:30-22:30 Kizomba Practica Thursdays: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Kizomba Practica Thursdays: Fall Series Details 20 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Join us every Thursday for Kizomba/Urbankiz classes. Intermediate 7:30PM-8:15pm Beginner 8:15pm-9:00pm Practica until 10:30pm Class only: $10 Class &amp; Practica: $15 or $10 for university students w/ID Practice only $10 Classes will be provided by your local Instructor (David Lamine) and assistants (Robyn, Becky) and occasionally by some out of town and International Instructors. Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C222" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3006474846197996/</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 30 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 27, 2025 | Lesson:  Intro class TBD Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro class TBD • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C223" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2637194793152555/</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 84 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 29, 2025 | Lesson:  Intro to Salsa Rueda with Sam and Katie Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa Rueda • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C224" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1184791909680061/</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Thursday 13 March 2025 from 19:30-23:00 Urban Kiz Workshop with Mannie Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 50 people responded Event by Becky Mowat and David Lamine Victoria Ukrainian Cultural Centre Duration: 3 hr 30 min Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C225" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1152065639712042/</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 20 20 Feb at 19:30 – 23 Feb at 23:00 Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Details 49 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 days Public · Anyone on or off Facebook Join us for our special edition Urbankiz &amp; Tarraxo workshops with Mike Ahombi Mike has been a big supporter of our VIKF and bringing his talent and low key vibe to the west coast. He is based out of Ottawa but you will find him at many different festivals and cities teaching Kizomba, Urbakiz and Tarraxo. We cannot wait for you all to have the opportunity to learn from such an incredible person and instructor. Details: Feb 20th Urbankiz Workshop 7:30pm-9:30pm Practica 9:30pm-11:00pm Feb 22nd Tarraxo Workshop 8:00pm-10:00pm Practica 10:00-11:30pm Price $90 Workshops only $70 Practica only $20 *** please e transfer to becksmith@hotmail.com *** Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C226" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3185065321631809/</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Saturday 15 March 2025 from 20:00-00:00 Urban Kiz Workshop with Mannie Method Studio - Victoria BC Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 48 people responded Event by Becky Mowat and David Lamine Victoria Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C227" s="3" t="n">
+        <v>45813.16810068287</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1813229489279716/</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Thursday 29 May 2025 from 19:55-21:00 Sensual Bachata 4 Week Series Method Studio - Victoria BC Thu, 15 May Thu, 22 May Thu, 29 May +1 About Discussion More About Discussion Sensual Bachata 4 Week Series Details 6 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 1 hr 5 min Public · Anyone on or off Facebook Ready to level up your Sensual Bachata? May 8, 15, 22, 29 Method Studio | 7:55–9:00 PM | $80 for all 4 classes Join us for an exciting and dynamic Bachata Sensual class designed for experienced beginners and intermediate dancers! We’re blending solid fundamentals with fresh, fun, and sensual combos to help you grow, challenge yourself, and have an amazing time on the dance floor. No partner needed — just bring yourself and your love for dance! Spots are limited — don’t miss out! Register by e-transferring $80 to maximumotion@gmail.com and mentioning “Bachata Sensual” in the notes. Get ready to connect, move, and elevate your dancing! P.S. All fees are non-refundable as they go directly toward securing the studio space and running the class. See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C228" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1300938064467261/</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Thursday 20 March 2025 from 20:00-22:00 Intermediate Sensual Bachata Workshop Method Studio - Victoria BC About Discussion More About Discussion Intermediate Sensual Bachata Workshop Details 24 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 2 hr Public · Anyone on or off Facebook Sensual Bachata Workshop in March! Intermediate workshop - March 20 Time: 8:00-9:30 PM + Practice 9:30-10:00 PM Location: Method Studio, 841 Fisgard St. Cost: $30 per workshop (includes 2 hours!) Intermediate workshop: Take your skills to a higher level! Master the advanced variations of the Madrid pass, smooth transitions and musicality. No partner needed, just bring your energy and comfortable shoes! Register at: maximumotion@gmail.com #BachataWorkshop #VictoriaBC #LearnToDance #BachataLovers See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C229" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1069894401564900/</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Monday Nights! 111 Superior St, Victoria, BC V8V 1T2, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion Sensual Bachata Series – Monday Nights! Details 15 people responded Event by Victoria Latin Dance Association 111 Superior St, Victoria, BC V8V 1T2, Canada Duration: 3 hr Public · Anyone on or off Facebook Sensual Bachata Series – Monday Nights! Mondays – April 7th, 14th, 21st &amp; 28th at 111 Superior Street Foundation Class (6:30–7:35 PM) Perfect for absolute beginners or dancers looking to strengthen their foundation! In this class, we’ll break down the essential steps, body movement, and partner connection in a fun environment. You’ll learn the basics with proper technique while also adding styling to make your dancing look and feel smooth on the dance floor. No experience or partner needed—just bring your curiosity and energy! Intermediate Class (7:35–8:40 PM) Ready to level up? This class is designed for dancers who already feel comfortable with the basics and want to challenge themselves. We’ll dive into more fun patterns while also exploring musicality—how to connect those movements to the music in a more expressive way. Get ready to build confidence, fluidity, and your own unique style! To Register: Send your e-transfer to maximumotion@gmail.com and include in the memo: Foundation, Intermediate, or Both + Lead or Follow Class Cancellation &amp; Refunds We understand that plans can change. However, due to limited spots, renting space in advance, and the preparation required for each class, we’re unable to offer refunds for cancellations. Please make sure you’re committed before signing up. We truly appreciate your understanding and support! See less Victoria, British Columbia 111 Superior St, Victoria, BC V8V 1T2, Canada 111 Superior St, Victoria, BC V8V 1T2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C230" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/692165093260868/</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 13:00-16:00 Salsa &amp; Bachata Masterclass with Adam &amp; Ghada Solwood Studio About Discussion More About Discussion Salsa &amp; Bachata Masterclass with Adam &amp; Ghada🔥 Details 60 people responded Event by Dancing Time Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook Hello everyone! Spring is here, and many things are happening, but I can’t but dance with you one last time before leaving for the entire summer!! To make things spicy, I am extremely happy to collaborate with Adam on a Salsa &amp; Bachata Masterclass! Get ready to learn details that will help you with creating flow – both as leads and follows – in addition to some socials-friendly tricks! Date: Saturday, May 10 Time: 1:00-2:30 | Salsa, 2:30-4:00 | Bachata Price: 25$ for one class, 35$ for two classes Location: Solwood studio, 1303 Broad st To register, please fill in this quick form and send an e-transfer to ghadacyoussef@gmail.com. https://forms.gle/4QThxT6yByd3h5KH8 Note: kindly understand that no-shows and cancellations made in less than 1 week from the workshop cannot be refunded. I will be happy to fully refund for earlier cancellations if need be. See less Victoria, British Columbia Solwood Studio Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C231" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1350929566137538/</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 4 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation August 10, 2025 | Lesson: Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C232" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/9677364319006080/</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 51 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation July 20, 2025 | Lesson:  Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C233" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1901245437276872/</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Friday 9 May 2025 from 20:00-00:00 Bachata Nights Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Details 40 people responded Event by Bachata Nights Victoria BC , Alysha Kopala and Sebastian Carmona Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights May 09 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @yourgirlalysha  and @davidch_78  will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person The evening starts with an Open-level Bachata lesson from 8:15 PM to 9:00 PM—great for all skill levels! Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C234" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1057471579628015/</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Friday 16 May 2025 at 17:00 Bachata Nights Victoria Bc Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Victoria Bc Details 9 people responded Event by Bachata Nights Victoria BC and Sebastian Carmona Method Studio - Victoria BC Public · Anyone on or off Facebook Join us on our next Bachata Nights May 23 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C235" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/717475250956404/</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Friday 30 May 2025 at 18:00 FREE Beginner Bachata Class 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 About Discussion More About Discussion FREE Beginner Bachata Class Details 65 people responded Event by Mayfair Shopping Centre and Victoria Latin Dance Association 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 Public · Anyone on or off Facebook Ready to get your groove on? We’re teaming up with the Victoria Latin Dance Association  for a FREE Beginner Bachata Class right here at Centre Court! Join us on Friday, May 30 at 6:00 PM for an evening of fun and dancing. FREE Beginner Bachata Class May 30th, Friday at 6PM NO partner or experience necessary! Bachata is a beautiful and easy-to-learn dance that’s great for meeting new people, getting active, and connecting with an amazing community. See less Dance Victoria, British Columbia 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 3147 Douglas St, Victoria, BC V8Z 3K3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C236" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342233713680795/</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Thursday 1 May 2025 at 21:00 Bachata &amp; Merengue- All Levels- May Series Studio 4 Athletics About Discussion More About Discussion Bachata &amp; Merengue- All Levels- May Series Details 3 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Bachata &amp; Merengue are both dances from the Dominican Republic. Bachata can be anywhere from slow and romantic with lots of dips, sway and body movement to more upbeat and percussive with lots of musical footwork. Merengue is carefree, flirtatious and fun! Classes are registered on a monthly basis and take place every Thursday from 8:00- 9:00pm, May 1, 8, 15, 22, 29. No experience required.  No partner is necessary as we rotate partners throughout the lesson.  Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C237" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3975145332748137/</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Friday 13 June 2025 from 20:00-00:00 Bachata Night Method Studio - Victoria BC About Discussion More About Discussion Bachata Night Interested Going Invite Details 47 people responded Event by Bachata Nights Victoria BC , Sebastian Carmona and Alysha Kopala Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights June 13 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C238" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1388695712154512/</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 67 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation June 22, 2025 | Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C239" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342792743590871/</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Monday 7 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- April series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, April 7, 14, 28. Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C240" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1382188962971661/</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Tuesday 1 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Fundamentals- April Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- April Series Details 9 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, Apr 1, 8, 15, 22, 29 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C241" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1298465587898458/</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Tuesday 4 March 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- March series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- March series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Mar 4, 11, 18, 25 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C242" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/966455485665576/</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Thursday 3 April 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- April series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Apr 1, 8, 15, 22, 29 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C243" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/679241811720932/</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Fundamentals- May Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- May Series Details 7 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, May 6, 13, 20, 27 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C244" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/669591372187091/</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 10:00-11:00 Salsa &amp; ChaCha Solo Westshore Dance Studios Sat, 17 May Sat, 24 May Sat, 31 May +7 About Discussion More About Discussion Salsa &amp; ChaCha Solo Details 2 people responded Event by Dance Praktika Westshore Dance Studios Duration: 1 hr Public · Anyone on or off Facebook Elevate your dance journey with our Ladies Solo Class. Join our exciting series and learn the basics of Salsa and Cha Cha. Perfect for beginners looking to spice up their dance skills! Class Highlights: - Learn exciting dance moves tailored for solo dancers; - Fun and welcoming environment; - Suitable for absolute beginners. Come dance with us and let the rhythm guide you! To register to April classes please use links at "Tickets". See less Langford, British Columbia Westshore Dance Studios 109-2675 Wilfert Road, Victoria www.westshoredance.com 2years+ Competitive&amp;Production a space for everyone with a love of dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C245" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/10048344358532607/</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- May series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. May 6, 13, 20, 27 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C246" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2233725973712106/</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Monday 3 March 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- March series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- March series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, Mar 3, 10, 17, 24, 31 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C247" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2214494908966327/</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Monday 5 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Int/ Adv- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- May series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, May 5, 12, 26 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C248" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1239163193996279/</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 14 Saturday 14 June 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Tickets · CA$17.31 www.eventbrite.com/e/caliente-salsa-saturdays-tickets-1390062838369 Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in May. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Tickets Find Tickets Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 49 people interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Janine and 4 friends are interested 956 people interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends 47 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C249" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/624858640069610/</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 Friday 22 August 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 7 friends 216 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 41 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 67 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C250" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1636237610432412/</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Saturday 16 August 2025 from 20:00-23:59 Salsa Sunset Latin Party – August 16th! Latin Dance Canada About Discussion More About Discussion 🌅🔥 Salsa Sunset Latin Party – August 16th! 🔥🌅 Interested Going Invite Details 29 people responded Event by Latin Dance Canada Latin Dance Canada Duration: 3 hr 59 min Public · Anyone on or off Facebook Salsa Sunset Latin Party – August 16th! Get ready for a magical summer night filled with Latin rhythms, sunset vibes, and non-stop dancing! Join us for the Salsa Sunset Latin Party, where the Salsa, Bachata, and Merengue beats will keep you moving all night long under the stunning sunset sky! Dress Code: Wear your best sunset-inspired outfit – think bright, tropical colors, and beach party vibes! Dance to the best Salsa, Bachata, Merengue &amp; Latin hits all night! No partner? No problem! Join our fun intro class at 8:00 PM! Location: Ukrainian Cultural Centre, 3277 Douglas St., Victoria, BC Date: Saturday, August 16, 2025 Intro Class: 8:00 PM | Social Dance: 8:30 PM - Late Entry: $15 at the door – Bring cash, please! What to Expect: Vibrant salsa rhythms &amp; tropical vibes! Tropical-themed decorations &amp; stunning sunset views! A welcoming dance community &amp; unforgettable fun! Let’s dance as the sun sets and make it a night to remember! Tag your friends and let’s create memories under the summer sky! #SalsaSunsetLatinParty #SalsaBachata #LatinDanceParty #VictoriaBC #LatinDanceCanada See less Dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C251" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/939376108286434/</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Friday 27 June 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 16 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Ali and Dalie 35 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 67 people interested Interested This Saturday at 21:00 Goth Nite: UNDERGROUND Victoria, BC, Canada, British Columbia 179 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C252" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/884101187183426/</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 July 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in June. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Janine and 4 friends are interested 956 people interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends 47 people interested Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 7 friends 216 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C253" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/530862806349067/</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Sunday 30 March 2025 from 13:00-17:00 Salsa Gonzales tasting! 🍋‍🟩 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia About Discussion More About Discussion Salsa Gonzales tasting! 🍋‍🟩 Details 6 people responded Event by THE ROOT CELLAR | village green grocer 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia Duration: 4 hr Public · Anyone on or off Facebook Hey friends! It's time to get those tastebuds tingling - you're invited to come and join us for a Salsa Gonzales tasting at our McKenzie Corner store! Salsa Gonzales is a little condiment company with a big personality! Nestled on Gonzales Beach in Victoria, they craft salsas, hot sauces, pickles, preserves, and more – all with a generous splash of love and a fiery kick. When: Sunday March 30th, 1pm-5pm Where: Our McKenzie Corner location We're looking forward to seeing you there! XO See less Victoria, British Columbia 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia 1286 McKenzie Ave, Saanich, BC V8P 5P2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C254" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3899920353641309/</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 9 Saturday 9 August 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in July. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 177 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 49 people interested Interested Mon, 30 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne and Ali 22 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C255" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/909522138040202/</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Friday 28 November 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 7 friends 216 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 41 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 67 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C256" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1059622278965884/</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 8 Saturday 8 November 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in October. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 177 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Sophia, Lorne and 10 friends 1091 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Lorne and 3 friends 67 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C257" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1618420955545842/</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Tomorrow from 18:00-19:30 Ladies Styling Bootcamp With Hannah Aylene Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 30 Friday 30 May 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing at an all ages venue with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 9 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 2 friends 56 people interested Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Roy and 7 friends 216 people interested Interested Mon, 30 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne and Ali 22 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C258" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2251848171850840/</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Tomorrow from 18:00-19:30 Ladies Styling Bootcamp With Hannah Aylene Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 Saturday 10 May 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in April. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 177 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 49 people interested Interested This Saturday at 21:00 Goth Nite: UNDERGROUND Victoria, BC, Canada, British Columbia 179 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C259" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1624603351798270/</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Tomorrow from 18:00-19:30 Ladies Styling Bootcamp With Hannah Aylene Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 April 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 14 Jun at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 177 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 49 people interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends 47 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C260" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1356293392177099/</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Monday 3 March 2025 from 18:30-21:30 Open House | FREE Classes - Bachata Sensual &amp; Brazilian Zouk 1709 Blanshard St, Victoria, BC V8W 2J8, Canada About Discussion More About Discussion Open House | FREE Classes - Bachata Sensual &amp; Brazilian Zouk Details 28 people responded Event by Bachata and Zouk with Javi in Victoria and Javi Zouker 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 3 hr Public · Anyone on or off Facebook Join us for our Open House / Free classes on Monday March 3rd with Javi Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on body awareness, lead and follow techniques, musicality, styling, and how to have lots of fun dancing with new friends!  Learn with Javi, with over ten Years of teaching experience.  Learn dance with clear, fun, and inspiring teachings open to all levels! Schedule: Monday March 3rd 6:30-6:45pm | Meet &amp; Greet 6:45-7:30pm | Traditional Bachata - Beginner 7:40-8:25pm | Sensual Bachata - Intermediate 8:35-9:20pm | Brazilian Zouk - Beginner 9:20-9:30pm | Sharing circle Tuition = FREE Space is Limited:  Please email us to register your spot and please share if you are leading or following or open to either. email:  danceinflow@gmail.com 4 week session on Monday March 10-31st Phillippine Bayanihan Community Centre - 1709 Blanshard st, Victoria, BC See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C261" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1106484714432492/</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Wednesday 11 June 2025 from 18:30-21:00 Zouk practica and social White Eagle Hall, 90 Dock St, Victoria BC Wed, 28 May Wed, 4 Jun Wed, 11 Jun Wed, 18 Jun +29 About Discussion More About Discussion Zouk practica and social Interested Going Invite Details 2 people responded Event by Victoria Zouk Collective and Victoria Zouk Collective Group White Eagle Hall, 90 Dock St, Victoria BC Duration: 2 hr 30 min Public · Anyone on or off Facebook Drop-in zouk practica by donation - everyone welcome! White Eagle Polish Hall every Wednesday 6:30-9 pm Shared warm up, free dance time, review material from lessons and congresses, connect and share knowledge! Help is always available. Minimum $5 donation. Cash at the door, or etransfer to oceanzouk@gmail.com Enter the lower hall by the side door on Niagara Street just beside the Polka food truck. Also available in Victoria are zouk lessons with Javi, an amazing instructor from Vancouver! More info at https://www.facebook.com/Sabor.Asi.Dance.Salsa.Victoria or email danceinflow@gmail.com See you there! See less Victoria, British Columbia White Eagle Hall, 90 Dock St, Victoria BC 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C262" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1411005319893067/</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Monday 28 April 2025 from 18:30-22:30 Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion 🔥Bachata &amp; Brazilian Zouk 🌊 dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard Details 7 people responded Event by Bachata and Zouk with Javi in Victoria 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 4 hr Public · Anyone on or off Facebook Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard street | Victoria Join us for a 4 week course exploring the joy and magic of Brazilian Zouk &amp; Bachata dancing! Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on enhancing body awareness, building confidence in dance vocabulary with lead and follow techniques, exploring musicality, and loving yourself deeper with styling! Be prepared to have lots of fun dancing with new friends! Register today! Schedule: Monday April 7 - 28th 6:30-7:25pm | Brazilian Zouk - Level 2 (ask Javi for permission) 7:30-8:25pm | Brazilian Zouk - Level 1 8:30-9:25pm | Sensual Bachata - Beginner Foundations 9:30-10:30pm | Sensual Bachata - Intermediate "Trending Moves" Tuition: $20 | 1 Class $35 | 2 Classes (Brazilian Zouk 1&amp;2, or Brazilian Zouk 1 &amp; Bachata, Bachata 1&amp;2) $50| 3 Classes (3 classes, BEST value) 1709 Blanshard St, Victoria, BC Registration: E-transfer to: danceinflow@gmail.com or send us a message on Whatsapp: 7785877665 (Also accepting credit card/cash at the door) Please add a note if you're registering as a "Leader", "Follower", or "Open to both" Space is limited. Register in advance to reserve your spot! Looking fwd to dancing and flowing with you, Warmly, Javi See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C263" s="3" t="n">
+        <v>45813.17928960648</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/544121845403419/</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 13:00-23:55 Swing Session: Balboa with Yoshi and Etsuko Solwood Studio About Discussion More About Discussion Swing Session: Balboa with Yoshi and Etsuko Details 108 people responded Event by Swing Dance Association of Victoria , Dave Henderson and 2 others Solwood Studio Duration: 10 hr 55 min Public · Anyone on or off Facebook Lace up your shoes on May 31, 2025 for an afternoon of Balboa Classes and an evening of Social Dancing with Yoshi and Etsuko Uemura. 4 Classes for everyone &amp; 1 Social Dance! Passes go on sale April 19 at noon at our SDAV Square Shop! You must know and be comfortable with Balboa basics for all of these classes - they won't be covered at this workshop. All the specifics are available at swingvictoria.net , but here are the notes: May 31st, at Solwood Studio, with doors at 12:30pm . Bring indoor shoes, please! 4 classes for everyone and there's a dance from 9-12am. Passes go on sale April 19th at noon. See less Victoria, British Columbia Solwood Studio 1303 Broad St, Victoria, BC V8W 2A8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C264" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1692156731689650/</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Tuesday 17 June 2025 from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 Tue, 27 May Tue, 3 Jun Tue, 17 Jun Tue, 24 Jun +22 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Interested Going Invite Details 2 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Saanich, BC V8Z 3S3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C265" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/402729737034904/</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Thursday 5 September 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Details 123 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for our second fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C266" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1594011994641933/</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Tuesday 22 April 2025 from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Details 9 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. No street shoes. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C267" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/634773653668605/</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Saturday Night West Coast Swing BC Swing Dance Club Victoria 15 Jun 2019 22 Jun 2019 29 Jun 2019 +2 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night West Coast Swing Details 9 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook June means summertime and sunny days! Along with the weather, things for BC Swing Dance Cub Victoria will be changing too. Here's what is happening this month: 7 - 8pm 1st Saturday of the Month: Lesson with Meaghan, plus an assistant from our dance community 7 - 8pm Remaining Saturdays each month: TBD (stay tuned for workshops, activities or practices - updates will be posted on each event page) Note:  The 7 - 8pm weekly timeslot is included in the dance entrance price. -------------------------------------------------- Come join us every Saturday all year long for a fabulous WCS social dance from 8 - 11pm. Just $10 for the ($5 for students). Meaghan Efford and Bob Gebbie 's lesson on June 1st (starting PROMPTLY at 7pm) will be the only lesson in June, and it will be a great way to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity.  The lesson is included in the dance entrance price.  No experience or partner is required. -------------------------------------------------- • 6:45 pm - Doors open • 7:00 pm - TBD each week* • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *lesson with Meaghan and Bob on June 1st Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C268" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/417338985546213/</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Thursday 29 August 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - August 29! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - August 29! Details 109 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for a fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C269" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663135653237580/</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Method Studio - Victoria BC Canice Ma invited you Interested Going About Discussion More About Discussion WACK! Another West Coast Swing Social Dance Invite Details 37 people responded Event by Canice Ma and Wyatt Ritchie Method Studio - Victoria BC Duration: 3 hr 30 min Public · Anyone on or off Facebook Guess who's back, it's WACK! (please ignore the fact that it's been 2 years...) The schmucks are back with another spontaneous west coast swing social dance, featuring music by DJs Topknot and Amandance from Vancouver! DETAILS: • Friday, June 20th, 2025 • Method Studio, 841 Fisgard St, Victoria, BC • 7:30-11 pm: social dancing with 100% west coast swing (sorry, no lesson!) • Admission: $10 • Water and AC on us (and maybe some bonus chocolate) • Please keep in mind that parking is limited at the venue GENERAL SOCIAL DANCE ETIQUETTE: • Consent is cool- don't be creepy. • Shake off any shyness and get out there! Ask people to dance regardless if you’re a lead or follow, dancing for 10 years or started yesterday- it's more fun that way! • No teaching or unsolicited feedback on the dance floor. Good vibes only! • If you would like to partake in a steal dance, try to remain with that group for the whole song. • Bring a water bottle! The studio is known to get warm with more bodies in the space so we want you to stay healthy and hydrated. • Personal hygiene is important! Consider bringing a towel and/or a spare shirt to change into if you sweat easily. Our studio has a bathroom and change rooms available for all to use. • We recommend wearing clothes that are easy to move in, especially pants given the nature of the dance. • Clean, comfortable shoes (ideally dance shoes) on the dance floor only! See less Victoria, British Columbia Method Studio - Victoria BC 833 Fisgard St, Victoria, BC V8W 1R9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C270" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663756533046485/</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Friday 11 April 2025 at 21:30 Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. Details 36 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Public · Anyone on or off Facebook Miguelito Valdes presents Contodo What happens when you bring together three Cuban and two Canadian musicians, with a deep love of all music and a wide range of musical experiences?  A joyful mix of party and deep groove, that's what! Guaranteed to make you want to dance, these brothers from other mothers bring it all. Con Todo! Featuring: Miguelito Valdes – brass/vocals/percussion Jose Sanchez – drumset/timbales Hector Ramos – congas/percussion Peter Dowse - bass Brooke Maxwell – keys/vocals See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C271" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1776457206589544/</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Friday 21 March 2025 from 18:30-20:30 Slim Sandy's Atomic Cocktails swing speakeasy party! The Coda About Discussion More About Discussion Slim Sandy's Atomic Cocktails swing speakeasy party! Details 72 people responded Event by Peter Sandmark and Trace Nelson The Coda Duration: 2 hr Public · Anyone on or off Facebook Join Slim Sandy's Atomic Cocktails and dance as they play 2 sets of swing jazz, jive and rhythm and blues from the 20’s to the 40’s. Slim, on guitar and harmonica, is joined by Willa Mae on vocals, “Big Daddy Bo” on bass, and Bryn Bad on trumpet.  Slim Sandy has been playing music for over 40 years with acts such as Ray Condo and the Crazy Rhythm Daddies.  In 2012, he and Willa Mae co-created the Slim Sandy band in Victoria!  They have played music festivals in Canada, France, Spain, Germany, Belgium, and the Netherlands.  In May they will be touring in Japan! See less Victoria, British Columbia The Coda 749 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C272" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/302778660295534/</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Sunday 19 August 2018 from 18:00-21:00 West Coast Swing in the Park! Cameron Bandshell @ Beacon Hill Park Carolyn Gebbie invited you About Discussion More About Discussion West Coast Swing in the Park! Details 58 people responded Event by Carolyn Gebbie Cameron Bandshell @ Beacon Hill Park Duration: 3 hr Public · Anyone on or off Facebook Come join us for another evening of fun and WCS dancing in Beacon Hill Park! WCS music will be provided by DJ Carolyn. For those who are familiar with the routine, the 2018 WCS Rally Song will be played at 6:30, 7:30 and 8:30pm. Sam Jackson and Meaghan Efford, from wcsmovementmethods.com will be on hand to answer questions about WCS or how to improve your WCS dancing. They will also demo some incredible WCS dancing at 7pm. Please invite your WCS dance friends by sharing this event! See less Victoria, British Columbia Cameron Bandshell @ Beacon Hill Park Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C273" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1035925295253912/</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Friday 18 April 2025 at 18:30 Swing out with the ATOMIC COCKTAILS 751 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Swing out with the ATOMIC COCKTAILS Details 64 people responded Event by Peter Sandmark 751 View St, Victoria, BC V8W 1J9, Canada Public · Anyone on or off Facebook Join the ATOMIC COCKTAILS as they swing out for their pre-Japan Tour dance party on April 18 at the Coda, 751 View Street.  Doors open 6 pn, show from 6:30-8:30 pm!  Tickets $20.  With songs from their new album BLUE LIGHT BOOGIE! See less Victoria, British Columbia 751 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C274" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/373500473108499/</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>Sunday Swing at Logan's Logan's Pub 10 Dec 2017 Debi Wong invited you About Discussion More About Discussion Sunday Swing at Logan's Details Event by Swing X Logan's Pub Duration: 3 hr 30 min Public · Anyone on or off Facebook Sunday Swing at Logan's is BACK! Come join us for some great tunes and we'll party like it's 1939. Bring your dancing shoes, sweet moves, and a few dollars for our fabulous DJ (and gracious bartenders). Feel free to come early to hang out and grab a bite to eat. 19+. NEW: Crash course 15min swing lesson at 8:30pm! This is intended to be the bare minimum for someone to show up and know the basics of swing dancing, nothing fancy! DETAILS: * 8:30pm Quickie 15min beginner lesson! * 8:45pm social dancing until as late as midnight (maybe!) * Usually gets bluesy after 11pm See less Victoria, British Columbia Logan's Pub 1821 Cook Street, Victoria Original - Authentic - Unique Guests See All</t>
+        </is>
+      </c>
+      <c r="C275" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2441697862726705/</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Sunday 30 June 2019 at 19:00 Journey’s 50th Birthday!!  A West Coast Swing dance party!! Eastern Star Hall Chapters No 5 &amp; No 17 Journeey Song invited you About Discussion More About Discussion Journey’s 50th Birthday!!  A West Coast Swing dance party!! Details 13 people responded Event by Journeey Song Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook 3281 Harriet Road, Victoria,BC Bring your own alcohol-free beverage... Bring a gluten-free appie if you’d like. Dance West Coast Swing until 10 pm to Blues, Pop, RnB, Swing, and a wee bit of Ballroom Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C276" s="3" t="n">
+        <v>45813.18556971065</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/644050564927019/</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends! A NEW SUNDAY AFTERNOON MILONGA! This is the first of a regular monthly milonga at a beautiful new venue…The Coda Club (formerly Hermann’s Upstairs) at 751 View Street, Victoria. Great ambience, nice wood floor, good sound system. So come join us for the warm hugs and close embrace and dance to the beautiful music of our very own DJ John Dewhirst. Sunday, 6 April 2025 2.00pm-5.00pm The Coda Club, 751 View Street, Victoria Admission $15 DJ: John Dewhirst Cash Bar is open for drinks Free Parking at View Street Parkade just next door Come celebrate this exciting day with us! See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C277" s="3" t="n">
+        <v>45813.18861127315</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1766891834185825/</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Interested Going Invite Details 38 people responded Event by Jeannie Kam and Alive Tango Victoria Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends SAVE THE DATE! The next Sunday afternoon Milonga is on 8 June 2025 1-4pm. The Coda Club (formerly Hermanns Upstairs) is a beautiful newly renovated venue with awesome ambience, nice wood floor and great sound system. Come join us for a wonderful afternoon of warm hugs and close embrace. Sunday 8June 2025 1-4pm The Coda, 751 View Street, Victoria Admission: $15 (plus tax) Special Guest DJ: Francis Nowaczynski (from Vancouver) Free parking at View Street Parkade (next door) or Broughton Parkade. Cash bar is open for drinks. See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C278" s="3" t="n">
+        <v>45813.18861127315</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/713923214640962/</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Sunday 4 May 2025 from 13:00-16:00 May 4th Afternoon Milonga Solwood Studio About Discussion More About Discussion May 4th Afternoon Milonga Details 45 people responded Event by Ingrid Love and Kathryn Stone Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook A one-time special afternoon milonga! Join us in celebrating the warmth of Spring and return to sunshine. Or, star wars, if you like. Featuring special guests Kimberly and Khang performing live music (violin/guitar) DJ Ingrid Hosts: Kathryn &amp; Ingrid $15 entry (cash only) 1:00pm-4:00pm Solwood Studio 1303 Broad St Victoria, BC See less Victoria, British Columbia Solwood Studio Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C279" s="3" t="n">
+        <v>45813.18861127315</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1838888640215250/</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Friday 28 February 2025 at 19:00 Argentine Tango for Beginner - level 2 1303 Broad St, Victoria, BC V8W 2A8, Canada About Discussion More About Discussion Argentine Tango for Beginner - level 2 Details 19 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria 1303 Broad St, Victoria, BC V8W 2A8, Canada Public · Anyone on or off Facebook We are happy to announce that we continue with Argentinian Tango for Beginners - level 2. This 6 weeks session is progressive and requires preregistration. It is designed for students who have completed Beginner - level 1 or would like to deepen their skills. If not sure where you are with your tango contact us To register email us : grazs@shaw.ca or PM Grazyna Feb 28th - April 4th Fridays 7-8pm Price per person : $80 series (6 weeks) See less Victoria, British Columbia 1303 Broad St, Victoria, BC V8W 2A8, Canada 1303 Broad St, Victoria, BC V8W 2A8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C280" s="3" t="n">
+        <v>45813.18861127315</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1318668532737609/</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 16 16 Apr at 18:30 – 18 Apr at 21:00 Tango week with Lya Alive Tango Victoria About Discussion More About Discussion Tango week with Lya Details 36 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 3 days Public · Anyone on or off Facebook Ignite Your Tango 16th of April, Wednesday 6:30-8:00 On &amp; Off Acis for social dance 18th of April, Friday 6:00 - 7:30 Follower technique 7:45 - 9:00 Switch role / connection Search - Grow &amp; Transform! Seminar series for Tango Dancers that want to transform their way of moving and connecting! We will travel through the Essentials of Tango in order to look for new answers and deeper understanding. What makes tango truly captivating? It’s the embrace, the connection, and the walk. These three fundamental elements are the heartbeat of tango, and mastering them is essential for creating an unforgettable dance experience. You will learn how to condition your body to move with control, fluidity, and elegance. You’ll discover how to find and perfect your axis, which is essential for maintaining balance and stability in every step. We will also explore dissociation, a technique that allows you to move the upper and lower body independently but associated. This workshop series will show you how to apply these principles in both the leader and follower roles, improving connection and response in every moment of the dance. We will apply all this to: The secrets to generating power for boleos effortlessly off and on axis special follower technique class Pro tips to dance with ease and confidence 90 min class - $30 All 3 classes - $80 To register email grazs@shaw.ca or pm me, or talk to me . See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C281" s="3" t="n">
+        <v>45813.18861127315</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1009684807956058/</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 17 17 May at 17:00 – 18 May at 13:30 Tango weekend with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Tango weekend with Jorge Olguín Details 28 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 17th 5pm-6pm solo technique all levels. ( no partner required) Please bring elastic bands!! 6.30pm-7.30pm for couples only ( need some experience) Sacadas, barridas and colgadas in an elastic embrace in order to create a circular movement. We will work with different orchestras to study the changes we need to do to introduce different tempos and rhythms. Get ready for a workout with musicality! 8pm milonga !!! Join us even if you didn’t take the classes. DJ Ingrid !! Free for people registered for the workshops. $10 for drop-ins. Sunday, 18th 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are June 21st &amp; 22nd Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C282" s="3" t="n">
+        <v>45813.18861127315</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3637725693193744/</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 22 Mar at 17:00 – 23 Mar at 13:30 Weekend with Tango with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Weekend with Tango with Jorge Olguín Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 22nd 5pm-6pm solo technique all levels. Balance and weight transfer while walking, change of dynamics to create a better connection with your body. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) Marathon is just around the corner so this month we continue with comfortable close embrace! We continue with dancing in small spaces!! Let’s move gracefully without affecting the partner's axis in elastic hugs of closed embrace. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 23rd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available only on Saturday. Sunday - sold out Next workshop dates are the May 17th &amp;18th Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C283" s="3" t="n">
+        <v>45813.18861127315</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1864555154338100/</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 21 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Alive Tango Victoria About Discussion More About Discussion Weekend with Tango Interested Going Invite Details 12 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 21st 5pm-6pm solo technique all levels. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) We will continue from May with the musicality for phrase change but this time we will add “double time” to help us with it, using examples of different orchestras. We will work with a “rebound” and half giros to change the direction within the phrase. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 22nd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are September 20th &amp; 21st. Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C284" s="3" t="n">
+        <v>45813.18861127315</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/967438905456066/</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Wednesday 26 March 2025 at 10:00 Victoria WCS Lesson and Dance at Eastern Star Hall Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria WCS Lesson and Dance at Eastern Star Hall Details 1 person responded Event by Donna Forsyth Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson by John de Pyffer from 7 to 8 pm Social dancing from 8 to 10:15pm Djs Amanda and Nel Cost $12 No need to register and no partner required. Please bring scuff-free indoor shoes or socks to dance in  and a water bottle. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C285" s="3" t="n">
+        <v>45813.19128471065</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2162855673833831/</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 11 May 2019 18 May 2019 25 May 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 8 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook Wow! April went by so quickly, which means it must've been super fun, which it definitely was.  Everyone at BC Swing Dance Club Victoria is so pleased with the way the first month of social dances went, and we hope to generate the same amount of enthusiasm in May. Let's make this month just as much fun! Come join us on May 4th for the first intro lesson and social dance of the month (plus every Saturday night after that). Just $10 for the lesson and/or social dance ($5 for students). No experience or partner required. • 6:45 pm - Doors open • 7:00 pm - Intro lesson with Sam Jackson and Meaghan Efford * • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *PLEASE NOTE that the weekly lessons will start PROMPTLY at 7pm.  It is disruptive to the flow of the lesson if participants arrive late. For anyone who's interested in building their West Coast Swing fundamentals quickly, note that May will be the last month we'll be offering weekly classes with both Sam and Meaghan. With summer approaching it's a great time to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity. Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C286" s="3" t="n">
+        <v>45813.19128471065</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2238975779474166/</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 13 Apr 2019 20 Apr 2019 27 Apr 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 23 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook A new month, a new social! Come and join in on the fun at our inaugural Saturday night dance and intro lesson on April 6 (and every Saturday night after that)! Just $10 for the Lesson and/or Social ($5 for Students). No experience or partner required. • 6:45 pm – Doors open • 7:00 pm – Beginner Lesson with Sam and Meaghan (this is perfect as a refresher class too!) • 8:00 – 11:00 pm Social Dancing featuring DJ Carolyn Please note the NEW START TIMES for the BC Swing Victoria Saturday night dances. See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C287" s="3" t="n">
+        <v>45813.19128471065</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1366072544640156/</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Saturday 17 May 2025 at 18:45 Victoria WCS Collective Beginner Lesson and Social Dancing Dance Victoria About Discussion More About Discussion Victoria WCS Collective Beginner Lesson and Social Dancing Details 9 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson from 7 to 8 pm by John de Pfyffer Social dancing from 8 to 10:15pm DJg by Donna and Nel Cost $15/ $12 for students No need to register and no need for dance experience.. Also, no partner necessary, we got you! Please bring indoor scuff-free dance shoes or socks to dance in. See less Victoria, British Columbia Dance Victoria 2750 Quadra St # 111, Victoria Dance Victoria brings the "World's Best Dance" to the Royal Theatre and supports new dance creation for the international stage from its studios. Guests See All</t>
+        </is>
+      </c>
+      <c r="C288" s="3" t="n">
+        <v>45813.19128471065</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1024182725709172/</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Saturday April 19th Lesson and Social Dance Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 19th Lesson and Social Dance Details 4 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginner plus lesson with Pamela Podmoroff from 8 to 10:15 pm Social dancing from 8 to 10:15 pm DJs Donna and Amanda Cost $15/ $12 for students No need to register and no partner required. Please bring scuff-free indoor dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C289" s="3" t="n">
+        <v>45813.19128471065</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1225266505917189/</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Saturday Beginner Lesson and Social Dancing Dance Victoria Sat, 7 Jun Sat, 14 Jun Sat, 21 Jun +4 About Discussion More About Discussion Victoria WCS Collective hosts Saturday Beginner Lesson and Social Dancing Interested Going Invite Details 1 person responded Event by Donna Forsyth Dance Victoria Duration: 3 hr 30 min Public · Anyone on or off Facebook Back to AIR CONDITIONED comfort at Dance Victoria Studios Beginner lesson from 7 to 8 pm Social dancing  from 8 to 10:15 pm Cost $15/$12 for students No need to register and no need for previous dance experience or a partner. Please bring scuff-free inside low-heeled dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C290" s="3" t="n">
+        <v>45813.19128471065</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/641769172035949/</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>Saturday April 12 Beginner lesson and social dance at Dance Victoria Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 12 Beginner lesson and social dance at Dance Victoria Details 5 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginners lesson by Donna from 7 to 8 pm Social dancing from 8 to 10:15 pm DJs Andre and Nel Cost $15 /$12 for Students No need to register and no partner required. Please bring scuff-free inside dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C291" s="3" t="n">
+        <v>45813.19128471065</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/516994561244886/</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:45 Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING White Eagle Polish Association About Discussion More About Discussion Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING Details 15 people responded Event by Donna Forsyth , Andre Russo and Victoria West Coast Swing Collective White Eagle Polish Association Public · Anyone on or off Facebook Doors open at 6:45pm at this fabulous new venue! Advanced beginner/intermediate lesson by Chantelle Pianetta from 7 to 8 pm Social dancing for 3 HOURS from 8 to 11 pm DJs Donna and Andre Cost $15 /$12 for students ALL at the spacious White Eagle Hall No need to register and you do not need a dance partner. Please bring scuff-free dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia White Eagle Polish Association 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C292" s="3" t="n">
+        <v>45813.19128471065</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3513597908934465/</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Saturday 12 April 2025 from 12:00-20:00 Live Music Benefit Event for Veteran's House 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion Live Music Benefit Event for Veteran's House Details 34 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 8 hr Public · Anyone on or off Facebook Admission by Donation (Non-Perishable Food Items, Charitable Donations, Gift Cards, accepted). Enjoy live music throughout the day by Bryce Allan, Love Cats, OTR, Donny Peterson &amp; the Tone Rangers, Helen Davies, and David Carl Trio. See less Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C293" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1399479741193649/</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Saxe Point Public House About Discussion More About Discussion TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Details 4 people responded Event by Tom Watson Saxe Point Public House Public · Anyone on or off Facebook Join Vinyl Wave at the lovely Saxe Point Pub for a couple of hours of smooth tunes that'll help ease you into the week! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C294" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1975172826621817/</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>(20+) Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Thursday 12 June 2025 from 19:00-20:30 Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Little Fernwood Gallery. About Discussion More About Discussion Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Interested Going Invite Details Event by Anna Bigland-Pritchard Little Fernwood Gallery. Tickets www.annabiglandpritchard.com/event-details/rest-resonate-restorative-yoga-ft-cozy-live-music Public · Anyone on or off Facebook Do you need some R&amp;R? Join Anna &amp; Roxie for a dreamy candlelit evening of restorative yoga, live music, and guided journalling. Facilitated by Roxie Fehr of Across the Water | Yoga Anna Bigland-Pritchard of ABP Music Studio | Music As experienced, intuitive space-holders, our goal to support your Nervous System and capacity for hope with a feast of restful offerings. We know life is stressful and we want to help you feel more connected to your intuition so you can not only survive, but also have the capacity to take the next right step in your life in a way that positively impacts the world. The space will be dreamy, there will be tea, guided journalling, poetry, restorative yoga shapes that can be adapted for any body, and LIVE MUSIC! Anna will be playing guitar, creating dreamy sound worlds with vocal looping, and singing you lullabies all evening. What to bring Yoga mat (We'll have a few available to borrow) Journal &amp; pen/pencil (We'll also have some spare paper and writing/drawing utensils) Yourself in your comfy cozies Details June 12, 7-8:30pm at Little Fernwood $42 Accessibility This event is on the ground floor There is a unisex/non-gendered bathroom on the same level We care about making this event accessible, so please let us know if you have any questions or accessibility needs. This will be a VERY gentle practice, and modifications will be offered. Happy pride! As members of and allies of the 2SLGBTQIA community, we (Anna &amp; Roxie) will create a supportive, inclusive, affirming environment and expect all participants to do the same. If cost is a barrier, please contact us directly as we have a limited number of discount codes available This is our first time offering this class, and we hope it will be a hit so we can make it a regular thing. Come as you are, leave nourished by your dreams See less Victoria, British Columbia Tickets Find Tickets Little Fernwood Gallery. 1923 Fernwood Ave., Victoria Meet your host Anna Bigland-Pritchard 5 past events · Page · Musician/band Based in Lekwungen territory (Victoria, BC), Anna Bigland-Pritchard is a: -Soprano -Voice teacher… Follow Suggested events Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested 6113 people interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends 47 people interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Janine and 4 friends are interested 956 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C295" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1142760357225336/</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 26 26 Jul at 10:00 – 27 Jul at 17:00 ArtisTREE Festival 1401 rockland ave, Victoria, BC, Canada About Discussion More About Discussion ArtisTREE Festival Interested Going Invite Details 1K people responded Event by Artistree Festival , MORENA CLOTHING and Cory Judge 1401 rockland ave, Victoria, BC, Canada Duration: 2 days Public · Anyone on or off Facebook Saturday July 26 10-7pm Sunday July 27 10-5pm Government House of BC 1402 Rockland Ave Celebration of Creativity profiling 130 Juried Artisans, Live Music, Installation and Performance Art, Indigenous Makers and Traditions, Kids section, Live Painters, Delicious Food and Ice cream. See less Shopping Victoria, British Columbia 1401 rockland ave, Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C296" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/979769967649565/</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 15:00-18:00 Live Music at the Legion 102-622 Admirals Rd, V9A 2N7 Sat, 17 May Sat, 24 May Sat, 31 May +2 About Discussion More About Discussion Live Music at the Legion Details 8 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Come enjoy live music on Saturdays 3-6 p. Dancing encouraged! Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C297" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1217747446718881/</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 18:00-22:00 Maifest - Evening of Live Music Edelweiss Club About Discussion More About Discussion Maifest - Evening of Live Music Details 36 people responded Event by Cindy Kent and Victoria Edelweiss Club Edelweiss Club Duration: 4 hr Public · Anyone on or off Facebook Join the Edelweiss Club for a lively evening of music and dance with Bijoux du Bayou and The Helen Davies Band. Let the infectious Zydeco beats and soulful rhythms set the tone for a night of fun, complete with delicious German snacks from the kitchen. Don’t miss out on this high-energy event! Get your tickets online or call 250-383-4823. www.victoriaedelweiss.ca/events See less Victoria, British Columbia Edelweiss Club 108 Niagara Street, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C298" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/4223643791110348/</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Sunday 22 June 2025 at 13:00 Victoria Italian Day 195 Bay St, Victoria, BC V9A 3K4, Canada About Discussion More About Discussion Victoria Italian Day Interested Going Invite Details 3 people responded Event by Calabrisella 195 Bay St, Victoria, BC V9A 3K4, Canada Public · Anyone on or off Facebook Join us for live music, food, gelato, games, cars, cultural exhibits, vendors, bike valets and much more - Free admission !! Victoria, British Columbia 195 Bay St, Victoria, BC V9A 3K4, Canada 195 Bay St, Victoria, BC V9A 3K4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C299" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1198411931645258/</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Saturday 26 April 2025 from 15:00-18:00 LIVE MUSIC - The City Slickers 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion LIVE MUSIC - The City Slickers Details 21 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Members $5, Guests $10 Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C300" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/639017139056190/</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Saturday 19 April 2025 from 15:00-18:00 Live Music - Love Cats 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion Live Music - Love Cats Details 22 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Members $5, Guests $10 Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C301" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2579625309035667/</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Sunday 18 May 2025 from 12:00-18:00 Live Music @ Junction (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Live Music @ Junction (RAIN OR SHINE) Details 125 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Here we go again, its a long weekend so let's get our Sunday Funday on. First Live Music of the year at Junction Up first is-  Emergency Exit  are playing from 1230-230pm To take us home is - An &amp; Ben are playing from 3-5pm Tasting Room and Picnic Area are open 12-6pm Oh and if you haven't heard me say it before ITS RAIN OR SHINE. Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Cider ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Mini Market and a Beautiful location ⠀⠀⠀⠀⠀⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your well behaved two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C302" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/686146924271113/</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>(20+) Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Spring Series Lorne and Ali Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 4 friends 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Recommended events See all Tomorrow from 16:00-22:00 Oak Bay Tea Party Roy and 7 friends Sunday from 13:00-16:00 Sunday Afternoon Milonga Dalie Sunday from 07:00-19:00 Oak Bay Tea Party Roy and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 5 Today from 19:00-22:00 Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz 753 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz Interested Going Invite Details Event by Adonis Puentes and Brent Jarvis 753 View St, Victoria, BC V8W 1J9, Canada Tickets hermannsjazz.com/reservations&amp;event_id=741898 Public · Anyone on or off Facebook An evening of Jazzy Cuban Fusion Music; traditional, contemporary, romance and dance. Juno &amp; Grammy Nominated vocalist, Adonis Puentes, will be joined by the Jazz Bohemians, featuring Brent Jarvis (piano), Ken Lister (bass), Nicholas Marquez (percussion) and Brooke Maxwell (Sax). Adonis Puentes opens up the marvelous world of Cuban music to his audience the second they hear his rich voice. When the other players kick in with their tight, multi-layered arrangements, it becomes clear that Adonis is a powerful bandleader. Fronting an acoustic band, Adonis' vocals are surrounded by piano, bass, strings, and percussion. Music reflects the present and Adonis Puentes is a Cuban Sonero for our times. Adonis thrives on the growth and acclaim for his original sonero sound. As he puts it, "I feel like a messenger of my roots and tradition, blessed that with me I have taken my music and heritage to many different places in the world; from Cuba, to Canada, USA, Mexico, Europe and Asia. My mission is to make you dance and enjoy my melodies and rhythms." Musician Line-Up: Adonis Puentes - Vocals Brent Jarvis - Piano Ken Lister - Bass Nicolas Marquez - Percussion Brooke Maxwell - Sax See less Music and audio Victoria, British Columbia Tickets Find Tickets 753 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Meet your hosts Adonis Puentes 34 past events · Page · Musician/band Adonis Puentes is a great singer and an elegant composer and lyricist grounded and nourished by his Cuban roots and worldly experience. Message Brent Jarvis 37 past events · Profile · Musician Message Suggested events Wed, 18 Jun at 16:00 Victoria Ska &amp; Reggae Fest Kickoff: Waahli, The Resignators, Hezron, Gun Street Ghouls &amp; Cabin Fever Victoria, BC, Canada, British Columbia 490 people interested Interested This Saturday at 21:00 Goth Nite: UNDERGROUND Victoria, BC, Canada, British Columbia 179 people interested Interested Thu, 19 Jun at 16:00 Victoria Ska &amp; Reggae Fest: Turbulence, La Severa Matacera, Spiritual Warriors, Sonic Alley &amp; Ari DL Victoria, BC, Canada, British Columbia 231 people interested Interested Popular with friends Tomorrow at 16:00 Oak Bay Tea Party Willows Park Roy, Veronica and 6 friends are interested Interested This Sunday at 10:00 Cook Street Village Block Party! 🥳 Cook Street Village Sophia, Roy and 4 friends are interested Interested Fri, 13 Jun at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 5 friends Interested This Saturday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested This Sunday at 07:00 Oak Bay Tea Party Willows Park Roy, Robin and 5 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C303" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/986310396630042/</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>SATURDAY SONG-A-THON 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada About Discussion More About Discussion THE SATURDAY SONG-A-THON Details 9 people responded Event by Bucket Crab Johnny and CRAB BUCKET STUFF 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada Duration: 5 hr Public · Anyone on or off Facebook an INDOOR PICNIC PARTY with FREE LIVE MUSIC Click on the Photo at the top to see the whole poster and zoom in on the details. Victoria, British Columbia 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada 1507 Glentana Rd, View Royal, BC V9A 4K1, Canada THE SATURDAY SONG-A-THON 1 member active Open chat Guests See All</t>
+        </is>
+      </c>
+      <c r="C304" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/665127126496204/</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Tuesday 27 May 2025 at 19:30 Live Music at the Saxe Point Public House Saxe Point Public House About Discussion More About Discussion Live Music at the Saxe Point Public House Details 9 people responded Event by VINYL WAVE Saxe Point Public House Public · Anyone on or off Facebook Live Music every other Tuesday starting May 27th! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C305" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/651664851189740/</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 12:00-18:00 Music in the Orchard (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Music in the Orchard (RAIN OR SHINE) Interested Going Invite Details 146 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Come enjoy the start of the summer in the orchard. We have two amazing artists for you, some delicious fun summer ciders for you to try and amazing food to enjoy to complete the experience. Delicious Cider Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀ Beautiful location ⠀⠀⠀⠀ Dog Friendly ⠀⠀ ⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your WELL BEHAVED two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C306" s="3" t="n">
+        <v>45813.19727147696</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1414577976223422/</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 19:00-23:00 Solstice Slammer 3 - Moon Under Water, Victoria The Moon Under Water Brewpub About Discussion More About Discussion Solstice Slammer 3 - Moon Under Water, Victoria Interested Going Invite Details 32 people responded Event by Electric Druids and Gate Theory The Moon Under Water Brewpub Tickets · CA$10 www.eventbrite.com/e/solstice-slammer-3-tickets-1389012316229 Public · Anyone on or off Facebook Come join us for Solstice Slammer III at Moon Under Water Brewpub and Distillery! Get ready to celebrate with Electric Druids, Gate Theory and Insulam, hefty drinks and good vibes. Whether you're a craft beer enthusiast or just an enthusiast, there's something for everyone at this epic night of live music. Don't miss out - mark your calendars! See less Music and audio Victoria, British Columbia Tickets Find Tickets The Moon Under Water Brewpub 5435 Fowler Rd, Saanich, BC V8Y 1Y4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C307" s="3" t="n">
+        <v>45813.19727147696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Error in write_events_to_db. Somehow, either parent_url or calendar_url was coming in as a float. Forced them to string at top of method.
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C307"/>
+  <dimension ref="A1:C421"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4832,7 +4832,7 @@
         </is>
       </c>
       <c r="C293" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="294">
@@ -4847,7 +4847,7 @@
         </is>
       </c>
       <c r="C294" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="295">
@@ -4862,7 +4862,7 @@
         </is>
       </c>
       <c r="C295" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="296">
@@ -4877,7 +4877,7 @@
         </is>
       </c>
       <c r="C296" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="297">
@@ -4892,7 +4892,7 @@
         </is>
       </c>
       <c r="C297" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="298">
@@ -4907,7 +4907,7 @@
         </is>
       </c>
       <c r="C298" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="299">
@@ -4922,7 +4922,7 @@
         </is>
       </c>
       <c r="C299" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="300">
@@ -4937,7 +4937,7 @@
         </is>
       </c>
       <c r="C300" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="301">
@@ -4952,7 +4952,7 @@
         </is>
       </c>
       <c r="C301" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="302">
@@ -4967,7 +4967,7 @@
         </is>
       </c>
       <c r="C302" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="303">
@@ -4982,7 +4982,7 @@
         </is>
       </c>
       <c r="C303" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="304">
@@ -4997,7 +4997,7 @@
         </is>
       </c>
       <c r="C304" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="305">
@@ -5012,7 +5012,7 @@
         </is>
       </c>
       <c r="C305" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="306">
@@ -5027,7 +5027,7 @@
         </is>
       </c>
       <c r="C306" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
       </c>
     </row>
     <row r="307">
@@ -5042,7 +5042,1730 @@
         </is>
       </c>
       <c r="C307" s="3" t="n">
-        <v>45813.19727147696</v>
+        <v>45813.19727148148</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1363696181561219/</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:00-22:00 Pride Contra Dance Fairfield United About Discussion More About Discussion Pride Contra Dance Interested Going Invite Details 70 people responded Event by Victoria Contra Dance and Code Tron Fairfield United Duration: 3 hr Public · Anyone on or off Facebook 𝕍𝕀ℂ𝕋𝕆ℝ𝕀𝔸 ℂ𝕆ℕ𝕋ℝ𝔸 𝔻𝔸ℕℂ𝔼 𝕊𝕆ℂ𝕀𝔼𝕋𝕐 ℙℝ𝔼𝕊𝔼ℕ𝕋𝕊: The return of our ℚ𝕌𝔼𝔼ℝ Contra Dance to celebrate the month of Pride! All Dancers welcome! Join us Friday, June 20th at the United Commons Fellowship Hall to do-si-do the night away to sprightly fiddle tunes and stellar performances from our two favorite drag performers! We'll have more capacity than our previous Valentines Day Dance, but we still might sell out, so grab your tickets online here! https://clannamorna.ca/.../ticket-victoria-pride-contra.../ ......................................................................................................... 𝕄𝕦𝕤𝕚𝕔 𝔹𝕪: 𝐑𝐨𝐬𝐞 𝐉𝐚𝐜𝐤𝐬𝐨𝐧: she/her Coming up in the rich folk scene of western Massachusetts, Rose is based in Montague, MA, where she studied under fiddler Becky Tracy from whom she inherited a wide repertoire of music from Quebec, New England, Ireland, and France, a deep love for old tunes, and the intuitive sense of rhythm and danceability which infuses her playing. Equally at home in the concert hall and on the dance stage, she’s taught fiddle, song, and dance at camps and festivals around New England, toured nationally with her band Polaris and now tours with her quartet Stove Dragon and duo Helen &amp; Rose. https://www.rose-jackson.com/ 𝐇𝐞𝐥𝐞𝐧 𝐊𝐮𝐡𝐚𝐫: they/them Hailing from Seattle, Washington, Helen currently resides in Cambridge, MA. Helen began exploring their connection to folk and Celtic music in 2020 while studying with renowned contra guitarist Alex Sturbaum. Upon moving to Cambridge in 2022, Helen dove into the thriving celtic music scene, playing contra dances, Irish sessions, and concerts around New England and the Pacific Northwest. Since then, Helen has developed their style as a contra accompanist, Irish session backer, and vocalist. https://www.helenkuharmusic.com/ 𝐅𝐢𝐝𝐝𝐥𝐢𝐧' 𝐅𝐢𝐧𝐧: they/them A professional fiddler, singer and banjo player living on the territories of the lekwungen and W̱SÁNEĆ people, colonially known as Victoria BC. Finn has a passion for Irish, Scottish, English, North American and Eastern European folk music, and are known for their dynamic fiddling and soulful voice. They delve into traditional material - bringing a fresh interpretation of songs and tunes from many different places, as well as writing their own material. From the Appalachian mountains to Quebec, to melodic Irish and Scottish tunes, they cover wide musical ground with articulate playing. Finn also performs frequently in Canada and the U.S. with their bands Clanna Morna and Ghostly Hounds. https://finnletourneau.com/ ℂ𝕒𝕝𝕝𝕚𝕟𝕘 𝔹𝕪: 𝐕𝐢𝐜𝐭𝐨𝐫𝐢𝐚 𝐁𝐞𝐚𝐮𝐜𝐡𝐞𝐬𝐧𝐞 One of our local communities up and coming callers! 𝔻𝕣𝕒𝕘 𝕡𝕖𝕣𝕗𝕠𝕣𝕞𝕒𝕟𝕔𝕖𝕤 𝕓𝕪: Aries Moon: Making country gay one song at a time Leo Moon: The island's premiere tap dancing drag thing ......................................................................................................... 6:30 - doors open 7:00 - dancing starts with a beginner friendly dance lesson Everyone welcome, no experience necessary. $12 - Youth $20 - Everyone who is willing and able to NOTAFLOF Poster Art by Sonya Chwyl See less Victoria, British Columbia Fairfield United 925 Balmoral Rd, Victoria, BC V8T 1A7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C308" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1185783966345055/</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 10:00-13:00 Shuffle Dance Workshop Victoria, BC About Discussion More About Discussion Shuffle Dance Workshop Details 12 people responded Event by Adelène Buchanan Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another SHUFFLE WORKSHOP coming your way!! Join our Shuffle Dance Workshop and learn a full shuffle choreography set to an energetic electronic track. We’ll guide you through each step, focusing on key shuffle movements, while incorporating them into a dynamic routine. Perfect for ALL LEVELS! This workshop will help you improve your footwork, coordination, and cardiovascular stamina as you master a complete choreography. Here’s what you need to know: DATE: Sunday, May 25th TIME: 10am - 1pm PLACE: The Beat Clinic (1303 Broad Street) Sign-up link here https://www.thebeatclinic.ca/ See less Victoria, British Columbia Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C309" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1187402793186660/</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 08:00-12:00 Global Underscore Solstice Dance 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada About Discussion More About Discussion Global Underscore Solstice Dance Interested Going Invite Details 45 people responded Event by Arunimá McNeish , Michael McAmmond and Victoria Contact Improv Jam 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada Duration: 4 hr Public · Anyone on or off Facebook Sweet dancers, This summer solstice we extend a warm invitation to join us in expanding and deepening our practice of Contact Improvisation with participation in The Global Underscore. Please arrive at 8am to join a 40 minute talk-through, introducing the concepts of the Underscore. This is mandatory if you have never attended an Underscore before. The Underscore will begin promptly at 8:45am. If you have attended a talk-through before you're welcome to arrive at this time. We will all start and end together. This is a closed container and we will not be allowing late-comers. TIMELINE: 8am-8:40am Underscore Talk-Through with Arunima 8:45am-11:30am Underscore 11:30am-11:50am Closing Circle COST: $15-$20  etransfer or pay cash at the door if pre-registered (if money is a barrier please reach out to discuss options). Please contact Arunima at ode.to.thylacine@gmail.com for registration, etransfer, questions, etc. VENUE: Victoria Truth Centre (2815 Cedar Hill Rd, Victoria, BC). MORE INFO: The Underscore, which has been evolving since 1990, is a vehicle for incorporating Contact Improvisation into the broader arena of improvisational dance practice; developing greater ease dancing in spherical space—alone and with others; and for integrating kinesthetic and compositional aspects while improvising. It allows for a full spectrum of energetic and physical expressions, embodying a range of forms and changing states. Its practice is familiar yet unpredictable. The practice progresses through a broad range of dynamic states, including long periods of very small, private, and quiet internal activity and other times of higher energy and interactive dancing. There are 20+ phases, 12+ connections, and 7 aspects of the Underscore—each with a name and a graphic symbol—which create a general map for the dancers. Within that frame, dancers are free to create their own movements, dynamics, and relationships—with themselves, each other, the group, and the environment. Each Underscore is unique, providing rich and often inspiring experiences of the human and artistic phenomena of dance improvisation. https://globalunderscore.com/ https://nancystarksmith.com/underscore/ See less Victoria, British Columbia 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C310" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/514087011782400/</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Thursday 5 June 2025 at 18:00 80s Dance Party 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion 80s Dance Party Details 42 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Public · Anyone on or off Facebook Join Kai Aris and Friends for an evening of upbeat 80s dance, pop, and rock classics. Featuring some of Victoria’s best young musicians: Lily Gyles Thomas on vocals, Josh Warren on bass, Ava Creed on drums, Alex Gwillim on guitar, and Kai Aris on Synthesizer. Enjoy some drinks and dance the night away! See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C311" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3639802496153228/</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Sunday 11 May 2025 from 11:00-12:30 Dance Temple w/ Lila Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Lila Details 69 people responded Event by Dance Temple Victoria , Lyndsay Lila and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, May 11th features Lila Spencer as our facilitator/dj! Details for Sunday, May 11th: Facilitation and music set by Lila Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C312" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1682353965754886/</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Saturday from 18:00-20:30 Mamas' Dance Party! 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Sat, 5 Apr Sat, 10 May Sat, 14 Jun About Discussion More About Discussion Mamas' Dance Party! Interested Going Invite Details 28 people responded Event by Fairfield Gonzales Community Association 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Duration: 2 hr 30 min Public · Anyone on or off Facebook Calling all mamas, grand-mamas, aunties &amp; mamas-to-be! Join us for a night curated for all mamas (in any season of their motherhood or reproductive journey) to connect through creative expression, freedom of movement and community building! There will be an opening &amp; closing circle and time to connect over light refreshments as the night concludes. Feel free to come for it all, or leave when needed. We can't wait to dance, groove, and connect with you all soon. This is an inclusive space for ALL those who mother. Admission by-donation: suggested donation $5 This event is presented by the FGCA's Neighbourhood Improvement Committee See less Victoria, British Columbia 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 1330 Fairfield Rd, Victoria, BC V8S 5J1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C313" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1206582580433662/</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Monday 16 June 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 41 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Salsa with Sebastian and Hannah— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C314" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663135653237580/</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Method Studio - Victoria BC Canice Ma invited you Interested Going About Discussion More About Discussion WACK! Another West Coast Swing Social Dance Invite Details 37 people responded Event by Canice Ma and Wyatt Ritchie Method Studio - Victoria BC Duration: 3 hr 30 min Public · Anyone on or off Facebook Guess who's back, it's WACK! (please ignore the fact that it's been 2 years...) The schmucks are back with another spontaneous west coast swing social dance, featuring music by DJs Topknot and Amandance from Vancouver! DETAILS: • Friday, June 20th, 2025 • Method Studio, 841 Fisgard St, Victoria, BC • 7:30-11 pm: social dancing with 100% west coast swing (sorry, no lesson!) • Admission: $10 • Water and AC on us (and maybe some bonus chocolate) • Please keep in mind that parking is limited at the venue GENERAL SOCIAL DANCE ETIQUETTE: • Consent is cool- don't be creepy. • Shake off any shyness and get out there! Ask people to dance regardless if you’re a lead or follow, dancing for 10 years or started yesterday- it's more fun that way! • No teaching or unsolicited feedback on the dance floor. Good vibes only! • If you would like to partake in a steal dance, try to remain with that group for the whole song. • Bring a water bottle! The studio is known to get warm with more bodies in the space so we want you to stay healthy and hydrated. • Personal hygiene is important! Consider bringing a towel and/or a spare shirt to change into if you sweat easily. Our studio has a bathroom and change rooms available for all to use. • We recommend wearing clothes that are easy to move in, especially pants given the nature of the dance. • Clean, comfortable shoes (ideally dance shoes) on the dance floor only! See less Victoria, British Columbia Method Studio - Victoria BC 833 Fisgard St, Victoria, BC V8W 1R9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C315" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1904863453602318/</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 19:00-22:00 Private Dance Saanichton, BC About Discussion More About Discussion Private Dance Details 8 people responded Event by HAMMERdown - Victoria, BC Saanichton, BC Duration: 3 hr Public · Anyone on or off Facebook We are excited for our gig on May 31 at Saanichton Bay. It is a private event. There will be good rocking tonight. Victoria, British Columbia Saanichton, BC Saanich, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C316" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2576922459305643/</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Sunday from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Interested Going Invite Details 13 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 15th features Cedar Mathias as our facilitator/dj! Details for Sunday, June 15th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C317" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/589043697010919/</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 66 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, May 25th features Cedar Mathias as our facilitator/dj! Details for Sunday, May 25th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C318" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/909522138040202/</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Friday 28 November 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 232 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 46 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Roy and 3 friends 70 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C319" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/939376108286434/</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Friday 27 June 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 16 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Ali and Dalie 41 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Roy and 3 friends 70 people interested Interested This Saturday at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 182 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C320" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/624858640069610/</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 Friday 22 August 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 232 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 46 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Roy and 3 friends 70 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C321" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/691138080073761/</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Monday 23 June 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 232 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Kizomba with Aaron and Fernanda— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C322" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1031573525615192/</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Sunday 29 June 2025 at 19:00 GROOVE KITCHEN'S JUNEFEST DANCE!! Hermann's Jazz Club About Discussion More About Discussion GROOVE KITCHEN'S JUNEFEST DANCE!! Interested Going Invite Details 64 people responded Event by Groove Kitchen and Hermann's Jazz Club Hermann's Jazz Club Tickets hermannsjazz.com/show/737557/view Public · Anyone on or off Facebook The festival is over and it seems you still wanna celebrate music, but also... wanna get down and boogie?? You're our kind of people!! Observe the top of Summer with song and funky steps as the kitchen's groove moves your body like they've done before at spots like the Butchart Gardens, The Esquimalt Ribfest, The Osbourne Bay Pub, or the hottest rooms in and outta town. The Chefs are ready to serve their mouthwatering melange of funk, pop, soul, Latin, and flavours to party to the end!! Join us... Doors 5:30 PM / 7:00 PM Show, Sunday June 29th Hermann's Jazz Club 753 View Street Victoria, BC V8W 1J9 https://hermannsjazz.com/show/737557/view See less Victoria, British Columbia Tickets Find Tickets Hermann's Jazz Club 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C323" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1618420955545842/</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 30 Friday 30 May 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing at an all ages venue with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 232 people interested Interested Mon, 4 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Ali 10 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 46 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C324" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/667083456006099/</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT Details 11 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 753 View Street (2nd floor, Hermmans Jazz Club) Date: Saturday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C325" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1910904133047825/</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY The Coda About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY Details 81 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 751 View Street (2nd floor, Hermmans Jazz Club) Date: Friday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia The Coda 751 View St, Victoria, BC Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C326" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1132427048350776/</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com or 15$ cash/e-transfer at the door. Formed in the heart of Chinatown, Rosebuds is a dynamic ensemble that brings the vibrant sounds of jazz, blues &amp; swing to life.  The group plays a mixture of originals and jazz standards, and is influenced by artists like Louis Armstrong, Billie Holiday, Lester Young, and Lionel Hampton. Featuring Rebecca Wells (vocals/guitar), Alex Moore (guitar/keys) Bryden Amos (guitar/keys), Matisse Gubby-Hurtig (bass), Owen Chow (trumpet), and Andrew Greenwood (tenor saxophone). Samba e Sol is a newly formed Brazilian bossa nova jazz trio featuring Andrew Greenwood (flute), Alex Moore (guitar), and Matisse Gubby-Hurtig (bass), playing music by artists like Antonio Carlos Jobim, Marcos Valle, Luiz Bonfa, and more. Instagram: https://www.instagram.com/rosebudsband/ See less Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C327" s="3" t="n">
+        <v>45819.86023413194</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2637194793152555/</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 91 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 29, 2025 | Lesson:  Intro to Salsa Rueda with Sam and Katie Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa Rueda • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C328" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/947213690692385/</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C329" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1743571267040445/</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Ali Jorgensen invited you About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Details 54 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 8, 2025 | Lesson: Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C330" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1794066937801722/</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Saturday 8 March 2025 from 20:30-23:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 26 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C331" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1293301738436581/</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Sunday 6 April 2025 at 17:00 Kizomba Sundown Party: Free of charge Method Studio - Victoria BC David Lamine Victoria invited you About Discussion More About Discussion Kizomba Sundown Party: Free of charge Details 58 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Method Studio - Victoria BC Public · Anyone on or off Facebook Free Pre-VIKFest party. Bring snack and drink. Expect great music, great energy, great atmosphere. "Dance with your heart. your feet will follow" Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria, BC Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C332" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1337760257449745/</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 5 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 10, 2025 | Lesson:   Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C333" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1079226067560481/</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 46 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 6, 2025 | Lesson:  Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C334" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/960236445839425/</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Saturday 22 June 2024 from 18:00-21:00 Kizomba/UrbanKiz at Clover Clover Pt, Victoria, BC V8S, Canada About Discussion More About Discussion Kizomba/UrbanKiz at Clover Interested Details 56 people responded Event by Becky Mowat Clover Pt, Victoria, BC V8S, Canada Duration: 3 hr Public · Anyone on or off Facebook Come join us for our first time dancing at Clover Point! There will be no lesson beforehand and this is super casual. Just a bunch of friends hanging out and dancing. Bring snacks, something to drink, blankets, warm clothes (as it is typically cooler by the ocean). There isn't a lot of parking at Clover Point but you can park along Dallas Rd and just walk down. Feel free to invite friends and family. Hope to see you all there! See less Victoria, British Columbia Clover Pt, Victoria, BC V8S, Canada 1301 Clover Pt, Victoria, BC V8S, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C335" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3006474846197996/</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 38 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 27, 2025 | Lesson:  Intro class TBD Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro class TBD • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C336" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1861230087752141/</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 4 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 31, 2025 | Lesson:  Intro to Salsa with Adam &amp; Alicia Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C337" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1029869435768837/</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Saturday 22 March 2025 at 20:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC This event has been cancelled. You cannot share this event, but you can still post. About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 14 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C338" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/372311028526699/</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Saturday 9 December 2023 from 20:30-23:30 Victoria Kizomba Social: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Social: Fall Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C339" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1179097320623502/</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 37 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C340" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1060779176049104/</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Thursday 3 October 2024 from 19:30-22:30 Kizomba Practica Thursdays: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Kizomba Practica Thursdays: Fall Series Details 20 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Join us every Thursday for Kizomba/Urbankiz classes. Intermediate 7:30PM-8:15pm Beginner 8:15pm-9:00pm Practica until 10:30pm Class only: $10 Class &amp; Practica: $15 or $10 for university students w/ID Practice only $10 Classes will be provided by your local Instructor (David Lamine) and assistants (Robyn, Becky) and occasionally by some out of town and International Instructors. Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C341" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3185065321631809/</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Saturday 15 March 2025 from 20:00-00:00 Urban Kiz Workshop with Mannie Method Studio - Victoria BC Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 48 people responded Event by Becky Mowat and David Lamine Victoria Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria, BC Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C342" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1184791909680061/</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Thursday 13 March 2025 from 19:30-23:00 Urban Kiz Workshop with Mannie Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 50 people responded Event by Becky Mowat and David Lamine Victoria Ukrainian Cultural Centre Duration: 3 hr 30 min Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C343" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1152065639712042/</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 20 20 Feb at 19:30 – 23 Feb at 23:00 Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Details 49 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 days Public · Anyone on or off Facebook Join us for our special edition Urbankiz &amp; Tarraxo workshops with Mike Ahombi Mike has been a big supporter of our VIKF and bringing his talent and low key vibe to the west coast. He is based out of Ottawa but you will find him at many different festivals and cities teaching Kizomba, Urbakiz and Tarraxo. We cannot wait for you all to have the opportunity to learn from such an incredible person and instructor. Details: Feb 20th Urbankiz Workshop 7:30pm-9:30pm Practica 9:30pm-11:00pm Feb 22nd Tarraxo Workshop 8:00pm-10:00pm Practica 10:00-11:30pm Price $90 Workshops only $70 Practica only $20 *** please e transfer to becksmith@hotmail.com *** Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C344" s="3" t="n">
+        <v>45819.86811199074</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/9677364319006080/</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 54 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation July 20, 2025 | Lesson:  Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C345" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1813229489279716/</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Thursday 29 May 2025 from 19:55-21:00 Sensual Bachata 4 Week Series Method Studio - Victoria BC Thu, 15 May Thu, 22 May Thu, 29 May +1 About Discussion More About Discussion Sensual Bachata 4 Week Series Details 6 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 1 hr 5 min Public · Anyone on or off Facebook Ready to level up your Sensual Bachata? May 8, 15, 22, 29 Method Studio | 7:55–9:00 PM | $80 for all 4 classes Join us for an exciting and dynamic Bachata Sensual class designed for experienced beginners and intermediate dancers! We’re blending solid fundamentals with fresh, fun, and sensual combos to help you grow, challenge yourself, and have an amazing time on the dance floor. No partner needed — just bring yourself and your love for dance! Spots are limited — don’t miss out! Register by e-transferring $80 to maximumotion@gmail.com and mentioning “Bachata Sensual” in the notes. Get ready to connect, move, and elevate your dancing! P.S. All fees are non-refundable as they go directly toward securing the studio space and running the class. See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria, BC Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C346" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1300938064467261/</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Thursday 20 March 2025 from 20:00-22:00 Intermediate Sensual Bachata Workshop Method Studio - Victoria BC About Discussion More About Discussion Intermediate Sensual Bachata Workshop Details 24 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 2 hr Public · Anyone on or off Facebook Sensual Bachata Workshop in March! Intermediate workshop - March 20 Time: 8:00-9:30 PM + Practice 9:30-10:00 PM Location: Method Studio, 841 Fisgard St. Cost: $30 per workshop (includes 2 hours!) Intermediate workshop: Take your skills to a higher level! Master the advanced variations of the Madrid pass, smooth transitions and musicality. No partner needed, just bring your energy and comfortable shoes! Register at: maximumotion@gmail.com #BachataWorkshop #VictoriaBC #LearnToDance #BachataLovers See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria, BC Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C347" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/692165093260868/</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 13:00-16:00 Salsa &amp; Bachata Masterclass with Adam &amp; Ghada Solwood Studio About Discussion More About Discussion Salsa &amp; Bachata Masterclass with Adam &amp; Ghada🔥 Details 60 people responded Event by Dancing Time Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook Hello everyone! Spring is here, and many things are happening, but I can’t but dance with you one last time before leaving for the entire summer!! To make things spicy, I am extremely happy to collaborate with Adam on a Salsa &amp; Bachata Masterclass! Get ready to learn details that will help you with creating flow – both as leads and follows – in addition to some socials-friendly tricks! Date: Saturday, May 10 Time: 1:00-2:30 | Salsa, 2:30-4:00 | Bachata Price: 25$ for one class, 35$ for two classes Location: Solwood studio, 1303 Broad st To register, please fill in this quick form and send an e-transfer to ghadacyoussef@gmail.com. https://forms.gle/4QThxT6yByd3h5KH8 Note: kindly understand that no-shows and cancellations made in less than 1 week from the workshop cannot be refunded. I will be happy to fully refund for earlier cancellations if need be. See less Victoria, British Columbia Solwood Studio Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C348" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3975145332748137/</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Friday from 20:00-00:00 Bachata Night Method Studio - Victoria BC About Discussion More About Discussion Bachata Night Interested Going Invite Details 66 people responded Event by Bachata Nights Victoria BC , Sebastian Carmona and Alysha Kopala Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights June 13 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria, BC Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C349" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1069894401564900/</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Monday Nights! 111 Superior St, Victoria, BC V8V 1T2, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion Sensual Bachata Series – Monday Nights! Details 15 people responded Event by Victoria Latin Dance Association 111 Superior St, Victoria, BC V8V 1T2, Canada Duration: 3 hr Public · Anyone on or off Facebook Sensual Bachata Series – Monday Nights! Mondays – April 7th, 14th, 21st &amp; 28th at 111 Superior Street Foundation Class (6:30–7:35 PM) Perfect for absolute beginners or dancers looking to strengthen their foundation! In this class, we’ll break down the essential steps, body movement, and partner connection in a fun environment. You’ll learn the basics with proper technique while also adding styling to make your dancing look and feel smooth on the dance floor. No experience or partner needed—just bring your curiosity and energy! Intermediate Class (7:35–8:40 PM) Ready to level up? This class is designed for dancers who already feel comfortable with the basics and want to challenge themselves. We’ll dive into more fun patterns while also exploring musicality—how to connect those movements to the music in a more expressive way. Get ready to build confidence, fluidity, and your own unique style! To Register: Send your e-transfer to maximumotion@gmail.com and include in the memo: Foundation, Intermediate, or Both + Lead or Follow Class Cancellation &amp; Refunds We understand that plans can change. However, due to limited spots, renting space in advance, and the preparation required for each class, we’re unable to offer refunds for cancellations. Please make sure you’re committed before signing up. We truly appreciate your understanding and support! See less Victoria, British Columbia 111 Superior St, Victoria, BC V8V 1T2, Canada 111 Superior St, Victoria, BC V8V 1T2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C350" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1388695712154512/</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 70 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation June 22, 2025 | Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C351" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1350929566137538/</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 5 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation August 10, 2025 | Lesson: Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C352" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/717475250956404/</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Friday 30 May 2025 at 18:00 FREE Beginner Bachata Class 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 About Discussion More About Discussion FREE Beginner Bachata Class Details 65 people responded Event by Mayfair Shopping Centre and Victoria Latin Dance Association 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 Public · Anyone on or off Facebook Ready to get your groove on? We’re teaming up with the Victoria Latin Dance Association  for a FREE Beginner Bachata Class right here at Centre Court! Join us on Friday, May 30 at 6:00 PM for an evening of fun and dancing. FREE Beginner Bachata Class May 30th, Friday at 6PM NO partner or experience necessary! Bachata is a beautiful and easy-to-learn dance that’s great for meeting new people, getting active, and connecting with an amazing community. See less Dance Victoria, British Columbia 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 3147 Douglas St, Victoria, BC V8Z 3K3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C353" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342233713680795/</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Thursday 1 May 2025 at 21:00 Bachata &amp; Merengue- All Levels- May Series Studio 4 Athletics About Discussion More About Discussion Bachata &amp; Merengue- All Levels- May Series Details 3 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Bachata &amp; Merengue are both dances from the Dominican Republic. Bachata can be anywhere from slow and romantic with lots of dips, sway and body movement to more upbeat and percussive with lots of musical footwork. Merengue is carefree, flirtatious and fun! Classes are registered on a monthly basis and take place every Thursday from 8:00- 9:00pm, May 1, 8, 15, 22, 29. No experience required.  No partner is necessary as we rotate partners throughout the lesson.  Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C354" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1901245437276872/</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Friday 9 May 2025 from 20:00-00:00 Bachata Nights Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Details 40 people responded Event by Bachata Nights Victoria BC , Alysha Kopala and Sebastian Carmona Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights May 09 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @yourgirlalysha  and @davidch_78  will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person The evening starts with an Open-level Bachata lesson from 8:15 PM to 9:00 PM—great for all skill levels! Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria, BC Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C355" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1057471579628015/</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Friday 16 May 2025 at 17:00 Bachata Nights Victoria Bc Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Victoria Bc Details 9 people responded Event by Bachata Nights Victoria BC and Sebastian Carmona Method Studio - Victoria BC Public · Anyone on or off Facebook Join us on our next Bachata Nights May 23 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria, BC Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C356" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1382188962971661/</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Tuesday 1 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Fundamentals- April Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- April Series Details 9 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, Apr 1, 8, 15, 22, 29 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C357" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/966455485665576/</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Thursday 3 April 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- April series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Apr 1, 8, 15, 22, 29 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C358" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/10048344358532607/</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- May series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. May 6, 13, 20, 27 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C359" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2214494908966327/</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Monday 5 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Int/ Adv- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- May series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, May 5, 12, 26 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C360" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/669591372187091/</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 10:00-11:00 Salsa &amp; ChaCha Solo Westshore Dance Studios Sat, 17 May Sat, 24 May Sat, 31 May +7 About Discussion More About Discussion Salsa &amp; ChaCha Solo Details 2 people responded Event by Dance Praktika Westshore Dance Studios Duration: 1 hr Public · Anyone on or off Facebook Elevate your dance journey with our Ladies Solo Class. Join our exciting series and learn the basics of Salsa and Cha Cha. Perfect for beginners looking to spice up their dance skills! Class Highlights: - Learn exciting dance moves tailored for solo dancers; - Fun and welcoming environment; - Suitable for absolute beginners. Come dance with us and let the rhythm guide you! To register to April classes please use links at "Tickets". See less Langford, British Columbia Westshore Dance Studios 109-2675 Wilfert Road, Victoria, BC www.westshoredance.com 2years+ Competitive&amp;Production a space for everyone with a love of dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C361" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342792743590871/</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Monday 7 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- April series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, April 7, 14, 28. Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C362" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2233725973712106/</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Monday 3 March 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- March series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- March series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, Mar 3, 10, 17, 24, 31 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C363" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/679241811720932/</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Fundamentals- May Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- May Series Details 7 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, May 6, 13, 20, 27 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C364" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1298465587898458/</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Tuesday 4 March 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- March series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- March series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Mar 4, 11, 18, 25 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C365" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1059622278965884/</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Active now Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 8 Saturday 8 November 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in October. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events This Saturday at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 182 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Sophia, Roy and 9 friends 1176 people interested Interested Sun, 22 Jun at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Sophia, Roy and 3 friends 70 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C366" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3899920353641309/</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Active now Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 9 Saturday 9 August 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in July. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events This Saturday at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 182 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 52 people interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends 66 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C367" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1239163193996279/</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Active now Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 14 Saturday at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Tickets · CA$17.31 www.eventbrite.com/e/caliente-salsa-saturdays-tickets-1390062838369 Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in May. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Tickets Find Tickets Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Fri, 11 Jul at 21:00 Locarno 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 13 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 52 people interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends 66 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C368" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1624603351798270/</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Active now Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 April 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 5 Jul at 19:00 Josh Warren Presents: The Path (LIVE @ Hermann's!) Hermann's Jazz Club 22 people interested Interested This Saturday at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 182 people interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends 66 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C369" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2251848171850840/</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Active now Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 Saturday 10 May 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in April. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Fri, 11 Jul at 21:00 Locarno 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 13 people interested Interested This Saturday at 21:00 Vibrate - Mood Change (YVR), Ageless, Big Body 1325 Government Street,Victoria,V8W 1M5,CA 182 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 52 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C370" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/530862806349067/</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Sunday 30 March 2025 from 13:00-17:00 Salsa Gonzales tasting! 🍋‍🟩 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia About Discussion More About Discussion Salsa Gonzales tasting! 🍋‍🟩 Details 6 people responded Event by THE ROOT CELLAR | village green grocer 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia Duration: 4 hr Public · Anyone on or off Facebook Hey friends! It's time to get those tastebuds tingling - you're invited to come and join us for a Salsa Gonzales tasting at our McKenzie Corner store! Salsa Gonzales is a little condiment company with a big personality! Nestled on Gonzales Beach in Victoria, they craft salsas, hot sauces, pickles, preserves, and more – all with a generous splash of love and a fiery kick. When: Sunday March 30th, 1pm-5pm Where: Our McKenzie Corner location We're looking forward to seeing you there! XO See less Victoria, British Columbia 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia 1286 McKenzie Ave, Saanich, BC V8P 5P2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C371" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/884101187183426/</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Active now Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 July 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in June. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1920 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends 66 people interested Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 232 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 46 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C372" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1636237610432412/</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Saturday 16 August 2025 from 20:00-23:59 Salsa Sunset Latin Party – August 16th! Latin Dance Canada About Discussion More About Discussion 🌅🔥 Salsa Sunset Latin Party – August 16th! 🔥🌅 Interested Going Invite Details 29 people responded Event by Latin Dance Canada Latin Dance Canada Duration: 3 hr 59 min Public · Anyone on or off Facebook Salsa Sunset Latin Party – August 16th! Get ready for a magical summer night filled with Latin rhythms, sunset vibes, and non-stop dancing! Join us for the Salsa Sunset Latin Party, where the Salsa, Bachata, and Merengue beats will keep you moving all night long under the stunning sunset sky! Dress Code: Wear your best sunset-inspired outfit – think bright, tropical colors, and beach party vibes! Dance to the best Salsa, Bachata, Merengue &amp; Latin hits all night! No partner? No problem! Join our fun intro class at 8:00 PM! Location: Ukrainian Cultural Centre, 3277 Douglas St., Victoria, BC Date: Saturday, August 16, 2025 Intro Class: 8:00 PM | Social Dance: 8:30 PM - Late Entry: $15 at the door – Bring cash, please! What to Expect: Vibrant salsa rhythms &amp; tropical vibes! Tropical-themed decorations &amp; stunning sunset views! A welcoming dance community &amp; unforgettable fun! Let’s dance as the sun sets and make it a night to remember! Tag your friends and let’s create memories under the summer sky! #SalsaSunsetLatinParty #SalsaBachata #LatinDanceParty #VictoriaBC #LatinDanceCanada See less Dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C373" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1356293392177099/</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Monday 3 March 2025 from 18:30-21:30 Open House | FREE Classes - Bachata Sensual &amp; Brazilian Zouk 1709 Blanshard St, Victoria, BC V8W 2J8, Canada About Discussion More About Discussion Open House | FREE Classes - Bachata Sensual &amp; Brazilian Zouk Details 28 people responded Event by Bachata and Zouk with Javi in Victoria and Javi Zouker 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 3 hr Public · Anyone on or off Facebook Join us for our Open House / Free classes on Monday March 3rd with Javi Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on body awareness, lead and follow techniques, musicality, styling, and how to have lots of fun dancing with new friends!  Learn with Javi, with over ten Years of teaching experience.  Learn dance with clear, fun, and inspiring teachings open to all levels! Schedule: Monday March 3rd 6:30-6:45pm | Meet &amp; Greet 6:45-7:30pm | Traditional Bachata - Beginner 7:40-8:25pm | Sensual Bachata - Intermediate 8:35-9:20pm | Brazilian Zouk - Beginner 9:20-9:30pm | Sharing circle Tuition = FREE Space is Limited:  Please email us to register your spot and please share if you are leading or following or open to either. email:  danceinflow@gmail.com 4 week session on Monday March 10-31st Phillippine Bayanihan Community Centre - 1709 Blanshard st, Victoria, BC See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C374" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1106484714432492/</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Wednesday 25 June 2025 from 18:30-21:00 Zouk practica and social White Eagle Hall, 90 Dock St, Victoria BC Wed, 4 Jun Wed, 25 Jun Wed, 2 Jul +41 About Discussion More About Discussion Zouk practica and social Interested Going Invite Details 3 people responded Event by Victoria Zouk Collective and Victoria Zouk Collective Group White Eagle Hall, 90 Dock St, Victoria BC Duration: 2 hr 30 min Public · Anyone on or off Facebook Drop-in zouk practica by donation - everyone welcome! White Eagle Polish Hall every Wednesday 6:30-9 pm Shared warm up, free dance time, review material from lessons and congresses, connect and share knowledge! Help is always available. Minimum $5 donation. Cash at the door, or etransfer to oceanzouk@gmail.com Enter the lower hall by the side door on Niagara Street just beside the Polka food truck. Also available in Victoria are zouk lessons with Javi, an amazing instructor from Vancouver! More info at https://www.facebook.com/Sabor.Asi.Dance.Salsa.Victoria or email danceinflow@gmail.com See you there! See less Victoria, British Columbia White Eagle Hall, 90 Dock St, Victoria BC 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C375" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1411005319893067/</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Monday 28 April 2025 from 18:30-22:30 Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion 🔥Bachata &amp; Brazilian Zouk 🌊 dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard Details 7 people responded Event by Bachata and Zouk with Javi in Victoria 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 4 hr Public · Anyone on or off Facebook Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard street | Victoria Join us for a 4 week course exploring the joy and magic of Brazilian Zouk &amp; Bachata dancing! Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on enhancing body awareness, building confidence in dance vocabulary with lead and follow techniques, exploring musicality, and loving yourself deeper with styling! Be prepared to have lots of fun dancing with new friends! Register today! Schedule: Monday April 7 - 28th 6:30-7:25pm | Brazilian Zouk - Level 2 (ask Javi for permission) 7:30-8:25pm | Brazilian Zouk - Level 1 8:30-9:25pm | Sensual Bachata - Beginner Foundations 9:30-10:30pm | Sensual Bachata - Intermediate "Trending Moves" Tuition: $20 | 1 Class $35 | 2 Classes (Brazilian Zouk 1&amp;2, or Brazilian Zouk 1 &amp; Bachata, Bachata 1&amp;2) $50| 3 Classes (3 classes, BEST value) 1709 Blanshard St, Victoria, BC Registration: E-transfer to: danceinflow@gmail.com or send us a message on Whatsapp: 7785877665 (Also accepting credit card/cash at the door) Please add a note if you're registering as a "Leader", "Follower", or "Open to both" Space is limited. Register in advance to reserve your spot! Looking fwd to dancing and flowing with you, Warmly, Javi See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C376" s="3" t="n">
+        <v>45819.87887427083</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/544121845403419/</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 13:00-23:55 Swing Session: Balboa with Yoshi and Etsuko Solwood Studio About Discussion More About Discussion Swing Session: Balboa with Yoshi and Etsuko Details 108 people responded Event by Swing Dance Association of Victoria , Dave Henderson and 2 others Solwood Studio Duration: 10 hr 55 min Public · Anyone on or off Facebook Lace up your shoes on May 31, 2025 for an afternoon of Balboa Classes and an evening of Social Dancing with Yoshi and Etsuko Uemura. 4 Classes for everyone &amp; 1 Social Dance! Passes go on sale April 19 at noon at our SDAV Square Shop! You must know and be comfortable with Balboa basics for all of these classes - they won't be covered at this workshop. All the specifics are available at swingvictoria.net , but here are the notes: May 31st, at Solwood Studio, with doors at 12:30pm . Bring indoor shoes, please! 4 classes for everyone and there's a dance from 9-12am. Passes go on sale April 19th at noon. See less Victoria, British Columbia Solwood Studio 1303 Broad St, Victoria, BC V8W 2A8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C377" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/302778660295534/</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Sunday 19 August 2018 from 18:00-21:00 West Coast Swing in the Park! Cameron Bandshell @ Beacon Hill Park Carolyn Gebbie invited you About Discussion More About Discussion West Coast Swing in the Park! Details 58 people responded Event by Carolyn Gebbie Cameron Bandshell @ Beacon Hill Park Duration: 3 hr Public · Anyone on or off Facebook Come join us for another evening of fun and WCS dancing in Beacon Hill Park! WCS music will be provided by DJ Carolyn. For those who are familiar with the routine, the 2018 WCS Rally Song will be played at 6:30, 7:30 and 8:30pm. Sam Jackson and Meaghan Efford, from wcsmovementmethods.com will be on hand to answer questions about WCS or how to improve your WCS dancing. They will also demo some incredible WCS dancing at 7pm. Please invite your WCS dance friends by sharing this event! See less Victoria, British Columbia Cameron Bandshell @ Beacon Hill Park Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C378" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1692156731689650/</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Tuesday 17 June 2025 from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 Tue, 27 May Tue, 3 Jun Tue, 17 Jun Tue, 24 Jun +22 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Interested Going Invite Details 2 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Saanich, BC V8Z 3S3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C379" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/417338985546213/</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Thursday 29 August 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - August 29! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - August 29! Details 109 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for a fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria, BC Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C380" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2441697862726705/</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Sunday 30 June 2019 at 19:00 Journey’s 50th Birthday!!  A West Coast Swing dance party!! Eastern Star Hall Chapters No 5 &amp; No 17 Journeey Song invited you About Discussion More About Discussion Journey’s 50th Birthday!!  A West Coast Swing dance party!! Details 13 people responded Event by Journeey Song Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook 3281 Harriet Road, Victoria,BC Bring your own alcohol-free beverage... Bring a gluten-free appie if you’d like. Dance West Coast Swing until 10 pm to Blues, Pop, RnB, Swing, and a wee bit of Ballroom Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C381" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663756533046485/</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Friday 11 April 2025 at 21:30 Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. Details 36 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Public · Anyone on or off Facebook Miguelito Valdes presents Contodo What happens when you bring together three Cuban and two Canadian musicians, with a deep love of all music and a wide range of musical experiences?  A joyful mix of party and deep groove, that's what! Guaranteed to make you want to dance, these brothers from other mothers bring it all. Con Todo! Featuring: Miguelito Valdes – brass/vocals/percussion Jose Sanchez – drumset/timbales Hector Ramos – congas/percussion Peter Dowse - bass Brooke Maxwell – keys/vocals See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C382" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/402729737034904/</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Thursday 5 September 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Details 123 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for our second fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria, BC Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C383" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1594011994641933/</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Tuesday 22 April 2025 from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Details 9 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. No street shoes. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C384" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1035925295253912/</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Friday 18 April 2025 at 18:30 Swing out with the ATOMIC COCKTAILS 751 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Swing out with the ATOMIC COCKTAILS Details 64 people responded Event by Peter Sandmark 751 View St, Victoria, BC V8W 1J9, Canada Public · Anyone on or off Facebook Join the ATOMIC COCKTAILS as they swing out for their pre-Japan Tour dance party on April 18 at the Coda, 751 View Street.  Doors open 6 pn, show from 6:30-8:30 pm!  Tickets $20.  With songs from their new album BLUE LIGHT BOOGIE! See less Victoria, British Columbia 751 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C385" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/634773653668605/</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Saturday Night West Coast Swing BC Swing Dance Club Victoria 15 Jun 2019 22 Jun 2019 29 Jun 2019 +2 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night West Coast Swing Details 9 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook June means summertime and sunny days! Along with the weather, things for BC Swing Dance Cub Victoria will be changing too. Here's what is happening this month: 7 - 8pm 1st Saturday of the Month: Lesson with Meaghan, plus an assistant from our dance community 7 - 8pm Remaining Saturdays each month: TBD (stay tuned for workshops, activities or practices - updates will be posted on each event page) Note:  The 7 - 8pm weekly timeslot is included in the dance entrance price. -------------------------------------------------- Come join us every Saturday all year long for a fabulous WCS social dance from 8 - 11pm. Just $10 for the ($5 for students). Meaghan Efford and Bob Gebbie 's lesson on June 1st (starting PROMPTLY at 7pm) will be the only lesson in June, and it will be a great way to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity.  The lesson is included in the dance entrance price.  No experience or partner is required. -------------------------------------------------- • 6:45 pm - Doors open • 7:00 pm - TBD each week* • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *lesson with Meaghan and Bob on June 1st Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C386" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/373500473108499/</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Sunday Swing at Logan's Logan's Pub 10 Dec 2017 Debi Wong invited you About Discussion More About Discussion Sunday Swing at Logan's Details Event by Swing X Logan's Pub Duration: 3 hr 30 min Public · Anyone on or off Facebook Sunday Swing at Logan's is BACK! Come join us for some great tunes and we'll party like it's 1939. Bring your dancing shoes, sweet moves, and a few dollars for our fabulous DJ (and gracious bartenders). Feel free to come early to hang out and grab a bite to eat. 19+. NEW: Crash course 15min swing lesson at 8:30pm! This is intended to be the bare minimum for someone to show up and know the basics of swing dancing, nothing fancy! DETAILS: * 8:30pm Quickie 15min beginner lesson! * 8:45pm social dancing until as late as midnight (maybe!) * Usually gets bluesy after 11pm See less Victoria, British Columbia Logan's Pub 1821 Cook Street, Victoria, BC Original - Authentic - Unique Guests See All</t>
+        </is>
+      </c>
+      <c r="C387" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1776457206589544/</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Friday 21 March 2025 from 18:30-20:30 Slim Sandy's Atomic Cocktails swing speakeasy party! The Coda About Discussion More About Discussion Slim Sandy's Atomic Cocktails swing speakeasy party! Details 72 people responded Event by Peter Sandmark and Trace Nelson The Coda Duration: 2 hr Public · Anyone on or off Facebook Join Slim Sandy's Atomic Cocktails and dance as they play 2 sets of swing jazz, jive and rhythm and blues from the 20’s to the 40’s. Slim, on guitar and harmonica, is joined by Willa Mae on vocals, “Big Daddy Bo” on bass, and Bryn Bad on trumpet.  Slim Sandy has been playing music for over 40 years with acts such as Ray Condo and the Crazy Rhythm Daddies.  In 2012, he and Willa Mae co-created the Slim Sandy band in Victoria!  They have played music festivals in Canada, France, Spain, Germany, Belgium, and the Netherlands.  In May they will be touring in Japan! See less Victoria, British Columbia The Coda 749 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C388" s="3" t="n">
+        <v>45819.88538226852</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1009684807956058/</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 17 17 May at 17:00 – 18 May at 13:30 Tango weekend with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Tango weekend with Jorge Olguín Details 28 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 17th 5pm-6pm solo technique all levels. ( no partner required) Please bring elastic bands!! 6.30pm-7.30pm for couples only ( need some experience) Sacadas, barridas and colgadas in an elastic embrace in order to create a circular movement. We will work with different orchestras to study the changes we need to do to introduce different tempos and rhythms. Get ready for a workout with musicality! 8pm milonga !!! Join us even if you didn’t take the classes. DJ Ingrid !! Free for people registered for the workshops. $10 for drop-ins. Sunday, 18th 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are June 21st &amp; 22nd Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria, BC Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C389" s="3" t="n">
+        <v>45819.88756766204</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1864555154338100/</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 21 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Alive Tango Victoria About Discussion More About Discussion Weekend with Tango Interested Going Invite Details 15 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 21st 5pm-6pm solo technique all levels. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) We will continue from May with the musicality for phrase change but this time we will add “double time” to help us with it, using examples of different orchestras. We will work with a “rebound” and half giros to change the direction within the phrase. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 22nd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are September 20th &amp; 21st. Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria, BC Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C390" s="3" t="n">
+        <v>45819.88756766204</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1766891834185825/</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Victoria, BC About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam and Alive Tango Victoria Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends SAVE THE DATE! The next Sunday afternoon Milonga is on 8 June 2025 1-4pm. The Coda Club (formerly Hermanns Upstairs) is a beautiful newly renovated venue with awesome ambience, nice wood floor and great sound system. Come join us for a wonderful afternoon of warm hugs and close embrace. Sunday 8June 2025 1-4pm The Coda, 751 View Street, Victoria Admission: $15 (plus tax) Special Guest DJ: Francis Nowaczynski (from Vancouver) Free parking at View Street Parkade (next door) or Broughton Parkade. Cash bar is open for drinks. See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C391" s="3" t="n">
+        <v>45819.88756766204</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1318668532737609/</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 16 16 Apr at 18:30 – 18 Apr at 21:00 Tango week with Lya Alive Tango Victoria About Discussion More About Discussion Tango week with Lya Details 36 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 3 days Public · Anyone on or off Facebook Ignite Your Tango 16th of April, Wednesday 6:30-8:00 On &amp; Off Acis for social dance 18th of April, Friday 6:00 - 7:30 Follower technique 7:45 - 9:00 Switch role / connection Search - Grow &amp; Transform! Seminar series for Tango Dancers that want to transform their way of moving and connecting! We will travel through the Essentials of Tango in order to look for new answers and deeper understanding. What makes tango truly captivating? It’s the embrace, the connection, and the walk. These three fundamental elements are the heartbeat of tango, and mastering them is essential for creating an unforgettable dance experience. You will learn how to condition your body to move with control, fluidity, and elegance. You’ll discover how to find and perfect your axis, which is essential for maintaining balance and stability in every step. We will also explore dissociation, a technique that allows you to move the upper and lower body independently but associated. This workshop series will show you how to apply these principles in both the leader and follower roles, improving connection and response in every moment of the dance. We will apply all this to: The secrets to generating power for boleos effortlessly off and on axis special follower technique class Pro tips to dance with ease and confidence 90 min class - $30 All 3 classes - $80 To register email grazs@shaw.ca or pm me, or talk to me . See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria, BC Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C392" s="3" t="n">
+        <v>45819.88756766204</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3637725693193744/</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 22 Mar at 17:00 – 23 Mar at 13:30 Weekend with Tango with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Weekend with Tango with Jorge Olguín Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 22nd 5pm-6pm solo technique all levels. Balance and weight transfer while walking, change of dynamics to create a better connection with your body. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) Marathon is just around the corner so this month we continue with comfortable close embrace! We continue with dancing in small spaces!! Let’s move gracefully without affecting the partner's axis in elastic hugs of closed embrace. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 23rd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available only on Saturday. Sunday - sold out Next workshop dates are the May 17th &amp;18th Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria, BC Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C393" s="3" t="n">
+        <v>45819.88756766204</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/641769172035949/</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Saturday April 12 Beginner lesson and social dance at Dance Victoria Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 12 Beginner lesson and social dance at Dance Victoria Details 5 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginners lesson by Donna from 7 to 8 pm Social dancing from 8 to 10:15 pm DJs Andre and Nel Cost $15 /$12 for Students No need to register and no partner required. Please bring scuff-free inside dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C394" s="3" t="n">
+        <v>45819.89009380787</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1366072544640156/</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Saturday 17 May 2025 at 18:45 Victoria WCS Collective Beginner Lesson and Social Dancing Dance Victoria About Discussion More About Discussion Victoria WCS Collective Beginner Lesson and Social Dancing Details 9 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson from 7 to 8 pm by John de Pfyffer Social dancing from 8 to 10:15pm DJg by Donna and Nel Cost $15/ $12 for students No need to register and no need for dance experience.. Also, no partner necessary, we got you! Please bring indoor scuff-free dance shoes or socks to dance in. See less Victoria, British Columbia Dance Victoria 2750 Quadra St # 111, Victoria, BC Dance Victoria brings the "World's Best Dance" to the Royal Theatre and supports new dance creation for the international stage from its studios. Guests See All</t>
+        </is>
+      </c>
+      <c r="C395" s="3" t="n">
+        <v>45819.89009380787</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2162855673833831/</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 11 May 2019 18 May 2019 25 May 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 8 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook Wow! April went by so quickly, which means it must've been super fun, which it definitely was.  Everyone at BC Swing Dance Club Victoria is so pleased with the way the first month of social dances went, and we hope to generate the same amount of enthusiasm in May. Let's make this month just as much fun! Come join us on May 4th for the first intro lesson and social dance of the month (plus every Saturday night after that). Just $10 for the lesson and/or social dance ($5 for students). No experience or partner required. • 6:45 pm - Doors open • 7:00 pm - Intro lesson with Sam Jackson and Meaghan Efford * • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *PLEASE NOTE that the weekly lessons will start PROMPTLY at 7pm.  It is disruptive to the flow of the lesson if participants arrive late. For anyone who's interested in building their West Coast Swing fundamentals quickly, note that May will be the last month we'll be offering weekly classes with both Sam and Meaghan. With summer approaching it's a great time to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity. Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C396" s="3" t="n">
+        <v>45819.89009380787</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1225266505917189/</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Saturday Beginner Lesson and Social Dancing Dance Victoria Sat, 7 Jun Sat, 14 Jun Sat, 21 Jun +4 About Discussion More About Discussion Victoria WCS Collective hosts Saturday Beginner Lesson and Social Dancing Interested Going Invite Details 4 people responded Event by Donna Forsyth Dance Victoria Duration: 3 hr 30 min Public · Anyone on or off Facebook Back to AIR CONDITIONED comfort at Dance Victoria Studios Beginner lesson from 7 to 8 pm Social dancing  from 8 to 10:15 pm Cost $15/$12 for students No need to register and no need for previous dance experience or a partner. Please bring scuff-free inside low-heeled dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C397" s="3" t="n">
+        <v>45819.89009380787</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1024182725709172/</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Saturday April 19th Lesson and Social Dance Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 19th Lesson and Social Dance Details 4 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginner plus lesson with Pamela Podmoroff from 8 to 10:15 pm Social dancing from 8 to 10:15 pm DJs Donna and Amanda Cost $15/ $12 for students No need to register and no partner required. Please bring scuff-free indoor dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C398" s="3" t="n">
+        <v>45819.89009380787</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2238975779474166/</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 13 Apr 2019 20 Apr 2019 27 Apr 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 23 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook A new month, a new social! Come and join in on the fun at our inaugural Saturday night dance and intro lesson on April 6 (and every Saturday night after that)! Just $10 for the Lesson and/or Social ($5 for Students). No experience or partner required. • 6:45 pm – Doors open • 7:00 pm – Beginner Lesson with Sam and Meaghan (this is perfect as a refresher class too!) • 8:00 – 11:00 pm Social Dancing featuring DJ Carolyn Please note the NEW START TIMES for the BC Swing Victoria Saturday night dances. See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C399" s="3" t="n">
+        <v>45819.89009380787</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/516994561244886/</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:45 Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING White Eagle Polish Association About Discussion More About Discussion Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING Details 15 people responded Event by Donna Forsyth , Andre Russo and Victoria West Coast Swing Collective White Eagle Polish Association Public · Anyone on or off Facebook Doors open at 6:45pm at this fabulous new venue! Advanced beginner/intermediate lesson by Chantelle Pianetta from 7 to 8 pm Social dancing for 3 HOURS from 8 to 11 pm DJs Donna and Andre Cost $15 /$12 for students ALL at the spacious White Eagle Hall No need to register and you do not need a dance partner. Please bring scuff-free dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia White Eagle Polish Association 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C400" s="3" t="n">
+        <v>45819.89009380787</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/967438905456066/</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Wednesday 26 March 2025 at 10:00 Victoria WCS Lesson and Dance at Eastern Star Hall Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria WCS Lesson and Dance at Eastern Star Hall Details 1 person responded Event by Donna Forsyth Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson by John de Pyffer from 7 to 8 pm Social dancing from 8 to 10:15pm Djs Amanda and Nel Cost $12 No need to register and no partner required. Please bring scuff-free indoor shoes or socks to dance in  and a water bottle. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C401" s="3" t="n">
+        <v>45819.89009380787</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/644050564927019/</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Victoria, BC About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends! A NEW SUNDAY AFTERNOON MILONGA! This is the first of a regular monthly milonga at a beautiful new venue…The Coda Club (formerly Hermann’s Upstairs) at 751 View Street, Victoria. Great ambience, nice wood floor, good sound system. So come join us for the warm hugs and close embrace and dance to the beautiful music of our very own DJ John Dewhirst. Sunday, 6 April 2025 2.00pm-5.00pm The Coda Club, 751 View Street, Victoria Admission $15 DJ: John Dewhirst Cash Bar is open for drinks Free Parking at View Street Parkade just next door Come celebrate this exciting day with us! See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C402" s="3" t="n">
+        <v>45819.89157356481</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1022330066692643/</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Wednesday 2 July 2025 at 18:30 Technique and Milonga with Monica Parra Alive Tango Victoria About Discussion More About Discussion Technique and Milonga with Monica Parra Interested Going Invite Details 22 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Public · Anyone on or off Facebook 2nd of July , Wednesday 6.30-8pm Follower’s technique: Pivots and turns • Dissociation technique and axis control. • Free leg preparation before the turn. • Turns in tight spaces (useful in a close embrace!!) 90 minutes, $30 9th of July , Wednesday 6.30-8pm Couple workshop: Milonga Lisa and Milonga with traspie using different tempo. 90 minutes, $30 Both workshops (July 2nd and 9th)$50 Register with Grazyna (grazs@shaw.ca, Messenger or simply talk to me) Contact me personally for privates with Monica. See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria, BC Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C403" s="3" t="n">
+        <v>45819.89157356481</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/713923214640962/</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Sunday 4 May 2025 from 13:00-16:00 May 4th Afternoon Milonga Solwood Studio About Discussion More About Discussion May 4th Afternoon Milonga Details 45 people responded Event by Ingrid Love and Kathryn Stone Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook A one-time special afternoon milonga! Join us in celebrating the warmth of Spring and return to sunshine. Or, star wars, if you like. Featuring special guests Kimberly and Khang performing live music (violin/guitar) DJ Ingrid Hosts: Kathryn &amp; Ingrid $15 entry (cash only) 1:00pm-4:00pm Solwood Studio 1303 Broad St Victoria, BC See less Victoria, British Columbia Solwood Studio Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C404" s="3" t="n">
+        <v>45819.89157356481</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1414577976223422/</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 19:00-23:00 Solstice Slammer 3 - Moon Under Water, Victoria The Moon Under Water Brewpub About Discussion More About Discussion Solstice Slammer 3 - Moon Under Water, Victoria Interested Going Invite Details 49 people responded Event by Electric Druids and Gate Theory The Moon Under Water Brewpub Tickets · CA$10 www.eventbrite.com/e/solstice-slammer-3-tickets-1389012316229 Public · Anyone on or off Facebook Come join us for Solstice Slammer III at Moon Under Water Brewpub and Distillery! Get ready to celebrate with Electric Druids, Gate Theory and West Street Children, hefty drinks and good vibes. Whether you're a craft beer enthusiast or just an enthusiast, there's something for everyone at this epic night of live music. Don't miss out - mark your calendars! See less Music and audio Victoria, British Columbia Tickets Find Tickets The Moon Under Water Brewpub 5435 Fowler Rd, Saanich, BC V8Y 1Y4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C405" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1142760357225336/</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 26 26 Jul at 10:00 – 27 Jul at 17:00 ArtisTREE Festival 1401 rockland ave, Victoria, BC, Canada About Discussion More About Discussion ArtisTREE Festival Interested Going Invite Details 1.1K people responded Event by Artistree Festival , MORENA CLOTHING and Cory Judge 1401 rockland ave, Victoria, BC, Canada Duration: 2 days Public · Anyone on or off Facebook Saturday July 26 10-7pm Sunday July 27 10-5pm Government House of BC 1402 Rockland Ave Celebration of Creativity profiling 130 Juried Artisans, Live Music, Installation and Performance Art, Indigenous Makers and Traditions, Kids section, Live Painters, Delicious Food and Ice cream. See less Shopping Victoria, British Columbia 1401 rockland ave, Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C406" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3513597908934465/</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Saturday 12 April 2025 from 12:00-20:00 Live Music Benefit Event for Veteran's House 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion Live Music Benefit Event for Veteran's House Details 34 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 8 hr Public · Anyone on or off Facebook Admission by Donation (Non-Perishable Food Items, Charitable Donations, Gift Cards, accepted). Enjoy live music throughout the day by Bryce Allan, Love Cats, OTR, Donny Peterson &amp; the Tone Rangers, Helen Davies, and David Carl Trio. See less Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C407" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/979769967649565/</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 15:00-18:00 Live Music at the Legion 102-622 Admirals Rd, V9A 2N7 Sat, 17 May Sat, 24 May Sat, 31 May +2 About Discussion More About Discussion Live Music at the Legion Details 8 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Come enjoy live music on Saturdays 3-6 p. Dancing encouraged! Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C408" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/651664851189740/</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Sunday from 12:00-18:00 Music in the Orchard (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Music in the Orchard (RAIN OR SHINE) Interested Going Invite Details 169 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Come enjoy the start of the summer in the orchard. We have two amazing artists for you, some delicious fun summer ciders for you to try and amazing food to enjoy to complete the experience. Delicious Cider Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀ Beautiful location ⠀⠀⠀⠀ Dog Friendly ⠀⠀ ⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your WELL BEHAVED two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C409" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/639017139056190/</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Saturday 19 April 2025 from 15:00-18:00 Live Music - Love Cats 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion Live Music - Love Cats Details 22 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Members $5, Guests $10 Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C410" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1198411931645258/</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Saturday 26 April 2025 from 15:00-18:00 LIVE MUSIC - The City Slickers 102-622 Admirals Rd, V9A 2N7 About Discussion More About Discussion LIVE MUSIC - The City Slickers Details 21 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Members $5, Guests $10 Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C411" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1093118172681618/</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>(20+) The Joan Bessie Cabaret: a celebration of original  live music and dance | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Active now Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 29 Sunday 29 June 2025 from 19:00-22:00 The Joan Bessie Cabaret: a celebration of original  live music and dance Metro Studio Theatre About Discussion More About Discussion The Joan Bessie Cabaret: a celebration of original  live music and dance Interested Going Invite Details Event by Joan Bessie Metro Studio Theatre Tickets · CA$5-CA$35 www.eventbrite.ca/e/joan-bessie-cabaret-tickets-1248762816199 Public · Anyone on or off Facebook Get ready to experience a night of songs and choreography at this one-of-a-kind indie cabaret. Licensed all ages event. Music and audio Victoria, British Columbia Tickets Find Tickets Metro Studio Theatre 1411 Quadra Street at Johnson Street, Victoria, BC Meet your host Joan Bessie 13 past events · Page · Musician/band Joan Bessie is a chart topping Canadian artist. This page shares releases &amp; live tour information Message Suggested events This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends 66 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Sophia, Roy and 9 friends 1178 people interested Interested Sat, 5 Jul at 12:00 Victoria, BC - Victoria Folk Music Festival, Royal Athletic Park Royal Athletic Park Debi and Carmie are interested 1194 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C412" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2579625309035667/</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Sunday 18 May 2025 from 12:00-18:00 Live Music @ Junction (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Live Music @ Junction (RAIN OR SHINE) Details 125 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Here we go again, its a long weekend so let's get our Sunday Funday on. First Live Music of the year at Junction Up first is-  Emergency Exit  are playing from 1230-230pm To take us home is - An &amp; Ben are playing from 3-5pm Tasting Room and Picnic Area are open 12-6pm Oh and if you haven't heard me say it before ITS RAIN OR SHINE. Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Cider ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Mini Market and a Beautiful location ⠀⠀⠀⠀⠀⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your well behaved two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C413" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/665127126496204/</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Tuesday 27 May 2025 at 19:30 Live Music at the Saxe Point Public House Saxe Point Public House About Discussion More About Discussion Live Music at the Saxe Point Public House Details 9 people responded Event by VINYL WAVE Saxe Point Public House Public · Anyone on or off Facebook Live Music every other Tuesday starting May 27th! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria, BC The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C414" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1975172826621817/</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>(20+) Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Active now Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Tomorrow from 19:00-20:30 Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Little Fernwood Gallery. About Discussion More About Discussion Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Interested Going Invite Details Event by Anna Bigland-Pritchard Little Fernwood Gallery. Tickets www.annabiglandpritchard.com/event-details/rest-resonate-restorative-yoga-ft-cozy-live-music Public · Anyone on or off Facebook Do you need some R&amp;R? Join Anna &amp; Roxie for a dreamy candlelit evening of restorative yoga, live music, and guided journalling. Facilitated by Roxie Fehr of Across the Water | Yoga Anna Bigland-Pritchard of ABP Music Studio | Music As experienced, intuitive space-holders, our goal to support your Nervous System and capacity for hope with a feast of restful offerings. We know life is stressful and we want to help you feel more connected to your intuition so you can not only survive, but also have the capacity to take the next right step in your life in a way that positively impacts the world. The space will be dreamy, there will be tea, guided journalling, poetry, restorative yoga shapes that can be adapted for any body, and LIVE MUSIC! Anna will be playing guitar, creating dreamy sound worlds with vocal looping, and singing you lullabies all evening. What to bring Yoga mat (We'll have a few available to borrow) Journal &amp; pen/pencil (We'll also have some spare paper and writing/drawing utensils) Yourself in your comfy cozies Details June 12, 7-8:30pm at Little Fernwood $42 Accessibility This event is on the ground floor There is a unisex/non-gendered bathroom on the same level We care about making this event accessible, so please let us know if you have any questions or accessibility needs. This will be a VERY gentle practice, and modifications will be offered. Happy pride! As members of and allies of the 2SLGBTQIA community, we (Anna &amp; Roxie) will create a supportive, inclusive, affirming environment and expect all participants to do the same. If cost is a barrier, please contact us directly as we have a limited number of discount codes available This is our first time offering this class, and we hope it will be a hit so we can make it a regular thing. Come as you are, leave nourished by your dreams See less Victoria, British Columbia Tickets Find Tickets Little Fernwood Gallery. 1923 Fernwood Ave., Victoria, BC Meet your host Anna Bigland-Pritchard 5 past events · Page · Musician/band Based in Lekwungen territory (Victoria, BC), Anna Bigland-Pritchard is a: -Soprano -Voice teacher… Follow Suggested events Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested 6615 people interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends 66 people interested Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 232 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C415" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/4223643791110348/</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Sunday 22 June 2025 at 13:00 Victoria Italian Day 195 Bay St, Victoria, BC V9A 3K4, Canada About Discussion More About Discussion Victoria Italian Day Interested Going Invite Details 5 people responded Event by Calabrisella 195 Bay St, Victoria, BC V9A 3K4, Canada Public · Anyone on or off Facebook Join us for live music, food, gelato, games, cars, cultural exhibits, vendors, bike valets and much more - Free admission !! Victoria, British Columbia 195 Bay St, Victoria, BC V9A 3K4, Canada 195 Bay St, Victoria, BC V9A 3K4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C416" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/686146924271113/</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>(20+) Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Marketplace 3 new messages · 1d Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 2d Active now Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 2d Murray McAllindon Messages and calls are secured with end-to-end encryption. · 4d Aylene Kirchner Messages and calls are secured with end-to-end encryption. · 2w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 2w Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 2w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 4w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 4w Sue Holloway Messages and calls are secured with end-to-end encryption. · 4w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 5w Mary, Aylene Aylene: u  and your dancing looked great!
+enjoy guest · 5w Gail Grant Messages and calls are secured with end-to-end encryption. · 5w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all 13 Jun at 20:00 – 15 Jun at 01:00 Becky's Birthday Bash &amp; Fundraiser Mary and 8 friends Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Sophia and 4 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Friday from 20:00-00:00 Bachata Night Roy and 7 friends Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 5 Thursday 5 June 2025 from 19:00-22:00 Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz 753 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz Details Event by Adonis Puentes and Brent Jarvis 753 View St, Victoria, BC V8W 1J9, Canada Duration: 3 hr Public · Anyone on or off Facebook An evening of Jazzy Cuban Fusion Music; traditional, contemporary, romance and dance. Juno &amp; Grammy Nominated vocalist, Adonis Puentes, will be joined by the Jazz Bohemians, featuring Brent Jarvis (piano), Ken Lister (bass), Nicholas Marquez (percussion) and Brooke Maxwell (Sax). Adonis Puentes opens up the marvelous world of Cuban music to his audience the second they hear his rich voice. When the other players kick in with their tight, multi-layered arrangements, it becomes clear that Adonis is a powerful bandleader. Fronting an acoustic band, Adonis' vocals are surrounded by piano, bass, strings, and percussion. Music reflects the present and Adonis Puentes is a Cuban Sonero for our times. Adonis thrives on the growth and acclaim for his original sonero sound. As he puts it, "I feel like a messenger of my roots and tradition, blessed that with me I have taken my music and heritage to many different places in the world; from Cuba, to Canada, USA, Mexico, Europe and Asia. My mission is to make you dance and enjoy my melodies and rhythms." Musician Line-Up: Adonis Puentes - Vocals Brent Jarvis - Piano Ken Lister - Bass Nicolas Marquez - Percussion Brooke Maxwell - Sax See less Music and audio Victoria, British Columbia 753 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Meet your hosts Adonis Puentes 34 past events · Page · Musician/band Adonis Puentes is a great singer and an elegant composer and lyricist grounded and nourished by his Cuban roots and worldly experience. Message Brent Jarvis 37 past events · Profile · Musician Message Suggested events Sun, 22 Jun at 14:00 Victoria Ska &amp; Reggae Fest Finale feat. illScarlett, MonteBong, Devon Kay, Brasser, Razorvoice Victoria, BC, Canada, British Columbia 341 people interested Interested Wed, 18 Jun at 16:00 Victoria Ska &amp; Reggae Fest Kickoff: Waahli, The Resignators, Hezron, Gun Street Ghouls &amp; Cabin Fever Victoria, BC, Canada, British Columbia 531 people interested Interested Thu, 19 Jun at 16:00 Victoria Ska &amp; Reggae Fest: Turbulence, La Severa Matacera, Spiritual Warriors, Sonic Alley &amp; Ari DL Victoria, BC, Canada, British Columbia 247 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Sophia, Lorne and 3 friends are interested Interested This Friday at 20:00 Bachata Night Method Studio - Victoria BC Roy, Lorne and 6 friends Interested Fri, 13 Jun-14 Jun FernFest 2025 Fernwood Square Sophia, Roy and 8 friends are interested Interested Sun, 29 Jun at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Sophia, Roy and 5 friends are interested Interested Sat, 14 Jun-15 Jun Mabuhay! Celebrating Filipino Heritage Month Centennial Square Ali, Jon and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C417" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1217747446718881/</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 18:00-22:00 Maifest - Evening of Live Music Edelweiss Club About Discussion More About Discussion Maifest - Evening of Live Music Details 36 people responded Event by Cindy Kent and Victoria Edelweiss Club Edelweiss Club Duration: 4 hr Public · Anyone on or off Facebook Join the Edelweiss Club for a lively evening of music and dance with Bijoux du Bayou and The Helen Davies Band. Let the infectious Zydeco beats and soulful rhythms set the tone for a night of fun, complete with delicious German snacks from the kitchen. Don’t miss out on this high-energy event! Get your tickets online or call 250-383-4823. www.victoriaedelweiss.ca/events See less Victoria, British Columbia Edelweiss Club 108 Niagara Street, Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C418" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1399479741193649/</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Saxe Point Public House About Discussion More About Discussion TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Details 4 people responded Event by Tom Watson Saxe Point Public House Public · Anyone on or off Facebook Join Vinyl Wave at the lovely Saxe Point Pub for a couple of hours of smooth tunes that'll help ease you into the week! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria, BC The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C419" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1110747367748372/</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Saturday 5 July 2025 at 12:00 Victoria Folk Music Festival Royal Athletic Park About Discussion More About Discussion Victoria Folk Music Festival Interested Going Invite Details 910 people responded Event by Victoria Folk Music Festival and Cascadia Concerts Royal Athletic Park Tickets · Free-CA$86.53 vicfolkfest.eventbrite.ca Public · Anyone on or off Facebook Date: July 5, 2025 Location: Royal Athletic Park, Victoria, BC Tickets: Available now at vicfolkfest.eventbrite.ca Gates Open: 12:00 PM Victoria Folk Music Festival Join us for a joyful weekend of music, community, and celebration at Victoria Folk Music Festival, on July 5th set in beautiful Royal Athletic Park . Featuring a world-class lineup including Frazey Ford, Joel Plaskett, Kacy &amp; Clayton, Harry Manx, Ferron, Old Man Luedecke, Vince Vaccaro, Canadian Beauty, Daneil Lapp's BC Fiddle Orchestra and more, this family-friendly event brings together the best in folk, roots, and Americana music. With two stages of live performances, the Victoria Folk Music Festival offers a full day of entertainment and community celebration. Explore the ReLove Vintage Pop-Up Market, showcasing top local vendors with the best in thrift, retro, and vintage wear. Enjoy a variety of Artisan goods and vendors, delicious food from Fresh Coast, Deadbeetz, Taco Revolution, and more. Families will love the vibrant children’s area—complete with a jumping castle! Dance in the grass to local Bluegrass groups and explore vendor booth from local music groups &amp; organizations. A community-driven atmosphere with world-class music at its heart, this festival is set to be a summer highlight for music lovers of all ages. Whether you're dancing barefoot in the grass, discovering your new favorite artist, or relaxing in the shade with friends, the Victoria Folk Music Festival is more than a concert — it’s a celebration of sound, soul, and connection. Don’t miss the unforgettable music and summer moments —July 5th at Royal Athletic Park! See less Music and audio Victoria, British Columbia Tickets Find Tickets Royal Athletic Park 1014 Caledonia Ave, Victoria, BC Royal Athletic Park is a multi-purpose, fully lit stadium in Victoria, British Columbia. It is primarily used for baseball, soccer, softball and football, but also hosts special events, such as the annual Great Canadian Beer Festival and Rifflandia Music Festival. It is approximately a ten-minute walk from the city centre.HistoryIn 1907 the burgeoning summer athletic teams did not have enough facilities for senior teams with paid attendances. Baseball in particular was challenged to find available dates at Oak Bay Grounds to operate due to a preference for lacrosse.Subsequently, the supporters of Canada's national summer sport lacrosse, at a meeting chaired by BC Premier McBride formed the Royal Victoria Athletic Association on March 26, 1908, and a senior lacrosse team was founded to enable the best intermediate (Under 21) players to play in the British Columbia Amateur Lacrosse Association (BCALA) League. The Oak Bay Grounds were put under the management of the senior baseball team and then later the Rugby Football Club. The lacrosse group, later shortened to the Royal Athletic Association, issued shares at $25 each with deposits of 10% and biannual calls of 10% to raise $25,000 for improvements to the grounds. The lease was signed for 5 acres at the corner of Cook and Pembroke Streets for the grounds.Contracts had been let by May 12, 1908 and $4,000 from the share offering and gate receipts was spent by June on the construction of a perimeter fence, 2 ticket offices, an inner fence, grandstand, and carriage parking area. The inner fence enclosed the 500 ft x 285 ft (152m x 87m) playing field. The grandstand on the south side of the playing field was 150 ft long x 25 ft deep with 10 rows of seats for more than 1000 spectators. Beneath the grandstand were dressing rooms and concessions. The original layout of the field and grandstand was essentially the same as today's; however based on maps used in advertising the original field also included half of the city block to the west between Quadra and Vancouver Streets. The carriage parking was on the east side off Cook Street. Guests See All</t>
+        </is>
+      </c>
+      <c r="C420" s="3" t="n">
+        <v>45819.89709724909</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1050242777151793/</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Friday from 18:00-19:30 Ladies Styling Bootcamp With Hannah 13 Jun at 17:00 – 14 Jun at 22:00 FernFest 2025 Sophia and 9 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 10 Jun at 09:00 – 15 Jun at 19:00 KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Victoria ,BC About Discussion More About Discussion KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Interested Going Invite Details 42 people responded Event by Congregation Emanu-El, Victoria, British Columbia Victoria ,BC Duration: 6 days Public · Anyone on or off Facebook Registration required for both in person and virtual attendance. https://klezcadia.org https://congregationemanuelnews.wordpress.com/.../klezca.../ Locations of performances and workshops provided upon registration. See less Victoria, British Columbia Victoria ,BC 528 Broughton St, Victoria, BC V8W 1C6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C421" s="3" t="n">
+        <v>45819.89709724909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Came up with a convention for logging names for all .py scripts. Updated pipeline.py to reflect that.
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -16,9 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -430,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C421"/>
+  <dimension ref="A1:C441"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6522,7 +6521,7 @@
         </is>
       </c>
       <c r="C405" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="406">
@@ -6537,7 +6536,7 @@
         </is>
       </c>
       <c r="C406" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="407">
@@ -6552,7 +6551,7 @@
         </is>
       </c>
       <c r="C407" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="408">
@@ -6567,7 +6566,7 @@
         </is>
       </c>
       <c r="C408" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="409">
@@ -6582,7 +6581,7 @@
         </is>
       </c>
       <c r="C409" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="410">
@@ -6597,7 +6596,7 @@
         </is>
       </c>
       <c r="C410" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="411">
@@ -6612,7 +6611,7 @@
         </is>
       </c>
       <c r="C411" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="412">
@@ -6628,7 +6627,7 @@
         </is>
       </c>
       <c r="C412" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="413">
@@ -6643,7 +6642,7 @@
         </is>
       </c>
       <c r="C413" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="414">
@@ -6658,7 +6657,7 @@
         </is>
       </c>
       <c r="C414" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="415">
@@ -6674,7 +6673,7 @@
         </is>
       </c>
       <c r="C415" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="416">
@@ -6689,7 +6688,7 @@
         </is>
       </c>
       <c r="C416" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="417">
@@ -6705,7 +6704,7 @@
         </is>
       </c>
       <c r="C417" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="418">
@@ -6720,7 +6719,7 @@
         </is>
       </c>
       <c r="C418" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="419">
@@ -6735,7 +6734,7 @@
         </is>
       </c>
       <c r="C419" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="420">
@@ -6750,7 +6749,7 @@
         </is>
       </c>
       <c r="C420" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
       </c>
     </row>
     <row r="421">
@@ -6765,7 +6764,311 @@
         </is>
       </c>
       <c r="C421" s="3" t="n">
-        <v>45819.89709724909</v>
+        <v>45819.89709724537</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/589043697010919/</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 66 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, May 25th features Cedar Mathias as our facilitator/dj! Details for Sunday, May 25th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C422" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663135653237580/</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Method Studio - Victoria BC Canice Ma invited you Interested Going About Discussion More About Discussion WACK! Another West Coast Swing Social Dance Invite Details 40 people responded Event by Canice Ma and Wyatt Ritchie Method Studio - Victoria BC Duration: 3 hr 30 min Public · Anyone on or off Facebook Guess who's back, it's WACK! (please ignore the fact that it's been 2 years...) The schmucks are back with another spontaneous west coast swing social dance, featuring music by DJs Topknot and Amandance from Vancouver! DETAILS: • Friday, June 20th, 2025 • Method Studio, 841 Fisgard St, Victoria, BC • 7:30-8:30 pm: "Shake That" line dance lesson featuring Kaitlyn • 8:30-11 pm: social dancing with 100% west coast swing • Admission: $10 • Water and AC on us (and maybe some bonus chocolate) • Please keep in mind that parking is limited at the venue GENERAL SOCIAL DANCE ETIQUETTE: • Consent is cool- don't be creepy. • Shake off any shyness and get out there! Ask people to dance regardless if you’re a lead or follow, dancing for 10 years or started yesterday- it's more fun that way! • No teaching or unsolicited feedback on the dance floor. Good vibes only! • If you would like to partake in a steal dance, try to remain with that group for the whole song. • Bring a water bottle! The studio is known to get warm with more bodies in the space so we want you to stay healthy and hydrated. • Personal hygiene is important! Consider bringing a towel and/or a spare shirt to change into if you sweat easily. Our studio has a bathroom and change rooms available for all to use. • We recommend wearing clothes that are easy to move in, especially pants given the nature of the dance. • Clean, comfortable shoes (ideally dance shoes) on the dance floor only! See less Victoria, British Columbia Method Studio - Victoria BC 833 Fisgard St, Victoria, BC V8W 1R9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C423" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/939376108286434/</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 17:30-19:00 Ladies Styling Bootcamp With Hannah 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Saturday at 14:00 Victoria Ska &amp; Reggae Fest: The Pharcyde, Sister Nancy, Marlon Asher, Dancehall Biz &amp; Tank Gyal! Becky and 2 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Friday 27 June 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Tickets · CA$17.31 www.eventbrite.com/e/salsa-night-dance-city-tickets-1415720962509 Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Tickets Find Tickets Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 240 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 52 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Ali Jorgensen invited you 91 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C424" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/514087011782400/</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Thursday 5 June 2025 at 18:00 80s Dance Party 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion 80s Dance Party Details 42 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Public · Anyone on or off Facebook Join Kai Aris and Friends for an evening of upbeat 80s dance, pop, and rock classics. Featuring some of Victoria’s best young musicians: Lily Gyles Thomas on vocals, Josh Warren on bass, Ava Creed on drums, Alex Gwillim on guitar, and Kai Aris on Synthesizer. Enjoy some drinks and dance the night away! See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C425" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1904863453602318/</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 19:00-22:00 Private Dance Saanichton, BC About Discussion More About Discussion Private Dance Details 8 people responded Event by HAMMERdown - Victoria, BC Saanichton, BC Duration: 3 hr Public · Anyone on or off Facebook We are excited for our gig on May 31 at Saanichton Bay. It is a private event. There will be good rocking tonight. Victoria, British Columbia Saanichton, BC Saanich Guests See All</t>
+        </is>
+      </c>
+      <c r="C426" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1031573525615192/</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Sunday 29 June 2025 at 19:00 GROOVE KITCHEN'S JUNEFEST DANCE!! Hermann's Jazz Club About Discussion More About Discussion GROOVE KITCHEN'S JUNEFEST DANCE!! Interested Going Invite Details 82 people responded Event by Groove Kitchen and Hermann's Jazz Club Hermann's Jazz Club Tickets hermannsjazz.com/show/737557/view Public · Anyone on or off Facebook The festival is over and it seems you still wanna celebrate music, but also... wanna get down and boogie?? You're our kind of people!! Observe the top of Summer with song and funky steps as the kitchen's groove moves your body like they've done before at spots like the Butchart Gardens, The Esquimalt Ribfest, The Osbourne Bay Pub, or the hottest rooms in and outta town. The Chefs are ready to serve their mouthwatering melange of funk, pop, soul, Latin, and flavours to party to the end!! Join us... Doors 5:30 PM / 7:00 PM Show, Sunday June 29th Hermann's Jazz Club 753 View Street Victoria, BC V8W 1J9 https://hermannsjazz.com/show/737557/view See less Victoria, British Columbia Tickets Find Tickets Hermann's Jazz Club 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C427" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1185783966345055/</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 10:00-13:00 Shuffle Dance Workshop Victoria, BC About Discussion More About Discussion Shuffle Dance Workshop Details 12 people responded Event by Adelène Buchanan Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another SHUFFLE WORKSHOP coming your way!! Join our Shuffle Dance Workshop and learn a full shuffle choreography set to an energetic electronic track. We’ll guide you through each step, focusing on key shuffle movements, while incorporating them into a dynamic routine. Perfect for ALL LEVELS! This workshop will help you improve your footwork, coordination, and cardiovascular stamina as you master a complete choreography. Here’s what you need to know: DATE: Sunday, May 25th TIME: 10am - 1pm PLACE: The Beat Clinic (1303 Broad Street) Sign-up link here https://www.thebeatclinic.ca/ See less Victoria, British Columbia Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C428" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1187402793186660/</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Saturday from 08:00-12:00 Global Underscore Solstice Dance 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada About Discussion More About Discussion Global Underscore Solstice Dance Interested Going Invite Details 50 people responded Event by Arunimá McNeish , Michael McAmmond and Victoria Contact Improv Jam 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada Duration: 4 hr Public · Anyone on or off Facebook Sweet dancers, This summer solstice we extend a warm invitation to join us in expanding and deepening our practice of Contact Improvisation with participation in The Global Underscore. Please arrive at 8am to join a 40 minute talk-through, introducing the concepts of the Underscore. This is mandatory if you have never attended an Underscore before. The Underscore will begin promptly at 8:45am. If you have attended a talk-through before you're welcome to arrive at this time. We will all start and end together. This is a closed container and we will not be allowing late-comers. TIMELINE: 8am-8:40am Underscore Talk-Through with Arunima 8:45am-11:30am Underscore 11:30am-11:50am Closing Circle COST: $15-$20  etransfer or pay cash at the door if pre-registered (if money is a barrier please reach out to discuss options). Please contact Arunima at ode.to.thylacine@gmail.com for registration, etransfer, questions, etc. VENUE: Victoria Truth Centre (2815 Cedar Hill Rd, Victoria, BC). MORE INFO: The Underscore, which has been evolving since 1990, is a vehicle for incorporating Contact Improvisation into the broader arena of improvisational dance practice; developing greater ease dancing in spherical space—alone and with others; and for integrating kinesthetic and compositional aspects while improvising. It allows for a full spectrum of energetic and physical expressions, embodying a range of forms and changing states. Its practice is familiar yet unpredictable. The practice progresses through a broad range of dynamic states, including long periods of very small, private, and quiet internal activity and other times of higher energy and interactive dancing. There are 20+ phases, 12+ connections, and 7 aspects of the Underscore—each with a name and a graphic symbol—which create a general map for the dancers. Within that frame, dancers are free to create their own movements, dynamics, and relationships—with themselves, each other, the group, and the environment. Each Underscore is unique, providing rich and often inspiring experiences of the human and artistic phenomena of dance improvisation. https://globalunderscore.com/ https://nancystarksmith.com/underscore/ See less Victoria, British Columbia 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C429" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/691138080073761/</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Monday 23 June 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 240 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Kizomba with Aaron and Fernanda— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C430" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1618420955545842/</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 17:30-19:00 Ladies Styling Bootcamp With Hannah 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Saturday at 14:00 Victoria Ska &amp; Reggae Fest: The Pharcyde, Sister Nancy, Marlon Asher, Dancehall Biz &amp; Tank Gyal! Becky and 2 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 30 Friday 30 May 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing at an all ages venue with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 240 people interested Interested Mon, 4 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Ali 11 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 52 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C431" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/556816543734629/</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Monday 7 July 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 41 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Merengue with Sebastian and Hannah— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C432" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3854957174726232/</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Monday 30 June 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 38 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Urban Kizomba with Aaron and Fernanda— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C433" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1682353965754886/</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Saturday 14 June 2025 from 18:00-20:30 Mamas' Dance Party! 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Sat, 5 Apr Sat, 10 May Sat, 14 Jun About Discussion More About Discussion Mamas' Dance Party! Details 31 people responded Event by Fairfield Gonzales Community Association 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Duration: 2 hr 30 min Public · Anyone on or off Facebook Calling all mamas, grand-mamas, aunties &amp; mamas-to-be! Join us for a night curated for all mamas (in any season of their motherhood or reproductive journey) to connect through creative expression, freedom of movement and community building! There will be an opening &amp; closing circle and time to connect over light refreshments as the night concludes. Feel free to come for it all, or leave when needed. We can't wait to dance, groove, and connect with you all soon. This is an inclusive space for ALL those who mother. Admission by-donation: suggested donation $5 This event is presented by the FGCA's Neighbourhood Improvement Committee See less Victoria, British Columbia 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 1330 Fairfield Rd, Victoria, BC V8S 5J1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C434" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/909522138040202/</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities More All Has new content Unread Groups Communities Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Active now Aylene Kirchner Unless you guys wanna make a A fun.
+Trip and stay overnight the night before · 1m Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 1d Velma Sproul Messages and calls are secured with end-to-end encryption. · 3d Active now Mary, Aylene, Jan Jan: Hi, we will be at Bard &amp; Banker at 3:30 ish.  Sorry won't make it to FW, but I know you'll all have fun there.  Maybe see you, M &amp; L, at the BB.  Cheers! · 5d Marketplace · 5d Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 1w Active now Murray McAllindon Messages and calls are secured with end-to-end encryption. · 1w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 3w Active now Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 3w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 5w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 5w Sue Holloway Messages and calls are secured with end-to-end encryption. · 5w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 6w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 17:30-19:00 Ladies Styling Bootcamp With Hannah 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Saturday at 14:00 Victoria Ska &amp; Reggae Fest: The Pharcyde, Sister Nancy, Marlon Asher, Dancehall Biz &amp; Tank Gyal! Becky and 2 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Friday 28 November 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 240 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 52 people interested Interested Sun, 29 Jun at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Ali and 2 friends 97 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025 Active now Aylene Kirchner Active now 2 April 2 Apr 2025, 20:53 You replied to Aylene Sorry, we have other plans but please have fun Enter 3 April 3 Apr 2025, 08:36 Aylene cool Enter New messages and calls are secured with end-to-end encryption. Only people in this chat can read, listen to or share them. Learn more Enter Messages are missing. Restore now Enter Today at 10:11 10:11 Aylene Oh no , we come back the same night Enter Aylene Unless you guys wanna make a A fun.
+Trip and stay overnight the night before Enter Aa</t>
+        </is>
+      </c>
+      <c r="C435" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1363696181561219/</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Friday from 19:00-22:00 Pride Contra Dance Fairfield United About Discussion More About Discussion Pride Contra Dance Interested Going Invite Details 84 people responded Event by Victoria Contra Dance , Code Tron and Rose Jackson Fairfield United Duration: 3 hr Public · Anyone on or off Facebook 𝕍𝕀ℂ𝕋𝕆ℝ𝕀𝔸 ℂ𝕆ℕ𝕋ℝ𝔸 𝔻𝔸ℕℂ𝔼 𝕊𝕆ℂ𝕀𝔼𝕋𝕐 ℙℝ𝔼𝕊𝔼ℕ𝕋𝕊: The return of our ℚ𝕌𝔼𝔼ℝ Contra Dance to celebrate the month of Pride! All Dancers welcome! Join us Friday, June 20th at the United Commons Fellowship Hall to do-si-do the night away to sprightly fiddle tunes and stellar performances from our two favorite drag performers! We'll have more capacity than our previous Valentines Day Dance, but we still might sell out, so grab your tickets online here! https://clannamorna.ca/.../ticket-victoria-pride-contra.../ ......................................................................................................... 𝕄𝕦𝕤𝕚𝕔 𝔹𝕪: 𝐑𝐨𝐬𝐞 𝐉𝐚𝐜𝐤𝐬𝐨𝐧: she/her Coming up in the rich folk scene of western Massachusetts, Rose is based in Montague, MA, where she studied under fiddler Becky Tracy from whom she inherited a wide repertoire of music from Quebec, New England, Ireland, and France, a deep love for old tunes, and the intuitive sense of rhythm and danceability which infuses her playing. Equally at home in the concert hall and on the dance stage, she’s taught fiddle, song, and dance at camps and festivals around New England, toured nationally with her band Polaris and now tours with her quartet Stove Dragon and duo Helen &amp; Rose. https://www.rose-jackson.com/ 𝐇𝐞𝐥𝐞𝐧 𝐊𝐮𝐡𝐚𝐫: they/them Hailing from Seattle, Washington, Helen currently resides in Cambridge, MA. Helen began exploring their connection to folk and Celtic music in 2020 while studying with renowned contra guitarist Alex Sturbaum. Upon moving to Cambridge in 2022, Helen dove into the thriving celtic music scene, playing contra dances, Irish sessions, and concerts around New England and the Pacific Northwest. Since then, Helen has developed their style as a contra accompanist, Irish session backer, and vocalist. https://www.helenkuharmusic.com/ 𝐅𝐢𝐝𝐝𝐥𝐢𝐧' 𝐅𝐢𝐧𝐧: they/them A professional fiddler, singer and banjo player living on the territories of the lekwungen and W̱SÁNEĆ people, colonially known as Victoria BC. Finn has a passion for Irish, Scottish, English, North American and Eastern European folk music, and are known for their dynamic fiddling and soulful voice. They delve into traditional material - bringing a fresh interpretation of songs and tunes from many different places, as well as writing their own material. From the Appalachian mountains to Quebec, to melodic Irish and Scottish tunes, they cover wide musical ground with articulate playing. Finn also performs frequently in Canada and the U.S. with their bands Clanna Morna and Ghostly Hounds. https://finnletourneau.com/ ℂ𝕒𝕝𝕝𝕚𝕟𝕘 𝔹𝕪: 𝐕𝐢𝐜𝐭𝐨𝐫𝐢𝐚 𝐁𝐞𝐚𝐮𝐜𝐡𝐞𝐬𝐧𝐞 One of our local communities up and coming callers! 𝔻𝕣𝕒𝕘 𝕡𝕖𝕣𝕗𝕠𝕣𝕞𝕒𝕟𝕔𝕖𝕤 𝕓𝕪: Aries Moon: Making country gay one song at a time Leo Moon: The island's premiere tap dancing drag thing ......................................................................................................... 6:30 - doors open 7:00 - dancing starts with a beginner friendly dance lesson Everyone welcome, no experience necessary. $12 - Youth $20 - Everyone who is willing and able to NOTAFLOF Poster Art by Sonya Chwyl See less Victoria, British Columbia Fairfield United 925 Balmoral Rd, Victoria, BC V8T 1A7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C436" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/624858640069610/</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook 1 unread chats 1 Number of unread notifications 20+ Chats All Has new content Unread Groups Communities Has new content More All Has new content Unread Groups Communities Has new content Chat history is missing Enter your PIN to restore chat history. - - - - - - Use a one-time code instead Active now Aylene Kirchner Unless you guys wanna make a A fun.
+Trip and stay overnight the night before · 1m Mary K. Nixon Messages and calls are secured with end-to-end encryption. · 1d Velma Sproul Messages and calls are secured with end-to-end encryption. · 3d Active now Mary, Aylene, Jan Jan: Hi, we will be at Bard &amp; Banker at 3:30 ish.  Sorry won't make it to FW, but I know you'll all have fun there.  Maybe see you, M &amp; L, at the BB.  Cheers! · 5d Marketplace · 5d Olga  Zhestkova Messages and calls are secured with end-to-end encryption. · 1w Active now Murray McAllindon Messages and calls are secured with end-to-end encryption. · 1w Active now Becky Mowat Messages and calls are secured with end-to-end encryption. · 3w Mary, Nita, Navtej, Clayton, Kathy, Harjit Kathy: https://www.eventbrite.ca/e/thirsty-chef-11th-anniversary-tickets-1359154450549?fbclid=IwZXh0bgNhZW0CMTEAAR6vBMazgmhA2skjMdDWbIbnPUkIM9C-rlHtE6oUdSOrCO6LiUr4vjV7-Kd-vw_aem_ND21ICQhoL4ldLwd7A-2PA · 3w Darlene Pinch Messages and calls are secured with end-to-end encryption. · 5w Active now Message request Journeey Song Messages and calls are secured with end-to-end encryption. · 5w Sue Holloway Messages and calls are secured with end-to-end encryption. · 5w Quinn Johnson Messages and calls are secured with end-to-end encryption. · 5w Mary, Velma Velma sent an attachment. · 6w See all in Messenger Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 17:30-19:00 Ladies Styling Bootcamp With Hannah 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Saturday at 14:00 Victoria Ska &amp; Reggae Fest: The Pharcyde, Sister Nancy, Marlon Asher, Dancehall Biz &amp; Tank Gyal! Becky and 2 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 Friday 22 August 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 240 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 52 people interested Interested Sun, 29 Jun at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Ali and 2 friends 97 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025 Active now Aylene Kirchner Active now 2 April 2 Apr 2025, 20:53 You replied to Aylene Sorry, we have other plans but please have fun Enter 3 April 3 Apr 2025, 08:36 Aylene cool Enter New messages and calls are secured with end-to-end encryption. Only people in this chat can read, listen to or share them. Learn more Enter Messages are missing. Restore now Enter Today at 10:11 10:11 Aylene Oh no , we come back the same night Enter Aylene Unless you guys wanna make a A fun.
+Trip and stay overnight the night before Enter Aa</t>
+        </is>
+      </c>
+      <c r="C437" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/667083456006099/</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT Details 11 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled… See more Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C438" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1910904133047825/</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY The Coda About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY Details 81 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 751 View Street (2nd floor, Hermmans Jazz Club) Date: Friday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C439" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/650657144184821/</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Saturday 19 July 2025 from 21:00-02:00 COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY The Coda About Discussion More About Discussion COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY Interested Going Invite Details 30 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 5 hr Public · Anyone on or off Facebook Colombian Summer Rumba: “Tierra Querida” Party Saturday, July 19th Doors: 9:00 PM | Show: 9:30 PM 19+ | ID Required Celebrate Colombian Independence Day with us with the vibrant “Tierra Querida” Party — an amazing night of live music, dance, culture, and pure rumba energy! Start the night with a live tribute to Colombian music by the talented Daniel Sar &amp; Sofia Leonne. Their performance will honor legendary Colombian artists such as Juanes, Maluma, Fonseca, Rodolfo Aicardi, Herencia de Timbiquí, Mon Laferte, and more—blending pop, tropical rhythms, and heartfelt Latin ballads into a powerful musical journey. At 10:30 PM, DJ Miro, straight from Cali, Colombia, will take over with a fiery mix of Colombian beats. Later, resident DJ Alex King will close out the night, turning up the heat with Latin hits and ending strong with the latest reggaetón summer vibes. At midnight, enjoy a special folkloric performance by Danza Colombia, followed by a unifying moment as we wave our flag souvenirs and sing the national anthem together. Savor delicious cocktails, soak in vibrant downtown vibes, and enjoy a night filled with alegría, culture, and  Colombian vibes! Get your tickets NOW! First-tier: $20 | Second-tier: $25 Limited tickets available at the door for $27 - Act fast before they are sold out! Party ends at 2:00 AM Each ticket includes a Colombian flag souvenir. Take a piece of the celebration home with you! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C440" s="3" t="n">
+        <v>45826.42809952546</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1132427048350776/</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com … See more Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C441" s="3" t="n">
+        <v>45826.42809952546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced llm.extract_and_parse_json() with a new parser.
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -429,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C441"/>
+  <dimension ref="A1:C551"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7071,6 +7072,1656 @@
         <v>45826.42809952546</v>
       </c>
     </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3854957174726232/</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Monday 30 June 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 38 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Urban Kizomba with Aaron and Fernanda— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C442" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1187402793186660/</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Saturday from 08:00-12:00 Global Underscore Solstice Dance 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada About Discussion More About Discussion Global Underscore Solstice Dance Interested Going Invite Details 50 people responded Event by Arunimá McNeish , Michael McAmmond and Victoria Contact Improv Jam 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada Duration: 4 hr Public · Anyone on or off Facebook Sweet dancers, This summer solstice we extend a warm invitation to join us in expanding and deepening our practice of Contact Improvisation with participation in The Global Underscore. Please arrive at 8am to join a 40 minute talk-through, introducing the concepts of the Underscore. This is mandatory if you have never attended an Underscore before. The Underscore will begin promptly at 8:45am. If you have attended a talk-through before you're welcome to arrive at this time. We will all start and end together. This is a closed container and we will not be allowing late-comers. TIMELINE: 8am-8:40am Underscore Talk-Through with Arunima 8:45am-11:30am Underscore 11:30am-11:50am Closing Circle COST: $15-$20  etransfer or pay cash at the door if pre-registered (if money is a barrier please reach out to discuss options). Please contact Arunima at ode.to.thylacine@gmail.com for registration, etransfer, questions, etc. VENUE: Victoria Truth Centre (2815 Cedar Hill Rd, Victoria, BC). MORE INFO: The Underscore, which has been evolving since 1990, is a vehicle for incorporating Contact Improvisation into the broader arena of improvisational dance practice; developing greater ease dancing in spherical space—alone and with others; and for integrating kinesthetic and compositional aspects while improvising. It allows for a full spectrum of energetic and physical expressions, embodying a range of forms and changing states. Its practice is familiar yet unpredictable. The practice progresses through a broad range of dynamic states, including long periods of very small, private, and quiet internal activity and other times of higher energy and interactive dancing. There are 20+ phases, 12+ connections, and 7 aspects of the Underscore—each with a name and a graphic symbol—which create a general map for the dancers. Within that frame, dancers are free to create their own movements, dynamics, and relationships—with themselves, each other, the group, and the environment. Each Underscore is unique, providing rich and often inspiring experiences of the human and artistic phenomena of dance improvisation. https://globalunderscore.com/ https://nancystarksmith.com/underscore/ See less Victoria, British Columbia 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada 2815 Cedar Hill Rd, Victoria, BC V8T 3H6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C443" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/909522138040202/</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Friday 28 November 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 243 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 52 people interested Interested Sun, 29 Jun at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Ali and 2 friends 97 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C444" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/589043697010919/</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 66 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, May 25th features Cedar Mathias as our facilitator/dj! Details for Sunday, May 25th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C445" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/556816543734629/</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Monday 7 July 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 41 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Merengue with Sebastian and Hannah— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C446" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/939376108286434/</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Friday 27 June 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Tickets · CA$17.31 www.eventbrite.com/e/salsa-night-dance-city-tickets-1415720962509 Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Tickets Find Tickets Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 243 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 52 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Ali Jorgensen invited you 91 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C447" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/624858640069610/</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 Friday 22 August 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 243 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 52 people interested Interested Sun, 29 Jun at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Ali and 2 friends 97 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C448" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/691138080073761/</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Monday 23 June 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 243 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Kizomba with Aaron and Fernanda— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C449" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/514087011782400/</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Thursday 5 June 2025 at 18:00 80s Dance Party 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion 80s Dance Party Details 42 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Public · Anyone on or off Facebook Join Kai Aris and Friends for an evening of upbeat 80s dance, pop, and rock classics. Featuring some of Victoria’s best young musicians: Lily Gyles Thomas on vocals, Josh Warren on bass, Ava Creed on drums, Alex Gwillim on guitar, and Kai Aris on Synthesizer. Enjoy some drinks and dance the night away! See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C450" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1618420955545842/</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 30 Friday 30 May 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing at an all ages venue with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 243 people interested Interested Mon, 4 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Ali 11 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 52 people interested Interested Popular with friends Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C451" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1031573525615192/</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Sunday 29 June 2025 at 19:00 GROOVE KITCHEN'S JUNEFEST DANCE!! Hermann's Jazz Club About Discussion More About Discussion GROOVE KITCHEN'S JUNEFEST DANCE!! Interested Going Invite Details 82 people responded Event by Groove Kitchen and Hermann's Jazz Club Hermann's Jazz Club Tickets hermannsjazz.com/show/737557/view Public · Anyone on or off Facebook The festival is over and it seems you still wanna celebrate music, but also... wanna get down and boogie?? You're our kind of people!! Observe the top of Summer with song and funky steps as the kitchen's groove moves your body like they've done before at spots like the Butchart Gardens, The Esquimalt Ribfest, The Osbourne Bay Pub, or the hottest rooms in and outta town. The Chefs are ready to serve their mouthwatering melange of funk, pop, soul, Latin, and flavours to party to the end!! Join us... Doors 5:30 PM / 7:00 PM Show, Sunday June 29th Hermann's Jazz Club 753 View Street Victoria, BC V8W 1J9 https://hermannsjazz.com/show/737557/view See less Victoria, British Columbia Tickets Find Tickets Hermann's Jazz Club 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C452" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1363696181561219/</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Friday from 19:00-22:00 Pride Contra Dance Fairfield United About Discussion More About Discussion Pride Contra Dance Interested Going Invite Details 85 people responded Event by Victoria Contra Dance , Code Tron and Rose Jackson Fairfield United Duration: 3 hr Public · Anyone on or off Facebook 𝕍𝕀ℂ𝕋𝕆ℝ𝕀𝔸 ℂ𝕆ℕ𝕋ℝ𝔸 𝔻𝔸ℕℂ𝔼 𝕊𝕆ℂ𝕀𝔼𝕋𝕐 ℙℝ𝔼𝕊𝔼ℕ𝕋𝕊: The return of our ℚ𝕌𝔼𝔼ℝ Contra Dance to celebrate the month of Pride! All Dancers welcome! Join us Friday, June 20th at the United Commons Fellowship Hall to do-si-do the night away to sprightly fiddle tunes and stellar performances from our two favorite drag performers! We'll have more capacity than our previous Valentines Day Dance, but we still might sell out, so grab your tickets online here! https://clannamorna.ca/.../ticket-victoria-pride-contra.../ ......................................................................................................... 𝕄𝕦𝕤𝕚𝕔 𝔹𝕪: 𝐑𝐨𝐬𝐞 𝐉𝐚𝐜𝐤𝐬𝐨𝐧: she/her Coming up in the rich folk scene of western Massachusetts, Rose is based in Montague, MA, where she studied under fiddler Becky Tracy from whom she inherited a wide repertoire of music from Quebec, New England, Ireland, and France, a deep love for old tunes, and the intuitive sense of rhythm and danceability which infuses her playing. Equally at home in the concert hall and on the dance stage, she’s taught fiddle, song, and dance at camps and festivals around New England, toured nationally with her band Polaris and now tours with her quartet Stove Dragon and duo Helen &amp; Rose. https://www.rose-jackson.com/ 𝐇𝐞𝐥𝐞𝐧 𝐊𝐮𝐡𝐚𝐫: they/them Hailing from Seattle, Washington, Helen currently resides in Cambridge, MA. Helen began exploring their connection to folk and Celtic music in 2020 while studying with renowned contra guitarist Alex Sturbaum. Upon moving to Cambridge in 2022, Helen dove into the thriving celtic music scene, playing contra dances, Irish sessions, and concerts around New England and the Pacific Northwest. Since then, Helen has developed their style as a contra accompanist, Irish session backer, and vocalist. https://www.helenkuharmusic.com/ 𝐅𝐢𝐝𝐝𝐥𝐢𝐧' 𝐅𝐢𝐧𝐧: they/them A professional fiddler, singer and banjo player living on the territories of the lekwungen and W̱SÁNEĆ people, colonially known as Victoria BC. Finn has a passion for Irish, Scottish, English, North American and Eastern European folk music, and are known for their dynamic fiddling and soulful voice. They delve into traditional material - bringing a fresh interpretation of songs and tunes from many different places, as well as writing their own material. From the Appalachian mountains to Quebec, to melodic Irish and Scottish tunes, they cover wide musical ground with articulate playing. Finn also performs frequently in Canada and the U.S. with their bands Clanna Morna and Ghostly Hounds. https://finnletourneau.com/ ℂ𝕒𝕝𝕝𝕚𝕟𝕘 𝔹𝕪: 𝐕𝐢𝐜𝐭𝐨𝐫𝐢𝐚 𝐁𝐞𝐚𝐮𝐜𝐡𝐞𝐬𝐧𝐞 One of our local communities up and coming callers! 𝔻𝕣𝕒𝕘 𝕡𝕖𝕣𝕗𝕠𝕣𝕞𝕒𝕟𝕔𝕖𝕤 𝕓𝕪: Aries Moon: Making country gay one song at a time Leo Moon: The island's premiere tap dancing drag thing ......................................................................................................... 6:30 - doors open 7:00 - dancing starts with a beginner friendly dance lesson Everyone welcome, no experience necessary. $12 - Youth $20 - Everyone who is willing and able to NOTAFLOF Poster Art by Sonya Chwyl See less Victoria, British Columbia Fairfield United 925 Balmoral Rd, Victoria, BC V8T 1A7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C453" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663135653237580/</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Method Studio - Victoria BC Canice Ma invited you Interested Going About Discussion More About Discussion WACK! Another West Coast Swing Social Dance Invite Details 40 people responded Event by Canice Ma and Wyatt Ritchie Method Studio - Victoria BC Duration: 3 hr 30 min Public · Anyone on or off Facebook Guess who's back, it's WACK! (please ignore the fact that it's been 2 years...) The schmucks are back with another spontaneous west coast swing social dance, featuring music by DJs Topknot and Amandance from Vancouver! DETAILS: • Friday, June 20th, 2025 • Method Studio, 841 Fisgard St, Victoria, BC • 7:30-8:30 pm: "Shake That" line dance lesson featuring Kaitlyn • 8:30-11 pm: social dancing with 100% west coast swing • Admission: $10 • Water and AC on us (and maybe some bonus chocolate) • Please keep in mind that parking is limited at the venue GENERAL SOCIAL DANCE ETIQUETTE: • Consent is cool- don't be creepy. • Shake off any shyness and get out there! Ask people to dance regardless if you’re a lead or follow, dancing for 10 years or started yesterday- it's more fun that way! • No teaching or unsolicited feedback on the dance floor. Good vibes only! • If you would like to partake in a steal dance, try to remain with that group for the whole song. • Bring a water bottle! The studio is known to get warm with more bodies in the space so we want you to stay healthy and hydrated. • Personal hygiene is important! Consider bringing a towel and/or a spare shirt to change into if you sweat easily. Our studio has a bathroom and change rooms available for all to use. • We recommend wearing clothes that are easy to move in, especially pants given the nature of the dance. • Clean, comfortable shoes (ideally dance shoes) on the dance floor only! See less Victoria, British Columbia Method Studio - Victoria BC 833 Fisgard St, Victoria, BC V8W 1R9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C454" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1904863453602318/</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 19:00-22:00 Private Dance Saanichton, BC About Discussion More About Discussion Private Dance Details 8 people responded Event by HAMMERdown - Victoria, BC Saanichton, BC Duration: 3 hr Public · Anyone on or off Facebook We are excited for our gig on May 31 at Saanichton Bay. It is a private event. There will be good rocking tonight. Victoria, British Columbia Saanichton, BC Saanich Guests See All</t>
+        </is>
+      </c>
+      <c r="C455" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1185783966345055/</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 10:00-13:00 Shuffle Dance Workshop Victoria, BC About Discussion More About Discussion Shuffle Dance Workshop Details 12 people responded Event by Adelène Buchanan Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another SHUFFLE WORKSHOP coming your way!! Join our Shuffle Dance Workshop and learn a full shuffle choreography set to an energetic electronic track. We’ll guide you through each step, focusing on key shuffle movements, while incorporating them into a dynamic routine. Perfect for ALL LEVELS! This workshop will help you improve your footwork, coordination, and cardiovascular stamina as you master a complete choreography. Here’s what you need to know: DATE: Sunday, May 25th TIME: 10am - 1pm PLACE: The Beat Clinic (1303 Broad Street) Sign-up link here https://www.thebeatclinic.ca/ See less Victoria, British Columbia Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C456" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1910904133047825/</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY The Coda About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL PARTY Details 81 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 751 View Street (2nd floor, Hermmans Jazz Club) Date: Friday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C457" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/650657144184821/</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Saturday 19 July 2025 from 21:00-02:00 COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY The Coda About Discussion More About Discussion COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY Interested Going Invite Details 31 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 5 hr Public · Anyone on or off Facebook Colombian Summer Rumba: “Tierra Querida” Party Saturday, July 19th Doors: 9:00 PM | Show: 9:30 PM 19+ | ID Required Celebrate Colombian Independence Day with us with the vibrant “Tierra Querida” Party — an amazing night of live music, dance, culture, and pure rumba energy! Start the night with a live tribute to Colombian music by the talented Daniel Sar &amp; Sofia Leonne. Their performance will honor legendary Colombian artists such as Juanes, Maluma, Fonseca, Rodolfo Aicardi, Herencia de Timbiquí, Mon Laferte, and more—blending pop, tropical rhythms, and heartfelt Latin ballads into a powerful musical journey. At 10:30 PM, DJ Miro, straight from Cali, Colombia, will take over with a fiery mix of Colombian beats. Later, resident DJ Alex King will close out the night, turning up the heat with Latin hits and ending strong with the latest reggaetón summer vibes. At midnight, enjoy a special folkloric performance by Danza Colombia, followed by a unifying moment as we wave our flag souvenirs and sing the national anthem together. Savor delicious cocktails, soak in vibrant downtown vibes, and enjoy a night filled with alegría, culture, and  Colombian vibes! Get your tickets NOW! First-tier: $20 | Second-tier: $25 Limited tickets available at the door for $27 - Act fast before they are sold out! Party ends at 2:00 AM Each ticket includes a Colombian flag souvenir. Take a piece of the celebration home with you! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C458" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/667083456006099/</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Friday 14 March 2025 from 21:30-01:30 COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion COLOMBIAN RUMBA - BARRANQUILLA CARNIVAL NIGHT Details 11 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Duration: 4 hr Public · Anyone on or off Facebook Are you ready to feel the sizzling energy and captivating beats of Colombia's legendary Barranquilla Carnival right here in Victoria? Get set for an unforgettable night filled with the vibrant rhythms, pulsating music, and electric atmosphere of one of Latin America's most exhilarating celebrations! Join us as we dive into a kaleidoscope of Caribbean rhythms, from cumbia and champeta to reggaeton, salsa, and merengue - all fueled by the hottest Latin vibes! Immerse yourself in a high-energy dance class Feel the thrill of live Colombian music “Parrandon Vallenato” and get swept away by the magic of electrifying DJ sets by Alex King and Dj Miro from Colombia. Lose yourself in spectacular performances by Fusion Chibcha “Colombian Culture Society” Show off your Carnival spirit with a colorful, eye-catching dress code, and have the chance of winning a surprise prize. Embrace the wild and wonderful world of Barranquilla Carnival with your most dazzling outfit! A fantastic surprise prize awaits the attendee who steals the show with the best costume! Venue: Coda - 753 View Street (2nd floor, Hermmans Jazz Club) Date: Saturday, March 14th, 2025 Time: 9:30 PM - 1:30 AM Presale Tickets: $30 (limited capacity, hurry up to assure your tickets) Legal drinking age required + two photo IDs Brought to you by Victoria Viva la Fiesta, get your tickets now and prepare to experience the heart-pounding excitement and magical ambiance of Carnaval in Canada! It's time to let loose, embrace your Latin side, and create memories that will last a lifetime! See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C459" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1132427048350776/</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com or 15$ cash/e-transfer at the door. Formed in the heart of Chinatown, Rosebuds is a dynamic ensemble that brings the vibrant sounds of jazz, blues &amp; swing to life.  The group plays a mixture of originals and jazz standards, and is influenced by artists like Louis Armstrong, Billie Holiday, Lester Young, and Lionel Hampton. Featuring Rebecca Wells (vocals/guitar), Alex Moore (guitar/keys) Bryden Amos (guitar/keys), Matisse Gubby-Hurtig (bass), Owen Chow (trumpet), and Andrew Greenwood (tenor saxophone). Samba e Sol is a newly formed Brazilian bossa nova jazz trio featuring Andrew Greenwood (flute), Alex Moore (guitar), and Matisse Gubby-Hurtig (bass), playing music by artists like Antonio Carlos Jobim, Marcos Valle, Luiz Bonfa, and more. Instagram: https://www.instagram.com/rosebudsband/ See less Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C460" s="3" t="n">
+        <v>45826.51645584491</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1079226067560481/</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 52 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 6, 2025 | Lesson:  Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C461" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1861230087752141/</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 5 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 31, 2025 | Lesson:  Intro to Salsa with Adam &amp; Alicia Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C462" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1179097320623502/</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 37 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C463" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1029869435768837/</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Saturday 22 March 2025 at 20:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC This event has been cancelled. You cannot share this event, but you can still post. About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 14 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C464" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1743571267040445/</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Ali Jorgensen invited you About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Details 55 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 8, 2025 | Lesson: Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C465" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2637194793152555/</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 97 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 29, 2025 | Lesson:  Intro to Salsa Rueda with Sam and Katie Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa Rueda • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C466" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/947213690692385/</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C467" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1293301738436581/</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Sunday 6 April 2025 at 17:00 Kizomba Sundown Party: Free of charge Method Studio - Victoria BC David Lamine Victoria invited you About Discussion More About Discussion Kizomba Sundown Party: Free of charge Details 58 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Method Studio - Victoria BC Public · Anyone on or off Facebook Free Pre-VIKFest party. Bring snack and drink. Expect great music, great energy, great atmosphere. "Dance with your heart. your feet will follow" Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C468" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/960236445839425/</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Saturday 22 June 2024 from 18:00-21:00 Kizomba/UrbanKiz at Clover Clover Pt, Victoria, BC V8S, Canada About Discussion More About Discussion Kizomba/UrbanKiz at Clover Interested Details 56 people responded Event by Becky Mowat Clover Pt, Victoria, BC V8S, Canada Duration: 3 hr Public · Anyone on or off Facebook Come join us for our first time dancing at Clover Point! There will be no lesson beforehand and this is super casual. Just a bunch of friends hanging out and dancing. Bring snacks, something to drink, blankets, warm clothes (as it is typically cooler by the ocean). There isn't a lot of parking at Clover Point but you can park along Dallas Rd and just walk down. Feel free to invite friends and family. Hope to see you all there! See less Victoria, British Columbia Clover Pt, Victoria, BC V8S, Canada 1301 Clover Pt, Victoria, BC V8S, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C469" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1337760257449745/</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 5 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 10, 2025 | Lesson:   Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C470" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3006474846197996/</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 43 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 27, 2025 | Lesson:  Intro class TBD Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro class TBD • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C471" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1794066937801722/</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Saturday 8 March 2025 from 20:30-23:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 26 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C472" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/372311028526699/</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Saturday 9 December 2023 from 20:30-23:30 Victoria Kizomba Social: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Social: Fall Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C473" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1060779176049104/</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Thursday 3 October 2024 from 19:30-22:30 Kizomba Practica Thursdays: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Kizomba Practica Thursdays: Fall Series Details 20 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Join us every Thursday for Kizomba/Urbankiz classes. Intermediate 7:30PM-8:15pm Beginner 8:15pm-9:00pm Practica until 10:30pm Class only: $10 Class &amp; Practica: $15 or $10 for university students w/ID Practice only $10 Classes will be provided by your local Instructor (David Lamine) and assistants (Robyn, Becky) and occasionally by some out of town and International Instructors. Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C474" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1184791909680061/</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Thursday 13 March 2025 from 19:30-23:00 Urban Kiz Workshop with Mannie Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 50 people responded Event by Becky Mowat and David Lamine Victoria Ukrainian Cultural Centre Duration: 3 hr 30 min Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C475" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3185065321631809/</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Saturday 15 March 2025 from 20:00-00:00 Urban Kiz Workshop with Mannie Method Studio - Victoria BC Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 48 people responded Event by Becky Mowat and David Lamine Victoria Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C476" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1334757257408713/</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Saturday 25 January 2025 from 19:00-23:30 Special Edition Urbankiz Workshop w/ Kenny Odumosu Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Special Edition Urbankiz Workshop w/ Kenny Odumosu Details 50 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 hr 30 min Public · Anyone on or off Facebook SPECIAL EDITION WORKSHOP Join us Saturday January 25th for a 2hr Urbankiz workshop. Joining us from Calgary to share his knowledge and love for Urbankiz. Kenny finished first for the Kizomba/Semba category at the North American Olympiads. With his background in Kizomba/Semba Kenny will help you incorporate techniques and smoothness into your Urbankiz. We are really looking forward to having him here! Schedule 7:00pm-9:00pm (workshop) 9:00pm-11:30pm (social) Price: $40 (includes workshop &amp; social dance) e-transfer to:  becksmith@hotmail.com please include the name you go by if different from your e-transfer account. Thanks See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C477" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1152065639712042/</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 20 20 Feb at 19:30 – 23 Feb at 23:00 Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Details 49 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 days Public · Anyone on or off Facebook Join us for our special edition Urbankiz &amp; Tarraxo workshops with Mike Ahombi Mike has been a big supporter of our VIKF and bringing his talent and low key vibe to the west coast. He is based out of Ottawa but you will find him at many different festivals and cities teaching Kizomba, Urbakiz and Tarraxo. We cannot wait for you all to have the opportunity to learn from such an incredible person and instructor. Details: Feb 20th Urbankiz Workshop 7:30pm-9:30pm Practica 9:30pm-11:00pm Feb 22nd Tarraxo Workshop 8:00pm-10:00pm Practica 10:00-11:30pm Price $90 Workshops only $70 Practica only $20 *** please e transfer to becksmith@hotmail.com *** Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C478" s="3" t="n">
+        <v>45826.5235294213</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1813229489279716/</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Thursday 29 May 2025 from 19:55-21:00 Sensual Bachata 4 Week Series Method Studio - Victoria BC Thu, 15 May Thu, 22 May Thu, 29 May +1 About Discussion More About Discussion Sensual Bachata 4 Week Series Details 6 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 1 hr 5 min Public · Anyone on or off Facebook Ready to level up your Sensual Bachata? May 8, 15, 22, 29 Method Studio | 7:55–9:00 PM | $80 for all 4 classes Join us for an exciting and dynamic Bachata Sensual class designed for experienced beginners and intermediate dancers! We’re blending solid fundamentals with fresh, fun, and sensual combos to help you grow, challenge yourself, and have an amazing time on the dance floor. No partner needed — just bring yourself and your love for dance! Spots are limited — don’t miss out! Register by e-transferring $80 to maximumotion@gmail.com and mentioning “Bachata Sensual” in the notes. Get ready to connect, move, and elevate your dancing! P.S. All fees are non-refundable as they go directly toward securing the studio space and running the class. See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C479" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1350929566137538/</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 6 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation August 10, 2025 | Lesson: Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C480" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1388695712154512/</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Ali Jorgensen invited you Interested Going About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Invite Details 91 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation June 22, 2025 | Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C481" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/692165093260868/</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 13:00-16:00 Salsa &amp; Bachata Masterclass with Adam &amp; Ghada Solwood Studio About Discussion More About Discussion Salsa &amp; Bachata Masterclass with Adam &amp; Ghada🔥 Details 60 people responded Event by Dancing Time Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook Hello everyone! Spring is here, and many things are happening, but I can’t but dance with you one last time before leaving for the entire summer!! To make things spicy, I am extremely happy to collaborate with Adam on a Salsa &amp; Bachata Masterclass! Get ready to learn details that will help you with creating flow – both as leads and follows – in addition to some socials-friendly tricks! Date: Saturday, May 10 Time: 1:00-2:30 | Salsa, 2:30-4:00 | Bachata Price: 25$ for one class, 35$ for two classes Location: Solwood studio, 1303 Broad st To register, please fill in this quick form and send an e-transfer to ghadacyoussef@gmail.com. https://forms.gle/4QThxT6yByd3h5KH8 Note: kindly understand that no-shows and cancellations made in less than 1 week from the workshop cannot be refunded. I will be happy to fully refund for earlier cancellations if need be. See less Victoria, British Columbia Solwood Studio Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C482" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1057471579628015/</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Friday 16 May 2025 at 17:00 Bachata Nights Victoria Bc Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Victoria Bc Details 9 people responded Event by Bachata Nights Victoria BC and Sebastian Carmona Method Studio - Victoria BC Public · Anyone on or off Facebook Join us on our next Bachata Nights May 23 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C483" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1300938064467261/</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Thursday 20 March 2025 from 20:00-22:00 Intermediate Sensual Bachata Workshop Method Studio - Victoria BC About Discussion More About Discussion Intermediate Sensual Bachata Workshop Details 24 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 2 hr Public · Anyone on or off Facebook Sensual Bachata Workshop in March! Intermediate workshop - March 20 Time: 8:00-9:30 PM + Practice 9:30-10:00 PM Location: Method Studio, 841 Fisgard St. Cost: $30 per workshop (includes 2 hours!) Intermediate workshop: Take your skills to a higher level! Master the advanced variations of the Madrid pass, smooth transitions and musicality. No partner needed, just bring your energy and comfortable shoes! Register at: maximumotion@gmail.com #BachataWorkshop #VictoriaBC #LearnToDance #BachataLovers See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C484" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1069894401564900/</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Monday Nights! 111 Superior St, Victoria, BC V8V 1T2, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion Sensual Bachata Series – Monday Nights! Details 15 people responded Event by Victoria Latin Dance Association 111 Superior St, Victoria, BC V8V 1T2, Canada Duration: 3 hr Public · Anyone on or off Facebook Sensual Bachata Series – Monday Nights! Mondays – April 7th, 14th, 21st &amp; 28th at 111 Superior Street Foundation Class (6:30–7:35 PM) Perfect for absolute beginners or dancers looking to strengthen their foundation! In this class, we’ll break down the essential steps, body movement, and partner connection in a fun environment. You’ll learn the basics with proper technique while also adding styling to make your dancing look and feel smooth on the dance floor. No experience or partner needed—just bring your curiosity and energy! Intermediate Class (7:35–8:40 PM) Ready to level up? This class is designed for dancers who already feel comfortable with the basics and want to challenge themselves. We’ll dive into more fun patterns while also exploring musicality—how to connect those movements to the music in a more expressive way. Get ready to build confidence, fluidity, and your own unique style! To Register: Send your e-transfer to maximumotion@gmail.com and include in the memo: Foundation, Intermediate, or Both + Lead or Follow Class Cancellation &amp; Refunds We understand that plans can change. However, due to limited spots, renting space in advance, and the preparation required for each class, we’re unable to offer refunds for cancellations. Please make sure you’re committed before signing up. We truly appreciate your understanding and support! See less Victoria, British Columbia 111 Superior St, Victoria, BC V8V 1T2, Canada 111 Superior St, Victoria, BC V8V 1T2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C485" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1730246844256904/</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre About Discussion More About Discussion Saturday Salsa/Bachata Social June 28th Interested Going Invite Details 20 people responded Event by Latin Dance Canada Ukrainian Cultural Centre Duration: 3 hr 59 min Public · Anyone on or off Facebook Saturday Salsa/Bachata Social June 28th 3277 Douglas st, Victoria BC Cost? $15 CASH ONLY PLEASE! When? Saturday, June 28th 8:00 pm - 8:30 pm beginner dance lesson 8:30 pm - 12 am Social dancing What? We will be playing a mix of salsa, bachata and more. Where? Ukrainian Cultural Centre 3277 Douglas Street, Victoria See less Dance Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C486" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342233713680795/</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Thursday 1 May 2025 at 21:00 Bachata &amp; Merengue- All Levels- May Series Studio 4 Athletics About Discussion More About Discussion Bachata &amp; Merengue- All Levels- May Series Details 3 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Bachata &amp; Merengue are both dances from the Dominican Republic. Bachata can be anywhere from slow and romantic with lots of dips, sway and body movement to more upbeat and percussive with lots of musical footwork. Merengue is carefree, flirtatious and fun! Classes are registered on a monthly basis and take place every Thursday from 8:00- 9:00pm, May 1, 8, 15, 22, 29. No experience required.  No partner is necessary as we rotate partners throughout the lesson.  Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C487" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/717475250956404/</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Friday 30 May 2025 at 18:00 FREE Beginner Bachata Class 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 About Discussion More About Discussion FREE Beginner Bachata Class Details 65 people responded Event by Mayfair Shopping Centre and Victoria Latin Dance Association 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 Public · Anyone on or off Facebook Ready to get your groove on? We’re teaming up with the Victoria Latin Dance Association  for a FREE Beginner Bachata Class right here at Centre Court! Join us on Friday, May 30 at 6:00 PM for an evening of fun and dancing. FREE Beginner Bachata Class May 30th, Friday at 6PM NO partner or experience necessary! Bachata is a beautiful and easy-to-learn dance that’s great for meeting new people, getting active, and connecting with an amazing community. See less Dance Victoria, British Columbia 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 3147 Douglas St, Victoria, BC V8Z 3K3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C488" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/9677364319006080/</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 57 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation July 20, 2025 | Lesson:  Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C489" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1901245437276872/</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Friday 9 May 2025 from 20:00-00:00 Bachata Nights Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Details 40 people responded Event by Bachata Nights Victoria BC , Alysha Kopala and Sebastian Carmona Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights May 09 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @yourgirlalysha  and @davidch_78  will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person The evening starts with an Open-level Bachata lesson from 8:15 PM to 9:00 PM—great for all skill levels! Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C490" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/679241811720932/</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Fundamentals- May Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- May Series Details 7 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, May 6, 13, 20, 27 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C491" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1382188962971661/</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Tuesday 1 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Fundamentals- April Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- April Series Details 9 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, Apr 1, 8, 15, 22, 29 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C492" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342792743590871/</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Monday 7 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- April series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, April 7, 14, 28. Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C493" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/10048344358532607/</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- May series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. May 6, 13, 20, 27 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C494" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/966455485665576/</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Thursday 3 April 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- April series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Apr 1, 8, 15, 22, 29 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C495" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/669591372187091/</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 10:00-11:00 Salsa &amp; ChaCha Solo Westshore Dance Studios Sat, 17 May Sat, 24 May Sat, 31 May +7 About Discussion More About Discussion Salsa &amp; ChaCha Solo Details 2 people responded Event by Dance Praktika Westshore Dance Studios Duration: 1 hr Public · Anyone on or off Facebook Elevate your dance journey with our Ladies Solo Class. Join our exciting series and learn the basics of Salsa and Cha Cha. Perfect for beginners looking to spice up their dance skills! Class Highlights: - Learn exciting dance moves tailored for solo dancers; - Fun and welcoming environment; - Suitable for absolute beginners. Come dance with us and let the rhythm guide you! To register to April classes please use links at "Tickets". See less Langford, British Columbia Westshore Dance Studios 109-2675 Wilfert Road, Victoria www.westshoredance.com 2years+ Competitive&amp;Production a space for everyone with a love of dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C496" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2214494908966327/</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Monday 5 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Int/ Adv- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- May series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, May 5, 12, 26 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C497" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1059622278965884/</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 8 Saturday 8 November 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in October. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Roy, Lorne and 10 friends 1338 people interested Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 243 people interested Interested This Friday at 19:00 Pride Contra Dance Fairfield United Adam is interested 85 people interested Interested Popular with friends Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C498" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/530862806349067/</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Sunday 30 March 2025 from 13:00-17:00 Salsa Gonzales tasting! 🍋‍🟩 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia About Discussion More About Discussion Salsa Gonzales tasting! 🍋‍🟩 Details 6 people responded Event by THE ROOT CELLAR | village green grocer 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia Duration: 4 hr Public · Anyone on or off Facebook Hey friends! It's time to get those tastebuds tingling - you're invited to come and join us for a Salsa Gonzales tasting at our McKenzie Corner store! Salsa Gonzales is a little condiment company with a big personality! Nestled on Gonzales Beach in Victoria, they craft salsas, hot sauces, pickles, preserves, and more – all with a generous splash of love and a fiery kick. When: Sunday March 30th, 1pm-5pm Where: Our McKenzie Corner location We're looking forward to seeing you there! XO See less Victoria, British Columbia 1286 McKenzie Avenue, Victoria, BC, Canada, British Columbia 1286 McKenzie Ave, Saanich, BC V8P 5P2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C499" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1636237610432412/</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Saturday 16 August 2025 from 20:00-23:59 Salsa Sunset Latin Party – August 16th! Latin Dance Canada About Discussion More About Discussion 🌅🔥 Salsa Sunset Latin Party – August 16th! 🔥🌅 Interested Going Invite Details 29 people responded Event by Latin Dance Canada Latin Dance Canada Duration: 3 hr 59 min Public · Anyone on or off Facebook Salsa Sunset Latin Party – August 16th! Get ready for a magical summer night filled with Latin rhythms, sunset vibes, and non-stop dancing! Join us for the Salsa Sunset Latin Party, where the Salsa, Bachata, and Merengue beats will keep you moving all night long under the stunning sunset sky! Dress Code: Wear your best sunset-inspired outfit – think bright, tropical colors, and beach party vibes! Dance to the best Salsa, Bachata, Merengue &amp; Latin hits all night! No partner? No problem! Join our fun intro class at 8:00 PM! Location: Ukrainian Cultural Centre, 3277 Douglas St., Victoria, BC Date: Saturday, August 16, 2025 Intro Class: 8:00 PM | Social Dance: 8:30 PM - Late Entry: $15 at the door – Bring cash, please! What to Expect: Vibrant salsa rhythms &amp; tropical vibes! Tropical-themed decorations &amp; stunning sunset views! A welcoming dance community &amp; unforgettable fun! Let’s dance as the sun sets and make it a night to remember! Tag your friends and let’s create memories under the summer sky! #SalsaSunsetLatinParty #SalsaBachata #LatinDanceParty #VictoriaBC #LatinDanceCanada See less Dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C500" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2251848171850840/</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 Saturday 10 May 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in April. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Fri, 11 Jul at 21:00 Locarno 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Carmie is interested 19 people interested Interested Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 55 people interested Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 243 people interested Interested Popular with friends Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C501" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/884101187183426/</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 July 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Tickets · CA$17.31 www.eventbrite.com/e/caliente-salsa-saturdays-tickets-1415724884239 Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in June. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Tickets Find Tickets Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 243 people interested Interested This Friday at 19:00 Pride Contra Dance Fairfield United Adam is interested 85 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 52 people interested Interested Popular with friends Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C502" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3899920353641309/</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 9 Saturday 9 August 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in July. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1922 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Wed, 25 Jun at 20:30 TD JazzFest 2025: Matteo Mancuso Wicket Hall Carmie is interested 55 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Roy, Lorne and 10 friends 1338 people interested Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 243 people interested Interested Popular with friends Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C503" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1411005319893067/</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Monday 28 April 2025 from 18:30-22:30 Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion 🔥Bachata &amp; Brazilian Zouk 🌊 dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard Details 7 people responded Event by Bachata and Zouk with Javi in Victoria 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 4 hr Public · Anyone on or off Facebook Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard street | Victoria Join us for a 4 week course exploring the joy and magic of Brazilian Zouk &amp; Bachata dancing! Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on enhancing body awareness, building confidence in dance vocabulary with lead and follow techniques, exploring musicality, and loving yourself deeper with styling! Be prepared to have lots of fun dancing with new friends! Register today! Schedule: Monday April 7 - 28th 6:30-7:25pm | Brazilian Zouk - Level 2 (ask Javi for permission) 7:30-8:25pm | Brazilian Zouk - Level 1 8:30-9:25pm | Sensual Bachata - Beginner Foundations 9:30-10:30pm | Sensual Bachata - Intermediate "Trending Moves" Tuition: $20 | 1 Class $35 | 2 Classes (Brazilian Zouk 1&amp;2, or Brazilian Zouk 1 &amp; Bachata, Bachata 1&amp;2) $50| 3 Classes (3 classes, BEST value) 1709 Blanshard St, Victoria, BC Registration: E-transfer to: danceinflow@gmail.com or send us a message on Whatsapp: 7785877665 (Also accepting credit card/cash at the door) Please add a note if you're registering as a "Leader", "Follower", or "Open to both" Space is limited. Register in advance to reserve your spot! Looking fwd to dancing and flowing with you, Warmly, Javi See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C504" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1106484714432492/</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Wednesday 25 June 2025 from 18:30-21:00 Zouk practica and social White Eagle Hall, 90 Dock St, Victoria BC Wed, 28 May Wed, 4 Jun Wed, 25 Jun Wed, 2 Jul +40 About Discussion More About Discussion Zouk practica and social Interested Going Invite Details 3 people responded Event by Victoria Zouk Collective and Victoria Zouk Collective Group White Eagle Hall, 90 Dock St, Victoria BC Duration: 2 hr 30 min Public · Anyone on or off Facebook Drop-in zouk practica by donation - everyone welcome! White Eagle Polish Hall every Wednesday 6:30-9 pm Shared warm up, free dance time, review material from lessons and congresses, connect and share knowledge! Help is always available. Minimum $5 donation. Cash at the door, or etransfer to oceanzouk@gmail.com Enter the lower hall by the side door on Niagara Street just beside the Polka food truck. Also available in Victoria are zouk lessons with Javi, an amazing instructor from Vancouver! More info at https://www.facebook.com/Sabor.Asi.Dance.Salsa.Victoria or email danceinflow@gmail.com See you there! See less Victoria, British Columbia White Eagle Hall, 90 Dock St, Victoria BC 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C505" s="3" t="n">
+        <v>45826.53331826389</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/544121845403419/</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 13:00-23:55 Swing Session: Balboa with Yoshi and Etsuko Solwood Studio About Discussion More About Discussion Swing Session: Balboa with Yoshi and Etsuko Details 108 people responded Event by Swing Dance Association of Victoria , Dave Henderson and 2 others Solwood Studio Duration: 10 hr 55 min Public · Anyone on or off Facebook Lace up your shoes on May 31, 2025 for an afternoon of Balboa Classes and an evening of Social Dancing with Yoshi and Etsuko Uemura. 4 Classes for everyone &amp; 1 Social Dance! Passes go on sale April 19 at noon at our SDAV Square Shop! You must know and be comfortable with Balboa basics for all of these classes - they won't be covered at this workshop. All the specifics are available at swingvictoria.net , but here are the notes: May 31st, at Solwood Studio, with doors at 12:30pm . Bring indoor shoes, please! 4 classes for everyone and there's a dance from 9-12am. Passes go on sale April 19th at noon. See less Victoria, British Columbia Solwood Studio 1303 Broad St, Victoria, BC V8W 2A8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C506" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/302778660295534/</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Sunday 19 August 2018 from 18:00-21:00 West Coast Swing in the Park! Cameron Bandshell @ Beacon Hill Park Carolyn Gebbie invited you About Discussion More About Discussion West Coast Swing in the Park! Details 58 people responded Event by Carolyn Gebbie Cameron Bandshell @ Beacon Hill Park Duration: 3 hr Public · Anyone on or off Facebook Come join us for another evening of fun and WCS dancing in Beacon Hill Park! WCS music will be provided by DJ Carolyn. For those who are familiar with the routine, the 2018 WCS Rally Song will be played at 6:30, 7:30 and 8:30pm. Sam Jackson and Meaghan Efford, from wcsmovementmethods.com will be on hand to answer questions about WCS or how to improve your WCS dancing. They will also demo some incredible WCS dancing at 7pm. Please invite your WCS dance friends by sharing this event! See less Victoria, British Columbia Cameron Bandshell @ Beacon Hill Park Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C507" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/417338985546213/</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Thursday 29 August 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - August 29! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - August 29! Details 109 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for a fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C508" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/634773653668605/</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Saturday Night West Coast Swing BC Swing Dance Club Victoria 15 Jun 2019 22 Jun 2019 29 Jun 2019 +2 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night West Coast Swing Details 9 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook June means summertime and sunny days! Along with the weather, things for BC Swing Dance Cub Victoria will be changing too. Here's what is happening this month: 7 - 8pm 1st Saturday of the Month: Lesson with Meaghan, plus an assistant from our dance community 7 - 8pm Remaining Saturdays each month: TBD (stay tuned for workshops, activities or practices - updates will be posted on each event page) Note:  The 7 - 8pm weekly timeslot is included in the dance entrance price. -------------------------------------------------- Come join us every Saturday all year long for a fabulous WCS social dance from 8 - 11pm. Just $10 for the ($5 for students). Meaghan Efford and Bob Gebbie 's lesson on June 1st (starting PROMPTLY at 7pm) will be the only lesson in June, and it will be a great way to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity.  The lesson is included in the dance entrance price.  No experience or partner is required. -------------------------------------------------- • 6:45 pm - Doors open • 7:00 pm - TBD each week* • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *lesson with Meaghan and Bob on June 1st Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C509" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1692156731689650/</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Tuesday 24 June 2025 from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 Tue, 3 Jun Tue, 17 Jun Tue, 24 Jun Tue, 1 Jul +22 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Interested Going Invite Details 2 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Saanich, BC V8Z 3S3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C510" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1594011994641933/</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Tuesday 22 April 2025 from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Details 9 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. No street shoes. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C511" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/373500473108499/</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Sunday Swing at Logan's Logan's Pub 10 Dec 2017 Debi Wong invited you About Discussion More About Discussion Sunday Swing at Logan's Details Event by Swing X Logan's Pub Duration: 3 hr 30 min Public · Anyone on or off Facebook Sunday Swing at Logan's is BACK! Come join us for some great tunes and we'll party like it's 1939. Bring your dancing shoes, sweet moves, and a few dollars for our fabulous DJ (and gracious bartenders). Feel free to come early to hang out and grab a bite to eat. 19+. NEW: Crash course 15min swing lesson at 8:30pm! This is intended to be the bare minimum for someone to show up and know the basics of swing dancing, nothing fancy! DETAILS: * 8:30pm Quickie 15min beginner lesson! * 8:45pm social dancing until as late as midnight (maybe!) * Usually gets bluesy after 11pm See less Victoria, British Columbia Logan's Pub 1821 Cook Street, Victoria Original - Authentic - Unique Guests See All</t>
+        </is>
+      </c>
+      <c r="C512" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1776457206589544/</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Friday 21 March 2025 from 18:30-20:30 Slim Sandy's Atomic Cocktails swing speakeasy party! The Coda About Discussion More About Discussion Slim Sandy's Atomic Cocktails swing speakeasy party! Details 72 people responded Event by Peter Sandmark and Trace Nelson The Coda Duration: 2 hr Public · Anyone on or off Facebook Join Slim Sandy's Atomic Cocktails and dance as they play 2 sets of swing jazz, jive and rhythm and blues from the 20’s to the 40’s. Slim, on guitar and harmonica, is joined by Willa Mae on vocals, “Big Daddy Bo” on bass, and Bryn Bad on trumpet.  Slim Sandy has been playing music for over 40 years with acts such as Ray Condo and the Crazy Rhythm Daddies.  In 2012, he and Willa Mae co-created the Slim Sandy band in Victoria!  They have played music festivals in Canada, France, Spain, Germany, Belgium, and the Netherlands.  In May they will be touring in Japan! See less Victoria, British Columbia The Coda 749 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C513" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2441697862726705/</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Sunday 30 June 2019 at 19:00 Journey’s 50th Birthday!!  A West Coast Swing dance party!! Eastern Star Hall Chapters No 5 &amp; No 17 Journeey Song invited you About Discussion More About Discussion Journey’s 50th Birthday!!  A West Coast Swing dance party!! Details 13 people responded Event by Journeey Song Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook 3281 Harriet Road, Victoria,BC Bring your own alcohol-free beverage... Bring a gluten-free appie if you’d like. Dance West Coast Swing until 10 pm to Blues, Pop, RnB, Swing, and a wee bit of Ballroom Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C514" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1035925295253912/</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Friday 18 April 2025 at 18:30 Swing out with the ATOMIC COCKTAILS 751 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Swing out with the ATOMIC COCKTAILS Details 64 people responded Event by Peter Sandmark 751 View St, Victoria, BC V8W 1J9, Canada Public · Anyone on or off Facebook Join the ATOMIC COCKTAILS as they swing out for their pre-Japan Tour dance party on April 18 at the Coda, 751 View Street.  Doors open 6 pn, show from 6:30-8:30 pm!  Tickets $20.  With songs from their new album BLUE LIGHT BOOGIE! See less Victoria, British Columbia 751 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C515" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663756533046485/</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Friday 11 April 2025 at 21:30 Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. Details 36 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Public · Anyone on or off Facebook Miguelito Valdes presents Contodo What happens when you bring together three Cuban and two Canadian musicians, with a deep love of all music and a wide range of musical experiences?  A joyful mix of party and deep groove, that's what! Guaranteed to make you want to dance, these brothers from other mothers bring it all. Con Todo! Featuring: Miguelito Valdes – brass/vocals/percussion Jose Sanchez – drumset/timbales Hector Ramos – congas/percussion Peter Dowse - bass Brooke Maxwell – keys/vocals See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C516" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/402729737034904/</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Thursday 5 September 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Details 123 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for our second fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C517" s="3" t="n">
+        <v>45826.53868971065</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1864555154338100/</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 21 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Alive Tango Victoria About Discussion More About Discussion Weekend with Tango Interested Going Invite Details 17 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 21st 5pm-6pm solo technique all levels. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) We will continue from May with the musicality for phrase change but this time we will add “double time” to help us with it, using examples of different orchestras. We will work with a “rebound” and half giros to change the direction within the phrase. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 22nd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are September 20th &amp; 21st. Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C518" s="3" t="n">
+        <v>45826.54105788194</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1766891834185825/</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam and Alive Tango Victoria Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends SAVE THE DATE! The next Sunday afternoon Milonga is on 8 June 2025 1-4pm. The Coda Club (formerly Hermanns Upstairs) is a beautiful newly renovated venue with awesome ambience, nice wood floor and great sound system. Come join us for a wonderful afternoon of warm hugs and close embrace. Sunday 8June 2025 1-4pm The Coda, 751 View Street, Victoria Admission: $15 (plus tax) Special Guest DJ: Francis Nowaczynski (from Vancouver) Free parking at View Street Parkade (next door) or Broughton Parkade. Cash bar is open for drinks. See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C519" s="3" t="n">
+        <v>45826.54105788194</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1318668532737609/</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 16 16 Apr at 18:30 – 18 Apr at 21:00 Tango week with Lya Alive Tango Victoria About Discussion More About Discussion Tango week with Lya Details 36 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 3 days Public · Anyone on or off Facebook Ignite Your Tango 16th of April, Wednesday 6:30-8:00 On &amp; Off Acis for social dance 18th of April, Friday 6:00 - 7:30 Follower technique 7:45 - 9:00 Switch role / connection Search - Grow &amp; Transform! Seminar series for Tango Dancers that want to transform their way of moving and connecting! We will travel through the Essentials of Tango in order to look for new answers and deeper understanding. What makes tango truly captivating? It’s the embrace, the connection, and the walk. These three fundamental elements are the heartbeat of tango, and mastering them is essential for creating an unforgettable dance experience. You will learn how to condition your body to move with control, fluidity, and elegance. You’ll discover how to find and perfect your axis, which is essential for maintaining balance and stability in every step. We will also explore dissociation, a technique that allows you to move the upper and lower body independently but associated. This workshop series will show you how to apply these principles in both the leader and follower roles, improving connection and response in every moment of the dance. We will apply all this to: The secrets to generating power for boleos effortlessly off and on axis special follower technique class Pro tips to dance with ease and confidence 90 min class - $30 All 3 classes - $80 To register email grazs@shaw.ca or pm me, or talk to me . See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C520" s="3" t="n">
+        <v>45826.54105788194</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3637725693193744/</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 22 Mar at 17:00 – 23 Mar at 13:30 Weekend with Tango with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Weekend with Tango with Jorge Olguín Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 22nd 5pm-6pm solo technique all levels. Balance and weight transfer while walking, change of dynamics to create a better connection with your body. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) Marathon is just around the corner so this month we continue with comfortable close embrace! We continue with dancing in small spaces!! Let’s move gracefully without affecting the partner's axis in elastic hugs of closed embrace. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 23rd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available only on Saturday. Sunday - sold out Next workshop dates are the May 17th &amp;18th Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C521" s="3" t="n">
+        <v>45826.54105788194</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1009684807956058/</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 17 17 May at 17:00 – 18 May at 13:30 Tango weekend with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Tango weekend with Jorge Olguín Details 28 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 17th 5pm-6pm solo technique all levels. ( no partner required) Please bring elastic bands!! 6.30pm-7.30pm for couples only ( need some experience) Sacadas, barridas and colgadas in an elastic embrace in order to create a circular movement. We will work with different orchestras to study the changes we need to do to introduce different tempos and rhythms. Get ready for a workout with musicality! 8pm milonga !!! Join us even if you didn’t take the classes. DJ Ingrid !! Free for people registered for the workshops. $10 for drop-ins. Sunday, 18th 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are June 21st &amp; 22nd Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C522" s="3" t="n">
+        <v>45826.54105788194</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2162855673833831/</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 11 May 2019 18 May 2019 25 May 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 8 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook Wow! April went by so quickly, which means it must've been super fun, which it definitely was.  Everyone at BC Swing Dance Club Victoria is so pleased with the way the first month of social dances went, and we hope to generate the same amount of enthusiasm in May. Let's make this month just as much fun! Come join us on May 4th for the first intro lesson and social dance of the month (plus every Saturday night after that). Just $10 for the lesson and/or social dance ($5 for students). No experience or partner required. • 6:45 pm - Doors open • 7:00 pm - Intro lesson with Sam Jackson and Meaghan Efford * • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *PLEASE NOTE that the weekly lessons will start PROMPTLY at 7pm.  It is disruptive to the flow of the lesson if participants arrive late. For anyone who's interested in building their West Coast Swing fundamentals quickly, note that May will be the last month we'll be offering weekly classes with both Sam and Meaghan. With summer approaching it's a great time to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity. Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C523" s="3" t="n">
+        <v>45826.54371428241</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2238975779474166/</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 13 Apr 2019 20 Apr 2019 27 Apr 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 23 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook A new month, a new social! Come and join in on the fun at our inaugural Saturday night dance and intro lesson on April 6 (and every Saturday night after that)! Just $10 for the Lesson and/or Social ($5 for Students). No experience or partner required. • 6:45 pm – Doors open • 7:00 pm – Beginner Lesson with Sam and Meaghan (this is perfect as a refresher class too!) • 8:00 – 11:00 pm Social Dancing featuring DJ Carolyn Please note the NEW START TIMES for the BC Swing Victoria Saturday night dances. See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C524" s="3" t="n">
+        <v>45826.54371428241</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/516994561244886/</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:45 Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING White Eagle Polish Association About Discussion More About Discussion Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING Details 15 people responded Event by Donna Forsyth , Andre Russo and Victoria West Coast Swing Collective White Eagle Polish Association Public · Anyone on or off Facebook Doors open at 6:45pm at this fabulous new venue! Advanced beginner/intermediate lesson by Chantelle Pianetta from 7 to 8 pm Social dancing for 3 HOURS from 8 to 11 pm DJs Donna and Andre Cost $15 /$12 for students ALL at the spacious White Eagle Hall No need to register and you do not need a dance partner. Please bring scuff-free dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia White Eagle Polish Association 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C525" s="3" t="n">
+        <v>45826.54371428241</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1024182725709172/</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Saturday April 19th Lesson and Social Dance Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 19th Lesson and Social Dance Details 4 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginner plus lesson with Pamela Podmoroff from 8 to 10:15 pm Social dancing from 8 to 10:15 pm DJs Donna and Amanda Cost $15/ $12 for students No need to register and no partner required. Please bring scuff-free indoor dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C526" s="3" t="n">
+        <v>45826.54371428241</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1225266505917189/</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Saturday Beginner Lesson and Social Dancing Dance Victoria Sat, 7 Jun Sat, 14 Jun Sat, 21 Jun Sat, 28 Jun +3 About Discussion More About Discussion Victoria WCS Collective hosts Saturday Beginner Lesson and Social Dancing Interested Going Invite Details 3 people responded Event by Donna Forsyth Dance Victoria Duration: 3 hr 30 min Public · Anyone on or off Facebook Back to AIR CONDITIONED comfort at Dance Victoria Studios Beginner lesson from 7 to 8 pm Social dancing  from 8 to 10:15 pm Cost $15/$12 for students No need to register and no need for previous dance experience or a partner. Please bring scuff-free inside low-heeled dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C527" s="3" t="n">
+        <v>45826.54371428241</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/641769172035949/</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Saturday April 12 Beginner lesson and social dance at Dance Victoria Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 12 Beginner lesson and social dance at Dance Victoria Details 5 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginners lesson by Donna from 7 to 8 pm Social dancing from 8 to 10:15 pm DJs Andre and Nel Cost $15 /$12 for Students No need to register and no partner required. Please bring scuff-free inside dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C528" s="3" t="n">
+        <v>45826.54371428241</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1366072544640156/</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Saturday 17 May 2025 at 18:45 Victoria WCS Collective Beginner Lesson and Social Dancing Dance Victoria About Discussion More About Discussion Victoria WCS Collective Beginner Lesson and Social Dancing Details 9 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson from 7 to 8 pm by John de Pfyffer Social dancing from 8 to 10:15pm DJg by Donna and Nel Cost $15/ $12 for students No need to register and no need for dance experience.. Also, no partner necessary, we got you! Please bring indoor scuff-free dance shoes or socks to dance in. See less Victoria, British Columbia Dance Victoria 2750 Quadra St # 111, Victoria Dance Victoria brings the "World's Best Dance" to the Royal Theatre and supports new dance creation for the international stage from its studios. Guests See All</t>
+        </is>
+      </c>
+      <c r="C529" s="3" t="n">
+        <v>45826.54371428241</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/967438905456066/</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Wednesday 26 March 2025 at 10:00 Victoria WCS Lesson and Dance at Eastern Star Hall Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria WCS Lesson and Dance at Eastern Star Hall Details 1 person responded Event by Donna Forsyth Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson by John de Pyffer from 7 to 8 pm Social dancing from 8 to 10:15pm Djs Amanda and Nel Cost $12 No need to register and no partner required. Please bring scuff-free indoor shoes or socks to dance in  and a water bottle. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C530" s="3" t="n">
+        <v>45826.54371428241</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/644050564927019/</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends! A NEW SUNDAY AFTERNOON MILONGA! This is the first of a regular monthly milonga at a beautiful new venue…The Coda Club (formerly Hermann’s Upstairs) at 751 View Street, Victoria. Great ambience, nice wood floor, good sound system. So come join us for the warm hugs and close embrace and dance to the beautiful music of our very own DJ John Dewhirst. Sunday, 6 April 2025 2.00pm-5.00pm The Coda Club, 751 View Street, Victoria Admission $15 DJ: John Dewhirst Cash Bar is open for drinks Free Parking at View Street Parkade just next door Come celebrate this exciting day with us! See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C531" s="3" t="n">
+        <v>45826.54500648148</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1022330066692643/</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Wednesday 2 July 2025 at 18:30 Technique and Milonga with Monica Parra Alive Tango Victoria About Discussion More About Discussion Technique and Milonga with Monica Parra Interested Going Invite Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Public · Anyone on or off Facebook 2nd of July , Wednesday 6.30-8pm Follower’s technique: Pivots and turns • Dissociation technique and axis control. • Free leg preparation before the turn. • Turns in tight spaces (useful in a close embrace!!) 90 minutes, $30 9th of July , Wednesday 6.30-8pm Couple workshop: Milonga Lisa and Milonga with traspie using different tempo. 90 minutes, $30 Both workshops (July 2nd and 9th)$50 Register with Grazyna (grazs@shaw.ca, Messenger or simply talk to me) Contact me personally for privates with Monica. See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C532" s="3" t="n">
+        <v>45826.54500648148</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/713923214640962/</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Sunday 4 May 2025 from 13:00-16:00 May 4th Afternoon Milonga Solwood Studio About Discussion More About Discussion May 4th Afternoon Milonga Details 45 people responded Event by Ingrid Love and Kathryn Stone Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook A one-time special afternoon milonga! Join us in celebrating the warmth of Spring and return to sunshine. Or, star wars, if you like. Featuring special guests Kimberly and Khang performing live music (violin/guitar) DJ Ingrid Hosts: Kathryn &amp; Ingrid $15 entry (cash only) 1:00pm-4:00pm Solwood Studio 1303 Broad St Victoria, BC See less Victoria, British Columbia Solwood Studio Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C533" s="3" t="n">
+        <v>45826.54500648148</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1142760357225336/</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 26 26 Jul at 10:00 – 27 Jul at 17:00 ArtisTREE Festival 1401 rockland ave, Victoria, BC, Canada About Discussion More About Discussion ArtisTREE Festival Interested Going Invite Details 1.2K people responded Event by Artistree Festival , MORENA CLOTHING and Cory Judge 1401 rockland ave, Victoria, BC, Canada Duration: 2 days Public · Anyone on or off Facebook Saturday July 26 10-7pm Sunday July 27 10-5pm Government House of BC 1402 Rockland Ave Celebration of Creativity profiling 130 Juried Artisans, Live Music, Installation and Performance Art, Indigenous Makers and Traditions, Kids section, Live Painters, Delicious Food and Ice cream. See less Shopping Victoria, British Columbia 1401 rockland ave, Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C534" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1217747446718881/</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 18:00-22:00 Maifest - Evening of Live Music Edelweiss Club About Discussion More About Discussion Maifest - Evening of Live Music Details 36 people responded Event by Cindy Kent and Victoria Edelweiss Club Edelweiss Club Duration: 4 hr Public · Anyone on or off Facebook Join the Edelweiss Club for a lively evening of music and dance with Bijoux du Bayou and The Helen Davies Band. Let the infectious Zydeco beats and soulful rhythms set the tone for a night of fun, complete with delicious German snacks from the kitchen. Don’t miss out on this high-energy event! Get your tickets online or call 250-383-4823. www.victoriaedelweiss.ca/events See less Victoria, British Columbia Edelweiss Club 108 Niagara Street, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C535" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/651664851189740/</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 12:00-18:00 Music in the Orchard (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Music in the Orchard (RAIN OR SHINE) Details 330 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Come enjoy the start of the summer in the orchard. We have two amazing artists for you, some delicious fun summer ciders for you to try and amazing food to enjoy to complete the experience. Delicious Cider Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀ Beautiful location ⠀⠀⠀⠀ Dog Friendly ⠀⠀ ⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your WELL BEHAVED two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C536" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1414577976223422/</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Saturday from 19:00-23:00 Solstice Slammer 3 - Moon Under Water, Victoria The Moon Under Water Brewpub About Discussion More About Discussion Solstice Slammer 3 - Moon Under Water, Victoria Interested Going Invite Details 60 people responded Event by Electric Druids and Gate Theory The Moon Under Water Brewpub Tickets · CA$10 www.eventbrite.com/e/solstice-slammer-3-tickets-1389012316229 Public · Anyone on or off Facebook Come join us for Solstice Slammer III at Moon Under Water Brewpub and Distillery! Get ready to celebrate with Electric Druids, Gate Theory and West Street Children, hefty drinks and good vibes. Whether you're a craft beer enthusiast or just an enthusiast, there's something for everyone at this epic night of live music. Don't miss out - mark your calendars! See less Music and audio Victoria, British Columbia Tickets Find Tickets The Moon Under Water Brewpub 5435 Fowler Rd, Saanich, BC V8Y 1Y4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C537" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1235598461330700/</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 19 Tomorrow at 19:00 Alfie Zappacosta Live at Hermann's Jazz Club Hermann's Jazz Club About Discussion More About Discussion Alfie Zappacosta Live at Hermann's Jazz Club Interested Going Invite Details 41 people responded Event by AZ Live Vancouver Island Hermann's Jazz Club Public · Anyone on or off Facebook Two time Juno award winner singer songwriter Alfie Zappacosta delivers a performance like no other. A sophisticated musician with international poise Alfie sings in both English and Italian; studied in jazz and classical guitar. He is a virtuoso composer and seasoned live performer. Alfie's rich soaring vocals have always been his signature and his songs diverse drawing from pop, jazz and rock elements. Five decades committed to his craft Alfie has invested in a lot of hard work to reach a capacity to produce complex and impactful music. Much more it is his underlying fabric, a talent, a natural affinity and introspective ability to create music that touches the hearts and souls of his audience. Alfie’s vocal dexterity and song writing proficiency was uncovered by a publisher while writing for his first original band “Surrender, a five-piece group that recorded three albums in the late 1970s into the early 1980s. As a solo artist Alfie's career took off with a legacy of hits that brought him to the world's attention. "Start Again”, “Passion”, “When I Fall in Love Again” and “Nothing Can Stand In Your Way” written with David Foster. In 1988 he was awarded JUNOs for “Album of The Year’ and “Most Promising Artist”, and American Music Award for “Most Popular Album of The Year”. These hit songs were originally written for acoustic and jazz presentations. Writing for radio began to rub against Alfie’s musical integrity and he became frustrated with the demands of music trends. Alfie broke from the stereotype and began to write the lyrics and melodies that were authentically him, revealing his insight into relationships and his advanced knowledge of music. See less Victoria, British Columbia Hermann's Jazz Club 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C538" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/665127126496204/</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Tuesday 27 May 2025 at 19:30 Live Music at the Saxe Point Public House Saxe Point Public House About Discussion More About Discussion Live Music at the Saxe Point Public House Details 9 people responded Event by VINYL WAVE Saxe Point Public House Public · Anyone on or off Facebook Live Music every other Tuesday starting May 27th! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C539" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1093118172681618/</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>(20+) The Joan Bessie Cabaret: a celebration of original  live music and dance | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 29 Sunday 29 June 2025 from 19:00-22:00 The Joan Bessie Cabaret: a celebration of original  live music and dance Metro Studio Theatre About Discussion More About Discussion The Joan Bessie Cabaret: a celebration of original  live music and dance Interested Going Invite Details Event by Joan Bessie Metro Studio Theatre Tickets · CA$5-CA$35 www.eventbrite.ca/e/joan-bessie-cabaret-tickets-1248762816199 Public · Anyone on or off Facebook Get ready to experience a night of songs and choreography at this one-of-a-kind indie cabaret. Licensed all ages event. Music and audio Victoria, British Columbia Tickets Find Tickets Metro Studio Theatre 1411 Quadra Street at Johnson Street, Victoria Meet your host Joan Bessie 13 past events · Page · Musician/band Joan Bessie is a chart topping Canadian artist. This page shares releases &amp; live tour information Message Suggested events This Friday at 19:00 Pride Contra Dance Fairfield United Adam is interested 85 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Roy, Lorne and 10 friends 1340 people interested Interested Sat, 5 Jul at 12:00 Victoria, BC - Victoria Folk Music Festival, Royal Athletic Park Royal Athletic Park Debi and Carmie are interested 1234 people interested Interested Popular with friends Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C540" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1085685423617722/</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Thursday 25 September 2025 at 10:00 The Men in Black: A Tribute to the Music of Johnny Cash Mcpherson Playhouse About Discussion More About Discussion The Men in Black: A Tribute to the Music of Johnny Cash Interested Going Invite Details 2 people responded Event by Jeff Scott and Victoria Live Music - @BarsnbandsYYJ Mcpherson Playhouse Public · Anyone on or off Facebook The Men in Black: The Songs and stories of Johnny Cash, presented Live onstage in this Multimedia production. Featuring special guest Tracee Rees singing the parts of June Carter Cash. Tickets on sale from the McPherson Box Office: https://www.rmts.bc.ca/.../2025.../the-men-in-black/ See less Victoria, British Columbia Mcpherson Playhouse 48.428809, -123.366838 Guests See All</t>
+        </is>
+      </c>
+      <c r="C541" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1975172826621817/</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>(20+) Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Thursday 12 June 2025 from 19:00-20:30 Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Little Fernwood Gallery. About Discussion More About Discussion Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Details Event by Anna Bigland-Pritchard Little Fernwood Gallery. Duration: 1 hr 30 min Public · Anyone on or off Facebook Do you need some R&amp;R? Join Anna &amp; Roxie for a dreamy candlelit evening of restorative yoga, live music, and guided journalling. Facilitated by Roxie Fehr of Across the Water | Yoga Anna Bigland-Pritchard of ABP Music Studio | Music As experienced, intuitive space-holders, our goal to support your Nervous System and capacity for hope with a feast of restful offerings. We know life is stressful and we want to help you feel more connected to your intuition so you can not only survive, but also have the capacity to take the next right step in your life in a way that positively impacts the world. The space will be dreamy, there will be tea, guided journalling, poetry, restorative yoga shapes that can be adapted for any body, and LIVE MUSIC! Anna will be playing guitar, creating dreamy sound worlds with vocal looping, and singing you lullabies all evening. What to bring Yoga mat (We'll have a few available to borrow) Journal &amp; pen/pencil (We'll also have some spare paper and writing/drawing utensils) Yourself in your comfy cozies Details June 12, 7-8:30pm at Little Fernwood $42 Accessibility This event is on the ground floor There is a unisex/non-gendered bathroom on the same level We care about making this event accessible, so please let us know if you have any questions or accessibility needs. This will be a VERY gentle practice, and modifications will be offered. Happy pride! As members of and allies of the 2SLGBTQIA community, we (Anna &amp; Roxie) will create a supportive, inclusive, affirming environment and expect all participants to do the same. If cost is a barrier, please contact us directly as we have a limited number of discount codes available This is our first time offering this class, and we hope it will be a hit so we can make it a regular thing. Come as you are, leave nourished by your dreams See less Victoria, British Columbia Little Fernwood Gallery. 1923 Fernwood Ave., Victoria Meet your host Anna Bigland-Pritchard 6 past events · Page · Musician/band Based in Lekwungen territory (Victoria, BC), Anna Bigland-Pritchard is a: -Soprano -Voice teacher… Follow Suggested events This Friday at 19:00 Pride Contra Dance Fairfield United Adam is interested 85 people interested Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends 243 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Roy, Lorne and Ali 52 people interested Interested Popular with friends Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C542" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/979769967649565/</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 15:00-18:00 Live Music at the Legion 102-622 Admirals Rd, V9A 2N7 Sat, 17 May Sat, 24 May Sat, 31 May +2 About Discussion More About Discussion Live Music at the Legion Details 8 people responded Event by Royal Canadian Legion, Esquimalt Dockyard #172 102-622 Admirals Rd, V9A 2N7 Duration: 3 hr Public · Anyone on or off Facebook Come enjoy live music on Saturdays 3-6 p. Dancing encouraged! Victoria, British Columbia 102-622 Admirals Rd, V9A 2N7 622 Admirals Rd, Esquimalt, BC V9A 2N7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C543" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/686146924271113/</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>(20+) Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Spring Series Lorne and David Friday from 19:30-23:00 WACK! Another West Coast Swing Social Dance Aylene and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Lorne and 4 friends Recommended events See all Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 5 Thursday 5 June 2025 from 19:00-22:00 Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz 753 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz Details Event by Adonis Puentes and Brent Jarvis 753 View St, Victoria, BC V8W 1J9, Canada Duration: 3 hr Public · Anyone on or off Facebook An evening of Jazzy Cuban Fusion Music; traditional, contemporary, romance and dance. Juno &amp; Grammy Nominated vocalist, Adonis Puentes, will be joined by the Jazz Bohemians, featuring Brent Jarvis (piano), Ken Lister (bass), Nicholas Marquez (percussion) and Brooke Maxwell (Sax). Adonis Puentes opens up the marvelous world of Cuban music to his audience the second they hear his rich voice. When the other players kick in with their tight, multi-layered arrangements, it becomes clear that Adonis is a powerful bandleader. Fronting an acoustic band, Adonis' vocals are surrounded by piano, bass, strings, and percussion. Music reflects the present and Adonis Puentes is a Cuban Sonero for our times. Adonis thrives on the growth and acclaim for his original sonero sound. As he puts it, "I feel like a messenger of my roots and tradition, blessed that with me I have taken my music and heritage to many different places in the world; from Cuba, to Canada, USA, Mexico, Europe and Asia. My mission is to make you dance and enjoy my melodies and rhythms." Musician Line-Up: Adonis Puentes - Vocals Brent Jarvis - Piano Ken Lister - Bass Nicolas Marquez - Percussion Brooke Maxwell - Sax See less Music and audio Victoria, British Columbia 753 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Meet your hosts Adonis Puentes 34 past events · Page · Musician/band Adonis Puentes is a great singer and an elegant composer and lyricist grounded and nourished by his Cuban roots and worldly experience. Message Brent Jarvis 37 past events · Profile · Musician Message Suggested events This Sunday at 14:00 Victoria Ska &amp; Reggae Fest Finale feat. illScarlett, MonteBong, Devon Kay, Brasser, Razorvoice Victoria, BC, Canada, British Columbia Carmie is interested 378 people interested Interested Today at 16:00 Victoria Ska &amp; Reggae Fest Kickoff: Waahli, The Resignators, Hezron, Gun Street Ghouls &amp; Cabin Fever Victoria, BC, Canada, British Columbia 623 people interested Interested Tomorrow at 16:00 Victoria Ska &amp; Reggae Fest: Turbulence, La Severa Matacera, Spiritual Warriors, Sonic Alley &amp; Ari DL Victoria, BC, Canada, British Columbia 329 people interested Interested Popular with friends Today at 18:30 Swing Dancing in City Square Duncan City Hall Carmie is interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Thu, 3 Jul at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested Sat, 28 Jun at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Roy, Lorne and 3 friends Interested Mon, 23 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Lorne and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C544" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2579625309035667/</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Sunday 18 May 2025 from 12:00-18:00 Live Music @ Junction (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Live Music @ Junction (RAIN OR SHINE) Details 125 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Here we go again, its a long weekend so let's get our Sunday Funday on. First Live Music of the year at Junction Up first is-  Emergency Exit  are playing from 1230-230pm To take us home is - An &amp; Ben are playing from 3-5pm Tasting Room and Picnic Area are open 12-6pm Oh and if you haven't heard me say it before ITS RAIN OR SHINE. Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Cider ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Mini Market and a Beautiful location ⠀⠀⠀⠀⠀⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your well behaved two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C545" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/4223643791110348/</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Sunday at 13:00 Victoria Italian Day 195 Bay St, Victoria, BC V9A 3K4, Canada About Discussion More About Discussion Victoria Italian Day Interested Going Invite Details 8 people responded Event by Calabrisella 195 Bay St, Victoria, BC V9A 3K4, Canada Public · Anyone on or off Facebook Join us for live music, food, gelato, games, cars, cultural exhibits, vendors, bike valets and much more - Free admission !! Victoria, British Columbia 195 Bay St, Victoria, BC V9A 3K4, Canada 195 Bay St, Victoria, BC V9A 3K4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C546" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1399479741193649/</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Saxe Point Public House About Discussion More About Discussion TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Details 4 people responded Event by Tom Watson Saxe Point Public House Public · Anyone on or off Facebook Join Vinyl Wave at the lovely Saxe Point Pub for a couple of hours of smooth tunes that'll help ease you into the week! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C547" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1110747367748372/</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Saturday 5 July 2025 at 12:00 Victoria Folk Music Festival Royal Athletic Park About Discussion More About Discussion Victoria Folk Music Festival Interested Going Invite Details 938 people responded Event by Victoria Folk Music Festival and Cascadia Concerts Royal Athletic Park Tickets · Free-CA$86.53 vicfolkfest.eventbrite.ca Public · Anyone on or off Facebook Date: July 5, 2025 Location: Royal Athletic Park, Victoria, BC Tickets: Available now at vicfolkfest.eventbrite.ca Gates Open: 12:00 PM Victoria Folk Music Festival Join us for a joyful weekend of music, community, and celebration at Victoria Folk Music Festival, on July 5th set in beautiful Royal Athletic Park . Featuring a world-class lineup including Frazey Ford, Joel Plaskett, Kacy &amp; Clayton, Harry Manx, Ferron, Old Man Luedecke, Vince Vaccaro, Canadian Beauty, Daneil Lapp's BC Fiddle Orchestra and more, this family-friendly event brings together the best in folk, roots, and Americana music. With two stages of live performances, the Victoria Folk Music Festival offers a full day of entertainment and community celebration. Explore the ReLove Vintage Pop-Up Market, showcasing top local vendors with the best in thrift, retro, and vintage wear. Enjoy a variety of Artisan goods and vendors, delicious food from Fresh Coast, Deadbeetz, Taco Revolution, and more. Families will love the vibrant children’s area—complete with a jumping castle! Dance in the grass to local Bluegrass groups and explore vendor booth from local music groups &amp; organizations. A community-driven atmosphere with world-class music at its heart, this festival is set to be a summer highlight for music lovers of all ages. Whether you're dancing barefoot in the grass, discovering your new favorite artist, or relaxing in the shade with friends, the Victoria Folk Music Festival is more than a concert — it’s a celebration of sound, soul, and connection. Don’t miss the unforgettable music and summer moments —July 5th at Royal Athletic Park! See less Music and audio Victoria, British Columbia Tickets Find Tickets Royal Athletic Park 1014 Caledonia Ave, Victoria Royal Athletic Park is a multi-purpose, fully lit stadium in Victoria, British Columbia. It is primarily used for baseball, soccer, softball and football, but also hosts special events, such as the annual Great Canadian Beer Festival and Rifflandia Music Festival. It is approximately a ten-minute walk from the city centre.HistoryIn 1907 the burgeoning summer athletic teams did not have enough facilities for senior teams with paid attendances. Baseball in particular was challenged to find available dates at Oak Bay Grounds to operate due to a preference for lacrosse.Subsequently, the supporters of Canada's national summer sport lacrosse, at a meeting chaired by BC Premier McBride formed the Royal Victoria Athletic Association on March 26, 1908, and a senior lacrosse team was founded to enable the best intermediate (Under 21) players to play in the British Columbia Amateur Lacrosse Association (BCALA) League. The Oak Bay Grounds were put under the management of the senior baseball team and then later the Rugby Football Club. The lacrosse group, later shortened to the Royal Athletic Association, issued shares at $25 each with deposits of 10% and biannual calls of 10% to raise $25,000 for improvements to the grounds. The lease was signed for 5 acres at the corner of Cook and Pembroke Streets for the grounds.Contracts had been let by May 12, 1908 and $4,000 from the share offering and gate receipts was spent by June on the construction of a perimeter fence, 2 ticket offices, an inner fence, grandstand, and carriage parking area. The inner fence enclosed the 500 ft x 285 ft (152m x 87m) playing field. The grandstand on the south side of the playing field was 150 ft long x 25 ft deep with 10 rows of seats for more than 1000 spectators. Beneath the grandstand were dressing rooms and concessions. The original layout of the field and grandstand was essentially the same as today's; however based on maps used in advertising the original field also included half of the city block to the west between Quadra and Vancouver Streets. The carriage parking was on the east side off Cook Street. Guests See All</t>
+        </is>
+      </c>
+      <c r="C548" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1050242777151793/</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Friday from 19:00-22:00 Pride Contra Dance Adam 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Dalie Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 10 Jun at 09:00 – 15 Jun at 19:00 KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Victoria ,BC About Discussion More About Discussion KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Details 46 people responded Event by Congregation Emanu-El, Victoria, British Columbia Victoria ,BC Duration: 6 days Public · Anyone on or off Facebook Registration required for both in person and virtual attendance. https://klezcadia.org https://congregationemanuelnews.wordpress.com/.../klezca.../ Locations of performances and workshops provided upon registration. See less Victoria, British Columbia Victoria ,BC 528 Broughton St, Victoria, BC V8W 1C6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C549" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1451663826076478/</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Sunday 6 July 2025 from 11:00-16:00 Saanich Strawberry Festival Beaver Lake Regional Park, 728 Beaver Lake Rd. About Discussion More About Discussion Saanich Strawberry Festival Interested Going Invite Details 456 people responded Event by Saanich Parks, Recreation &amp; Community Services Beaver Lake Regional Park, 728 Beaver Lake Rd. Duration: 5 hr Public · Anyone on or off Facebook Join Saanich in celebrating the 58th annual Strawberry Festival. This family-friendly, fun, free event features live music, kids' activities, bouncy castles, information booths, arts and craft stations and, of course, the traditional servings of strawberries and ice cream. Strawberries and ice cream sales and service will be from 2 to 4pm, or until sold out. $2/serving. For more details, including vendors, activities and performances, visit saanich.ca/strawberryfestival See less Foods Victoria, British Columbia Beaver Lake Regional Park, 728 Beaver Lake Rd. 728 Beaver Lake Rd, Saanich, BC V8Z 6K2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C550" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1514674672845802/</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Saturday 5 July 2025 at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park About Discussion More About Discussion Oak Bay Summer Concerts in the Park: Family Show Interested Going Invite Details 414 people responded Event by Oak Bay Parks, Recreation and Culture Willows Park Public · Anyone on or off Facebook Oak Bay Summer Concerts in the Park: Family Show With a stunning backdrop of Willows Beach, these outdoor concerts gather the community to celebrate music and the arts.  Presented by Oak Bay Parks, Recreation and Culture. Location: Willows Beach Park, Oak Bay Date: Saturday, July 5, 2025 Time: 2:00 p.m. Admission: Free Family Concert: lək̓ʷəŋən Traditional Dancers, Pacific Opera Victoria, STAGES Dance Company, and Marimba Mufaro. More information: https://www.oakbay.ca/.../oak-bay-summer-concerts-in-the.../ See less Victoria, British Columbia Willows Park 2778 Dalhousie St, Oak Bay, BC V8R, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C551" s="3" t="n">
+        <v>45826.55137051206</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added methods to clean_up.py that get rid of duplicate addresses. This uses transofmres, dbscan, and agglomerative clustering.
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -16,9 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -8464,7 +8463,7 @@
         </is>
       </c>
       <c r="C534" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="535">
@@ -8479,7 +8478,7 @@
         </is>
       </c>
       <c r="C535" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="536">
@@ -8494,7 +8493,7 @@
         </is>
       </c>
       <c r="C536" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="537">
@@ -8509,7 +8508,7 @@
         </is>
       </c>
       <c r="C537" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="538">
@@ -8524,7 +8523,7 @@
         </is>
       </c>
       <c r="C538" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="539">
@@ -8539,7 +8538,7 @@
         </is>
       </c>
       <c r="C539" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="540">
@@ -8554,7 +8553,7 @@
         </is>
       </c>
       <c r="C540" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="541">
@@ -8569,7 +8568,7 @@
         </is>
       </c>
       <c r="C541" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="542">
@@ -8584,7 +8583,7 @@
         </is>
       </c>
       <c r="C542" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="543">
@@ -8599,7 +8598,7 @@
         </is>
       </c>
       <c r="C543" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="544">
@@ -8614,7 +8613,7 @@
         </is>
       </c>
       <c r="C544" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="545">
@@ -8629,7 +8628,7 @@
         </is>
       </c>
       <c r="C545" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="546">
@@ -8644,7 +8643,7 @@
         </is>
       </c>
       <c r="C546" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="547">
@@ -8659,7 +8658,7 @@
         </is>
       </c>
       <c r="C547" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="548">
@@ -8674,7 +8673,7 @@
         </is>
       </c>
       <c r="C548" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="549">
@@ -8689,7 +8688,7 @@
         </is>
       </c>
       <c r="C549" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="550">
@@ -8704,7 +8703,7 @@
         </is>
       </c>
       <c r="C550" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
     <row r="551">
@@ -8719,7 +8718,7 @@
         </is>
       </c>
       <c r="C551" s="3" t="n">
-        <v>45826.55137051206</v>
+        <v>45826.55137050926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
not sure what happened but I deleted the generate_prompt() method in llm.py. I retrieved it from git. All good now. Just commiting it here.
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -429,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C551"/>
+  <dimension ref="A1:C569"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8721,6 +8722,276 @@
         <v>45826.55137050926</v>
       </c>
     </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1187402793186660/</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 08:00-12:00 Global Underscore Solstice Dance Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada About Discussion More About Discussion Global Underscore Solstice Dance Details 62 people responded Event by Arunimá McNeish , Michael McAmmond and Victoria Contact Improv Jam Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada Duration: 4 hr Public · Anyone on or off Facebook Sweet dancers, This summer solstice we extend a warm invitation to join us in expanding and deepening our practice of Contact Improvisation with participation in The Global Underscore. Please arrive at 8am to join a 40 minute talk-through, introducing the concepts of the Underscore. This is mandatory if you have never attended an Underscore before. The Underscore will begin promptly at 8:45am. If you have attended a talk-through before you're welcome to arrive at this time. We will all start and end together. This is a closed container and we will not be allowing late-comers. TIMELINE: 8am-8:40am Underscore Talk-Through with Arunima 8:45am-11:30am Underscore 11:30am-11:50am Closing Circle COST: $15-$20  etransfer or pay cash at the door if pre-registered (if money is a barrier please reach out to discuss options). Please contact Arunima at ode.to.thylacine@gmail.com for registration, etransfer, questions, etc. VENUE: Centennial United Church (612 David St, Victoria, BC). MORE INFO: The Underscore, which has been evolving since 1990, is a vehicle for incorporating Contact Improvisation into the broader arena of improvisational dance practice; developing greater ease dancing in spherical space—alone and with others; and for integrating kinesthetic and compositional aspects while improvising. It allows for a full spectrum of energetic and physical expressions, embodying a range of forms and changing states. Its practice is familiar yet unpredictable. The practice progresses through a broad range of dynamic states, including long periods of very small, private, and quiet internal activity and other times of higher energy and interactive dancing. There are 20+ phases, 12+ connections, and 7 aspects of the Underscore—each with a name and a graphic symbol—which create a general map for the dancers. Within that frame, dancers are free to create their own movements, dynamics, and relationships—with themselves, each other, the group, and the environment. Each Underscore is unique, providing rich and often inspiring experiences of the human and artistic phenomena of dance improvisation. https://globalunderscore.com/ https://nancystarksmith.com/underscore/ See less Victoria, British Columbia Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada 612 David St, Victoria, BC V8T 2E1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C552" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1363696181561219/</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:00-22:00 Pride Contra Dance Fairfield United About Discussion More About Discussion Pride Contra Dance Details 90 people responded Event by Victoria Contra Dance , Code Tron and Rose Jackson Fairfield United Duration: 3 hr Public · Anyone on or off Facebook 𝕍𝕀ℂ𝕋𝕆ℝ𝕀𝔸 ℂ𝕆ℕ𝕋ℝ𝔸 𝔻𝔸ℕℂ𝔼 𝕊𝕆ℂ𝕀𝔼𝕋𝕐 ℙℝ𝔼𝕊𝔼ℕ𝕋𝕊: The return of our ℚ𝕌𝔼𝔼ℝ Contra Dance to celebrate the month of Pride! All Dancers welcome! Join us Friday, June 20th at the United Commons Fellowship Hall to do-si-do the night away to sprightly fiddle tunes and stellar performances from our two favorite drag performers! We'll have more capacity than our previous Valentines Day Dance, but we still might sell out, so grab your tickets online here! https://clannamorna.ca/.../ticket-victoria-pride-contra.../ ......................................................................................................... 𝕄𝕦𝕤𝕚𝕔 𝔹𝕪: 𝐑𝐨𝐬𝐞 𝐉𝐚𝐜𝐤𝐬𝐨𝐧: she/her Coming up in the rich folk scene of western Massachusetts, Rose is based in Montague, MA, where she studied under fiddler Becky Tracy from whom she inherited a wide repertoire of music from Quebec, New England, Ireland, and France, a deep love for old tunes, and the intuitive sense of rhythm and danceability which infuses her playing. Equally at home in the concert hall and on the dance stage, she’s taught fiddle, song, and dance at camps and festivals around New England, toured nationally with her band Polaris and now tours with her quartet Stove Dragon and duo Helen &amp; Rose. https://www.rose-jackson.com/ 𝐇𝐞𝐥𝐞𝐧 𝐊𝐮𝐡𝐚𝐫: they/them Hailing from Seattle, Washington, Helen currently resides in Cambridge, MA. Helen began exploring their connection to folk and Celtic music in 2020 while studying with renowned contra guitarist Alex Sturbaum. Upon moving to Cambridge in 2022, Helen dove into the thriving celtic music scene, playing contra dances, Irish sessions, and concerts around New England and the Pacific Northwest. Since then, Helen has developed their style as a contra accompanist, Irish session backer, and vocalist. https://www.helenkuharmusic.com/ 𝐅𝐢𝐝𝐝𝐥𝐢𝐧' 𝐅𝐢𝐧𝐧: they/them A professional fiddler, singer and banjo player living on the territories of the lekwungen and W̱SÁNEĆ people, colonially known as Victoria BC. Finn has a passion for Irish, Scottish, English, North American and Eastern European folk music, and are known for their dynamic fiddling and soulful voice. They delve into traditional material - bringing a fresh interpretation of songs and tunes from many different places, as well as writing their own material. From the Appalachian mountains to Quebec, to melodic Irish and Scottish tunes, they cover wide musical ground with articulate playing. Finn also performs frequently in Canada and the U.S. with their bands Clanna Morna and Ghostly Hounds. https://finnletourneau.com/ ℂ𝕒𝕝𝕝𝕚𝕟𝕘 𝔹𝕪: 𝐕𝐢𝐜𝐭𝐨𝐫𝐢𝐚 𝐁𝐞𝐚𝐮𝐜𝐡𝐞𝐬𝐧𝐞 One of our local communities up and coming callers! 𝔻𝕣𝕒𝕘 𝕡𝕖𝕣𝕗𝕠𝕣𝕞𝕒𝕟𝕔𝕖𝕤 𝕓𝕪: Aries Moon: Making country gay one song at a time Leo Moon: The island's premiere tap dancing drag thing ......................................................................................................... 6:30 - doors open 7:00 - dancing starts with a beginner friendly dance lesson Everyone welcome, no experience necessary. $12 - Youth $20 - Everyone who is willing and able to NOTAFLOF Poster Art by Sonya Chwyl See less Victoria, British Columbia Fairfield United 925 Balmoral Rd, Victoria, BC V8T 1A7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C553" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/589043697010919/</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 66 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, May 25th features Cedar Mathias as our facilitator/dj! Details for Sunday, May 25th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C554" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1031573525615192/</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Sunday at 19:00 GROOVE KITCHEN'S JUNEFEST DANCE!! Hermann's Jazz Club About Discussion More About Discussion GROOVE KITCHEN'S JUNEFEST DANCE!! Interested Going Invite Details 97 people responded Event by Groove Kitchen and Hermann's Jazz Club Hermann's Jazz Club Tickets hermannsjazz.com/show/737557/view Public · Anyone on or off Facebook The festival is over and it seems you still wanna celebrate music, but also... wanna get down and boogie?? You're our kind of people!! Observe the top of Summer with song and funky steps as the kitchen's groove moves your body like they've done before at spots like the Butchart Gardens, The Esquimalt Ribfest, The Osbourne Bay Pub, or the hottest rooms in and outta town. The Chefs are ready to serve their mouthwatering melange of funk, pop, soul, Latin, and flavours to party to the end!! Join us... Doors 5:30 PM / 7:00 PM Show, Sunday June 29th Hermann's Jazz Club 753 View Street Victoria, BC V8W 1J9 https://hermannsjazz.com/show/737557/view See less Victoria, British Columbia Tickets Find Tickets Hermann's Jazz Club 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C555" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1238334523949776/</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Sunday from 11:00-12:30 Dance Temple w/ Alex King-Harris (aka Rara Avis) Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Alex King-Harris (aka Rara Avis) Interested Going Invite Details 66 people responded Event by Dance Temple Victoria , Alex King-Harris and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 29th features Alex King-Harris (aka Rara Avis) as our facilitator/dj. He is back in town for the summer! Details for Sunday, June 29th: Facilitation and music set by Alex King-Harris (Rara Avis) Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C556" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/734261429120710/</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Friday 6 June 2025 from 19:30-22:30 Dance City 108 Niagara St, Victoria, BC V8V 1E9, Canada About Discussion More About Discussion Dance City Details 9 people responded Event by Andrew Sanderson 108 Niagara St, Victoria, BC V8V 1E9, Canada Duration: 3 hr Public · Anyone on or off Facebook Beginner Cha Cha workshop with Jane and Andrew at 7:30pm Multi genres dance including Standard, Latin,  West Coast Swing, and more starting at 8:30pm dj Andrew Sanderson Cash Admission: $12/$10 Members See less Victoria, British Columbia 108 Niagara St, Victoria, BC V8V 1E9, Canada 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C557" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1408949946810887/</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Sunday 8 June 2025 from 11:00-12:30 Dance Temple w/ Lila Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Lila Details 32 people responded Event by Dance Temple Victoria , Lyndsay Lila and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 8th features Lila Spencer as our facilitator/dj! Details for Sunday, June 8th: Facilitation and music set by Lila Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C558" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1904863453602318/</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 19:00-22:00 Private Dance Saanichton, BC About Discussion More About Discussion Private Dance Details 8 people responded Event by HAMMERdown - Victoria, BC Saanichton, BC Duration: 3 hr Public · Anyone on or off Facebook We are excited for our gig on May 31 at Saanichton Bay. It is a private event. There will be good rocking tonight. Victoria, British Columbia Saanichton, BC Saanich Guests See All</t>
+        </is>
+      </c>
+      <c r="C559" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3854957174726232/</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Monday 30 June 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 49 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Urban Kizomba with Aaron and Fernanda— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C560" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2576922459305643/</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 51 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 15th features Cedar Mathias as our facilitator/dj! Details for Sunday, June 15th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C561" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1682353965754886/</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Saturday 14 June 2025 from 18:00-20:30 Mamas' Dance Party! 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Sat, 5 Apr Sat, 10 May Sat, 14 Jun About Discussion More About Discussion Mamas' Dance Party! Details 32 people responded Event by Fairfield Gonzales Community Association 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Duration: 2 hr 30 min Public · Anyone on or off Facebook Calling all mamas, grand-mamas, aunties &amp; mamas-to-be! Join us for a night curated for all mamas (in any season of their motherhood or reproductive journey) to connect through creative expression, freedom of movement and community building! There will be an opening &amp; closing circle and time to connect over light refreshments as the night concludes. Feel free to come for it all, or leave when needed. We can't wait to dance, groove, and connect with you all soon. This is an inclusive space for ALL those who mother. Admission by-donation: suggested donation $5 This event is presented by the FGCA's Neighbourhood Improvement Committee See less Victoria, British Columbia 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 1330 Fairfield Rd, Victoria, BC V8S 5J1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C562" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1185783966345055/</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 10:00-13:00 Shuffle Dance Workshop Victoria, BC About Discussion More About Discussion Shuffle Dance Workshop Details 12 people responded Event by Adelène Buchanan Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another SHUFFLE WORKSHOP coming your way!! Join our Shuffle Dance Workshop and learn a full shuffle choreography set to an energetic electronic track. We’ll guide you through each step, focusing on key shuffle movements, while incorporating them into a dynamic routine. Perfect for ALL LEVELS! This workshop will help you improve your footwork, coordination, and cardiovascular stamina as you master a complete choreography. Here’s what you need to know: DATE: Sunday, May 25th TIME: 10am - 1pm PLACE: The Beat Clinic (1303 Broad Street) Sign-up link here https://www.thebeatclinic.ca/ See less Victoria, British Columbia Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C563" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/909522138040202/</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today at 17:00 ReLove Night Market Janine and 3 friends Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Friday 28 November 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 127 people interested Interested Sun, 20 Jul at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Lorne, Roy and 2 friends 60 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Saturday at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C564" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/939376108286434/</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today at 17:00 ReLove Night Market Janine and 3 friends Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Tomorrow at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Tickets · CA$17.31 www.eventbrite.com/e/salsa-night-dance-city-tickets-1415720962509 Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Tickets Find Tickets Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 18 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Ali and Jon 27 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 127 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Saturday at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C565" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/624858640069610/</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today at 17:00 ReLove Night Market Janine and 3 friends Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 Friday 22 August 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 127 people interested Interested Sun, 20 Jul at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Lorne, Roy and 2 friends 60 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Saturday at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C566" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/556816543734629/</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Monday 7 July 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 46 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Merengue with Sebastian and Hannah— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C567" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/650657144184821/</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Saturday 19 July 2025 from 21:00-02:00 COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY The Coda About Discussion More About Discussion COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY Interested Going Invite Details 64 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 5 hr Public · Anyone on or off Facebook Colombian Summer Rumba: “Tierra Querida” Party Saturday, July 19th Doors: 9:00 PM | Show: 9:30 PM 19+ | ID Required Celebrate Colombian Independence Day with us with the vibrant “Tierra Querida” Party — an amazing night of live music, dance, culture, and pure rumba energy! Start the night with a live tribute to Colombian music by the talented Daniel Sar &amp; Sofia Leonne. Their performance will honor legendary Colombian artists such as Juanes, Maluma, Fonseca, Rodolfo Aicardi, Herencia de Timbiquí, Mon Laferte, and more—blending pop, tropical rhythms, and heartfelt Latin ballads into a powerful musical journey. At 10:30 PM, DJ Miro, straight from Cali, Colombia, will take over with a fiery mix of Colombian beats. Later, resident DJ Alex King will close out the night, turning up the heat with Latin hits and ending strong with the latest reggaetón summer vibes. At midnight, enjoy a special folkloric performance by Danza Colombia, followed by a unifying moment as we wave our flag souvenirs and sing the national anthem together. Savor delicious cocktails, soak in vibrant downtown vibes, and enjoy a night filled with alegría, culture, and  Colombian vibes! Get your tickets NOW! First-tier: $20 | Second-tier: $25 Limited tickets available at the door for $27 - Act fast before they are sold out! Party ends at 2:00 AM Each ticket includes a Colombian flag souvenir. Take a piece of the celebration home with you! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C568" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1132427048350776/</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com or 15$ cash/e-transfer at the door. Formed in the heart of Chinatown, Rosebuds is a dynamic ensemble that brings the vibrant sounds of jazz, blues &amp; swing to life.  The group plays a mixture of originals and jazz standards, and is influenced by artists like Louis Armstrong, Billie Holiday, Lester Young, and Lionel Hampton. Featuring Rebecca Wells (vocals/guitar), Alex Moore (guitar/keys) Bryden Amos (guitar/keys), Matisse Gubby-Hurtig (bass), Owen Chow (trumpet), and Andrew Greenwood (tenor saxophone). Samba e Sol is a newly formed Brazilian bossa nova jazz trio featuring Andrew Greenwood (flute), Alex Moore (guitar), and Matisse Gubby-Hurtig (bass), playing music by artists like Antonio Carlos Jobim, Marcos Valle, Luiz Bonfa, and more. Instagram: https://www.instagram.com/rosebudsband/ See less Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C569" s="3" t="n">
+        <v>45834.87827490307</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed the #'s that stopped the other methods running. All normal now.
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C569"/>
+  <dimension ref="A1:C605"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8734,7 +8734,7 @@
         </is>
       </c>
       <c r="C552" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="553">
@@ -8749,7 +8749,7 @@
         </is>
       </c>
       <c r="C553" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="554">
@@ -8764,7 +8764,7 @@
         </is>
       </c>
       <c r="C554" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="555">
@@ -8779,7 +8779,7 @@
         </is>
       </c>
       <c r="C555" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="556">
@@ -8794,7 +8794,7 @@
         </is>
       </c>
       <c r="C556" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="557">
@@ -8809,7 +8809,7 @@
         </is>
       </c>
       <c r="C557" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="558">
@@ -8824,7 +8824,7 @@
         </is>
       </c>
       <c r="C558" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="559">
@@ -8839,7 +8839,7 @@
         </is>
       </c>
       <c r="C559" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="560">
@@ -8854,7 +8854,7 @@
         </is>
       </c>
       <c r="C560" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="561">
@@ -8869,7 +8869,7 @@
         </is>
       </c>
       <c r="C561" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="562">
@@ -8884,7 +8884,7 @@
         </is>
       </c>
       <c r="C562" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="563">
@@ -8899,7 +8899,7 @@
         </is>
       </c>
       <c r="C563" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="564">
@@ -8914,7 +8914,7 @@
         </is>
       </c>
       <c r="C564" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="565">
@@ -8929,7 +8929,7 @@
         </is>
       </c>
       <c r="C565" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="566">
@@ -8944,7 +8944,7 @@
         </is>
       </c>
       <c r="C566" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="567">
@@ -8959,7 +8959,7 @@
         </is>
       </c>
       <c r="C567" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="568">
@@ -8974,7 +8974,7 @@
         </is>
       </c>
       <c r="C568" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
       </c>
     </row>
     <row r="569">
@@ -8989,7 +8989,547 @@
         </is>
       </c>
       <c r="C569" s="3" t="n">
-        <v>45834.87827490307</v>
+        <v>45834.87827490741</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/589043697010919/</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 66 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, May 25th features Cedar Mathias as our facilitator/dj! Details for Sunday, May 25th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C570" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1682353965754886/</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Saturday 14 June 2025 from 18:00-20:30 Mamas' Dance Party! 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Sat, 5 Apr Sat, 10 May Sat, 14 Jun About Discussion More About Discussion Mamas' Dance Party! Details 32 people responded Event by Fairfield Gonzales Community Association 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Duration: 2 hr 30 min Public · Anyone on or off Facebook Calling all mamas, grand-mamas, aunties &amp; mamas-to-be! Join us for a night curated for all mamas (in any season of their motherhood or reproductive journey) to connect through creative expression, freedom of movement and community building! There will be an opening &amp; closing circle and time to connect over light refreshments as the night concludes. Feel free to come for it all, or leave when needed. We can't wait to dance, groove, and connect with you all soon. This is an inclusive space for ALL those who mother. Admission by-donation: suggested donation $5 This event is presented by the FGCA's Neighbourhood Improvement Committee See less Victoria, British Columbia 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 1330 Fairfield Rd, Victoria, BC V8S 5J1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C571" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1187402793186660/</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 08:00-12:00 Global Underscore Solstice Dance Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada About Discussion More About Discussion Global Underscore Solstice Dance Details 62 people responded Event by Arunimá McNeish , Michael McAmmond and Victoria Contact Improv Jam Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada Duration: 4 hr Public · Anyone on or off Facebook Sweet dancers, This summer solstice we extend a warm invitation to join us in expanding and deepening our practice of Contact Improvisation with participation in The Global Underscore. Please arrive at 8am to join a 40 minute talk-through, introducing the concepts of the Underscore. This is mandatory if you have never attended an Underscore before. The Underscore will begin promptly at 8:45am. If you have attended a talk-through before you're welcome to arrive at this time. We will all start and end together. This is a closed container and we will not be allowing late-comers. TIMELINE: 8am-8:40am Underscore Talk-Through with Arunima 8:45am-11:30am Underscore 11:30am-11:50am Closing Circle COST: $15-$20  etransfer or pay cash at the door if pre-registered (if money is a barrier please reach out to discuss options). Please contact Arunima at ode.to.thylacine@gmail.com for registration, etransfer, questions, etc. VENUE: Centennial United Church (612 David St, Victoria, BC). MORE INFO: The Underscore, which has been evolving since 1990, is a vehicle for incorporating Contact Improvisation into the broader arena of improvisational dance practice; developing greater ease dancing in spherical space—alone and with others; and for integrating kinesthetic and compositional aspects while improvising. It allows for a full spectrum of energetic and physical expressions, embodying a range of forms and changing states. Its practice is familiar yet unpredictable. The practice progresses through a broad range of dynamic states, including long periods of very small, private, and quiet internal activity and other times of higher energy and interactive dancing. There are 20+ phases, 12+ connections, and 7 aspects of the Underscore—each with a name and a graphic symbol—which create a general map for the dancers. Within that frame, dancers are free to create their own movements, dynamics, and relationships—with themselves, each other, the group, and the environment. Each Underscore is unique, providing rich and often inspiring experiences of the human and artistic phenomena of dance improvisation. https://globalunderscore.com/ https://nancystarksmith.com/underscore/ See less Victoria, British Columbia Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada 612 David St, Victoria, BC V8T 2E1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C572" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1408949946810887/</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Sunday 8 June 2025 from 11:00-12:30 Dance Temple w/ Lila Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Lila Details 32 people responded Event by Dance Temple Victoria , Lyndsay Lila and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 8th features Lila Spencer as our facilitator/dj! Details for Sunday, June 8th: Facilitation and music set by Lila Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C573" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1363696181561219/</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:00-22:00 Pride Contra Dance Fairfield United About Discussion More About Discussion Pride Contra Dance Details 90 people responded Event by Victoria Contra Dance , Code Tron and Rose Jackson Fairfield United Duration: 3 hr Public · Anyone on or off Facebook 𝕍𝕀ℂ𝕋𝕆ℝ𝕀𝔸 ℂ𝕆ℕ𝕋ℝ𝔸 𝔻𝔸ℕℂ𝔼 𝕊𝕆ℂ𝕀𝔼𝕋𝕐 ℙℝ𝔼𝕊𝔼ℕ𝕋𝕊: The return of our ℚ𝕌𝔼𝔼ℝ Contra Dance to celebrate the month of Pride! All Dancers welcome! Join us Friday, June 20th at the United Commons Fellowship Hall to do-si-do the night away to sprightly fiddle tunes and stellar performances from our two favorite drag performers! We'll have more capacity than our previous Valentines Day Dance, but we still might sell out, so grab your tickets online here! https://clannamorna.ca/.../ticket-victoria-pride-contra.../ ......................................................................................................... 𝕄𝕦𝕤𝕚𝕔 𝔹𝕪: 𝐑𝐨𝐬𝐞 𝐉𝐚𝐜𝐤𝐬𝐨𝐧: she/her Coming up in the rich folk scene of western Massachusetts, Rose is based in Montague, MA, where she studied under fiddler Becky Tracy from whom she inherited a wide repertoire of music from Quebec, New England, Ireland, and France, a deep love for old tunes, and the intuitive sense of rhythm and danceability which infuses her playing. Equally at home in the concert hall and on the dance stage, she’s taught fiddle, song, and dance at camps and festivals around New England, toured nationally with her band Polaris and now tours with her quartet Stove Dragon and duo Helen &amp; Rose. https://www.rose-jackson.com/ 𝐇𝐞𝐥𝐞𝐧 𝐊𝐮𝐡𝐚𝐫: they/them Hailing from Seattle, Washington, Helen currently resides in Cambridge, MA. Helen began exploring their connection to folk and Celtic music in 2020 while studying with renowned contra guitarist Alex Sturbaum. Upon moving to Cambridge in 2022, Helen dove into the thriving celtic music scene, playing contra dances, Irish sessions, and concerts around New England and the Pacific Northwest. Since then, Helen has developed their style as a contra accompanist, Irish session backer, and vocalist. https://www.helenkuharmusic.com/ 𝐅𝐢𝐝𝐝𝐥𝐢𝐧' 𝐅𝐢𝐧𝐧: they/them A professional fiddler, singer and banjo player living on the territories of the lekwungen and W̱SÁNEĆ people, colonially known as Victoria BC. Finn has a passion for Irish, Scottish, English, North American and Eastern European folk music, and are known for their dynamic fiddling and soulful voice. They delve into traditional material - bringing a fresh interpretation of songs and tunes from many different places, as well as writing their own material. From the Appalachian mountains to Quebec, to melodic Irish and Scottish tunes, they cover wide musical ground with articulate playing. Finn also performs frequently in Canada and the U.S. with their bands Clanna Morna and Ghostly Hounds. https://finnletourneau.com/ ℂ𝕒𝕝𝕝𝕚𝕟𝕘 𝔹𝕪: 𝐕𝐢𝐜𝐭𝐨𝐫𝐢𝐚 𝐁𝐞𝐚𝐮𝐜𝐡𝐞𝐬𝐧𝐞 One of our local communities up and coming callers! 𝔻𝕣𝕒𝕘 𝕡𝕖𝕣𝕗𝕠𝕣𝕞𝕒𝕟𝕔𝕖𝕤 𝕓𝕪: Aries Moon: Making country gay one song at a time Leo Moon: The island's premiere tap dancing drag thing ......................................................................................................... 6:30 - doors open 7:00 - dancing starts with a beginner friendly dance lesson Everyone welcome, no experience necessary. $12 - Youth $20 - Everyone who is willing and able to NOTAFLOF Poster Art by Sonya Chwyl See less Victoria, British Columbia Fairfield United 925 Balmoral Rd, Victoria, BC V8T 1A7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C574" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1031573525615192/</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Sunday at 19:00 GROOVE KITCHEN'S JUNEFEST DANCE!! Hermann's Jazz Club About Discussion More About Discussion GROOVE KITCHEN'S JUNEFEST DANCE!! Interested Going Invite Details 97 people responded Event by Groove Kitchen and Hermann's Jazz Club Hermann's Jazz Club Tickets hermannsjazz.com/show/737557/view Public · Anyone on or off Facebook The festival is over and it seems you still wanna celebrate music, but also... wanna get down and boogie?? You're our kind of people!! Observe the top of Summer with song and funky steps as the kitchen's groove moves your body like they've done before at spots like the Butchart Gardens, The Esquimalt Ribfest, The Osbourne Bay Pub, or the hottest rooms in and outta town. The Chefs are ready to serve their mouthwatering melange of funk, pop, soul, Latin, and flavours to party to the end!! Join us... Doors 5:30 PM / 7:00 PM Show, Sunday June 29th Hermann's Jazz Club 753 View Street Victoria, BC V8W 1J9 https://hermannsjazz.com/show/737557/view See less Victoria, British Columbia Tickets Find Tickets Hermann's Jazz Club 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C575" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3854957174726232/</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Monday 30 June 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 49 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Urban Kizomba with Aaron and Fernanda— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C576" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2576922459305643/</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 51 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 15th features Cedar Mathias as our facilitator/dj! Details for Sunday, June 15th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C577" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/939376108286434/</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Today at 17:00 ReLove Night Market Janine and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Tomorrow at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Tickets · CA$17.31 www.eventbrite.com/e/salsa-night-dance-city-tickets-1415720962509 Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Tickets Find Tickets Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 18 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Ali and Jon 27 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 128 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C578" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1238334523949776/</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Sunday from 11:00-12:30 Dance Temple w/ Alex King-Harris (aka Rara Avis) Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Alex King-Harris (aka Rara Avis) Interested Going Invite Details 66 people responded Event by Dance Temple Victoria , Alex King-Harris and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 29th features Alex King-Harris (aka Rara Avis) as our facilitator/dj. He is back in town for the summer! Details for Sunday, June 29th: Facilitation and music set by Alex King-Harris (Rara Avis) Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C579" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1904863453602318/</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 19:00-22:00 Private Dance Saanichton, BC About Discussion More About Discussion Private Dance Details 8 people responded Event by HAMMERdown - Victoria, BC Saanichton, BC Duration: 3 hr Public · Anyone on or off Facebook We are excited for our gig on May 31 at Saanichton Bay. It is a private event. There will be good rocking tonight. Victoria, British Columbia Saanichton, BC Saanich Guests See All</t>
+        </is>
+      </c>
+      <c r="C580" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/624858640069610/</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Today at 17:00 ReLove Night Market Janine and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 Friday 22 August 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 128 people interested Interested Sun, 20 Jul at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Lorne, Roy and 2 friends 60 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C581" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/909522138040202/</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Today from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Today at 17:00 ReLove Night Market Janine and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Friday 28 November 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 128 people interested Interested Sun, 20 Jul at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Lorne, Roy and 2 friends 60 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C582" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1185783966345055/</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 10:00-13:00 Shuffle Dance Workshop Victoria, BC About Discussion More About Discussion Shuffle Dance Workshop Details 12 people responded Event by Adelène Buchanan Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another SHUFFLE WORKSHOP coming your way!! Join our Shuffle Dance Workshop and learn a full shuffle choreography set to an energetic electronic track. We’ll guide you through each step, focusing on key shuffle movements, while incorporating them into a dynamic routine. Perfect for ALL LEVELS! This workshop will help you improve your footwork, coordination, and cardiovascular stamina as you master a complete choreography. Here’s what you need to know: DATE: Sunday, May 25th TIME: 10am - 1pm PLACE: The Beat Clinic (1303 Broad Street) Sign-up link here https://www.thebeatclinic.ca/ See less Victoria, British Columbia Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C583" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/734261429120710/</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Friday 6 June 2025 from 19:30-22:30 Dance City 108 Niagara St, Victoria, BC V8V 1E9, Canada About Discussion More About Discussion Dance City Details 9 people responded Event by Andrew Sanderson 108 Niagara St, Victoria, BC V8V 1E9, Canada Duration: 3 hr Public · Anyone on or off Facebook Beginner Cha Cha workshop with Jane and Andrew at 7:30pm Multi genres dance including Standard, Latin,  West Coast Swing, and more starting at 8:30pm dj Andrew Sanderson Cash Admission: $12/$10 Members See less Victoria, British Columbia 108 Niagara St, Victoria, BC V8V 1E9, Canada 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C584" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/556816543734629/</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Monday 7 July 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 46 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Merengue with Sebastian and Hannah— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C585" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/650657144184821/</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Saturday 19 July 2025 from 21:00-02:00 COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY The Coda About Discussion More About Discussion COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY Interested Going Invite Details 64 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 5 hr Public · Anyone on or off Facebook Colombian Summer Rumba: “Tierra Querida” Party Saturday, July 19th Doors: 9:00 PM | Show: 9:30 PM 19+ | ID Required Celebrate Colombian Independence Day with us with the vibrant “Tierra Querida” Party — an amazing night of live music, dance, culture, and pure rumba energy! Start the night with a live tribute to Colombian music by the talented Daniel Sar &amp; Sofia Leonne. Their performance will honor legendary Colombian artists such as Juanes, Maluma, Fonseca, Rodolfo Aicardi, Herencia de Timbiquí, Mon Laferte, and more—blending pop, tropical rhythms, and heartfelt Latin ballads into a powerful musical journey. At 10:30 PM, DJ Miro, straight from Cali, Colombia, will take over with a fiery mix of Colombian beats. Later, resident DJ Alex King will close out the night, turning up the heat with Latin hits and ending strong with the latest reggaetón summer vibes. At midnight, enjoy a special folkloric performance by Danza Colombia, followed by a unifying moment as we wave our flag souvenirs and sing the national anthem together. Savor delicious cocktails, soak in vibrant downtown vibes, and enjoy a night filled with alegría, culture, and  Colombian vibes! Get your tickets NOW! First-tier: $20 | Second-tier: $25 Limited tickets available at the door for $27 - Act fast before they are sold out! Party ends at 2:00 AM Each ticket includes a Colombian flag souvenir. Take a piece of the celebration home with you! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C586" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1132427048350776/</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com or 15$ cash/e-transfer at the door. Formed in the heart of Chinatown, Rosebuds is a dynamic ensemble that brings the vibrant sounds of jazz, blues &amp; swing to life.  The group plays a mixture of originals and jazz standards, and is influenced by artists like Louis Armstrong, Billie Holiday, Lester Young, and Lionel Hampton. Featuring Rebecca Wells (vocals/guitar), Alex Moore (guitar/keys) Bryden Amos (guitar/keys), Matisse Gubby-Hurtig (bass), Owen Chow (trumpet), and Andrew Greenwood (tenor saxophone). Samba e Sol is a newly formed Brazilian bossa nova jazz trio featuring Andrew Greenwood (flute), Alex Moore (guitar), and Matisse Gubby-Hurtig (bass), playing music by artists like Antonio Carlos Jobim, Marcos Valle, Luiz Bonfa, and more. Instagram: https://www.instagram.com/rosebudsband/ See less Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C587" s="3" t="n">
+        <v>45834.93029778935</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/947213690692385/</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C588" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1029869435768837/</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Saturday 22 March 2025 at 20:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC This event has been cancelled. You cannot share this event, but you can still post. About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 14 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C589" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2637194793152555/</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 128 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 29, 2025 | Lesson:  Intro to Salsa Rueda with Sam and Katie Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa Rueda • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C590" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1060779176049104/</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Thursday 3 October 2024 from 19:30-22:30 Kizomba Practica Thursdays: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Kizomba Practica Thursdays: Fall Series Details 20 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Join us every Thursday for Kizomba/Urbankiz classes. Intermediate 7:30PM-8:15pm Beginner 8:15pm-9:00pm Practica until 10:30pm Class only: $10 Class &amp; Practica: $15 or $10 for university students w/ID Practice only $10 Classes will be provided by your local Instructor (David Lamine) and assistants (Robyn, Becky) and occasionally by some out of town and International Instructors. Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C591" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/960236445839425/</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Saturday 22 June 2024 from 18:00-21:00 Kizomba/UrbanKiz at Clover Clover Pt, Victoria, BC V8S, Canada About Discussion More About Discussion Kizomba/UrbanKiz at Clover Interested Details 56 people responded Event by Becky Mowat Clover Pt, Victoria, BC V8S, Canada Duration: 3 hr Public · Anyone on or off Facebook Come join us for our first time dancing at Clover Point! There will be no lesson beforehand and this is super casual. Just a bunch of friends hanging out and dancing. Bring snacks, something to drink, blankets, warm clothes (as it is typically cooler by the ocean). There isn't a lot of parking at Clover Point but you can park along Dallas Rd and just walk down. Feel free to invite friends and family. Hope to see you all there! See less Victoria, British Columbia Clover Pt, Victoria, BC V8S, Canada 1301 Clover Pt, Victoria, BC V8S, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C592" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1743571267040445/</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Ali Jorgensen invited you About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Details 55 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 8, 2025 | Lesson: Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C593" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1337760257449745/</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 6 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 10, 2025 | Lesson:   Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C594" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1459643825205914/</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Saturday from 10:00-12:00 KIZOMBA NA RUA – AfriCa Fest Victoria 2025 Centennial Square About Discussion More About Discussion KIZOMBA NA RUA – AfriCa Fest Victoria 2025 Interested Going Invite Details 9 people responded Event by African Arts &amp; Cultural Society - Centre Issamba Centre and Pulchérie N. Mboussi Centennial Square Duration: 2 hr Public · Anyone on or off Facebook KIZOMBA NA RUA – AfriCa Fest Victoria 2025 Date: Saturday, June 28, 2025 Time: 10:00 AM – 12:00 PM Location: Centennial Square, Victoria, BC Free &amp; open to the public! We’re inviting all Kizomba dancers to join us for a special Kizomba Na Rua moment at AfriCa Fest Victoria 2025! Dance under the morning sun and feel the rhythm of Afro-Lusophone vibes in the city's heart. This open-air morning dance club moment is for dancers of all levels — whether you're dancing or just enjoying the vibe, the energy will be electric! Let’s connect, move, and celebrate community, culture, and rhythm together. Don’t forget to bring your smiles and dancing shoes — it's going to be unforgettable! #KizombaNaRua #AfriCaFest2025 #DanceInTheSquare #VictoriaBC #AfroLusophoneVibes #AfriCaFestVictoria See less Dance Victoria, British Columbia Centennial Square 10 Centennial Sq, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C595" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1794066937801722/</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Saturday 8 March 2025 from 20:30-23:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 26 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C596" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3006474846197996/</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 45 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 27, 2025 | Lesson:  Intro class TBD Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro class TBD • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C597" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1179097320623502/</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 37 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C598" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1079226067560481/</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 57 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 6, 2025 | Lesson:  Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C599" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1293301738436581/</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Sunday 6 April 2025 at 17:00 Kizomba Sundown Party: Free of charge Method Studio - Victoria BC David Lamine Victoria invited you About Discussion More About Discussion Kizomba Sundown Party: Free of charge Details 58 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Method Studio - Victoria BC Public · Anyone on or off Facebook Free Pre-VIKFest party. Bring snack and drink. Expect great music, great energy, great atmosphere. "Dance with your heart. your feet will follow" Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C600" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1861230087752141/</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 6 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 31, 2025 | Lesson:  Intro to Salsa with Adam &amp; Alicia Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C601" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1334757257408713/</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Saturday 25 January 2025 from 19:00-23:30 Special Edition Urbankiz Workshop w/ Kenny Odumosu Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Special Edition Urbankiz Workshop w/ Kenny Odumosu Details 50 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 hr 30 min Public · Anyone on or off Facebook SPECIAL EDITION WORKSHOP Join us Saturday January 25th for a 2hr Urbankiz workshop. Joining us from Calgary to share his knowledge and love for Urbankiz. Kenny finished first for the Kizomba/Semba category at the North American Olympiads. With his background in Kizomba/Semba Kenny will help you incorporate techniques and smoothness into your Urbankiz. We are really looking forward to having him here! Schedule 7:00pm-9:00pm (workshop) 9:00pm-11:30pm (social) Price: $40 (includes workshop &amp; social dance) e-transfer to:  becksmith@hotmail.com please include the name you go by if different from your e-transfer account. Thanks See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C602" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1184791909680061/</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Thursday 13 March 2025 from 19:30-23:00 Urban Kiz Workshop with Mannie Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 50 people responded Event by Becky Mowat and David Lamine Victoria Ukrainian Cultural Centre Duration: 3 hr 30 min Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C603" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3185065321631809/</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Saturday 15 March 2025 from 20:00-00:00 Urban Kiz Workshop with Mannie Method Studio - Victoria BC Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 48 people responded Event by Becky Mowat and David Lamine Victoria Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C604" s="3" t="n">
+        <v>45834.93730209005</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1152065639712042/</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 20 20 Feb at 19:30 – 23 Feb at 23:00 Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Details 49 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 days Public · Anyone on or off Facebook Join us for our special edition Urbankiz &amp; Tarraxo workshops with Mike Ahombi Mike has been a big supporter of our VIKF and bringing his talent and low key vibe to the west coast. He is based out of Ottawa but you will find him at many different festivals and cities teaching Kizomba, Urbakiz and Tarraxo. We cannot wait for you all to have the opportunity to learn from such an incredible person and instructor. Details: Feb 20th Urbankiz Workshop 7:30pm-9:30pm Practica 9:30pm-11:00pm Feb 22nd Tarraxo Workshop 8:00pm-10:00pm Practica 10:00-11:30pm Price $90 Workshops only $70 Practica only $20 *** please e transfer to becksmith@hotmail.com *** Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C605" s="3" t="n">
+        <v>45834.93730209005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug in fb.py. Somehow db.write_url was being set as a variable. I must have done a replace all and ended up with problem.
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C605"/>
+  <dimension ref="A1:C804"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9274,7 +9274,7 @@
         </is>
       </c>
       <c r="C588" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="589">
@@ -9289,7 +9289,7 @@
         </is>
       </c>
       <c r="C589" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="590">
@@ -9304,7 +9304,7 @@
         </is>
       </c>
       <c r="C590" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="591">
@@ -9319,7 +9319,7 @@
         </is>
       </c>
       <c r="C591" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="592">
@@ -9334,7 +9334,7 @@
         </is>
       </c>
       <c r="C592" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="593">
@@ -9349,7 +9349,7 @@
         </is>
       </c>
       <c r="C593" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="594">
@@ -9364,7 +9364,7 @@
         </is>
       </c>
       <c r="C594" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="595">
@@ -9379,7 +9379,7 @@
         </is>
       </c>
       <c r="C595" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="596">
@@ -9394,7 +9394,7 @@
         </is>
       </c>
       <c r="C596" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="597">
@@ -9409,7 +9409,7 @@
         </is>
       </c>
       <c r="C597" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="598">
@@ -9424,7 +9424,7 @@
         </is>
       </c>
       <c r="C598" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="599">
@@ -9439,7 +9439,7 @@
         </is>
       </c>
       <c r="C599" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="600">
@@ -9454,7 +9454,7 @@
         </is>
       </c>
       <c r="C600" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="601">
@@ -9469,7 +9469,7 @@
         </is>
       </c>
       <c r="C601" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="602">
@@ -9484,7 +9484,7 @@
         </is>
       </c>
       <c r="C602" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="603">
@@ -9499,7 +9499,7 @@
         </is>
       </c>
       <c r="C603" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="604">
@@ -9514,7 +9514,7 @@
         </is>
       </c>
       <c r="C604" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
       </c>
     </row>
     <row r="605">
@@ -9529,7 +9529,2992 @@
         </is>
       </c>
       <c r="C605" s="3" t="n">
-        <v>45834.93730209005</v>
+        <v>45834.93730209491</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1300938064467261/</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Thursday 20 March 2025 from 20:00-22:00 Intermediate Sensual Bachata Workshop Method Studio - Victoria BC About Discussion More About Discussion Intermediate Sensual Bachata Workshop Details 24 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 2 hr Public · Anyone on or off Facebook Sensual Bachata Workshop in March! Intermediate workshop - March 20 Time: 8:00-9:30 PM + Practice 9:30-10:00 PM Location: Method Studio, 841 Fisgard St. Cost: $30 per workshop (includes 2 hours!) Intermediate workshop: Take your skills to a higher level! Master the advanced variations of the Madrid pass, smooth transitions and musicality. No partner needed, just bring your energy and comfortable shoes! Register at: maximumotion@gmail.com #BachataWorkshop #VictoriaBC #LearnToDance #BachataLovers See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C606" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/717475250956404/</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Friday 30 May 2025 at 18:00 FREE Beginner Bachata Class 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 About Discussion More About Discussion FREE Beginner Bachata Class Details 65 people responded Event by Mayfair Shopping Centre and Victoria Latin Dance Association 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 Public · Anyone on or off Facebook Ready to get your groove on? We’re teaming up with the Victoria Latin Dance Association  for a FREE Beginner Bachata Class right here at Centre Court! Join us on Friday, May 30 at 6:00 PM for an evening of fun and dancing. FREE Beginner Bachata Class May 30th, Friday at 6PM NO partner or experience necessary! Bachata is a beautiful and easy-to-learn dance that’s great for meeting new people, getting active, and connecting with an amazing community. See less Dance Victoria, British Columbia 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 3147 Douglas St, Victoria, BC V8Z 3K3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C607" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/729183856154450/</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Tomorrow from 20:00-00:00 Bachata Night Method Studio - Victoria BC About Discussion More About Discussion Bachata Night Interested Going Invite Details 28 people responded Event by Bachata Nights Victoria BC and Alysha Kopala Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights June 27 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance @yourgirlalysha  and @davidch_78 will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C608" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1730246844256904/</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre About Discussion More About Discussion Saturday Salsa/Bachata Social June 28th Interested Going Invite Details 44 people responded Event by Latin Dance Canada Ukrainian Cultural Centre Duration: 3 hr 59 min Public · Anyone on or off Facebook Saturday Salsa/Bachata Social June 28th 3277 Douglas st, Victoria BC Cost? $15 CASH ONLY PLEASE! When? Saturday, June 28th 8:00 pm - 8:30 pm beginner dance lesson 8:30 pm - 12 am Social dancing What? We will be playing a mix of salsa, bachata and more. Where? Ukrainian Cultural Centre 3277 Douglas Street, Victoria See less Dance Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C609" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/601131956358678/</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Thursday 3 July 2025 at 20:00 Bachata &amp; Merengue- All Levels- July Series Studio 4 Athletics About Discussion More About Discussion Bachata &amp; Merengue- All Levels- July Series Interested Going Invite Details 2 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Bachata &amp; Merengue are both dances from the Dominican Republic. Bachata can be anywhere from slow and romantic with lots of dips, sway and body movement to more upbeat and percussive with lots of musical footwork. Merengue is carefree, flirtatious and fun! Classes are registered on a monthly basis and take place every Thursday from 8:00- 9:00pm, July 3,10,17,24,31 No experience required.  No partner is necessary as we rotate partners throughout the lesson.  Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot!d See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C610" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1813229489279716/</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Thursday 29 May 2025 from 19:55-21:00 Sensual Bachata 4 Week Series Method Studio - Victoria BC Thu, 15 May Thu, 22 May Thu, 29 May +1 About Discussion More About Discussion Sensual Bachata 4 Week Series Details 6 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 1 hr 5 min Public · Anyone on or off Facebook Ready to level up your Sensual Bachata? May 8, 15, 22, 29 Method Studio | 7:55–9:00 PM | $80 for all 4 classes Join us for an exciting and dynamic Bachata Sensual class designed for experienced beginners and intermediate dancers! We’re blending solid fundamentals with fresh, fun, and sensual combos to help you grow, challenge yourself, and have an amazing time on the dance floor. No partner needed — just bring yourself and your love for dance! Spots are limited — don’t miss out! Register by e-transferring $80 to maximumotion@gmail.com and mentioning “Bachata Sensual” in the notes. Get ready to connect, move, and elevate your dancing! P.S. All fees are non-refundable as they go directly toward securing the studio space and running the class. See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C611" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1057471579628015/</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Friday 16 May 2025 at 17:00 Bachata Nights Victoria Bc Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Victoria Bc Details 9 people responded Event by Bachata Nights Victoria BC and Sebastian Carmona Method Studio - Victoria BC Public · Anyone on or off Facebook Join us on our next Bachata Nights May 23 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C612" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1350929566137538/</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 7 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation August 10, 2025 | Lesson: Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C613" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1388695712154512/</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Ali Jorgensen invited you About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Details 121 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation June 22, 2025 | Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C614" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/9677364319006080/</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 60 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation July 20, 2025 | Lesson:  Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C615" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3975145332748137/</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Friday 13 June 2025 from 20:00-00:00 Bachata Night Method Studio - Victoria BC About Discussion More About Discussion Bachata Night Details 77 people responded Event by Bachata Nights Victoria BC , Sebastian Carmona and Alysha Kopala Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights June 13 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C616" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1901245437276872/</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Friday 9 May 2025 from 20:00-00:00 Bachata Nights Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Details 40 people responded Event by Bachata Nights Victoria BC , Alysha Kopala and Sebastian Carmona Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights May 09 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @yourgirlalysha  and @davidch_78  will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person The evening starts with an Open-level Bachata lesson from 8:15 PM to 9:00 PM—great for all skill levels! Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C617" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342792743590871/</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Monday 7 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- April series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, April 7, 14, 28. Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C618" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/966455485665576/</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Thursday 3 April 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- April series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Apr 1, 8, 15, 22, 29 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C619" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/679241811720932/</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Fundamentals- May Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- May Series Details 7 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, May 6, 13, 20, 27 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C620" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1382188962971661/</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Tuesday 1 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Fundamentals- April Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- April Series Details 9 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, Apr 1, 8, 15, 22, 29 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C621" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/745466751313624/</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Tuesday 8 July 2025 at 20:00 Salsa &amp; Cha Cha Cha- Fundamentals- July Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- July Series Interested Going Invite Details 4 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, July 8,15,22,29 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C622" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/669591372187091/</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 10:00-11:00 Salsa &amp; ChaCha Solo Westshore Dance Studios Sat, 17 May Sat, 24 May Sat, 31 May +7 About Discussion More About Discussion Salsa &amp; ChaCha Solo Details 2 people responded Event by Dance Praktika Westshore Dance Studios Duration: 1 hr Public · Anyone on or off Facebook Elevate your dance journey with our Ladies Solo Class. Join our exciting series and learn the basics of Salsa and Cha Cha. Perfect for beginners looking to spice up their dance skills! Class Highlights: - Learn exciting dance moves tailored for solo dancers; - Fun and welcoming environment; - Suitable for absolute beginners. Come dance with us and let the rhythm guide you! To register to April classes please use links at "Tickets". See less Langford, British Columbia Westshore Dance Studios 109-2675 Wilfert Road, Victoria www.westshoredance.com 2years+ Competitive&amp;Production a space for everyone with a love of dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C623" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/10048344358532607/</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- May series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. May 6, 13, 20, 27 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C624" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2579272439096564/</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Tuesday 8 July 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- July series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- July series Interested Going Invite Details 4 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. July 8,15,22,29 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C625" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2214494908966327/</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Monday 5 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Int/ Adv- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- May series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, May 5, 12, 26 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C626" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/727053470038104/</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Monday 7 July 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ July series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ July series Interested Going Invite Details 4 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, July 7,14,21,28 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C627" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342233713680795/</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Thursday 1 May 2025 at 21:00 Bachata &amp; Merengue- All Levels- May Series Studio 4 Athletics About Discussion More About Discussion Bachata &amp; Merengue- All Levels- May Series Details 3 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Bachata &amp; Merengue are both dances from the Dominican Republic. Bachata can be anywhere from slow and romantic with lots of dips, sway and body movement to more upbeat and percussive with lots of musical footwork. Merengue is carefree, flirtatious and fun! Classes are registered on a monthly basis and take place every Thursday from 8:00- 9:00pm, May 1, 8, 15, 22, 29. No experience required.  No partner is necessary as we rotate partners throughout the lesson.  Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C628" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3899920353641309/</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Today at 17:00 ReLove Night Market Janine and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 9 Saturday 9 August 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in July. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Fri, 11 Jul at 21:00 Locarno at The Coda The Coda Nadia is interested 43 people interested Interested Sat, 5 Jul at 19:00 Josh Warren Presents: The Path (LIVE @ Hermann's!) Hermann's Jazz Club 23 people interested Interested Mon, 30 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Ali and Almeda 49 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C629" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1636237610432412/</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Saturday 16 August 2025 from 20:00-23:59 Salsa Sunset Latin Party – August 16th! Latin Dance Canada About Discussion More About Discussion 🌅🔥 Salsa Sunset Latin Party – August 16th! 🔥🌅 Interested Going Invite Details 29 people responded Event by Latin Dance Canada Latin Dance Canada Duration: 3 hr 59 min Public · Anyone on or off Facebook Salsa Sunset Latin Party – August 16th! Get ready for a magical summer night filled with Latin rhythms, sunset vibes, and non-stop dancing! Join us for the Salsa Sunset Latin Party, where the Salsa, Bachata, and Merengue beats will keep you moving all night long under the stunning sunset sky! Dress Code: Wear your best sunset-inspired outfit – think bright, tropical colors, and beach party vibes! Dance to the best Salsa, Bachata, Merengue &amp; Latin hits all night! No partner? No problem! Join our fun intro class at 8:00 PM! Location: Ukrainian Cultural Centre, 3277 Douglas St., Victoria, BC Date: Saturday, August 16, 2025 Intro Class: 8:00 PM | Social Dance: 8:30 PM - Late Entry: $15 at the door – Bring cash, please! What to Expect: Vibrant salsa rhythms &amp; tropical vibes! Tropical-themed decorations &amp; stunning sunset views! A welcoming dance community &amp; unforgettable fun! Let’s dance as the sun sets and make it a night to remember! Tag your friends and let’s create memories under the summer sky! #SalsaSunsetLatinParty #SalsaBachata #LatinDanceParty #VictoriaBC #LatinDanceCanada See less Dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C630" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2251848171850840/</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Today at 17:00 ReLove Night Market Janine and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 Saturday 10 May 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in April. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Fri, 11 Jul at 21:00 Locarno at The Coda The Coda Nadia is interested 43 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1498 people interested Interested Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested 28 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C631" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1479111682798589/</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Today at 17:00 ReLove Night Market Janine and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 13 Saturday 13 September 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in August. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1498 people interested Interested Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested 28 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C632" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1618420955545842/</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Today at 17:00 ReLove Night Market Janine and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 30 Friday 30 May 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing at an all ages venue with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 4 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Ali 13 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested Sun, 17 Aug at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Ali is going 2 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C633" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1059622278965884/</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Today at 17:00 ReLove Night Market Janine and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 8 Saturday 8 November 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in October. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1498 people interested Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends 184 people interested Interested Sat, 18 Oct at 20:00 ✨ White and Gold Latin Night – October 18th! ✨ Latin Dance Canada Carmie is interested 33 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C634" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/884101187183426/</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Today at 17:00 ReLove Night Market Janine and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 July 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Tickets · CA$17.31 www.eventbrite.com/e/caliente-salsa-saturdays-tickets-1415724884239 Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in June. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Tickets Find Tickets Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 5 Jul at 19:00 Josh Warren Presents: The Path (LIVE @ Hermann's!) Hermann's Jazz Club 23 people interested Interested Happening now Marquis Hill Jazz Fest 2025 Wicket Hall 919 Douglas Street, Victoria, BC, Canada 31 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1498 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested This Sunday at 11:00 BC CRABFEST - Serving an Authentic BC CrabBoil Ship Point, Wharf St, Victoria, British Columbia Roy, Debi and 4 friends are interested Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C635" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1106484714432492/</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Wednesday 2 July 2025 from 18:30-21:00 Zouk practica and social White Eagle Hall, 90 Dock St, Victoria BC Wed, 4 Jun Wed, 25 Jun Wed, 2 Jul Wed, 9 Jul +40 About Discussion More About Discussion Zouk practica and social Interested Going Invite Details 1 person responded Event by Victoria Zouk Collective and Victoria Zouk Collective Group White Eagle Hall, 90 Dock St, Victoria BC Duration: 2 hr 30 min Public · Anyone on or off Facebook Drop-in zouk practica by donation - everyone welcome! White Eagle Polish Hall every Wednesday 6:30-9 pm Shared warm up, free dance time, review material from lessons and congresses, connect and share knowledge! Help is always available. Minimum $5 donation. Cash at the door, or etransfer to oceanzouk@gmail.com Enter the lower hall by the side door on Niagara Street just beside the Polka food truck. Also available in Victoria are zouk lessons with Javi, an amazing instructor from Vancouver! More info at https://www.facebook.com/Sabor.Asi.Dance.Salsa.Victoria or email danceinflow@gmail.com See you there! See less Victoria, British Columbia White Eagle Hall, 90 Dock St, Victoria BC 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C636" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1411005319893067/</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Monday 28 April 2025 from 18:30-22:30 Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion 🔥Bachata &amp; Brazilian Zouk 🌊 dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard Details 7 people responded Event by Bachata and Zouk with Javi in Victoria 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 4 hr Public · Anyone on or off Facebook Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard street | Victoria Join us for a 4 week course exploring the joy and magic of Brazilian Zouk &amp; Bachata dancing! Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on enhancing body awareness, building confidence in dance vocabulary with lead and follow techniques, exploring musicality, and loving yourself deeper with styling! Be prepared to have lots of fun dancing with new friends! Register today! Schedule: Monday April 7 - 28th 6:30-7:25pm | Brazilian Zouk - Level 2 (ask Javi for permission) 7:30-8:25pm | Brazilian Zouk - Level 1 8:30-9:25pm | Sensual Bachata - Beginner Foundations 9:30-10:30pm | Sensual Bachata - Intermediate "Trending Moves" Tuition: $20 | 1 Class $35 | 2 Classes (Brazilian Zouk 1&amp;2, or Brazilian Zouk 1 &amp; Bachata, Bachata 1&amp;2) $50| 3 Classes (3 classes, BEST value) 1709 Blanshard St, Victoria, BC Registration: E-transfer to: danceinflow@gmail.com or send us a message on Whatsapp: 7785877665 (Also accepting credit card/cash at the door) Please add a note if you're registering as a "Leader", "Follower", or "Open to both" Space is limited. Register in advance to reserve your spot! Looking fwd to dancing and flowing with you, Warmly, Javi See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C637" s="3" t="n">
+        <v>45834.94694195602</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/544121845403419/</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 13:00-23:55 Swing Session: Balboa with Yoshi and Etsuko Solwood Studio About Discussion More About Discussion Swing Session: Balboa with Yoshi and Etsuko Details 108 people responded Event by Swing Dance Association of Victoria , Dave Henderson and 2 others Solwood Studio Duration: 10 hr 55 min Public · Anyone on or off Facebook Lace up your shoes on May 31, 2025 for an afternoon of Balboa Classes and an evening of Social Dancing with Yoshi and Etsuko Uemura. 4 Classes for everyone &amp; 1 Social Dance! Passes go on sale April 19 at noon at our SDAV Square Shop! You must know and be comfortable with Balboa basics for all of these classes - they won't be covered at this workshop. All the specifics are available at swingvictoria.net , but here are the notes: May 31st, at Solwood Studio, with doors at 12:30pm . Bring indoor shoes, please! 4 classes for everyone and there's a dance from 9-12am. Passes go on sale April 19th at noon. See less Victoria, British Columbia Solwood Studio 1303 Broad St, Victoria, BC V8W 2A8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C638" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1786895135557126/</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Monday 26 May 2025 at 19:00 The Jive Big Band and The Blue Bosses Hermann's Jazz Club About Discussion More About Discussion The Jive Big Band and The Blue Bosses Details 9 people responded Event by The Jive Big Band Hermann's Jazz Club Public · Anyone on or off Facebook Join the Jive Big Band for a fun night of music featuring big band classics, rock, funk, and the unexpected. Directed by Nick La Riviere, this band is always a good time! Joining them is the fantastic Blue Bosses jazz combo directed by Ashley Wey. Entry by donation to Arts on View, keeping music at Hermann’s alive and strong! See less Victoria, British Columbia Hermann's Jazz Club 753 View Street, Victoria Hermann's Jazz Club is the best place to visit for live jazz and blues in Victoria, BC. On July 15, Guests See All</t>
+        </is>
+      </c>
+      <c r="C639" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/634773653668605/</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Saturday Night West Coast Swing BC Swing Dance Club Victoria 15 Jun 2019 22 Jun 2019 29 Jun 2019 +2 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night West Coast Swing Details 9 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook June means summertime and sunny days! Along with the weather, things for BC Swing Dance Cub Victoria will be changing too. Here's what is happening this month: 7 - 8pm 1st Saturday of the Month: Lesson with Meaghan, plus an assistant from our dance community 7 - 8pm Remaining Saturdays each month: TBD (stay tuned for workshops, activities or practices - updates will be posted on each event page) Note:  The 7 - 8pm weekly timeslot is included in the dance entrance price. -------------------------------------------------- Come join us every Saturday all year long for a fabulous WCS social dance from 8 - 11pm. Just $10 for the ($5 for students). Meaghan Efford and Bob Gebbie 's lesson on June 1st (starting PROMPTLY at 7pm) will be the only lesson in June, and it will be a great way to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity.  The lesson is included in the dance entrance price.  No experience or partner is required. -------------------------------------------------- • 6:45 pm - Doors open • 7:00 pm - TBD each week* • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *lesson with Meaghan and Bob on June 1st Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C640" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/417338985546213/</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Thursday 29 August 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - August 29! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - August 29! Details 109 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for a fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C641" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1776457206589544/</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Friday 21 March 2025 from 18:30-20:30 Slim Sandy's Atomic Cocktails swing speakeasy party! The Coda About Discussion More About Discussion Slim Sandy's Atomic Cocktails swing speakeasy party! Details 72 people responded Event by Peter Sandmark and Trace Nelson The Coda Duration: 2 hr Public · Anyone on or off Facebook Join Slim Sandy's Atomic Cocktails and dance as they play 2 sets of swing jazz, jive and rhythm and blues from the 20’s to the 40’s. Slim, on guitar and harmonica, is joined by Willa Mae on vocals, “Big Daddy Bo” on bass, and Bryn Bad on trumpet.  Slim Sandy has been playing music for over 40 years with acts such as Ray Condo and the Crazy Rhythm Daddies.  In 2012, he and Willa Mae co-created the Slim Sandy band in Victoria!  They have played music festivals in Canada, France, Spain, Germany, Belgium, and the Netherlands.  In May they will be touring in Japan! See less Victoria, British Columbia The Coda 749 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C642" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1594011994641933/</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Tuesday 22 April 2025 from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Details 9 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. No street shoes. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C643" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/402729737034904/</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Thursday 5 September 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Details 123 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for our second fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C644" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663135653237580/</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Method Studio - Victoria BC Canice Ma invited you About Discussion More About Discussion WACK! Another West Coast Swing Social Dance Details 40 people responded Event by Canice Ma and Wyatt Ritchie Method Studio - Victoria BC Duration: 3 hr 30 min Public · Anyone on or off Facebook Guess who's back, it's WACK! (please ignore the fact that it's been 2 years...) The schmucks are back with another spontaneous west coast swing social dance, featuring music by DJs Topknot and Amandance from Vancouver! DETAILS: • Friday, June 20th, 2025 • Method Studio, 841 Fisgard St, Victoria, BC • 7:30-8:30 pm: "Shake That" line dance lesson featuring Kaitlyn • 8:30-11 pm: social dancing with 100% west coast swing • Admission: $10 • Water and AC on us (and maybe some bonus chocolate) • Please keep in mind that parking is limited at the venue GENERAL SOCIAL DANCE ETIQUETTE: • Consent is cool- don't be creepy. • Shake off any shyness and get out there! Ask people to dance regardless if you’re a lead or follow, dancing for 10 years or started yesterday- it's more fun that way! • No teaching or unsolicited feedback on the dance floor. Good vibes only! • If you would like to partake in a steal dance, try to remain with that group for the whole song. • Bring a water bottle! The studio is known to get warm with more bodies in the space so we want you to stay healthy and hydrated. • Personal hygiene is important! Consider bringing a towel and/or a spare shirt to change into if you sweat easily. Our studio has a bathroom and change rooms available for all to use. • We recommend wearing clothes that are easy to move in, especially pants given the nature of the dance. • Clean, comfortable shoes (ideally dance shoes) on the dance floor only! See less Victoria, British Columbia Method Studio - Victoria BC 833 Fisgard St, Victoria, BC V8W 1R9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C645" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1035925295253912/</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Friday 18 April 2025 at 18:30 Swing out with the ATOMIC COCKTAILS 751 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Swing out with the ATOMIC COCKTAILS Details 64 people responded Event by Peter Sandmark 751 View St, Victoria, BC V8W 1J9, Canada Public · Anyone on or off Facebook Join the ATOMIC COCKTAILS as they swing out for their pre-Japan Tour dance party on April 18 at the Coda, 751 View Street.  Doors open 6 pn, show from 6:30-8:30 pm!  Tickets $20.  With songs from their new album BLUE LIGHT BOOGIE! See less Victoria, British Columbia 751 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C646" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663756533046485/</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Friday 11 April 2025 at 21:30 Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. Details 36 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Public · Anyone on or off Facebook Miguelito Valdes presents Contodo What happens when you bring together three Cuban and two Canadian musicians, with a deep love of all music and a wide range of musical experiences?  A joyful mix of party and deep groove, that's what! Guaranteed to make you want to dance, these brothers from other mothers bring it all. Con Todo! Featuring: Miguelito Valdes – brass/vocals/percussion Jose Sanchez – drumset/timbales Hector Ramos – congas/percussion Peter Dowse - bass Brooke Maxwell – keys/vocals See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C647" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2441697862726705/</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Sunday 30 June 2019 at 19:00 Journey’s 50th Birthday!!  A West Coast Swing dance party!! Eastern Star Hall Chapters No 5 &amp; No 17 Journeey Song invited you About Discussion More About Discussion Journey’s 50th Birthday!!  A West Coast Swing dance party!! Details 13 people responded Event by Journeey Song Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook 3281 Harriet Road, Victoria,BC Bring your own alcohol-free beverage... Bring a gluten-free appie if you’d like. Dance West Coast Swing until 10 pm to Blues, Pop, RnB, Swing, and a wee bit of Ballroom Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C648" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/302778660295534/</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Sunday 19 August 2018 from 18:00-21:00 West Coast Swing in the Park! Cameron Bandshell @ Beacon Hill Park Carolyn Gebbie invited you About Discussion More About Discussion West Coast Swing in the Park! Details 58 people responded Event by Carolyn Gebbie Cameron Bandshell @ Beacon Hill Park Duration: 3 hr Public · Anyone on or off Facebook Come join us for another evening of fun and WCS dancing in Beacon Hill Park! WCS music will be provided by DJ Carolyn. For those who are familiar with the routine, the 2018 WCS Rally Song will be played at 6:30, 7:30 and 8:30pm. Sam Jackson and Meaghan Efford, from wcsmovementmethods.com will be on hand to answer questions about WCS or how to improve your WCS dancing. They will also demo some incredible WCS dancing at 7pm. Please invite your WCS dance friends by sharing this event! See less Victoria, British Columbia Cameron Bandshell @ Beacon Hill Park Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C649" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/373500473108499/</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Sunday Swing at Logan's Logan's Pub 10 Dec 2017 Debi Wong invited you About Discussion More About Discussion Sunday Swing at Logan's Details Event by Swing X Logan's Pub Duration: 3 hr 30 min Public · Anyone on or off Facebook Sunday Swing at Logan's is BACK! Come join us for some great tunes and we'll party like it's 1939. Bring your dancing shoes, sweet moves, and a few dollars for our fabulous DJ (and gracious bartenders). Feel free to come early to hang out and grab a bite to eat. 19+. NEW: Crash course 15min swing lesson at 8:30pm! This is intended to be the bare minimum for someone to show up and know the basics of swing dancing, nothing fancy! DETAILS: * 8:30pm Quickie 15min beginner lesson! * 8:45pm social dancing until as late as midnight (maybe!) * Usually gets bluesy after 11pm See less Victoria, British Columbia Logan's Pub 1821 Cook Street, Victoria Original - Authentic - Unique Guests See All</t>
+        </is>
+      </c>
+      <c r="C650" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/717783180949020/</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>FRIDAY ! Fort Tectoria About Discussion More About Discussion THIS FRIDAY 🌹🌹ROSEBUDS //swing band -&amp;- MISHA MANOUCHE //gypsy jazz @ Fort Techtoria THIS FRIDAY ! Interested Going Invite Details 29 people responded Event by Rebecca Rose , Bryden Amos and Alex Q Moore Fort Tectoria Public · Anyone on or off Facebook Bring your dancing shoes, we have a whole floor to boogie on this Friday!  We are taking it back to the 30's and 40's with a night of gypsy jazz, swing and blues for you. ROSEBUDS 8pm Victoria's hot new Swing Band, formed in the heart of China Town. Playing old time swing jazz classics and original tunes with bluesy grit.  Rebecca Wells//lead singer, Alex Quincy Moore &amp; Bryden Amos// guitar + keys, Andrew Greenwood//tenor sax, Owen Chow// trumpet, Matisse Gubby-Hurtig//upright bass. We invite you to rock the night away with us, swinging our way into summer. **MISHA MANOUCHE **7pm Kicking off the night, gypsy jazz duo Misha Manouche will be bringing us velvety melodies and the spirit of Django Reinhardt to the room. Adam Paquette &amp; Alex Gnaedinger// Guitar and vocals. Catch us Fort Techtoria this Friday! 777 Fort Street Victoria BC June 27th 6:30pm Doors open Buy Pre sale ticket at 15$ by e transfering rosebudsband@gmail.com Or 20$ tickets at door See you folks there See less Victoria, British Columbia Fort Tectoria 777 Fort Street, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C651" s="3" t="n">
+        <v>45834.95276986111</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/754259983939888/</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Sunday 20 July 2025 from 12:00-17:00 Anniversary Milonga Alive Tango Victoria About Discussion More About Discussion Anniversary Milonga Interested Going Invite Details 22 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 5 hr Public · Anyone on or off Facebook 10 years of Alive Tango in Victoria! 10 years of friendships, events and exploring the music, the movement, the possibilities. 10 years of mutual support in tango and life. So many people came and moved on  but everyone left something behind, built a small piece of Alive. So many of you came but stayed building, creating and shaping us. It takes a village and we all are part of it!!! Afternoon Anniversary Milonga ! Cake (made by Danusia!!)and bubbly ( we encourage you to bring your own water bottle or a cup .. we might run out of the ones in the studio ). Let us know if you can come 12pm-5pm $10 Two amazing DJs : Carol Horowitz ( Montreal) and Dan Boccia ( Anchorage) ( the artwork by Rasanga Weerasinghe) See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C652" s="3" t="n">
+        <v>45834.95611695602</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1864555154338100/</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 21 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Alive Tango Victoria About Discussion More About Discussion Weekend with Tango Details 18 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 21st 5pm-6pm solo technique all levels. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) We will continue from May with the musicality for phrase change but this time we will add “double time” to help us with it, using examples of different orchestras. We will work with a “rebound” and half giros to change the direction within the phrase. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 22nd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are September 20th &amp; 21st. Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C653" s="3" t="n">
+        <v>45834.95611695602</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1766891834185825/</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam and Alive Tango Victoria Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends SAVE THE DATE! The next Sunday afternoon Milonga is on 8 June 2025 1-4pm. The Coda Club (formerly Hermanns Upstairs) is a beautiful newly renovated venue with awesome ambience, nice wood floor and great sound system. Come join us for a wonderful afternoon of warm hugs and close embrace. Sunday 8June 2025 1-4pm The Coda, 751 View Street, Victoria Admission: $15 (plus tax) Special Guest DJ: Francis Nowaczynski (from Vancouver) Free parking at View Street Parkade (next door) or Broughton Parkade. Cash bar is open for drinks. See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C654" s="3" t="n">
+        <v>45834.95611695602</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3637725693193744/</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 22 Mar at 17:00 – 23 Mar at 13:30 Weekend with Tango with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Weekend with Tango with Jorge Olguín Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 22nd 5pm-6pm solo technique all levels. Balance and weight transfer while walking, change of dynamics to create a better connection with your body. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) Marathon is just around the corner so this month we continue with comfortable close embrace! We continue with dancing in small spaces!! Let’s move gracefully without affecting the partner's axis in elastic hugs of closed embrace. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 23rd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available only on Saturday. Sunday - sold out Next workshop dates are the May 17th &amp;18th Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C655" s="3" t="n">
+        <v>45834.95611695602</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1318668532737609/</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 16 16 Apr at 18:30 – 18 Apr at 21:00 Tango week with Lya Alive Tango Victoria About Discussion More About Discussion Tango week with Lya Details 36 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 3 days Public · Anyone on or off Facebook Ignite Your Tango 16th of April, Wednesday 6:30-8:00 On &amp; Off Acis for social dance 18th of April, Friday 6:00 - 7:30 Follower technique 7:45 - 9:00 Switch role / connection Search - Grow &amp; Transform! Seminar series for Tango Dancers that want to transform their way of moving and connecting! We will travel through the Essentials of Tango in order to look for new answers and deeper understanding. What makes tango truly captivating? It’s the embrace, the connection, and the walk. These three fundamental elements are the heartbeat of tango, and mastering them is essential for creating an unforgettable dance experience. You will learn how to condition your body to move with control, fluidity, and elegance. You’ll discover how to find and perfect your axis, which is essential for maintaining balance and stability in every step. We will also explore dissociation, a technique that allows you to move the upper and lower body independently but associated. This workshop series will show you how to apply these principles in both the leader and follower roles, improving connection and response in every moment of the dance. We will apply all this to: The secrets to generating power for boleos effortlessly off and on axis special follower technique class Pro tips to dance with ease and confidence 90 min class - $30 All 3 classes - $80 To register email grazs@shaw.ca or pm me, or talk to me . See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C656" s="3" t="n">
+        <v>45834.95611695602</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1009684807956058/</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 17 17 May at 17:00 – 18 May at 13:30 Tango weekend with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Tango weekend with Jorge Olguín Details 28 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 17th 5pm-6pm solo technique all levels. ( no partner required) Please bring elastic bands!! 6.30pm-7.30pm for couples only ( need some experience) Sacadas, barridas and colgadas in an elastic embrace in order to create a circular movement. We will work with different orchestras to study the changes we need to do to introduce different tempos and rhythms. Get ready for a workout with musicality! 8pm milonga !!! Join us even if you didn’t take the classes. DJ Ingrid !! Free for people registered for the workshops. $10 for drop-ins. Sunday, 18th 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are June 21st &amp; 22nd Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C657" s="3" t="n">
+        <v>45834.95611695602</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/516994561244886/</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:45 Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING White Eagle Polish Association About Discussion More About Discussion Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING Details 15 people responded Event by Donna Forsyth , Andre Russo and Victoria West Coast Swing Collective White Eagle Polish Association Public · Anyone on or off Facebook Doors open at 6:45pm at this fabulous new venue! Advanced beginner/intermediate lesson by Chantelle Pianetta from 7 to 8 pm Social dancing for 3 HOURS from 8 to 11 pm DJs Donna and Andre Cost $15 /$12 for students ALL at the spacious White Eagle Hall No need to register and you do not need a dance partner. Please bring scuff-free dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia White Eagle Polish Association 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C658" s="3" t="n">
+        <v>45834.95884658565</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/967438905456066/</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Wednesday 26 March 2025 at 10:00 Victoria WCS Lesson and Dance at Eastern Star Hall Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria WCS Lesson and Dance at Eastern Star Hall Details 1 person responded Event by Donna Forsyth Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson by John de Pyffer from 7 to 8 pm Social dancing from 8 to 10:15pm Djs Amanda and Nel Cost $12 No need to register and no partner required. Please bring scuff-free indoor shoes or socks to dance in  and a water bottle. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C659" s="3" t="n">
+        <v>45834.95884658565</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/641769172035949/</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Saturday April 12 Beginner lesson and social dance at Dance Victoria Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 12 Beginner lesson and social dance at Dance Victoria Details 5 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginners lesson by Donna from 7 to 8 pm Social dancing from 8 to 10:15 pm DJs Andre and Nel Cost $15 /$12 for Students No need to register and no partner required. Please bring scuff-free inside dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C660" s="3" t="n">
+        <v>45834.95884658565</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1366072544640156/</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Saturday 17 May 2025 at 18:45 Victoria WCS Collective Beginner Lesson and Social Dancing Dance Victoria About Discussion More About Discussion Victoria WCS Collective Beginner Lesson and Social Dancing Details 9 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson from 7 to 8 pm by John de Pfyffer Social dancing from 8 to 10:15pm DJg by Donna and Nel Cost $15/ $12 for students No need to register and no need for dance experience.. Also, no partner necessary, we got you! Please bring indoor scuff-free dance shoes or socks to dance in. See less Victoria, British Columbia Dance Victoria 2750 Quadra St # 111, Victoria Dance Victoria brings the "World's Best Dance" to the Royal Theatre and supports new dance creation for the international stage from its studios. Guests See All</t>
+        </is>
+      </c>
+      <c r="C661" s="3" t="n">
+        <v>45834.95884658565</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1024182725709172/</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Saturday April 19th Lesson and Social Dance Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 19th Lesson and Social Dance Details 4 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginner plus lesson with Pamela Podmoroff from 8 to 10:15 pm Social dancing from 8 to 10:15 pm DJs Donna and Amanda Cost $15/ $12 for students No need to register and no partner required. Please bring scuff-free indoor dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C662" s="3" t="n">
+        <v>45834.95884658565</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3963074663954670/</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Tuesday dances Eastern Star Hall Chapters No 5 &amp; No 17 Tue, 15 Jul Tue, 22 Jul Tue, 29 Jul About Discussion More About Discussion VIctoria WCS Collective Tuesday dances Interested Going Invite Details 1 person responded Event by Donna Forsyth and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 6 hr 45 min Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Saanich, BC V8Z 3S3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C663" s="3" t="n">
+        <v>45834.95884658565</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2162855673833831/</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 11 May 2019 18 May 2019 25 May 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 8 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook Wow! April went by so quickly, which means it must've been super fun, which it definitely was.  Everyone at BC Swing Dance Club Victoria is so pleased with the way the first month of social dances went, and we hope to generate the same amount of enthusiasm in May. Let's make this month just as much fun! Come join us on May 4th for the first intro lesson and social dance of the month (plus every Saturday night after that). Just $10 for the lesson and/or social dance ($5 for students). No experience or partner required. • 6:45 pm - Doors open • 7:00 pm - Intro lesson with Sam Jackson and Meaghan Efford * • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *PLEASE NOTE that the weekly lessons will start PROMPTLY at 7pm.  It is disruptive to the flow of the lesson if participants arrive late. For anyone who's interested in building their West Coast Swing fundamentals quickly, note that May will be the last month we'll be offering weekly classes with both Sam and Meaghan. With summer approaching it's a great time to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity. Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C664" s="3" t="n">
+        <v>45834.95884658565</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1225266505917189/</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Saturday Beginner Lesson and Social Dancing Dance Victoria Sat, 14 Jun Sat, 21 Jun Sat, 28 Jun Sat, 12 Jul +3 About Discussion More About Discussion Victoria WCS Collective hosts Saturday Beginner Lesson and Social Dancing Interested Going Invite Details 7 people responded Event by Donna Forsyth Dance Victoria Duration: 3 hr 30 min Public · Anyone on or off Facebook Back to AIR CONDITIONED comfort at Dance Victoria Studios Beginner lesson from 7 to 8 pm Social dancing  from 8 to 10:15 pm Cost $15/$12 for students No need to register and no need for previous dance experience or a partner. Please bring scuff-free inside low-heeled dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C665" s="3" t="n">
+        <v>45834.95884658565</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1022330066692643/</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Wednesday 2 July 2025 at 18:30 Technique and Milonga with Monica Parra Alive Tango Victoria About Discussion More About Discussion Technique and Milonga with Monica Parra Interested Going Invite Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Public · Anyone on or off Facebook 2nd of July , Wednesday 6.30-8pm Follower’s technique: Pivots and turns • Dissociation technique and axis control. • Free leg preparation before the turn. • Turns in tight spaces (useful in a close embrace!!) 90 minutes, $30 9th of July , Wednesday 6.30-8pm Couple workshop: Milonga Lisa and Milonga with traspie using different tempo. 90 minutes, $30 Both workshops (July 2nd and 9th)$50 Register with Grazyna (grazs@shaw.ca, Messenger or simply talk to me) Contact me personally for privates with Monica. See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C666" s="3" t="n">
+        <v>45834.9603525</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/713923214640962/</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Sunday 4 May 2025 from 13:00-16:00 May 4th Afternoon Milonga Solwood Studio About Discussion More About Discussion May 4th Afternoon Milonga Details 45 people responded Event by Ingrid Love and Kathryn Stone Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook A one-time special afternoon milonga! Join us in celebrating the warmth of Spring and return to sunshine. Or, star wars, if you like. Featuring special guests Kimberly and Khang performing live music (violin/guitar) DJ Ingrid Hosts: Kathryn &amp; Ingrid $15 entry (cash only) 1:00pm-4:00pm Solwood Studio 1303 Broad St Victoria, BC See less Victoria, British Columbia Solwood Studio Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C667" s="3" t="n">
+        <v>45834.9603525</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/644050564927019/</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends! A NEW SUNDAY AFTERNOON MILONGA! This is the first of a regular monthly milonga at a beautiful new venue…The Coda Club (formerly Hermann’s Upstairs) at 751 View Street, Victoria. Great ambience, nice wood floor, good sound system. So come join us for the warm hugs and close embrace and dance to the beautiful music of our very own DJ John Dewhirst. Sunday, 6 April 2025 2.00pm-5.00pm The Coda Club, 751 View Street, Victoria Admission $15 DJ: John Dewhirst Cash Bar is open for drinks Free Parking at View Street Parkade just next door Come celebrate this exciting day with us! See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C668" s="3" t="n">
+        <v>45834.9603525</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2579625309035667/</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Sunday 18 May 2025 from 12:00-18:00 Live Music @ Junction (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Live Music @ Junction (RAIN OR SHINE) Details 125 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Here we go again, its a long weekend so let's get our Sunday Funday on. First Live Music of the year at Junction Up first is-  Emergency Exit  are playing from 1230-230pm To take us home is - An &amp; Ben are playing from 3-5pm Tasting Room and Picnic Area are open 12-6pm Oh and if you haven't heard me say it before ITS RAIN OR SHINE. Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Cider ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Mini Market and a Beautiful location ⠀⠀⠀⠀⠀⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your well behaved two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C669" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/686146924271113/</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>(20+) Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Saturday from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 5 Thursday 5 June 2025 from 19:00-22:00 Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz 753 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz Details Event by Adonis Puentes and Brent Jarvis 753 View St, Victoria, BC V8W 1J9, Canada Duration: 3 hr Public · Anyone on or off Facebook An evening of Jazzy Cuban Fusion Music; traditional, contemporary, romance and dance. Juno &amp; Grammy Nominated vocalist, Adonis Puentes, will be joined by the Jazz Bohemians, featuring Brent Jarvis (piano), Ken Lister (bass), Nicholas Marquez (percussion) and Brooke Maxwell (Sax). Adonis Puentes opens up the marvelous world of Cuban music to his audience the second they hear his rich voice. When the other players kick in with their tight, multi-layered arrangements, it becomes clear that Adonis is a powerful bandleader. Fronting an acoustic band, Adonis' vocals are surrounded by piano, bass, strings, and percussion. Music reflects the present and Adonis Puentes is a Cuban Sonero for our times. Adonis thrives on the growth and acclaim for his original sonero sound. As he puts it, "I feel like a messenger of my roots and tradition, blessed that with me I have taken my music and heritage to many different places in the world; from Cuba, to Canada, USA, Mexico, Europe and Asia. My mission is to make you dance and enjoy my melodies and rhythms." Musician Line-Up: Adonis Puentes - Vocals Brent Jarvis - Piano Ken Lister - Bass Nicolas Marquez - Percussion Brooke Maxwell - Sax See less Music and audio Victoria, British Columbia 753 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Meet your hosts Adonis Puentes 34 past events · Page · Musician/band Adonis Puentes is a great singer and an elegant composer and lyricist grounded and nourished by his Cuban roots and worldly experience. Message Brent Jarvis 37 past events · Profile · Musician Message Suggested events Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1499 people interested Interested Fri, 29 Aug at 19:00 GLOW • i-Land Fest Kick-Off Fete Ambrosia Banquet Nadia is interested 129 people interested Interested Thu, 18 Sep at 18:00 THE WAILERS NATURAL MYSTIC 30TH ANNIVERSARY TOUR - THUR. SEPT 18 AT ROYAL ATHLETIC PARK IN VICTORIA! Royal Athletic Park Linda is interested 580 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested This Saturday at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C670" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1414577976223422/</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 19:00-23:00 Solstice Slammer 3 - Moon Under Water, Victoria The Moon Under Water Brewpub About Discussion More About Discussion Solstice Slammer 3 - Moon Under Water, Victoria Details 68 people responded Event by Electric Druids and Gate Theory The Moon Under Water Brewpub Duration: 4 hr Public · Anyone on or off Facebook Come join us for Solstice Slammer III at Moon Under Water Brewpub and Distillery! Get ready to celebrate with Electric Druids, Gate Theory and West Street Children, hefty drinks and good vibes. Whether you're a craft beer enthusiast or just an enthusiast, there's something for everyone at this epic night of live music. Don't miss out - mark your calendars! See less Music and audio Victoria, British Columbia The Moon Under Water Brewpub 5435 Fowler Rd, Saanich, BC V8Y 1Y4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C671" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1239927167616785/</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Thursday 11 September 2025 at 19:00 Rest and Resonate - Restorative Yoga ft. cozy Live Music Fernwood Community and Arts Association About Discussion More About Discussion Rest and Resonate - Restorative Yoga ft. cozy Live Music Interested Going Invite Details 9 people responded Event by Across the Water Fernwood Community and Arts Association Tickets www.annabiglandpritchard.com/event-details/rest-resonate-restorative-yoga-ft-cozy-live-music-1-1 Public · Anyone on or off Facebook A dreamy and nourishing evening retreat offering restorative yoga, live music, and guided journalling. Still warm with the energy of the September full moon in Pisces (the Corn Moon) - this is a great time to celebrate and embrace life, nourishing our bodies so they can carry out our most impactful dreams. Facilitated by: Roxie Fehr of Across the Water | Yoga, Meditation, and Indian Head Massage &amp; Anna Bigland-Pritchard of Rose House | Music (harp, vocal looping, singing) and poetry reading What to bring: Yoga mat Journal &amp; pen/pencil Yoga bolster Yoga blocks Blanket Any other props you'd like to use Yourself as you are Details: Thursday September 11th, 7-8:30pm at Little Fernwood If cost is a barrier, please contact us directly as we have a limited number of discount codes available Come as you are, leave nourished by your dreams See less Victoria, British Columbia Tickets Find Tickets Fernwood Community and Arts Association 1923 Fernwood Rd., Victoria Welcome to the Fernwood Community and Arts Association FB page. This site is used to distribute updates on FCAA meetings, initiatives and events. Join or renew your membership at www.thefca.ca or our office 1923 Fernwood Rd. Guests See All</t>
+        </is>
+      </c>
+      <c r="C672" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1137992241425588/</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Tomorrow from 13:00-15:00 Music in Abkhazi Garden Abkhazi Garden Fri, 27 Jun Fri, 4 Jul Fri, 11 Jul +5 About Discussion More About Discussion Music in Abkhazi Garden Interested Going Invite Details 13 people responded Event by Victoria Conservatory of Music Abkhazi Garden Duration: 2 hr Public · Anyone on or off Facebook Abkhazi Garden hosts Victoria Conservatory of Music students and faculty for a season of live outdoor performances from June 13 to August 15, every Friday from 1:00pm to 3:00pm. Admission is by donation. The address of Abkhazi Garden is 1964 Fairfield Road, Victoria, BC V8S 1H4 See less Victoria, British Columbia Abkhazi Garden 1964 Fairfield Road, Victoria Explore a one-of-a-kind west coast, heritage garden in a quiet Victoria neighborhood on Vancouver Island. Open seven days a week 11 am – 5 pm. Last entrance, 4:00pm. Entrance by donation. We suggest $10/person. Guests See All</t>
+        </is>
+      </c>
+      <c r="C673" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1142760357225336/</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 26 26 Jul at 10:00 – 27 Jul at 17:00 ArtisTREE Festival 1401 rockland ave, Victoria, BC, Canada About Discussion More About Discussion ArtisTREE Festival Interested Going Invite Details 1.3K people responded Event by Artistree Festival , MORENA CLOTHING and Cory Judge 1401 rockland ave, Victoria, BC, Canada Duration: 2 days Public · Anyone on or off Facebook Saturday July 26 10-7pm Sunday July 27 10-5pm Government House of BC 1402 Rockland Ave Celebration of Creativity profiling 130 Juried Artisans, Live Music, Installation and Performance Art, Indigenous Makers and Traditions, Kids section, Live Painters, Delicious Food and Ice cream. See less Shopping Victoria, British Columbia 1401 rockland ave, Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C674" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1975172826621817/</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>(20+) Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Saturday from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Thursday 12 June 2025 from 19:00-20:30 Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Little Fernwood Gallery. About Discussion More About Discussion Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Details Event by Across the Water and Anna Bigland-Pritchard Little Fernwood Gallery. Duration: 1 hr 30 min Public · Anyone on or off Facebook Do you need some R&amp;R? Join Anna &amp; Roxie for a dreamy candlelit evening of restorative yoga, live music, and guided journalling. Facilitated by Roxie Fehr of Across the Water | Yoga Anna Bigland-Pritchard of ABP Music Studio | Music As experienced, intuitive space-holders, our goal to support your Nervous System and capacity for hope with a feast of restful offerings. We know life is stressful and we want to help you feel more connected to your intuition so you can not only survive, but also have the capacity to take the next right step in your life in a way that positively impacts the world. The space will be dreamy, there will be tea, guided journalling, poetry, restorative yoga shapes that can be adapted for any body, and LIVE MUSIC! Anna will be playing guitar, creating dreamy sound worlds with vocal looping, and singing you lullabies all evening. What to bring Yoga mat (We'll have a few available to borrow) Journal &amp; pen/pencil (We'll also have some spare paper and writing/drawing utensils) Yourself in your comfy cozies Details June 12, 7-8:30pm at Little Fernwood $42 Accessibility This event is on the ground floor There is a unisex/non-gendered bathroom on the same level We care about making this event accessible, so please let us know if you have any questions or accessibility needs. This will be a VERY gentle practice, and modifications will be offered. Happy pride! As members of and allies of the 2SLGBTQIA community, we (Anna &amp; Roxie) will create a supportive, inclusive, affirming environment and expect all participants to do the same. If cost is a barrier, please contact us directly as we have a limited number of discount codes available This is our first time offering this class, and we hope it will be a hit so we can make it a regular thing. Come as you are, leave nourished by your dreams See less Victoria, British Columbia Little Fernwood Gallery. 1923 Fernwood Ave., Victoria Meet your hosts Across the Water 2 past events · Page · Fitness trainer Across the Water facilitates Yoga and Group Fitness in Victoria, BC. We value community and connection and just love to have fun while moving ou… Contact Us Anna Bigland-Pritchard 6 past events · Page · Musician/band Based in Lekwungen territory (Victoria, BC), Anna Bigland-Pritchard is a: -Soprano -Voice teacher… Follow Suggested events Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested 28 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1499 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested This Saturday at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C675" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1482463219409922/</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Wednesday 2 July 2025 from 19:30-19:31 Live Music Sessions at Crafthouse Vic West #100 - 184 Wilson Street, Victoria, BC, Canada About Discussion More About Discussion Live Music Sessions at Crafthouse Vic West Interested Going Invite Details 1 person responded Event by Browns Crafthouse Vic West #100 - 184 Wilson Street, Victoria, BC, Canada Duration: 1 min Public · Anyone on or off Facebook Join us every Wednesday night for local live music starting at 730pm. 1/2 wings &amp; 1/2 bottles of wine. Victoria, British Columbia #100 - 184 Wilson Street, Victoria, BC, Canada 184 Wilson St, Victoria, BC V9A 7N6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C676" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1085685423617722/</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Thursday 25 September 2025 at 10:00 The Men in Black: A Tribute to the Music of Johnny Cash Mcpherson Playhouse About Discussion More About Discussion The Men in Black: A Tribute to the Music of Johnny Cash Interested Going Invite Details 3 people responded Event by Jeff Scott and Victoria Live Music - @BarsnbandsYYJ Mcpherson Playhouse Public · Anyone on or off Facebook The Men in Black: The Songs and stories of Johnny Cash, presented Live onstage in this Multimedia production. Featuring special guest Tracee Rees singing the parts of June Carter Cash. Tickets on sale from the McPherson Box Office: https://www.rmts.bc.ca/.../2025.../the-men-in-black/ See less Victoria, British Columbia Mcpherson Playhouse 48.428809, -123.366838 Guests See All</t>
+        </is>
+      </c>
+      <c r="C677" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/650159601522409/</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>(20+) Rest and Resonate - Restorative Yoga ft. cozy Live Music  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Saturday from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 9 Saturday 9 August 2025 at 19:30 Rest and Resonate - Restorative Yoga ft. cozy Live Music Fernwood Community and Arts Association About Discussion More About Discussion Rest and Resonate - Restorative Yoga ft. cozy Live Music Interested Going Invite Details Event by Across the Water Fernwood Community and Arts Association Tickets www.annabiglandpritchard.com/event-details/rest-resonate-restorative-yoga-ft-cozy-live-music-1 Public · Anyone on or off Facebook A dreamy and nourishing evening retreat offering restorative yoga, live music, and guided journalling. Fresh on the heels of the August full moon in Aquarius - this is a great time to charge up your batteries and dream up visionary ways to improve the state of world together. Facilitated by: Roxie Fehr of Across the Water Yoga and Wellness | Yoga, guided meditation, and Indian Head Massage  &amp; Anna Bigland-Pritchard of Rose House | Music (harp, vocal looping, singing) &amp; poetry reading What to bring: Yoga mat Journal &amp; pen/pencil Yoga bolster Yoga blocks Blanket Any other props you'd like to use Yourself as you are Details August 19, 7-8:30pm at Little Fernwood If cost is a barrier, please contact us directly as we have a limited number of discount codes available Come as you are, leave nourished by your dreams See less Music and audio Victoria, British Columbia Tickets Find Tickets Fernwood Community and Arts Association 1923 Fernwood Rd., Victoria Welcome to the Fernwood Community and Arts Association FB page. This site is used to distribute updates on FCAA meetings, initiatives and events. Join or renew your membership at www.thefca.ca or our office 1923 Fernwood Rd. Meet your host Across the Water 2 past events · Page · Fitness trainer Across the Water facilitates Yoga and Group Fitness in Victoria, BC. We value community and connection and just love to have fun while moving ou… Contact Us Suggested events Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested 28 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1499 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested This Saturday at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C678" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1399479741193649/</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Saxe Point Public House About Discussion More About Discussion TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Details 4 people responded Event by Tom Watson Saxe Point Public House Public · Anyone on or off Facebook Join Vinyl Wave at the lovely Saxe Point Pub for a couple of hours of smooth tunes that'll help ease you into the week! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C679" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1093118172681618/</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>(20+) The Joan Bessie Cabaret: a celebration of original  live music and dance | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Tomorrow from 20:00-00:00 Bachata Night Lorne and 3 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Saturday from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 29 Sunday from 19:00-22:00 The Joan Bessie Cabaret: a celebration of original  live music and dance Metro Studio Theatre About Discussion More About Discussion The Joan Bessie Cabaret: a celebration of original  live music and dance Interested Going Invite Details Event by Joan Bessie Metro Studio Theatre Tickets · CA$5-CA$35 www.eventbrite.ca/e/joan-bessie-cabaret-tickets-1248762816199 Public · Anyone on or off Facebook Get ready to experience a night of songs and choreography at this one-of-a-kind indie cabaret. Licensed all ages event. Music and audio Victoria, British Columbia Tickets Find Tickets Metro Studio Theatre 1411 Quadra Street at Johnson Street, Victoria Meet your host Joan Bessie 13 past events · Page · Musician/band Joan Bessie is a chart topping Canadian artist. This page shares releases &amp; live tour information Message Suggested events This Sunday at 19:00 GROOVE KITCHEN'S JUNEFEST DANCE!! Hermann's Jazz Club Carmie is interested 97 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1499 people interested Interested Sat, 5 Jul at 12:00 Victoria, BC - Victoria Folk Music Festival, Royal Athletic Park Royal Athletic Park Debi and Carmie are interested 1292 people interested Interested Popular with friends Tomorrow at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 2 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested This Saturday at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C680" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/665127126496204/</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Tuesday 27 May 2025 at 19:30 Live Music at the Saxe Point Public House Saxe Point Public House About Discussion More About Discussion Live Music at the Saxe Point Public House Details 9 people responded Event by VINYL WAVE Saxe Point Public House Public · Anyone on or off Facebook Live Music every other Tuesday starting May 27th! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C681" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1050242777151793/</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 10 Jun at 09:00 – 15 Jun at 19:00 KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Victoria ,BC About Discussion More About Discussion KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Details 46 people responded Event by Congregation Emanu-El, Victoria, British Columbia Victoria ,BC Duration: 6 days Public · Anyone on or off Facebook Registration required for both in person and virtual attendance. https://klezcadia.org https://congregationemanuelnews.wordpress.com/.../klezca.../ Locations of performances and workshops provided upon registration. See less Victoria, British Columbia Victoria ,BC 528 Broughton St, Victoria, BC V8W 1C6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C682" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1451663826076478/</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Sunday 6 July 2025 from 11:00-16:00 Saanich Strawberry Festival Beaver Lake Regional Park, 728 Beaver Lake Rd. About Discussion More About Discussion Saanich Strawberry Festival Interested Going Invite Details 996 people responded Event by Saanich Parks, Recreation &amp; Community Services Beaver Lake Regional Park, 728 Beaver Lake Rd. Duration: 5 hr Public · Anyone on or off Facebook Join Saanich in celebrating the 58th annual Strawberry Festival. This family-friendly, fun, free event features live music, kids' activities, bouncy castles, information booths, arts and craft stations and, of course, the traditional servings of strawberries and ice cream. Strawberries and ice cream sales and service will be from 2 to 4pm, or until sold out. $2/serving. For more details, including vendors, activities and performances, visit saanich.ca/strawberryfestival See less Foods Victoria, British Columbia Beaver Lake Regional Park, 728 Beaver Lake Rd. 728 Beaver Lake Rd, Saanich, BC V8Z 6K2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C683" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1225611168970110/</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 25 25 Jul at 17:30 – 26 Jul at 20:00 Indigenous Music Festival Hampton Park About Discussion More About Discussion Indigenous Music Festival Interested Going Invite Details 633 people responded Event by Saanich Parks, Recreation &amp; Community Services Hampton Park Duration: 2 days Public · Anyone on or off Facebook Celebrate the 5th Annual Indigenous Music Festival at Hampton Park! A free two-night celebration of Indigenous performers from across Vancouver Island. Craft market and food vendors on site as well. Friday, July 25, 2025, from 5:30 to 8:00pm -Esquimalt Drummers and Dancers -OTR (Off the Reservation) -James Vickers Band Saturday, July 26, 2025, from  5:00 to 8:00pm -Lekwungen Traditional Dancers -Killed Instantly -Yellow Wolf w/ Benny the Jet -Nate Harris - Nate Harris Band featuring Madison Olsen Learn more at saanich.ca/indigenousmusicfestival See less Music and audio Victoria, British Columbia Hampton Park 224 Hampton Rd, Saanich Guests See All</t>
+        </is>
+      </c>
+      <c r="C684" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1110747367748372/</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Saturday 5 July 2025 at 12:00 Victoria Folk Music Festival Royal Athletic Park About Discussion More About Discussion Victoria Folk Music Festival Interested Going Invite Details 981 people responded Event by Victoria Folk Music Festival and Cascadia Concerts Royal Athletic Park Tickets · Free-CA$86.53 vicfolkfest.eventbrite.ca Public · Anyone on or off Facebook Date: July 5, 2025 Location: Royal Athletic Park, Victoria, BC Tickets: Available now at vicfolkfest.eventbrite.ca Gates Open: 12:00 PM Victoria Folk Music Festival Join us for a joyful weekend of music, community, and celebration at Victoria Folk Music Festival, on July 5th set in beautiful Royal Athletic Park . Featuring a world-class lineup including Frazey Ford, Joel Plaskett, Kacy &amp; Clayton, Harry Manx, Ferron, Old Man Luedecke, Vince Vaccaro, Canadian Beauty, Daneil Lapp's BC Fiddle Orchestra and more, this family-friendly event brings together the best in folk, roots, and Americana music. With two stages of live performances, the Victoria Folk Music Festival offers a full day of entertainment and community celebration. Explore the ReLove Vintage Pop-Up Market, showcasing top local vendors with the best in thrift, retro, and vintage wear. Enjoy a variety of Artisan goods and vendors, delicious food from Fresh Coast, Deadbeetz, Taco Revolution, and more. Families will love the vibrant children’s area—complete with a jumping castle! Dance in the grass to local Bluegrass groups and explore vendor booth from local music groups &amp; organizations. A community-driven atmosphere with world-class music at its heart, this festival is set to be a summer highlight for music lovers of all ages. Whether you're dancing barefoot in the grass, discovering your new favorite artist, or relaxing in the shade with friends, the Victoria Folk Music Festival is more than a concert — it’s a celebration of sound, soul, and connection. Don’t miss the unforgettable music and summer moments —July 5th at Royal Athletic Park! See less Music and audio Victoria, British Columbia Tickets Find Tickets Royal Athletic Park 1014 Caledonia Ave, Victoria Royal Athletic Park is a multi-purpose, fully lit stadium in Victoria, British Columbia. It is primarily used for baseball, soccer, softball and football, but also hosts special events, such as the annual Great Canadian Beer Festival and Rifflandia Music Festival. It is approximately a ten-minute walk from the city centre.HistoryIn 1907 the burgeoning summer athletic teams did not have enough facilities for senior teams with paid attendances. Baseball in particular was challenged to find available dates at Oak Bay Grounds to operate due to a preference for lacrosse.Subsequently, the supporters of Canada's national summer sport lacrosse, at a meeting chaired by BC Premier McBride formed the Royal Victoria Athletic Association on March 26, 1908, and a senior lacrosse team was founded to enable the best intermediate (Under 21) players to play in the British Columbia Amateur Lacrosse Association (BCALA) League. The Oak Bay Grounds were put under the management of the senior baseball team and then later the Rugby Football Club. The lacrosse group, later shortened to the Royal Athletic Association, issued shares at $25 each with deposits of 10% and biannual calls of 10% to raise $25,000 for improvements to the grounds. The lease was signed for 5 acres at the corner of Cook and Pembroke Streets for the grounds.Contracts had been let by May 12, 1908 and $4,000 from the share offering and gate receipts was spent by June on the construction of a perimeter fence, 2 ticket offices, an inner fence, grandstand, and carriage parking area. The inner fence enclosed the 500 ft x 285 ft (152m x 87m) playing field. The grandstand on the south side of the playing field was 150 ft long x 25 ft deep with 10 rows of seats for more than 1000 spectators. Beneath the grandstand were dressing rooms and concessions. The original layout of the field and grandstand was essentially the same as today's; however based on maps used in advertising the original field also included half of the city block to the west between Quadra and Vancouver Streets. The carriage parking was on the east side off Cook Street. Guests See All</t>
+        </is>
+      </c>
+      <c r="C685" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/651664851189740/</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 12:00-18:00 Music in the Orchard (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Music in the Orchard (RAIN OR SHINE) Details 330 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Come enjoy the start of the summer in the orchard. We have two amazing artists for you, some delicious fun summer ciders for you to try and amazing food to enjoy to complete the experience. Delicious Cider Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀ Beautiful location ⠀⠀⠀⠀ Dog Friendly ⠀⠀ ⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your WELL BEHAVED two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C686" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1514674672845802/</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Saturday 5 July 2025 at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park About Discussion More About Discussion Oak Bay Summer Concerts in the Park: Family Show Interested Going Invite Details 745 people responded Event by Oak Bay Parks, Recreation and Culture Willows Park Public · Anyone on or off Facebook Oak Bay Summer Concerts in the Park: Family Show With a stunning backdrop of Willows Beach, these outdoor concerts gather the community to celebrate music and the arts.  Presented by Oak Bay Parks, Recreation and Culture. Location: Willows Beach Park, Oak Bay Date: Saturday, July 5, 2025 Time: 2:00 p.m. Admission: Free Family Concert: lək̓ʷəŋən Traditional Dancers, Pacific Opera Victoria, STAGES Dance Company, and Marimba Mufaro. More information: https://www.oakbay.ca/.../oak-bay-summer-concerts-in-the.../ See less Victoria, British Columbia Willows Park 2778 Dalhousie St, Oak Bay, BC V8R, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C687" s="3" t="n">
+        <v>45834.96916726852</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/939376108286434/</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Today at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Tickets · CA$17.31 www.eventbrite.com/e/salsa-night-dance-city-tickets-1415720962509 Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Tickets Find Tickets Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 18 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Ali and Jon 27 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 130 people interested Interested Sat, 5 Jul at 19:00 Josh Warren Presents: The Path (LIVE @ Hermann's!) Hermann's Jazz Club 23 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C688" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/589043697010919/</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 66 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, May 25th features Cedar Mathias as our facilitator/dj! Details for Sunday, May 25th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C689" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1682353965754886/</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Saturday 14 June 2025 from 18:00-20:30 Mamas' Dance Party! 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Sat, 5 Apr Sat, 10 May Sat, 14 Jun About Discussion More About Discussion Mamas' Dance Party! Details 32 people responded Event by Fairfield Gonzales Community Association 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Duration: 2 hr 30 min Public · Anyone on or off Facebook Calling all mamas, grand-mamas, aunties &amp; mamas-to-be! Join us for a night curated for all mamas (in any season of their motherhood or reproductive journey) to connect through creative expression, freedom of movement and community building! There will be an opening &amp; closing circle and time to connect over light refreshments as the night concludes. Feel free to come for it all, or leave when needed. We can't wait to dance, groove, and connect with you all soon. This is an inclusive space for ALL those who mother. Admission by-donation: suggested donation $5 This event is presented by the FGCA's Neighbourhood Improvement Committee See less Victoria, British Columbia 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 1330 Fairfield Rd, Victoria, BC V8S 5J1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C690" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/556816543734629/</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Monday 7 July 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 46 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Merengue with Sebastian and Hannah— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C691" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1031573525615192/</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Sunday at 19:00 GROOVE KITCHEN'S JUNEFEST DANCE!! Hermann's Jazz Club About Discussion More About Discussion GROOVE KITCHEN'S JUNEFEST DANCE!! Interested Going Invite Details 98 people responded Event by Groove Kitchen and Hermann's Jazz Club Hermann's Jazz Club Tickets hermannsjazz.com/show/737557/view Public · Anyone on or off Facebook The festival is over and it seems you still wanna celebrate music, but also... wanna get down and boogie?? You're our kind of people!! Observe the top of Summer with song and funky steps as the kitchen's groove moves your body like they've done before at spots like the Butchart Gardens, The Esquimalt Ribfest, The Osbourne Bay Pub, or the hottest rooms in and outta town. The Chefs are ready to serve their mouthwatering melange of funk, pop, soul, Latin, and flavours to party to the end!! Join us... Doors 5:30 PM / 7:00 PM Show, Sunday June 29th Hermann's Jazz Club 753 View Street Victoria, BC V8W 1J9 https://hermannsjazz.com/show/737557/view See less Victoria, British Columbia Tickets Find Tickets Hermann's Jazz Club 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C692" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2576922459305643/</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 51 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 15th features Cedar Mathias as our facilitator/dj! Details for Sunday, June 15th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C693" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3854957174726232/</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Monday from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 49 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Urban Kizomba with Aaron and Fernanda— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C694" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1363696181561219/</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:00-22:00 Pride Contra Dance Fairfield United About Discussion More About Discussion Pride Contra Dance Details 90 people responded Event by Victoria Contra Dance , Code Tron and Rose Jackson Fairfield United Duration: 3 hr Public · Anyone on or off Facebook 𝕍𝕀ℂ𝕋𝕆ℝ𝕀𝔸 ℂ𝕆ℕ𝕋ℝ𝔸 𝔻𝔸ℕℂ𝔼 𝕊𝕆ℂ𝕀𝔼𝕋𝕐 ℙℝ𝔼𝕊𝔼ℕ𝕋𝕊: The return of our ℚ𝕌𝔼𝔼ℝ Contra Dance to celebrate the month of Pride! All Dancers welcome! Join us Friday, June 20th at the United Commons Fellowship Hall to do-si-do the night away to sprightly fiddle tunes and stellar performances from our two favorite drag performers! We'll have more capacity than our previous Valentines Day Dance, but we still might sell out, so grab your tickets online here! https://clannamorna.ca/.../ticket-victoria-pride-contra.../ ......................................................................................................... 𝕄𝕦𝕤𝕚𝕔 𝔹𝕪: 𝐑𝐨𝐬𝐞 𝐉𝐚𝐜𝐤𝐬𝐨𝐧: she/her Coming up in the rich folk scene of western Massachusetts, Rose is based in Montague, MA, where she studied under fiddler Becky Tracy from whom she inherited a wide repertoire of music from Quebec, New England, Ireland, and France, a deep love for old tunes, and the intuitive sense of rhythm and danceability which infuses her playing. Equally at home in the concert hall and on the dance stage, she’s taught fiddle, song, and dance at camps and festivals around New England, toured nationally with her band Polaris and now tours with her quartet Stove Dragon and duo Helen &amp; Rose. https://www.rose-jackson.com/ 𝐇𝐞𝐥𝐞𝐧 𝐊𝐮𝐡𝐚𝐫: they/them Hailing from Seattle, Washington, Helen currently resides in Cambridge, MA. Helen began exploring their connection to folk and Celtic music in 2020 while studying with renowned contra guitarist Alex Sturbaum. Upon moving to Cambridge in 2022, Helen dove into the thriving celtic music scene, playing contra dances, Irish sessions, and concerts around New England and the Pacific Northwest. Since then, Helen has developed their style as a contra accompanist, Irish session backer, and vocalist. https://www.helenkuharmusic.com/ 𝐅𝐢𝐝𝐝𝐥𝐢𝐧' 𝐅𝐢𝐧𝐧: they/them A professional fiddler, singer and banjo player living on the territories of the lekwungen and W̱SÁNEĆ people, colonially known as Victoria BC. Finn has a passion for Irish, Scottish, English, North American and Eastern European folk music, and are known for their dynamic fiddling and soulful voice. They delve into traditional material - bringing a fresh interpretation of songs and tunes from many different places, as well as writing their own material. From the Appalachian mountains to Quebec, to melodic Irish and Scottish tunes, they cover wide musical ground with articulate playing. Finn also performs frequently in Canada and the U.S. with their bands Clanna Morna and Ghostly Hounds. https://finnletourneau.com/ ℂ𝕒𝕝𝕝𝕚𝕟𝕘 𝔹𝕪: 𝐕𝐢𝐜𝐭𝐨𝐫𝐢𝐚 𝐁𝐞𝐚𝐮𝐜𝐡𝐞𝐬𝐧𝐞 One of our local communities up and coming callers! 𝔻𝕣𝕒𝕘 𝕡𝕖𝕣𝕗𝕠𝕣𝕞𝕒𝕟𝕔𝕖𝕤 𝕓𝕪: Aries Moon: Making country gay one song at a time Leo Moon: The island's premiere tap dancing drag thing ......................................................................................................... 6:30 - doors open 7:00 - dancing starts with a beginner friendly dance lesson Everyone welcome, no experience necessary. $12 - Youth $20 - Everyone who is willing and able to NOTAFLOF Poster Art by Sonya Chwyl See less Victoria, British Columbia Fairfield United 925 Balmoral Rd, Victoria, BC V8T 1A7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C695" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/734261429120710/</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Friday 6 June 2025 from 19:30-22:30 Dance City 108 Niagara St, Victoria, BC V8V 1E9, Canada About Discussion More About Discussion Dance City Details 9 people responded Event by Andrew Sanderson 108 Niagara St, Victoria, BC V8V 1E9, Canada Duration: 3 hr Public · Anyone on or off Facebook Beginner Cha Cha workshop with Jane and Andrew at 7:30pm Multi genres dance including Standard, Latin,  West Coast Swing, and more starting at 8:30pm dj Andrew Sanderson Cash Admission: $12/$10 Members See less Victoria, British Columbia 108 Niagara St, Victoria, BC V8V 1E9, Canada 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C696" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/909522138040202/</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Friday 28 November 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 130 people interested Interested Sun, 27 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Ali and 3 friends 45 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C697" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1185783966345055/</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 10:00-13:00 Shuffle Dance Workshop Victoria, BC About Discussion More About Discussion Shuffle Dance Workshop Details 12 people responded Event by Adelène Buchanan Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another SHUFFLE WORKSHOP coming your way!! Join our Shuffle Dance Workshop and learn a full shuffle choreography set to an energetic electronic track. We’ll guide you through each step, focusing on key shuffle movements, while incorporating them into a dynamic routine. Perfect for ALL LEVELS! This workshop will help you improve your footwork, coordination, and cardiovascular stamina as you master a complete choreography. Here’s what you need to know: DATE: Sunday, May 25th TIME: 10am - 1pm PLACE: The Beat Clinic (1303 Broad Street) Sign-up link here https://www.thebeatclinic.ca/ See less Victoria, British Columbia Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C698" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1408949946810887/</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Sunday 8 June 2025 from 11:00-12:30 Dance Temple w/ Lila Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Lila Details 32 people responded Event by Dance Temple Victoria , Lyndsay Lila and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 8th features Lila Spencer as our facilitator/dj! Details for Sunday, June 8th: Facilitation and music set by Lila Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C699" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1187402793186660/</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 08:00-12:00 Global Underscore Solstice Dance Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada About Discussion More About Discussion Global Underscore Solstice Dance Details 62 people responded Event by Arunimá McNeish , Michael McAmmond and Victoria Contact Improv Jam Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada Duration: 4 hr Public · Anyone on or off Facebook Sweet dancers, This summer solstice we extend a warm invitation to join us in expanding and deepening our practice of Contact Improvisation with participation in The Global Underscore. Please arrive at 8am to join a 40 minute talk-through, introducing the concepts of the Underscore. This is mandatory if you have never attended an Underscore before. The Underscore will begin promptly at 8:45am. If you have attended a talk-through before you're welcome to arrive at this time. We will all start and end together. This is a closed container and we will not be allowing late-comers. TIMELINE: 8am-8:40am Underscore Talk-Through with Arunima 8:45am-11:30am Underscore 11:30am-11:50am Closing Circle COST: $15-$20  etransfer or pay cash at the door if pre-registered (if money is a barrier please reach out to discuss options). Please contact Arunima at ode.to.thylacine@gmail.com for registration, etransfer, questions, etc. VENUE: Centennial United Church (612 David St, Victoria, BC). MORE INFO: The Underscore, which has been evolving since 1990, is a vehicle for incorporating Contact Improvisation into the broader arena of improvisational dance practice; developing greater ease dancing in spherical space—alone and with others; and for integrating kinesthetic and compositional aspects while improvising. It allows for a full spectrum of energetic and physical expressions, embodying a range of forms and changing states. Its practice is familiar yet unpredictable. The practice progresses through a broad range of dynamic states, including long periods of very small, private, and quiet internal activity and other times of higher energy and interactive dancing. There are 20+ phases, 12+ connections, and 7 aspects of the Underscore—each with a name and a graphic symbol—which create a general map for the dancers. Within that frame, dancers are free to create their own movements, dynamics, and relationships—with themselves, each other, the group, and the environment. Each Underscore is unique, providing rich and often inspiring experiences of the human and artistic phenomena of dance improvisation. https://globalunderscore.com/ https://nancystarksmith.com/underscore/ See less Victoria, British Columbia Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada 612 David St, Victoria, BC V8T 2E1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C700" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/624858640069610/</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 Friday 22 August 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 130 people interested Interested Sun, 27 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Ali and 3 friends 45 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C701" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1238334523949776/</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Sunday from 11:00-12:30 Dance Temple w/ Alex King-Harris (aka Rara Avis) Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Alex King-Harris (aka Rara Avis) Interested Going Invite Details 68 people responded Event by Dance Temple Victoria , Alex King-Harris and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 29th features Alex King-Harris (aka Rara Avis) as our facilitator/dj. He is back in town for the summer! Details for Sunday, June 29th: Facilitation and music set by Alex King-Harris (Rara Avis) Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C702" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/650657144184821/</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Saturday 19 July 2025 from 21:00-02:00 COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY The Coda About Discussion More About Discussion COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY Interested Going Invite Details 64 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 5 hr Public · Anyone on or off Facebook Colombian Summer Rumba: “Tierra Querida” Party Saturday, July 19th Doors: 9:00 PM | Show: 9:30 PM 19+ | ID Required Celebrate Colombian Independence Day with us with the vibrant “Tierra Querida” Party — an amazing night of live music, dance, culture, and pure rumba energy! Start the night with a live tribute to Colombian music by the talented Daniel Sar &amp; Sofia Leonne. Their performance will honor legendary Colombian artists such as Juanes, Maluma, Fonseca, Rodolfo Aicardi, Herencia de Timbiquí, Mon Laferte, and more—blending pop, tropical rhythms, and heartfelt Latin ballads into a powerful musical journey. At 10:30 PM, DJ Miro, straight from Cali, Colombia, will take over with a fiery mix of Colombian beats. Later, resident DJ Alex King will close out the night, turning up the heat with Latin hits and ending strong with the latest reggaetón summer vibes. At midnight, enjoy a special folkloric performance by Danza Colombia, followed by a unifying moment as we wave our flag souvenirs and sing the national anthem together. Savor delicious cocktails, soak in vibrant downtown vibes, and enjoy a night filled with alegría, culture, and  Colombian vibes! Get your tickets NOW! First-tier: $20 | Second-tier: $25 Limited tickets available at the door for $27 - Act fast before they are sold out! Party ends at 2:00 AM Each ticket includes a Colombian flag souvenir. Take a piece of the celebration home with you! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C703" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1132427048350776/</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com or 15$ cash/e-transfer at the door. Formed in the heart of Chinatown, Rosebuds is a dynamic ensemble that brings the vibrant sounds of jazz, blues &amp; swing to life.  The group plays a mixture of originals and jazz standards, and is influenced by artists like Louis Armstrong, Billie Holiday, Lester Young, and Lionel Hampton. Featuring Rebecca Wells (vocals/guitar), Alex Moore (guitar/keys) Bryden Amos (guitar/keys), Matisse Gubby-Hurtig (bass), Owen Chow (trumpet), and Andrew Greenwood (tenor saxophone). Samba e Sol is a newly formed Brazilian bossa nova jazz trio featuring Andrew Greenwood (flute), Alex Moore (guitar), and Matisse Gubby-Hurtig (bass), playing music by artists like Antonio Carlos Jobim, Marcos Valle, Luiz Bonfa, and more. Instagram: https://www.instagram.com/rosebudsband/ See less Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C704" s="3" t="n">
+        <v>45835.37158289352</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1861230087752141/</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 6 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 31, 2025 | Lesson:  Intro to Salsa with Adam &amp; Alicia Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C705" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1743571267040445/</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Ali Jorgensen invited you About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Details 55 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 8, 2025 | Lesson: Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C706" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1079226067560481/</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 57 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 6, 2025 | Lesson:  Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C707" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1060779176049104/</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Thursday 3 October 2024 from 19:30-22:30 Kizomba Practica Thursdays: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Kizomba Practica Thursdays: Fall Series Details 20 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Join us every Thursday for Kizomba/Urbankiz classes. Intermediate 7:30PM-8:15pm Beginner 8:15pm-9:00pm Practica until 10:30pm Class only: $10 Class &amp; Practica: $15 or $10 for university students w/ID Practice only $10 Classes will be provided by your local Instructor (David Lamine) and assistants (Robyn, Becky) and occasionally by some out of town and International Instructors. Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C708" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/960236445839425/</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Saturday 22 June 2024 from 18:00-21:00 Kizomba/UrbanKiz at Clover Clover Pt, Victoria, BC V8S, Canada About Discussion More About Discussion Kizomba/UrbanKiz at Clover Interested Details 56 people responded Event by Becky Mowat Clover Pt, Victoria, BC V8S, Canada Duration: 3 hr Public · Anyone on or off Facebook Come join us for our first time dancing at Clover Point! There will be no lesson beforehand and this is super casual. Just a bunch of friends hanging out and dancing. Bring snacks, something to drink, blankets, warm clothes (as it is typically cooler by the ocean). There isn't a lot of parking at Clover Point but you can park along Dallas Rd and just walk down. Feel free to invite friends and family. Hope to see you all there! See less Victoria, British Columbia Clover Pt, Victoria, BC V8S, Canada 1301 Clover Pt, Victoria, BC V8S, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C709" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1029869435768837/</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Saturday 22 March 2025 at 20:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC This event has been cancelled. You cannot share this event, but you can still post. About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 14 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C710" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1179097320623502/</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 37 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C711" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1459643825205914/</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Tomorrow from 10:00-12:00 KIZOMBA NA RUA – AfriCa Fest Victoria 2025 Centennial Square About Discussion More About Discussion KIZOMBA NA RUA – AfriCa Fest Victoria 2025 Interested Going Invite Details 10 people responded Event by African Arts &amp; Cultural Society - Centre Issamba Centre and Pulchérie N. Mboussi Centennial Square Duration: 2 hr Public · Anyone on or off Facebook KIZOMBA NA RUA – AfriCa Fest Victoria 2025 Date: Saturday, June 28, 2025 Time: 10:00 AM – 12:00 PM Location: Centennial Square, Victoria, BC Free &amp; open to the public! We’re inviting all Kizomba dancers to join us for a special Kizomba Na Rua moment at AfriCa Fest Victoria 2025! Dance under the morning sun and feel the rhythm of Afro-Lusophone vibes in the city's heart. This open-air morning dance club moment is for dancers of all levels — whether you're dancing or just enjoying the vibe, the energy will be electric! Let’s connect, move, and celebrate community, culture, and rhythm together. Don’t forget to bring your smiles and dancing shoes — it's going to be unforgettable! #KizombaNaRua #AfriCaFest2025 #DanceInTheSquare #VictoriaBC #AfroLusophoneVibes #AfriCaFestVictoria See less Dance Victoria, British Columbia Centennial Square 10 Centennial Sq, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C712" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/947213690692385/</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C713" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2637194793152555/</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 130 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 29, 2025 | Lesson:  Intro to Salsa Rueda with Sam and Katie Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa Rueda • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C714" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1794066937801722/</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Saturday 8 March 2025 from 20:30-23:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 26 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C715" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1293301738436581/</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Sunday 6 April 2025 at 17:00 Kizomba Sundown Party: Free of charge Method Studio - Victoria BC David Lamine Victoria invited you About Discussion More About Discussion Kizomba Sundown Party: Free of charge Details 58 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Method Studio - Victoria BC Public · Anyone on or off Facebook Free Pre-VIKFest party. Bring snack and drink. Expect great music, great energy, great atmosphere. "Dance with your heart. your feet will follow" Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C716" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1337760257449745/</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 6 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 10, 2025 | Lesson:   Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C717" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3006474846197996/</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 45 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 27, 2025 | Lesson:  Intro class TBD Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro class TBD • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C718" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3185065321631809/</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Saturday 15 March 2025 from 20:00-00:00 Urban Kiz Workshop with Mannie Method Studio - Victoria BC Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 48 people responded Event by Becky Mowat and David Lamine Victoria Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C719" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1334757257408713/</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Saturday 25 January 2025 from 19:00-23:30 Special Edition Urbankiz Workshop w/ Kenny Odumosu Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Special Edition Urbankiz Workshop w/ Kenny Odumosu Details 50 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 hr 30 min Public · Anyone on or off Facebook SPECIAL EDITION WORKSHOP Join us Saturday January 25th for a 2hr Urbankiz workshop. Joining us from Calgary to share his knowledge and love for Urbankiz. Kenny finished first for the Kizomba/Semba category at the North American Olympiads. With his background in Kizomba/Semba Kenny will help you incorporate techniques and smoothness into your Urbankiz. We are really looking forward to having him here! Schedule 7:00pm-9:00pm (workshop) 9:00pm-11:30pm (social) Price: $40 (includes workshop &amp; social dance) e-transfer to:  becksmith@hotmail.com please include the name you go by if different from your e-transfer account. Thanks See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C720" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1152065639712042/</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 20 20 Feb at 19:30 – 23 Feb at 23:00 Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Details 49 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 days Public · Anyone on or off Facebook Join us for our special edition Urbankiz &amp; Tarraxo workshops with Mike Ahombi Mike has been a big supporter of our VIKF and bringing his talent and low key vibe to the west coast. He is based out of Ottawa but you will find him at many different festivals and cities teaching Kizomba, Urbakiz and Tarraxo. We cannot wait for you all to have the opportunity to learn from such an incredible person and instructor. Details: Feb 20th Urbankiz Workshop 7:30pm-9:30pm Practica 9:30pm-11:00pm Feb 22nd Tarraxo Workshop 8:00pm-10:00pm Practica 10:00-11:30pm Price $90 Workshops only $70 Practica only $20 *** please e transfer to becksmith@hotmail.com *** Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C721" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1184791909680061/</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Thursday 13 March 2025 from 19:30-23:00 Urban Kiz Workshop with Mannie Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 50 people responded Event by Becky Mowat and David Lamine Victoria Ukrainian Cultural Centre Duration: 3 hr 30 min Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C722" s="3" t="n">
+        <v>45835.37826666667</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/601131956358678/</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Thursday 3 July 2025 at 20:00 Bachata &amp; Merengue- All Levels- July Series Studio 4 Athletics About Discussion More About Discussion Bachata &amp; Merengue- All Levels- July Series Interested Going Invite Details 3 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Bachata &amp; Merengue are both dances from the Dominican Republic. Bachata can be anywhere from slow and romantic with lots of dips, sway and body movement to more upbeat and percussive with lots of musical footwork. Merengue is carefree, flirtatious and fun! Classes are registered on a monthly basis and take place every Thursday from 8:00- 9:00pm, July 3,10,17,24,31 No experience required.  No partner is necessary as we rotate partners throughout the lesson.  Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot!d See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C723" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/717475250956404/</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Friday 30 May 2025 at 18:00 FREE Beginner Bachata Class 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 About Discussion More About Discussion FREE Beginner Bachata Class Details 65 people responded Event by Mayfair Shopping Centre and Victoria Latin Dance Association 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 Public · Anyone on or off Facebook Ready to get your groove on? We’re teaming up with the Victoria Latin Dance Association  for a FREE Beginner Bachata Class right here at Centre Court! Join us on Friday, May 30 at 6:00 PM for an evening of fun and dancing. FREE Beginner Bachata Class May 30th, Friday at 6PM NO partner or experience necessary! Bachata is a beautiful and easy-to-learn dance that’s great for meeting new people, getting active, and connecting with an amazing community. See less Dance Victoria, British Columbia 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 3147 Douglas St, Victoria, BC V8Z 3K3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C724" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1300938064467261/</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Thursday 20 March 2025 from 20:00-22:00 Intermediate Sensual Bachata Workshop Method Studio - Victoria BC About Discussion More About Discussion Intermediate Sensual Bachata Workshop Details 24 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 2 hr Public · Anyone on or off Facebook Sensual Bachata Workshop in March! Intermediate workshop - March 20 Time: 8:00-9:30 PM + Practice 9:30-10:00 PM Location: Method Studio, 841 Fisgard St. Cost: $30 per workshop (includes 2 hours!) Intermediate workshop: Take your skills to a higher level! Master the advanced variations of the Madrid pass, smooth transitions and musicality. No partner needed, just bring your energy and comfortable shoes! Register at: maximumotion@gmail.com #BachataWorkshop #VictoriaBC #LearnToDance #BachataLovers See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C725" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3975145332748137/</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Friday 13 June 2025 from 20:00-00:00 Bachata Night Method Studio - Victoria BC About Discussion More About Discussion Bachata Night Details 77 people responded Event by Bachata Nights Victoria BC , Sebastian Carmona and Alysha Kopala Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights June 13 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C726" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1350929566137538/</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 7 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation August 10, 2025 | Lesson: Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C727" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1057471579628015/</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Friday 16 May 2025 at 17:00 Bachata Nights Victoria Bc Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Victoria Bc Details 9 people responded Event by Bachata Nights Victoria BC and Sebastian Carmona Method Studio - Victoria BC Public · Anyone on or off Facebook Join us on our next Bachata Nights May 23 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C728" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1813229489279716/</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Thursday 29 May 2025 from 19:55-21:00 Sensual Bachata 4 Week Series Method Studio - Victoria BC Thu, 15 May Thu, 22 May Thu, 29 May +1 About Discussion More About Discussion Sensual Bachata 4 Week Series Details 6 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 1 hr 5 min Public · Anyone on or off Facebook Ready to level up your Sensual Bachata? May 8, 15, 22, 29 Method Studio | 7:55–9:00 PM | $80 for all 4 classes Join us for an exciting and dynamic Bachata Sensual class designed for experienced beginners and intermediate dancers! We’re blending solid fundamentals with fresh, fun, and sensual combos to help you grow, challenge yourself, and have an amazing time on the dance floor. No partner needed — just bring yourself and your love for dance! Spots are limited — don’t miss out! Register by e-transferring $80 to maximumotion@gmail.com and mentioning “Bachata Sensual” in the notes. Get ready to connect, move, and elevate your dancing! P.S. All fees are non-refundable as they go directly toward securing the studio space and running the class. See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C729" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1730246844256904/</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre About Discussion More About Discussion Saturday Salsa/Bachata Social June 28th Interested Going Invite Details 46 people responded Event by Latin Dance Canada Ukrainian Cultural Centre Duration: 3 hr 59 min Public · Anyone on or off Facebook Saturday Salsa/Bachata Social June 28th 3277 Douglas st, Victoria BC Cost? $15 CASH ONLY PLEASE! When? Saturday, June 28th 8:00 pm - 8:30 pm beginner dance lesson 8:30 pm - 12 am Social dancing What? We will be playing a mix of salsa, bachata and more. Where? Ukrainian Cultural Centre 3277 Douglas Street, Victoria See less Dance Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C730" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1388695712154512/</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Ali Jorgensen invited you About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Details 121 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation June 22, 2025 | Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C731" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/729183856154450/</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Today from 20:00-00:00 Bachata Night Method Studio - Victoria BC About Discussion More About Discussion Bachata Night Interested Going Invite Details 31 people responded Event by Bachata Nights Victoria BC and Alysha Kopala Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights June 27 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance @yourgirlalysha  and @davidch_78 will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C732" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1901245437276872/</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Friday 9 May 2025 from 20:00-00:00 Bachata Nights Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Details 40 people responded Event by Bachata Nights Victoria BC , Alysha Kopala and Sebastian Carmona Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights May 09 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @yourgirlalysha  and @davidch_78  will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person The evening starts with an Open-level Bachata lesson from 8:15 PM to 9:00 PM—great for all skill levels! Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C733" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/9677364319006080/</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 61 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation July 20, 2025 | Lesson:  Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C734" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/745466751313624/</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Tuesday 8 July 2025 at 20:00 Salsa &amp; Cha Cha Cha- Fundamentals- July Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- July Series Interested Going Invite Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, July 8,15,22,29 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C735" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342792743590871/</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Monday 7 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- April series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, April 7, 14, 28. Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C736" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/966455485665576/</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Thursday 3 April 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- April series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Apr 1, 8, 15, 22, 29 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C737" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1382188962971661/</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Tuesday 1 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Fundamentals- April Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- April Series Details 9 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, Apr 1, 8, 15, 22, 29 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C738" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/669591372187091/</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 10:00-11:00 Salsa &amp; ChaCha Solo Westshore Dance Studios Sat, 17 May Sat, 24 May Sat, 31 May +7 About Discussion More About Discussion Salsa &amp; ChaCha Solo Details 2 people responded Event by Dance Praktika Westshore Dance Studios Duration: 1 hr Public · Anyone on or off Facebook Elevate your dance journey with our Ladies Solo Class. Join our exciting series and learn the basics of Salsa and Cha Cha. Perfect for beginners looking to spice up their dance skills! Class Highlights: - Learn exciting dance moves tailored for solo dancers; - Fun and welcoming environment; - Suitable for absolute beginners. Come dance with us and let the rhythm guide you! To register to April classes please use links at "Tickets". See less Langford, British Columbia Westshore Dance Studios 109-2675 Wilfert Road, Victoria www.westshoredance.com 2years+ Competitive&amp;Production a space for everyone with a love of dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C739" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2579272439096564/</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Tuesday 8 July 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- July series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- July series Interested Going Invite Details 4 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. July 8,15,22,29 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C740" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2214494908966327/</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Monday 5 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Int/ Adv- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- May series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, May 5, 12, 26 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C741" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/727053470038104/</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Monday 7 July 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/Adv- July series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/Adv- July series Interested Going Invite Details 4 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, July 7,14,21,28 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C742" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/679241811720932/</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Fundamentals- May Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- May Series Details 7 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, May 6, 13, 20, 27 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C743" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/10048344358532607/</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- May series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. May 6, 13, 20, 27 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C744" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342233713680795/</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Thursday 1 May 2025 at 21:00 Bachata &amp; Merengue- All Levels- May Series Studio 4 Athletics About Discussion More About Discussion Bachata &amp; Merengue- All Levels- May Series Details 3 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Bachata &amp; Merengue are both dances from the Dominican Republic. Bachata can be anywhere from slow and romantic with lots of dips, sway and body movement to more upbeat and percussive with lots of musical footwork. Merengue is carefree, flirtatious and fun! Classes are registered on a monthly basis and take place every Thursday from 8:00- 9:00pm, May 1, 8, 15, 22, 29. No experience required.  No partner is necessary as we rotate partners throughout the lesson.  Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C745" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1059622278965884/</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 8 Saturday 8 November 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in October. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1505 people interested Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends 184 people interested Interested Sat, 18 Oct at 20:00 ✨ White and Gold Latin Night – October 18th! ✨ Latin Dance Canada Carmie is interested 33 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C746" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1618420955545842/</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 30 Friday 30 May 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing at an all ages venue with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 4 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Ali 13 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested Sun, 17 Aug at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Ali is going 2 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C747" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/884101187183426/</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 July 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Tickets · CA$17.31 www.eventbrite.com/e/caliente-salsa-saturdays-tickets-1415724884239 Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in June. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Tickets Find Tickets Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 5 Jul at 19:00 Josh Warren Presents: The Path (LIVE @ Hermann's!) Hermann's Jazz Club 23 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1505 people interested Interested Happening now AfriCa Fest Victoria 12e Edition Centennial Square Ali, Debi and 2 friends 587 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C748" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2251848171850840/</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 Saturday 10 May 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in April. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Fri, 11 Jul at 21:00 Locarno at The Coda The Coda Nadia is interested 43 people interested Interested Sat, 5 Jul at 19:00 Josh Warren Presents: The Path (LIVE @ Hermann's!) Hermann's Jazz Club 23 people interested Interested Sun, 17 Aug at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Ali is going 2 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C749" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3899920353641309/</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 9 Saturday 9 August 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in July. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Fri, 11 Jul at 21:00 Locarno at The Coda The Coda Nadia is interested 43 people interested Interested Sat, 5 Jul at 19:00 Josh Warren Presents: The Path (LIVE @ Hermann's!) Hermann's Jazz Club 23 people interested Interested Mon, 30 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Ali and Almeda 49 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C750" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1636237610432412/</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Saturday 16 August 2025 from 20:00-23:59 Salsa Sunset Latin Party – August 16th! Latin Dance Canada About Discussion More About Discussion 🌅🔥 Salsa Sunset Latin Party – August 16th! 🔥🌅 Interested Going Invite Details 29 people responded Event by Latin Dance Canada Latin Dance Canada Duration: 3 hr 59 min Public · Anyone on or off Facebook Salsa Sunset Latin Party – August 16th! Get ready for a magical summer night filled with Latin rhythms, sunset vibes, and non-stop dancing! Join us for the Salsa Sunset Latin Party, where the Salsa, Bachata, and Merengue beats will keep you moving all night long under the stunning sunset sky! Dress Code: Wear your best sunset-inspired outfit – think bright, tropical colors, and beach party vibes! Dance to the best Salsa, Bachata, Merengue &amp; Latin hits all night! No partner? No problem! Join our fun intro class at 8:00 PM! Location: Ukrainian Cultural Centre, 3277 Douglas St., Victoria, BC Date: Saturday, August 16, 2025 Intro Class: 8:00 PM | Social Dance: 8:30 PM - Late Entry: $15 at the door – Bring cash, please! What to Expect: Vibrant salsa rhythms &amp; tropical vibes! Tropical-themed decorations &amp; stunning sunset views! A welcoming dance community &amp; unforgettable fun! Let’s dance as the sun sets and make it a night to remember! Tag your friends and let’s create memories under the summer sky! #SalsaSunsetLatinParty #SalsaBachata #LatinDanceParty #VictoriaBC #LatinDanceCanada See less Dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C751" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1479111682798589/</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 13 Saturday 13 September 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in August. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1505 people interested Interested Happening now AfriCa Fest Victoria 12e Edition Centennial Square Ali, Debi and 2 friends 587 people interested Interested Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested 31 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Sat, 5 Jul at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C752" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1411005319893067/</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Monday 28 April 2025 from 18:30-22:30 Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion 🔥Bachata &amp; Brazilian Zouk 🌊 dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard Details 7 people responded Event by Bachata and Zouk with Javi in Victoria 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 4 hr Public · Anyone on or off Facebook Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard street | Victoria Join us for a 4 week course exploring the joy and magic of Brazilian Zouk &amp; Bachata dancing! Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on enhancing body awareness, building confidence in dance vocabulary with lead and follow techniques, exploring musicality, and loving yourself deeper with styling! Be prepared to have lots of fun dancing with new friends! Register today! Schedule: Monday April 7 - 28th 6:30-7:25pm | Brazilian Zouk - Level 2 (ask Javi for permission) 7:30-8:25pm | Brazilian Zouk - Level 1 8:30-9:25pm | Sensual Bachata - Beginner Foundations 9:30-10:30pm | Sensual Bachata - Intermediate "Trending Moves" Tuition: $20 | 1 Class $35 | 2 Classes (Brazilian Zouk 1&amp;2, or Brazilian Zouk 1 &amp; Bachata, Bachata 1&amp;2) $50| 3 Classes (3 classes, BEST value) 1709 Blanshard St, Victoria, BC Registration: E-transfer to: danceinflow@gmail.com or send us a message on Whatsapp: 7785877665 (Also accepting credit card/cash at the door) Please add a note if you're registering as a "Leader", "Follower", or "Open to both" Space is limited. Register in advance to reserve your spot! Looking fwd to dancing and flowing with you, Warmly, Javi See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C753" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1106484714432492/</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Wednesday 2 July 2025 from 18:30-21:00 Zouk practica and social White Eagle Hall, 90 Dock St, Victoria BC Wed, 4 Jun Wed, 25 Jun Wed, 2 Jul Wed, 9 Jul +40 About Discussion More About Discussion Zouk practica and social Interested Going Invite Details 1 person responded Event by Victoria Zouk Collective and Victoria Zouk Collective Group White Eagle Hall, 90 Dock St, Victoria BC Duration: 2 hr 30 min Public · Anyone on or off Facebook Drop-in zouk practica by donation - everyone welcome! White Eagle Polish Hall every Wednesday 6:30-9 pm Shared warm up, free dance time, review material from lessons and congresses, connect and share knowledge! Help is always available. Minimum $5 donation. Cash at the door, or etransfer to oceanzouk@gmail.com Enter the lower hall by the side door on Niagara Street just beside the Polka food truck. Also available in Victoria are zouk lessons with Javi, an amazing instructor from Vancouver! More info at https://www.facebook.com/Sabor.Asi.Dance.Salsa.Victoria or email danceinflow@gmail.com See you there! See less Victoria, British Columbia White Eagle Hall, 90 Dock St, Victoria BC 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C754" s="3" t="n">
+        <v>45835.38804599537</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/544121845403419/</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 13:00-23:55 Swing Session: Balboa with Yoshi and Etsuko Solwood Studio About Discussion More About Discussion Swing Session: Balboa with Yoshi and Etsuko Details 108 people responded Event by Swing Dance Association of Victoria , Dave Henderson and 2 others Solwood Studio Duration: 10 hr 55 min Public · Anyone on or off Facebook Lace up your shoes on May 31, 2025 for an afternoon of Balboa Classes and an evening of Social Dancing with Yoshi and Etsuko Uemura. 4 Classes for everyone &amp; 1 Social Dance! Passes go on sale April 19 at noon at our SDAV Square Shop! You must know and be comfortable with Balboa basics for all of these classes - they won't be covered at this workshop. All the specifics are available at swingvictoria.net , but here are the notes: May 31st, at Solwood Studio, with doors at 12:30pm . Bring indoor shoes, please! 4 classes for everyone and there's a dance from 9-12am. Passes go on sale April 19th at noon. See less Victoria, British Columbia Solwood Studio 1303 Broad St, Victoria, BC V8W 2A8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C755" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1786895135557126/</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Monday 26 May 2025 at 19:00 The Jive Big Band and The Blue Bosses Hermann's Jazz Club About Discussion More About Discussion The Jive Big Band and The Blue Bosses Details 9 people responded Event by The Jive Big Band Hermann's Jazz Club Public · Anyone on or off Facebook Join the Jive Big Band for a fun night of music featuring big band classics, rock, funk, and the unexpected. Directed by Nick La Riviere, this band is always a good time! Joining them is the fantastic Blue Bosses jazz combo directed by Ashley Wey. Entry by donation to Arts on View, keeping music at Hermann’s alive and strong! See less Victoria, British Columbia Hermann's Jazz Club 753 View Street, Victoria Hermann's Jazz Club is the best place to visit for live jazz and blues in Victoria, BC. On July 15, Guests See All</t>
+        </is>
+      </c>
+      <c r="C756" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1594011994641933/</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Tuesday 22 April 2025 from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Details 9 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. No street shoes. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C757" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/634773653668605/</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Saturday Night West Coast Swing BC Swing Dance Club Victoria 15 Jun 2019 22 Jun 2019 29 Jun 2019 +2 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night West Coast Swing Details 9 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook June means summertime and sunny days! Along with the weather, things for BC Swing Dance Cub Victoria will be changing too. Here's what is happening this month: 7 - 8pm 1st Saturday of the Month: Lesson with Meaghan, plus an assistant from our dance community 7 - 8pm Remaining Saturdays each month: TBD (stay tuned for workshops, activities or practices - updates will be posted on each event page) Note:  The 7 - 8pm weekly timeslot is included in the dance entrance price. -------------------------------------------------- Come join us every Saturday all year long for a fabulous WCS social dance from 8 - 11pm. Just $10 for the ($5 for students). Meaghan Efford and Bob Gebbie 's lesson on June 1st (starting PROMPTLY at 7pm) will be the only lesson in June, and it will be a great way to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity.  The lesson is included in the dance entrance price.  No experience or partner is required. -------------------------------------------------- • 6:45 pm - Doors open • 7:00 pm - TBD each week* • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *lesson with Meaghan and Bob on June 1st Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C758" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/717783180949020/</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>FRIDAY ! Fort Tectoria About Discussion More About Discussion THIS FRIDAY 🌹🌹ROSEBUDS //swing band -&amp;- MISHA MANOUCHE //gypsy jazz @ Fort Techtoria THIS FRIDAY ! Interested Going Invite Details 33 people responded Event by Rebecca Rose , Bryden Amos and Alex Q Moore Fort Tectoria Public · Anyone on or off Facebook Bring your dancing shoes, we have a whole floor to boogie on this Friday!  We are taking it back to the 30's and 40's with a night of gypsy jazz, swing and blues for you. ROSEBUDS 8pm Victoria's hot new Swing Band, formed in the heart of China Town. Playing old time swing jazz classics and original tunes with bluesy grit.  Rebecca Wells//lead singer, Alex Quincy Moore &amp; Bryden Amos// guitar + keys, Andrew Greenwood//tenor sax, Owen Chow// trumpet, Matisse Gubby-Hurtig//upright bass. We invite you to rock the night away with us, swinging our way into summer. **MISHA MANOUCHE **7pm Kicking off the night, gypsy jazz duo Misha Manouche will be bringing us velvety melodies and the spirit of Django Reinhardt to the room. Adam Paquette &amp; Alex Gnaedinger// Guitar and vocals. Catch us Fort Techtoria this Friday! 777 Fort Street Victoria BC June 27th 6:30pm Doors open Buy Pre sale ticket at 15$ by e transfering rosebudsband@gmail.com Or 20$ tickets at door See you folks there See less Victoria, British Columbia Fort Tectoria 777 Fort Street, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C759" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1035925295253912/</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Friday 18 April 2025 at 18:30 Swing out with the ATOMIC COCKTAILS 751 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Swing out with the ATOMIC COCKTAILS Details 64 people responded Event by Peter Sandmark 751 View St, Victoria, BC V8W 1J9, Canada Public · Anyone on or off Facebook Join the ATOMIC COCKTAILS as they swing out for their pre-Japan Tour dance party on April 18 at the Coda, 751 View Street.  Doors open 6 pn, show from 6:30-8:30 pm!  Tickets $20.  With songs from their new album BLUE LIGHT BOOGIE! See less Victoria, British Columbia 751 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C760" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/373500473108499/</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Sunday Swing at Logan's Logan's Pub 10 Dec 2017 Debi Wong invited you About Discussion More About Discussion Sunday Swing at Logan's Details Event by Swing X Logan's Pub Duration: 3 hr 30 min Public · Anyone on or off Facebook Sunday Swing at Logan's is BACK! Come join us for some great tunes and we'll party like it's 1939. Bring your dancing shoes, sweet moves, and a few dollars for our fabulous DJ (and gracious bartenders). Feel free to come early to hang out and grab a bite to eat. 19+. NEW: Crash course 15min swing lesson at 8:30pm! This is intended to be the bare minimum for someone to show up and know the basics of swing dancing, nothing fancy! DETAILS: * 8:30pm Quickie 15min beginner lesson! * 8:45pm social dancing until as late as midnight (maybe!) * Usually gets bluesy after 11pm See less Victoria, British Columbia Logan's Pub 1821 Cook Street, Victoria Original - Authentic - Unique Guests See All</t>
+        </is>
+      </c>
+      <c r="C761" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1776457206589544/</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Friday 21 March 2025 from 18:30-20:30 Slim Sandy's Atomic Cocktails swing speakeasy party! The Coda About Discussion More About Discussion Slim Sandy's Atomic Cocktails swing speakeasy party! Details 72 people responded Event by Peter Sandmark and Trace Nelson The Coda Duration: 2 hr Public · Anyone on or off Facebook Join Slim Sandy's Atomic Cocktails and dance as they play 2 sets of swing jazz, jive and rhythm and blues from the 20’s to the 40’s. Slim, on guitar and harmonica, is joined by Willa Mae on vocals, “Big Daddy Bo” on bass, and Bryn Bad on trumpet.  Slim Sandy has been playing music for over 40 years with acts such as Ray Condo and the Crazy Rhythm Daddies.  In 2012, he and Willa Mae co-created the Slim Sandy band in Victoria!  They have played music festivals in Canada, France, Spain, Germany, Belgium, and the Netherlands.  In May they will be touring in Japan! See less Victoria, British Columbia The Coda 749 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C762" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/302778660295534/</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Sunday 19 August 2018 from 18:00-21:00 West Coast Swing in the Park! Cameron Bandshell @ Beacon Hill Park Carolyn Gebbie invited you About Discussion More About Discussion West Coast Swing in the Park! Details 58 people responded Event by Carolyn Gebbie Cameron Bandshell @ Beacon Hill Park Duration: 3 hr Public · Anyone on or off Facebook Come join us for another evening of fun and WCS dancing in Beacon Hill Park! WCS music will be provided by DJ Carolyn. For those who are familiar with the routine, the 2018 WCS Rally Song will be played at 6:30, 7:30 and 8:30pm. Sam Jackson and Meaghan Efford, from wcsmovementmethods.com will be on hand to answer questions about WCS or how to improve your WCS dancing. They will also demo some incredible WCS dancing at 7pm. Please invite your WCS dance friends by sharing this event! See less Victoria, British Columbia Cameron Bandshell @ Beacon Hill Park Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C763" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663756533046485/</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Friday 11 April 2025 at 21:30 Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. Details 36 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Public · Anyone on or off Facebook Miguelito Valdes presents Contodo What happens when you bring together three Cuban and two Canadian musicians, with a deep love of all music and a wide range of musical experiences?  A joyful mix of party and deep groove, that's what! Guaranteed to make you want to dance, these brothers from other mothers bring it all. Con Todo! Featuring: Miguelito Valdes – brass/vocals/percussion Jose Sanchez – drumset/timbales Hector Ramos – congas/percussion Peter Dowse - bass Brooke Maxwell – keys/vocals See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C764" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663135653237580/</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Method Studio - Victoria BC Canice Ma invited you About Discussion More About Discussion WACK! Another West Coast Swing Social Dance Details 40 people responded Event by Canice Ma and Wyatt Ritchie Method Studio - Victoria BC Duration: 3 hr 30 min Public · Anyone on or off Facebook Guess who's back, it's WACK! (please ignore the fact that it's been 2 years...) The schmucks are back with another spontaneous west coast swing social dance, featuring music by DJs Topknot and Amandance from Vancouver! DETAILS: • Friday, June 20th, 2025 • Method Studio, 841 Fisgard St, Victoria, BC • 7:30-8:30 pm: "Shake That" line dance lesson featuring Kaitlyn • 8:30-11 pm: social dancing with 100% west coast swing • Admission: $10 • Water and AC on us (and maybe some bonus chocolate) • Please keep in mind that parking is limited at the venue GENERAL SOCIAL DANCE ETIQUETTE: • Consent is cool- don't be creepy. • Shake off any shyness and get out there! Ask people to dance regardless if you’re a lead or follow, dancing for 10 years or started yesterday- it's more fun that way! • No teaching or unsolicited feedback on the dance floor. Good vibes only! • If you would like to partake in a steal dance, try to remain with that group for the whole song. • Bring a water bottle! The studio is known to get warm with more bodies in the space so we want you to stay healthy and hydrated. • Personal hygiene is important! Consider bringing a towel and/or a spare shirt to change into if you sweat easily. Our studio has a bathroom and change rooms available for all to use. • We recommend wearing clothes that are easy to move in, especially pants given the nature of the dance. • Clean, comfortable shoes (ideally dance shoes) on the dance floor only! See less Victoria, British Columbia Method Studio - Victoria BC 833 Fisgard St, Victoria, BC V8W 1R9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C765" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/417338985546213/</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Thursday 29 August 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - August 29! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - August 29! Details 109 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for a fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C766" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/402729737034904/</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Thursday 5 September 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Details 123 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for our second fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C767" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2441697862726705/</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Sunday 30 June 2019 at 19:00 Journey’s 50th Birthday!!  A West Coast Swing dance party!! Eastern Star Hall Chapters No 5 &amp; No 17 Journeey Song invited you About Discussion More About Discussion Journey’s 50th Birthday!!  A West Coast Swing dance party!! Details 13 people responded Event by Journeey Song Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook 3281 Harriet Road, Victoria,BC Bring your own alcohol-free beverage... Bring a gluten-free appie if you’d like. Dance West Coast Swing until 10 pm to Blues, Pop, RnB, Swing, and a wee bit of Ballroom Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C768" s="3" t="n">
+        <v>45835.39363462963</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1766891834185825/</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam and Alive Tango Victoria Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends SAVE THE DATE! The next Sunday afternoon Milonga is on 8 June 2025 1-4pm. The Coda Club (formerly Hermanns Upstairs) is a beautiful newly renovated venue with awesome ambience, nice wood floor and great sound system. Come join us for a wonderful afternoon of warm hugs and close embrace. Sunday 8June 2025 1-4pm The Coda, 751 View Street, Victoria Admission: $15 (plus tax) Special Guest DJ: Francis Nowaczynski (from Vancouver) Free parking at View Street Parkade (next door) or Broughton Parkade. Cash bar is open for drinks. See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C769" s="3" t="n">
+        <v>45835.39596427084</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/754259983939888/</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Sunday 20 July 2025 from 12:00-17:00 Anniversary Milonga Alive Tango Victoria About Discussion More About Discussion Anniversary Milonga Interested Going Invite Details 22 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 5 hr Public · Anyone on or off Facebook 10 years of Alive Tango in Victoria! 10 years of friendships, events and exploring the music, the movement, the possibilities. 10 years of mutual support in tango and life. So many people came and moved on  but everyone left something behind, built a small piece of Alive. So many of you came but stayed building, creating and shaping us. It takes a village and we all are part of it!!! Afternoon Anniversary Milonga ! Cake (made by Danusia!!)and bubbly ( we encourage you to bring your own water bottle or a cup .. we might run out of the ones in the studio ). Let us know if you can come 12pm-5pm $10 Two amazing DJs : Carol Horowitz ( Montreal) and Dan Boccia ( Anchorage) ( the artwork by Rasanga Weerasinghe) See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C770" s="3" t="n">
+        <v>45835.39596427084</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1864555154338100/</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 21 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Alive Tango Victoria About Discussion More About Discussion Weekend with Tango Details 18 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 21st 5pm-6pm solo technique all levels. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) We will continue from May with the musicality for phrase change but this time we will add “double time” to help us with it, using examples of different orchestras. We will work with a “rebound” and half giros to change the direction within the phrase. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 22nd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are September 20th &amp; 21st. Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C771" s="3" t="n">
+        <v>45835.39596427084</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1009684807956058/</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 17 17 May at 17:00 – 18 May at 13:30 Tango weekend with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Tango weekend with Jorge Olguín Details 28 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 17th 5pm-6pm solo technique all levels. ( no partner required) Please bring elastic bands!! 6.30pm-7.30pm for couples only ( need some experience) Sacadas, barridas and colgadas in an elastic embrace in order to create a circular movement. We will work with different orchestras to study the changes we need to do to introduce different tempos and rhythms. Get ready for a workout with musicality! 8pm milonga !!! Join us even if you didn’t take the classes. DJ Ingrid !! Free for people registered for the workshops. $10 for drop-ins. Sunday, 18th 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are June 21st &amp; 22nd Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C772" s="3" t="n">
+        <v>45835.39596427084</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1318668532737609/</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 16 16 Apr at 18:30 – 18 Apr at 21:00 Tango week with Lya Alive Tango Victoria About Discussion More About Discussion Tango week with Lya Details 36 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 3 days Public · Anyone on or off Facebook Ignite Your Tango 16th of April, Wednesday 6:30-8:00 On &amp; Off Acis for social dance 18th of April, Friday 6:00 - 7:30 Follower technique 7:45 - 9:00 Switch role / connection Search - Grow &amp; Transform! Seminar series for Tango Dancers that want to transform their way of moving and connecting! We will travel through the Essentials of Tango in order to look for new answers and deeper understanding. What makes tango truly captivating? It’s the embrace, the connection, and the walk. These three fundamental elements are the heartbeat of tango, and mastering them is essential for creating an unforgettable dance experience. You will learn how to condition your body to move with control, fluidity, and elegance. You’ll discover how to find and perfect your axis, which is essential for maintaining balance and stability in every step. We will also explore dissociation, a technique that allows you to move the upper and lower body independently but associated. This workshop series will show you how to apply these principles in both the leader and follower roles, improving connection and response in every moment of the dance. We will apply all this to: The secrets to generating power for boleos effortlessly off and on axis special follower technique class Pro tips to dance with ease and confidence 90 min class - $30 All 3 classes - $80 To register email grazs@shaw.ca or pm me, or talk to me . See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C773" s="3" t="n">
+        <v>45835.39596427084</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3637725693193744/</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 22 Mar at 17:00 – 23 Mar at 13:30 Weekend with Tango with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Weekend with Tango with Jorge Olguín Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 22nd 5pm-6pm solo technique all levels. Balance and weight transfer while walking, change of dynamics to create a better connection with your body. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) Marathon is just around the corner so this month we continue with comfortable close embrace! We continue with dancing in small spaces!! Let’s move gracefully without affecting the partner's axis in elastic hugs of closed embrace. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 23rd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available only on Saturday. Sunday - sold out Next workshop dates are the May 17th &amp;18th Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C774" s="3" t="n">
+        <v>45835.39596427084</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1024182725709172/</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Saturday April 19th Lesson and Social Dance Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 19th Lesson and Social Dance Details 4 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginner plus lesson with Pamela Podmoroff from 8 to 10:15 pm Social dancing from 8 to 10:15 pm DJs Donna and Amanda Cost $15/ $12 for students No need to register and no partner required. Please bring scuff-free indoor dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C775" s="3" t="n">
+        <v>45835.39859219908</v>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1366072544640156/</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Saturday 17 May 2025 at 18:45 Victoria WCS Collective Beginner Lesson and Social Dancing Dance Victoria About Discussion More About Discussion Victoria WCS Collective Beginner Lesson and Social Dancing Details 9 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson from 7 to 8 pm by John de Pfyffer Social dancing from 8 to 10:15pm DJg by Donna and Nel Cost $15/ $12 for students No need to register and no need for dance experience.. Also, no partner necessary, we got you! Please bring indoor scuff-free dance shoes or socks to dance in. See less Victoria, British Columbia Dance Victoria 2750 Quadra St # 111, Victoria Dance Victoria brings the "World's Best Dance" to the Royal Theatre and supports new dance creation for the international stage from its studios. Guests See All</t>
+        </is>
+      </c>
+      <c r="C776" s="3" t="n">
+        <v>45835.39859219908</v>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/516994561244886/</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:45 Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING White Eagle Polish Association About Discussion More About Discussion Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING Details 15 people responded Event by Donna Forsyth , Andre Russo and Victoria West Coast Swing Collective White Eagle Polish Association Public · Anyone on or off Facebook Doors open at 6:45pm at this fabulous new venue! Advanced beginner/intermediate lesson by Chantelle Pianetta from 7 to 8 pm Social dancing for 3 HOURS from 8 to 11 pm DJs Donna and Andre Cost $15 /$12 for students ALL at the spacious White Eagle Hall No need to register and you do not need a dance partner. Please bring scuff-free dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia White Eagle Polish Association 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C777" s="3" t="n">
+        <v>45835.39859219908</v>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1225266505917189/</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Saturday Beginner Lesson and Social Dancing Dance Victoria Sat, 14 Jun Sat, 21 Jun Sat, 28 Jun Sat, 12 Jul +3 About Discussion More About Discussion Victoria WCS Collective hosts Saturday Beginner Lesson and Social Dancing Interested Going Invite Details 8 people responded Event by Donna Forsyth Dance Victoria Duration: 3 hr 30 min Public · Anyone on or off Facebook Back to AIR CONDITIONED comfort at Dance Victoria Studios Beginner lesson from 7 to 8 pm Social dancing  from 8 to 10:15 pm Cost $15/$12 for students No need to register and no need for previous dance experience or a partner. Please bring scuff-free inside low-heeled dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C778" s="3" t="n">
+        <v>45835.39859219908</v>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/641769172035949/</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Saturday April 12 Beginner lesson and social dance at Dance Victoria Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 12 Beginner lesson and social dance at Dance Victoria Details 5 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginners lesson by Donna from 7 to 8 pm Social dancing from 8 to 10:15 pm DJs Andre and Nel Cost $15 /$12 for Students No need to register and no partner required. Please bring scuff-free inside dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C779" s="3" t="n">
+        <v>45835.39859219908</v>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/967438905456066/</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Wednesday 26 March 2025 at 10:00 Victoria WCS Lesson and Dance at Eastern Star Hall Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria WCS Lesson and Dance at Eastern Star Hall Details 1 person responded Event by Donna Forsyth Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson by John de Pyffer from 7 to 8 pm Social dancing from 8 to 10:15pm Djs Amanda and Nel Cost $12 No need to register and no partner required. Please bring scuff-free indoor shoes or socks to dance in  and a water bottle. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C780" s="3" t="n">
+        <v>45835.39859219908</v>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2162855673833831/</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 11 May 2019 18 May 2019 25 May 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 8 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook Wow! April went by so quickly, which means it must've been super fun, which it definitely was.  Everyone at BC Swing Dance Club Victoria is so pleased with the way the first month of social dances went, and we hope to generate the same amount of enthusiasm in May. Let's make this month just as much fun! Come join us on May 4th for the first intro lesson and social dance of the month (plus every Saturday night after that). Just $10 for the lesson and/or social dance ($5 for students). No experience or partner required. • 6:45 pm - Doors open • 7:00 pm - Intro lesson with Sam Jackson and Meaghan Efford * • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *PLEASE NOTE that the weekly lessons will start PROMPTLY at 7pm.  It is disruptive to the flow of the lesson if participants arrive late. For anyone who's interested in building their West Coast Swing fundamentals quickly, note that May will be the last month we'll be offering weekly classes with both Sam and Meaghan. With summer approaching it's a great time to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity. Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C781" s="3" t="n">
+        <v>45835.39859219908</v>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3963074663954670/</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Tuesday dances Eastern Star Hall Chapters No 5 &amp; No 17 Tue, 15 Jul Tue, 22 Jul Tue, 29 Jul About Discussion More About Discussion VIctoria WCS Collective Tuesday dances Interested Going Invite Details 1 person responded Event by Donna Forsyth and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 6 hr 45 min Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Saanich, BC V8Z 3S3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C782" s="3" t="n">
+        <v>45835.39859219908</v>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/713923214640962/</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Sunday 4 May 2025 from 13:00-16:00 May 4th Afternoon Milonga Solwood Studio About Discussion More About Discussion May 4th Afternoon Milonga Details 45 people responded Event by Ingrid Love and Kathryn Stone Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook A one-time special afternoon milonga! Join us in celebrating the warmth of Spring and return to sunshine. Or, star wars, if you like. Featuring special guests Kimberly and Khang performing live music (violin/guitar) DJ Ingrid Hosts: Kathryn &amp; Ingrid $15 entry (cash only) 1:00pm-4:00pm Solwood Studio 1303 Broad St Victoria, BC See less Victoria, British Columbia Solwood Studio Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C783" s="3" t="n">
+        <v>45835.3998534838</v>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/644050564927019/</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends! A NEW SUNDAY AFTERNOON MILONGA! This is the first of a regular monthly milonga at a beautiful new venue…The Coda Club (formerly Hermann’s Upstairs) at 751 View Street, Victoria. Great ambience, nice wood floor, good sound system. So come join us for the warm hugs and close embrace and dance to the beautiful music of our very own DJ John Dewhirst. Sunday, 6 April 2025 2.00pm-5.00pm The Coda Club, 751 View Street, Victoria Admission $15 DJ: John Dewhirst Cash Bar is open for drinks Free Parking at View Street Parkade just next door Come celebrate this exciting day with us! See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C784" s="3" t="n">
+        <v>45835.3998534838</v>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1022330066692643/</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Wednesday 2 July 2025 at 18:30 Technique and Milonga with Monica Parra Alive Tango Victoria About Discussion More About Discussion Technique and Milonga with Monica Parra Interested Going Invite Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Public · Anyone on or off Facebook 2nd of July , Wednesday 6.30-8pm Follower’s technique: Pivots and turns • Dissociation technique and axis control. • Free leg preparation before the turn. • Turns in tight spaces (useful in a close embrace!!) 90 minutes, $30 9th of July , Wednesday 6.30-8pm Couple workshop: Milonga Lisa and Milonga with traspie using different tempo. 90 minutes, $30 Both workshops (July 2nd and 9th)$50 Register with Grazyna (grazs@shaw.ca, Messenger or simply talk to me) Contact me personally for privates with Monica. See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C785" s="3" t="n">
+        <v>45835.3998534838</v>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1142760357225336/</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 26 26 Jul at 10:00 – 27 Jul at 17:00 ArtisTREE Festival 1401 rockland ave, Victoria, BC, Canada About Discussion More About Discussion ArtisTREE Festival Interested Going Invite Details 1.3K people responded Event by Artistree Festival , MORENA CLOTHING and Cory Judge 1401 rockland ave, Victoria, BC, Canada Duration: 2 days Public · Anyone on or off Facebook Saturday July 26 10-7pm Sunday July 27 10-5pm Government House of BC 1402 Rockland Ave Celebration of Creativity profiling 130 Juried Artisans, Live Music, Installation and Performance Art, Indigenous Makers and Traditions, Kids section, Live Painters, Delicious Food and Ice cream. See less Shopping Victoria, British Columbia 1401 rockland ave, Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C786" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/650159601522409/</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>(20+) Rest and Resonate - Restorative Yoga ft. cozy Live Music  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 9 Saturday 9 August 2025 at 19:30 Rest and Resonate - Restorative Yoga ft. cozy Live Music Fernwood Community and Arts Association About Discussion More About Discussion Rest and Resonate - Restorative Yoga ft. cozy Live Music Interested Going Invite Details Event by Across the Water Fernwood Community and Arts Association Tickets www.annabiglandpritchard.com/event-details/rest-resonate-restorative-yoga-ft-cozy-live-music-1 Public · Anyone on or off Facebook A dreamy and nourishing evening retreat offering restorative yoga, live music, and guided journalling. Fresh on the heels of the August full moon in Aquarius - this is a great time to charge up your batteries and dream up visionary ways to improve the state of world together. Facilitated by: Roxie Fehr of Across the Water Yoga and Wellness | Yoga, guided meditation, and Indian Head Massage  &amp; Anna Bigland-Pritchard of Rose House | Music (harp, vocal looping, singing) &amp; poetry reading What to bring: Yoga mat Journal &amp; pen/pencil Yoga bolster Yoga blocks Blanket Any other props you'd like to use Yourself as you are Details August 19, 7-8:30pm at Little Fernwood If cost is a barrier, please contact us directly as we have a limited number of discount codes available Come as you are, leave nourished by your dreams See less Music and audio Victoria, British Columbia Tickets Find Tickets Fernwood Community and Arts Association 1923 Fernwood Rd., Victoria Welcome to the Fernwood Community and Arts Association FB page. This site is used to distribute updates on FCAA meetings, initiatives and events. Join or renew your membership at www.thefca.ca or our office 1923 Fernwood Rd. Meet your host Across the Water 2 past events · Page · Fitness trainer Across the Water facilitates Yoga and Group Fitness in Victoria, BC. We value community and connection and just love to have fun while moving ou… Contact Us Suggested events Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested 31 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1505 people interested Interested Happening now AfriCa Fest Victoria 12e Edition Centennial Square Ali, Debi and 2 friends 589 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Today at 18:00 🎉 You're invited to AfriCa Fest Victoria’s Special African Drumming Night! 🥁 Victoria, Canada Sophia and Carmie are interested Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C787" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1093118172681618/</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>(20+) The Joan Bessie Cabaret: a celebration of original  live music and dance | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 29 Sunday from 19:00-22:00 The Joan Bessie Cabaret: a celebration of original  live music and dance Metro Studio Theatre About Discussion More About Discussion The Joan Bessie Cabaret: a celebration of original  live music and dance Interested Going Invite Details Event by Joan Bessie Metro Studio Theatre Tickets · CA$5-CA$35 www.eventbrite.ca/e/joan-bessie-cabaret-tickets-1248762816199 Public · Anyone on or off Facebook Get ready to experience a night of songs and choreography at this one-of-a-kind indie cabaret. Licensed all ages event. Music and audio Victoria, British Columbia Tickets Find Tickets Metro Studio Theatre 1411 Quadra Street at Johnson Street, Victoria Meet your host Joan Bessie 13 past events · Page · Musician/band Joan Bessie is a chart topping Canadian artist. This page shares releases &amp; live tour information Message Suggested events This Sunday at 19:00 GROOVE KITCHEN'S JUNEFEST DANCE!! Hermann's Jazz Club Carmie is interested 98 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1505 people interested Interested Sat, 5 Jul at 12:00 Victoria, BC - Victoria Folk Music Festival, Royal Athletic Park Royal Athletic Park Debi and Carmie are interested 1296 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Today at 18:00 🎉 You're invited to AfriCa Fest Victoria’s Special African Drumming Night! 🥁 Victoria, Canada Sophia and Carmie are interested Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C788" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1137992241425588/</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Today from 13:00-15:00 Music in Abkhazi Garden Abkhazi Garden Fri, 27 Jun Fri, 4 Jul Fri, 11 Jul +5 About Discussion More About Discussion Music in Abkhazi Garden Interested Going Invite Details 13 people responded Event by Victoria Conservatory of Music Abkhazi Garden Duration: 2 hr Public · Anyone on or off Facebook Abkhazi Garden hosts Victoria Conservatory of Music students and faculty for a season of live outdoor performances from June 13 to August 15, every Friday from 1:00pm to 3:00pm. Admission is by donation. The address of Abkhazi Garden is 1964 Fairfield Road, Victoria, BC V8S 1H4 See less Victoria, British Columbia Abkhazi Garden 1964 Fairfield Road, Victoria Explore a one-of-a-kind west coast, heritage garden in a quiet Victoria neighborhood on Vancouver Island. Open seven days a week 11 am – 5 pm. Last entrance, 4:00pm. Entrance by donation. We suggest $10/person. Guests See All</t>
+        </is>
+      </c>
+      <c r="C789" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1085685423617722/</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Thursday 25 September 2025 at 10:00 The Men in Black: A Tribute to the Music of Johnny Cash Mcpherson Playhouse About Discussion More About Discussion The Men in Black: A Tribute to the Music of Johnny Cash Interested Going Invite Details 3 people responded Event by Jeff Scott and Victoria Live Music - @BarsnbandsYYJ Mcpherson Playhouse Public · Anyone on or off Facebook The Men in Black: The Songs and stories of Johnny Cash, presented Live onstage in this Multimedia production. Featuring special guest Tracee Rees singing the parts of June Carter Cash. Tickets on sale from the McPherson Box Office: https://www.rmts.bc.ca/.../2025.../the-men-in-black/ See less Victoria, British Columbia Mcpherson Playhouse 48.428809, -123.366838 Guests See All</t>
+        </is>
+      </c>
+      <c r="C790" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1975172826621817/</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>(20+) Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Thursday 12 June 2025 from 19:00-20:30 Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Little Fernwood Gallery. About Discussion More About Discussion Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Details Event by Across the Water and Anna Bigland-Pritchard Little Fernwood Gallery. Duration: 1 hr 30 min Public · Anyone on or off Facebook Do you need some R&amp;R? Join Anna &amp; Roxie for a dreamy candlelit evening of restorative yoga, live music, and guided journalling. Facilitated by Roxie Fehr of Across the Water | Yoga Anna Bigland-Pritchard of ABP Music Studio | Music As experienced, intuitive space-holders, our goal to support your Nervous System and capacity for hope with a feast of restful offerings. We know life is stressful and we want to help you feel more connected to your intuition so you can not only survive, but also have the capacity to take the next right step in your life in a way that positively impacts the world. The space will be dreamy, there will be tea, guided journalling, poetry, restorative yoga shapes that can be adapted for any body, and LIVE MUSIC! Anna will be playing guitar, creating dreamy sound worlds with vocal looping, and singing you lullabies all evening. What to bring Yoga mat (We'll have a few available to borrow) Journal &amp; pen/pencil (We'll also have some spare paper and writing/drawing utensils) Yourself in your comfy cozies Details June 12, 7-8:30pm at Little Fernwood $42 Accessibility This event is on the ground floor There is a unisex/non-gendered bathroom on the same level We care about making this event accessible, so please let us know if you have any questions or accessibility needs. This will be a VERY gentle practice, and modifications will be offered. Happy pride! As members of and allies of the 2SLGBTQIA community, we (Anna &amp; Roxie) will create a supportive, inclusive, affirming environment and expect all participants to do the same. If cost is a barrier, please contact us directly as we have a limited number of discount codes available This is our first time offering this class, and we hope it will be a hit so we can make it a regular thing. Come as you are, leave nourished by your dreams See less Victoria, British Columbia Little Fernwood Gallery. 1923 Fernwood Ave., Victoria Meet your hosts Across the Water 2 past events · Page · Fitness trainer Across the Water facilitates Yoga and Group Fitness in Victoria, BC. We value community and connection and just love to have fun while moving ou… Contact Us Anna Bigland-Pritchard 6 past events · Page · Musician/band Based in Lekwungen territory (Victoria, BC), Anna Bigland-Pritchard is a: -Soprano -Voice teacher… Follow Suggested events Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested 31 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1505 people interested Interested Happening now AfriCa Fest Victoria 12e Edition Centennial Square Ali, Debi and 2 friends 589 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Today at 18:00 🎉 You're invited to AfriCa Fest Victoria’s Special African Drumming Night! 🥁 Victoria, Canada Sophia and Carmie are interested Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C791" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1239927167616785/</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Thursday 11 September 2025 at 19:00 Rest and Resonate - Restorative Yoga ft. cozy Live Music Fernwood Community and Arts Association About Discussion More About Discussion Rest and Resonate - Restorative Yoga ft. cozy Live Music Interested Going Invite Details 9 people responded Event by Across the Water Fernwood Community and Arts Association Tickets www.annabiglandpritchard.com/event-details/rest-resonate-restorative-yoga-ft-cozy-live-music-1-1 Public · Anyone on or off Facebook A dreamy and nourishing evening retreat offering restorative yoga, live music, and guided journalling. Still warm with the energy of the September full moon in Pisces (the Corn Moon) - this is a great time to celebrate and embrace life, nourishing our bodies so they can carry out our most impactful dreams. Facilitated by: Roxie Fehr of Across the Water | Yoga, Meditation, and Indian Head Massage &amp; Anna Bigland-Pritchard of Rose House | Music (harp, vocal looping, singing) and poetry reading What to bring: Yoga mat Journal &amp; pen/pencil Yoga bolster Yoga blocks Blanket Any other props you'd like to use Yourself as you are Details: Thursday September 11th, 7-8:30pm at Little Fernwood If cost is a barrier, please contact us directly as we have a limited number of discount codes available Come as you are, leave nourished by your dreams See less Victoria, British Columbia Tickets Find Tickets Fernwood Community and Arts Association 1923 Fernwood Rd., Victoria Welcome to the Fernwood Community and Arts Association FB page. This site is used to distribute updates on FCAA meetings, initiatives and events. Join or renew your membership at www.thefca.ca or our office 1923 Fernwood Rd. Guests See All</t>
+        </is>
+      </c>
+      <c r="C792" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/686146924271113/</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>(20+) Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 5 Thursday 5 June 2025 from 19:00-22:00 Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz 753 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz Details Event by Adonis Puentes and Brent Jarvis 753 View St, Victoria, BC V8W 1J9, Canada Duration: 3 hr Public · Anyone on or off Facebook An evening of Jazzy Cuban Fusion Music; traditional, contemporary, romance and dance. Juno &amp; Grammy Nominated vocalist, Adonis Puentes, will be joined by the Jazz Bohemians, featuring Brent Jarvis (piano), Ken Lister (bass), Nicholas Marquez (percussion) and Brooke Maxwell (Sax). Adonis Puentes opens up the marvelous world of Cuban music to his audience the second they hear his rich voice. When the other players kick in with their tight, multi-layered arrangements, it becomes clear that Adonis is a powerful bandleader. Fronting an acoustic band, Adonis' vocals are surrounded by piano, bass, strings, and percussion. Music reflects the present and Adonis Puentes is a Cuban Sonero for our times. Adonis thrives on the growth and acclaim for his original sonero sound. As he puts it, "I feel like a messenger of my roots and tradition, blessed that with me I have taken my music and heritage to many different places in the world; from Cuba, to Canada, USA, Mexico, Europe and Asia. My mission is to make you dance and enjoy my melodies and rhythms." Musician Line-Up: Adonis Puentes - Vocals Brent Jarvis - Piano Ken Lister - Bass Nicolas Marquez - Percussion Brooke Maxwell - Sax See less Music and audio Victoria, British Columbia 753 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Meet your hosts Adonis Puentes 34 past events · Page · Musician/band Adonis Puentes is a great singer and an elegant composer and lyricist grounded and nourished by his Cuban roots and worldly experience. Message Brent Jarvis 37 past events · Profile · Musician Message Suggested events Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1505 people interested Interested Fri, 29 Aug at 19:00 GLOW • i-Land Fest Kick-Off Fete Ambrosia Banquet Nadia is interested 129 people interested Interested Thu, 18 Sep at 18:00 THE WAILERS NATURAL MYSTIC 30TH ANNIVERSARY TOUR - THUR. SEPT 18 AT ROYAL ATHLETIC PARK IN VICTORIA! Royal Athletic Park Linda is interested 581 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Today at 18:00 🎉 You're invited to AfriCa Fest Victoria’s Special African Drumming Night! 🥁 Victoria, Canada Sophia and Carmie are interested Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C793" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1399479741193649/</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Saxe Point Public House About Discussion More About Discussion TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Details 4 people responded Event by Tom Watson Saxe Point Public House Public · Anyone on or off Facebook Join Vinyl Wave at the lovely Saxe Point Pub for a couple of hours of smooth tunes that'll help ease you into the week! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C794" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/665127126496204/</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Tuesday 27 May 2025 at 19:30 Live Music at the Saxe Point Public House Saxe Point Public House About Discussion More About Discussion Live Music at the Saxe Point Public House Details 9 people responded Event by VINYL WAVE Saxe Point Public House Public · Anyone on or off Facebook Live Music every other Tuesday starting May 27th! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C795" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1414577976223422/</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 19:00-23:00 Solstice Slammer 3 - Moon Under Water, Victoria The Moon Under Water Brewpub About Discussion More About Discussion Solstice Slammer 3 - Moon Under Water, Victoria Details 68 people responded Event by Electric Druids and Gate Theory The Moon Under Water Brewpub Duration: 4 hr Public · Anyone on or off Facebook Come join us for Solstice Slammer III at Moon Under Water Brewpub and Distillery! Get ready to celebrate with Electric Druids, Gate Theory and West Street Children, hefty drinks and good vibes. Whether you're a craft beer enthusiast or just an enthusiast, there's something for everyone at this epic night of live music. Don't miss out - mark your calendars! See less Music and audio Victoria, British Columbia The Moon Under Water Brewpub 5435 Fowler Rd, Saanich, BC V8Y 1Y4, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C796" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1482463219409922/</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Wednesday 2 July 2025 from 19:30-19:31 Live Music Sessions at Crafthouse Vic West #100 - 184 Wilson Street, Victoria, BC, Canada About Discussion More About Discussion Live Music Sessions at Crafthouse Vic West Interested Going Invite Details 1 person responded Event by Browns Crafthouse Vic West #100 - 184 Wilson Street, Victoria, BC, Canada Duration: 1 min Public · Anyone on or off Facebook Join us every Wednesday night for local live music starting at 730pm. 1/2 wings &amp; 1/2 bottles of wine. Victoria, British Columbia #100 - 184 Wilson Street, Victoria, BC, Canada 184 Wilson St, Victoria, BC V9A 7N6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C797" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2579625309035667/</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Sunday 18 May 2025 from 12:00-18:00 Live Music @ Junction (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Live Music @ Junction (RAIN OR SHINE) Details 125 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Here we go again, its a long weekend so let's get our Sunday Funday on. First Live Music of the year at Junction Up first is-  Emergency Exit  are playing from 1230-230pm To take us home is - An &amp; Ben are playing from 3-5pm Tasting Room and Picnic Area are open 12-6pm Oh and if you haven't heard me say it before ITS RAIN OR SHINE. Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Cider ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Mini Market and a Beautiful location ⠀⠀⠀⠀⠀⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your well behaved two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C798" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1225611168970110/</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends 26 Jun at 19:00 – 29 Jun at 20:00 AfriCa Fest Victoria 12e Edition Ali and 3 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 25 25 Jul at 17:30 – 26 Jul at 20:00 Indigenous Music Festival Hampton Park About Discussion More About Discussion Indigenous Music Festival Interested Going Invite Details 672 people responded Event by Saanich Parks, Recreation &amp; Community Services Hampton Park Duration: 2 days Public · Anyone on or off Facebook Celebrate the 5th Annual Indigenous Music Festival at Hampton Park! A free two-night celebration of Indigenous performers from across Vancouver Island. Craft market and food vendors on site as well. Friday, July 25, 2025, from 5:30 to 8:00pm -Esquimalt Drummers and Dancers -OTR (Off the Reservation) -James Vickers Band Saturday, July 26, 2025, from  5:00 to 8:00pm -Lekwungen Traditional Dancers -Killed Instantly -Yellow Wolf w/ Benny the Jet -Nate Harris - Nate Harris Band featuring Madison Olsen Learn more at saanich.ca/indigenousmusicfestival See less Music and audio Victoria, British Columbia Hampton Park 224 Hampton Rd, Saanich Guests See All</t>
+        </is>
+      </c>
+      <c r="C799" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1050242777151793/</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends 26 Jun at 19:00 – 29 Jun at 20:00 AfriCa Fest Victoria 12e Edition Ali and 3 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 10 Jun at 09:00 – 15 Jun at 19:00 KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Victoria ,BC About Discussion More About Discussion KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Details 46 people responded Event by Congregation Emanu-El, Victoria, British Columbia Victoria ,BC Duration: 6 days Public · Anyone on or off Facebook Registration required for both in person and virtual attendance. https://klezcadia.org https://congregationemanuelnews.wordpress.com/.../klezca.../ Locations of performances and workshops provided upon registration. See less Victoria, British Columbia Victoria ,BC 528 Broughton St, Victoria, BC V8W 1C6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C800" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1451663826076478/</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Sunday 6 July 2025 from 11:00-16:00 Saanich Strawberry Festival Beaver Lake Regional Park, 728 Beaver Lake Rd. About Discussion More About Discussion Saanich Strawberry Festival Interested Going Invite Details 1K people responded Event by Saanich Parks, Recreation &amp; Community Services Beaver Lake Regional Park, 728 Beaver Lake Rd. Duration: 5 hr Public · Anyone on or off Facebook Join Saanich in celebrating the 58th annual Strawberry Festival. This family-friendly, fun, free event features live music, kids' activities, bouncy castles, information booths, arts and craft stations and, of course, the traditional servings of strawberries and ice cream. Strawberries and ice cream sales and service will be from 2 to 4pm, or until sold out. $2/serving. For more details, including vendors, activities and performances, visit saanich.ca/strawberryfestival See less Foods Victoria, British Columbia Beaver Lake Regional Park, 728 Beaver Lake Rd. 728 Beaver Lake Rd, Saanich, BC V8Z 6K2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C801" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1110747367748372/</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Saturday 5 July 2025 at 12:00 Victoria Folk Music Festival Royal Athletic Park About Discussion More About Discussion Victoria Folk Music Festival Interested Going Invite Details 982 people responded Event by Victoria Folk Music Festival and Cascadia Concerts Royal Athletic Park Tickets · Free-CA$86.53 vicfolkfest.eventbrite.ca Public · Anyone on or off Facebook Date: July 5, 2025 Location: Royal Athletic Park, Victoria, BC Tickets: Available now at vicfolkfest.eventbrite.ca Gates Open: 12:00 PM Victoria Folk Music Festival Join us for a joyful weekend of music, community, and celebration at Victoria Folk Music Festival, on July 5th set in beautiful Royal Athletic Park . Featuring a world-class lineup including Frazey Ford, Joel Plaskett, Kacy &amp; Clayton, Harry Manx, Ferron, Old Man Luedecke, Vince Vaccaro, Canadian Beauty, Daneil Lapp's BC Fiddle Orchestra and more, this family-friendly event brings together the best in folk, roots, and Americana music. With two stages of live performances, the Victoria Folk Music Festival offers a full day of entertainment and community celebration. Explore the ReLove Vintage Pop-Up Market, showcasing top local vendors with the best in thrift, retro, and vintage wear. Enjoy a variety of Artisan goods and vendors, delicious food from Fresh Coast, Deadbeetz, Taco Revolution, and more. Families will love the vibrant children’s area—complete with a jumping castle! Dance in the grass to local Bluegrass groups and explore vendor booth from local music groups &amp; organizations. A community-driven atmosphere with world-class music at its heart, this festival is set to be a summer highlight for music lovers of all ages. Whether you're dancing barefoot in the grass, discovering your new favorite artist, or relaxing in the shade with friends, the Victoria Folk Music Festival is more than a concert — it’s a celebration of sound, soul, and connection. Don’t miss the unforgettable music and summer moments —July 5th at Royal Athletic Park! See less Music and audio Victoria, British Columbia Tickets Find Tickets Royal Athletic Park 1014 Caledonia Ave, Victoria Royal Athletic Park is a multi-purpose, fully lit stadium in Victoria, British Columbia. It is primarily used for baseball, soccer, softball and football, but also hosts special events, such as the annual Great Canadian Beer Festival and Rifflandia Music Festival. It is approximately a ten-minute walk from the city centre.HistoryIn 1907 the burgeoning summer athletic teams did not have enough facilities for senior teams with paid attendances. Baseball in particular was challenged to find available dates at Oak Bay Grounds to operate due to a preference for lacrosse.Subsequently, the supporters of Canada's national summer sport lacrosse, at a meeting chaired by BC Premier McBride formed the Royal Victoria Athletic Association on March 26, 1908, and a senior lacrosse team was founded to enable the best intermediate (Under 21) players to play in the British Columbia Amateur Lacrosse Association (BCALA) League. The Oak Bay Grounds were put under the management of the senior baseball team and then later the Rugby Football Club. The lacrosse group, later shortened to the Royal Athletic Association, issued shares at $25 each with deposits of 10% and biannual calls of 10% to raise $25,000 for improvements to the grounds. The lease was signed for 5 acres at the corner of Cook and Pembroke Streets for the grounds.Contracts had been let by May 12, 1908 and $4,000 from the share offering and gate receipts was spent by June on the construction of a perimeter fence, 2 ticket offices, an inner fence, grandstand, and carriage parking area. The inner fence enclosed the 500 ft x 285 ft (152m x 87m) playing field. The grandstand on the south side of the playing field was 150 ft long x 25 ft deep with 10 rows of seats for more than 1000 spectators. Beneath the grandstand were dressing rooms and concessions. The original layout of the field and grandstand was essentially the same as today's; however based on maps used in advertising the original field also included half of the city block to the west between Quadra and Vancouver Streets. The carriage parking was on the east side off Cook Street. Guests See All</t>
+        </is>
+      </c>
+      <c r="C802" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1514674672845802/</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Saturday 5 July 2025 at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park About Discussion More About Discussion Oak Bay Summer Concerts in the Park: Family Show Interested Going Invite Details 766 people responded Event by Oak Bay Parks, Recreation and Culture Willows Park Public · Anyone on or off Facebook Oak Bay Summer Concerts in the Park: Family Show With a stunning backdrop of Willows Beach, these outdoor concerts gather the community to celebrate music and the arts.  Presented by Oak Bay Parks, Recreation and Culture. Location: Willows Beach Park, Oak Bay Date: Saturday, July 5, 2025 Time: 2:00 p.m. Admission: Free Family Concert: lək̓ʷəŋən Traditional Dancers, Pacific Opera Victoria, STAGES Dance Company, and Marimba Mufaro. More information: https://www.oakbay.ca/.../oak-bay-summer-concerts-in-the.../ See less Victoria, British Columbia Willows Park 2778 Dalhousie St, Oak Bay, BC V8R, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C803" s="3" t="n">
+        <v>45835.40737312785</v>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/651664851189740/</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 12:00-18:00 Music in the Orchard (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Music in the Orchard (RAIN OR SHINE) Details 330 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Come enjoy the start of the summer in the orchard. We have two amazing artists for you, some delicious fun summer ciders for you to try and amazing food to enjoy to complete the experience. Delicious Cider Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀ Beautiful location ⠀⠀⠀⠀ Dog Friendly ⠀⠀ ⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your WELL BEHAVED two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C804" s="3" t="n">
+        <v>45835.40737312785</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uncommented the last bit of code that Google used to use in clean_up_address(). It now uses foursquare.
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C804"/>
+  <dimension ref="A1:C921"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12244,7 +12244,7 @@
         </is>
       </c>
       <c r="C786" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="787">
@@ -12259,7 +12259,7 @@
         </is>
       </c>
       <c r="C787" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="788">
@@ -12274,7 +12274,7 @@
         </is>
       </c>
       <c r="C788" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="789">
@@ -12289,7 +12289,7 @@
         </is>
       </c>
       <c r="C789" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="790">
@@ -12304,7 +12304,7 @@
         </is>
       </c>
       <c r="C790" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="791">
@@ -12319,7 +12319,7 @@
         </is>
       </c>
       <c r="C791" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="792">
@@ -12334,7 +12334,7 @@
         </is>
       </c>
       <c r="C792" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="793">
@@ -12349,7 +12349,7 @@
         </is>
       </c>
       <c r="C793" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="794">
@@ -12364,7 +12364,7 @@
         </is>
       </c>
       <c r="C794" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="795">
@@ -12379,7 +12379,7 @@
         </is>
       </c>
       <c r="C795" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="796">
@@ -12394,7 +12394,7 @@
         </is>
       </c>
       <c r="C796" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="797">
@@ -12409,7 +12409,7 @@
         </is>
       </c>
       <c r="C797" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="798">
@@ -12424,7 +12424,7 @@
         </is>
       </c>
       <c r="C798" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="799">
@@ -12439,7 +12439,7 @@
         </is>
       </c>
       <c r="C799" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="800">
@@ -12454,7 +12454,7 @@
         </is>
       </c>
       <c r="C800" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="801">
@@ -12469,7 +12469,7 @@
         </is>
       </c>
       <c r="C801" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="802">
@@ -12484,7 +12484,7 @@
         </is>
       </c>
       <c r="C802" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="803">
@@ -12499,7 +12499,7 @@
         </is>
       </c>
       <c r="C803" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
       </c>
     </row>
     <row r="804">
@@ -12514,7 +12514,1762 @@
         </is>
       </c>
       <c r="C804" s="3" t="n">
-        <v>45835.40737312785</v>
+        <v>45835.407373125</v>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1185783966345055/</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 10:00-13:00 Shuffle Dance Workshop Victoria, BC About Discussion More About Discussion Shuffle Dance Workshop Details 12 people responded Event by Adelène Buchanan Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another SHUFFLE WORKSHOP coming your way!! Join our Shuffle Dance Workshop and learn a full shuffle choreography set to an energetic electronic track. We’ll guide you through each step, focusing on key shuffle movements, while incorporating them into a dynamic routine. Perfect for ALL LEVELS! This workshop will help you improve your footwork, coordination, and cardiovascular stamina as you master a complete choreography. Here’s what you need to know: DATE: Sunday, May 25th TIME: 10am - 1pm PLACE: The Beat Clinic (1303 Broad Street) Sign-up link here https://www.thebeatclinic.ca/ See less Victoria, British Columbia Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C805" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/624858640069610/</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and Vivek Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 Friday 22 August 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 133 people interested Interested Sun, 27 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Ali and 3 friends 45 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C806" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1187402793186660/</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 08:00-12:00 Global Underscore Solstice Dance Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada About Discussion More About Discussion Global Underscore Solstice Dance Details 62 people responded Event by Arunimá McNeish , Michael McAmmond and Victoria Contact Improv Jam Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada Duration: 4 hr Public · Anyone on or off Facebook Sweet dancers, This summer solstice we extend a warm invitation to join us in expanding and deepening our practice of Contact Improvisation with participation in The Global Underscore. Please arrive at 8am to join a 40 minute talk-through, introducing the concepts of the Underscore. This is mandatory if you have never attended an Underscore before. The Underscore will begin promptly at 8:45am. If you have attended a talk-through before you're welcome to arrive at this time. We will all start and end together. This is a closed container and we will not be allowing late-comers. TIMELINE: 8am-8:40am Underscore Talk-Through with Arunima 8:45am-11:30am Underscore 11:30am-11:50am Closing Circle COST: $15-$20  etransfer or pay cash at the door if pre-registered (if money is a barrier please reach out to discuss options). Please contact Arunima at ode.to.thylacine@gmail.com for registration, etransfer, questions, etc. VENUE: Centennial United Church (612 David St, Victoria, BC). MORE INFO: The Underscore, which has been evolving since 1990, is a vehicle for incorporating Contact Improvisation into the broader arena of improvisational dance practice; developing greater ease dancing in spherical space—alone and with others; and for integrating kinesthetic and compositional aspects while improvising. It allows for a full spectrum of energetic and physical expressions, embodying a range of forms and changing states. Its practice is familiar yet unpredictable. The practice progresses through a broad range of dynamic states, including long periods of very small, private, and quiet internal activity and other times of higher energy and interactive dancing. There are 20+ phases, 12+ connections, and 7 aspects of the Underscore—each with a name and a graphic symbol—which create a general map for the dancers. Within that frame, dancers are free to create their own movements, dynamics, and relationships—with themselves, each other, the group, and the environment. Each Underscore is unique, providing rich and often inspiring experiences of the human and artistic phenomena of dance improvisation. https://globalunderscore.com/ https://nancystarksmith.com/underscore/ See less Victoria, British Columbia Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada 612 David St, Victoria, BC V8T 2E1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C807" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1363696181561219/</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:00-22:00 Pride Contra Dance Fairfield United About Discussion More About Discussion Pride Contra Dance Details 90 people responded Event by Victoria Contra Dance , Code Tron and Rose Jackson Fairfield United Duration: 3 hr Public · Anyone on or off Facebook 𝕍𝕀ℂ𝕋𝕆ℝ𝕀𝔸 ℂ𝕆ℕ𝕋ℝ𝔸 𝔻𝔸ℕℂ𝔼 𝕊𝕆ℂ𝕀𝔼𝕋𝕐 ℙℝ𝔼𝕊𝔼ℕ𝕋𝕊: The return of our ℚ𝕌𝔼𝔼ℝ Contra Dance to celebrate the month of Pride! All Dancers welcome! Join us Friday, June 20th at the United Commons Fellowship Hall to do-si-do the night away to sprightly fiddle tunes and stellar performances from our two favorite drag performers! We'll have more capacity than our previous Valentines Day Dance, but we still might sell out, so grab your tickets online here! https://clannamorna.ca/.../ticket-victoria-pride-contra.../ ......................................................................................................... 𝕄𝕦𝕤𝕚𝕔 𝔹𝕪: 𝐑𝐨𝐬𝐞 𝐉𝐚𝐜𝐤𝐬𝐨𝐧: she/her Coming up in the rich folk scene of western Massachusetts, Rose is based in Montague, MA, where she studied under fiddler Becky Tracy from whom she inherited a wide repertoire of music from Quebec, New England, Ireland, and France, a deep love for old tunes, and the intuitive sense of rhythm and danceability which infuses her playing. Equally at home in the concert hall and on the dance stage, she’s taught fiddle, song, and dance at camps and festivals around New England, toured nationally with her band Polaris and now tours with her quartet Stove Dragon and duo Helen &amp; Rose. https://www.rose-jackson.com/ 𝐇𝐞𝐥𝐞𝐧 𝐊𝐮𝐡𝐚𝐫: they/them Hailing from Seattle, Washington, Helen currently resides in Cambridge, MA. Helen began exploring their connection to folk and Celtic music in 2020 while studying with renowned contra guitarist Alex Sturbaum. Upon moving to Cambridge in 2022, Helen dove into the thriving celtic music scene, playing contra dances, Irish sessions, and concerts around New England and the Pacific Northwest. Since then, Helen has developed their style as a contra accompanist, Irish session backer, and vocalist. https://www.helenkuharmusic.com/ 𝐅𝐢𝐝𝐝𝐥𝐢𝐧' 𝐅𝐢𝐧𝐧: they/them A professional fiddler, singer and banjo player living on the territories of the lekwungen and W̱SÁNEĆ people, colonially known as Victoria BC. Finn has a passion for Irish, Scottish, English, North American and Eastern European folk music, and are known for their dynamic fiddling and soulful voice. They delve into traditional material - bringing a fresh interpretation of songs and tunes from many different places, as well as writing their own material. From the Appalachian mountains to Quebec, to melodic Irish and Scottish tunes, they cover wide musical ground with articulate playing. Finn also performs frequently in Canada and the U.S. with their bands Clanna Morna and Ghostly Hounds. https://finnletourneau.com/ ℂ𝕒𝕝𝕝𝕚𝕟𝕘 𝔹𝕪: 𝐕𝐢𝐜𝐭𝐨𝐫𝐢𝐚 𝐁𝐞𝐚𝐮𝐜𝐡𝐞𝐬𝐧𝐞 One of our local communities up and coming callers! 𝔻𝕣𝕒𝕘 𝕡𝕖𝕣𝕗𝕠𝕣𝕞𝕒𝕟𝕔𝕖𝕤 𝕓𝕪: Aries Moon: Making country gay one song at a time Leo Moon: The island's premiere tap dancing drag thing ......................................................................................................... 6:30 - doors open 7:00 - dancing starts with a beginner friendly dance lesson Everyone welcome, no experience necessary. $12 - Youth $20 - Everyone who is willing and able to NOTAFLOF Poster Art by Sonya Chwyl See less Victoria, British Columbia Fairfield United 925 Balmoral Rd, Victoria, BC V8T 1A7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C808" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/909522138040202/</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and Vivek Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Friday 28 November 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 133 people interested Interested Sun, 27 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Ali and 3 friends 45 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C809" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1031573525615192/</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Sunday at 19:00 GROOVE KITCHEN'S JUNEFEST DANCE!! Hermann's Jazz Club About Discussion More About Discussion GROOVE KITCHEN'S JUNEFEST DANCE!! Interested Going Invite Details 98 people responded Event by Groove Kitchen and Hermann's Jazz Club Hermann's Jazz Club Tickets hermannsjazz.com/show/737557/view Public · Anyone on or off Facebook The festival is over and it seems you still wanna celebrate music, but also... wanna get down and boogie?? You're our kind of people!! Observe the top of Summer with song and funky steps as the kitchen's groove moves your body like they've done before at spots like the Butchart Gardens, The Esquimalt Ribfest, The Osbourne Bay Pub, or the hottest rooms in and outta town. The Chefs are ready to serve their mouthwatering melange of funk, pop, soul, Latin, and flavours to party to the end!! Join us... Doors 5:30 PM / 7:00 PM Show, Sunday June 29th Hermann's Jazz Club 753 View Street Victoria, BC V8W 1J9 https://hermannsjazz.com/show/737557/view See less Victoria, British Columbia Tickets Find Tickets Hermann's Jazz Club 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C810" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3854957174726232/</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Monday from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 51 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Urban Kizomba with Aaron and Fernanda— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C811" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/589043697010919/</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 66 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, May 25th features Cedar Mathias as our facilitator/dj! Details for Sunday, May 25th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C812" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/556816543734629/</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Monday 7 July 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 47 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Merengue with Sebastian and Hannah— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C813" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1238334523949776/</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Sunday from 11:00-12:30 Dance Temple w/ Alex King-Harris (aka Rara Avis) Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Alex King-Harris (aka Rara Avis) Interested Going Invite Details 70 people responded Event by Dance Temple Victoria , Alex King-Harris and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 29th features Alex King-Harris (aka Rara Avis) as our facilitator/dj. He is back in town for the summer! Details for Sunday, June 29th: Facilitation and music set by Alex King-Harris (Rara Avis) Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C814" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1682353965754886/</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Saturday 14 June 2025 from 18:00-20:30 Mamas' Dance Party! 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Sat, 5 Apr Sat, 10 May Sat, 14 Jun About Discussion More About Discussion Mamas' Dance Party! Details 32 people responded Event by Fairfield Gonzales Community Association 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Duration: 2 hr 30 min Public · Anyone on or off Facebook Calling all mamas, grand-mamas, aunties &amp; mamas-to-be! Join us for a night curated for all mamas (in any season of their motherhood or reproductive journey) to connect through creative expression, freedom of movement and community building! There will be an opening &amp; closing circle and time to connect over light refreshments as the night concludes. Feel free to come for it all, or leave when needed. We can't wait to dance, groove, and connect with you all soon. This is an inclusive space for ALL those who mother. Admission by-donation: suggested donation $5 This event is presented by the FGCA's Neighbourhood Improvement Committee See less Victoria, British Columbia 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 1330 Fairfield Rd, Victoria, BC V8S 5J1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C815" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/939376108286434/</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and David Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 2 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Today at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Tickets · CA$17.31 www.eventbrite.com/e/salsa-night-dance-city-tickets-1415720962509 Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Tickets Find Tickets Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 18 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Ali and Jon 28 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends 133 people interested Interested Sat, 5 Jul at 19:00 Josh Warren Presents: The Path (LIVE @ Hermann's!) Hermann's Jazz Club 23 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C816" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1408949946810887/</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Sunday 8 June 2025 from 11:00-12:30 Dance Temple w/ Lila Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Lila Details 32 people responded Event by Dance Temple Victoria , Lyndsay Lila and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 8th features Lila Spencer as our facilitator/dj! Details for Sunday, June 8th: Facilitation and music set by Lila Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C817" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/734261429120710/</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Friday 6 June 2025 from 19:30-22:30 Dance City 108 Niagara St, Victoria, BC V8V 1E9, Canada About Discussion More About Discussion Dance City Details 9 people responded Event by Andrew Sanderson 108 Niagara St, Victoria, BC V8V 1E9, Canada Duration: 3 hr Public · Anyone on or off Facebook Beginner Cha Cha workshop with Jane and Andrew at 7:30pm Multi genres dance including Standard, Latin,  West Coast Swing, and more starting at 8:30pm dj Andrew Sanderson Cash Admission: $12/$10 Members See less Victoria, British Columbia 108 Niagara St, Victoria, BC V8V 1E9, Canada 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C818" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2576922459305643/</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 51 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 15th features Cedar Mathias as our facilitator/dj! Details for Sunday, June 15th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C819" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/650657144184821/</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Saturday 19 July 2025 from 21:00-02:00 COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY The Coda About Discussion More About Discussion COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY Interested Going Invite Details 65 people responded Event by Victoria Viva la Fiesta and Victoria LATIN Community Society The Coda Duration: 5 hr Public · Anyone on or off Facebook Colombian Summer Rumba: “Tierra Querida” Party Saturday, July 19th Doors: 9:00 PM | Show: 9:30 PM 19+ | ID Required Celebrate Colombian Independence Day with us with the vibrant “Tierra Querida” Party — an amazing night of live music, dance, culture, and pure rumba energy! Start the night with a live tribute to Colombian music by the talented Daniel Sar &amp; Sofia Leonne. Their performance will honor legendary Colombian artists such as Juanes, Maluma, Fonseca, Rodolfo Aicardi, Herencia de Timbiquí, Mon Laferte, and more—blending pop, tropical rhythms, and heartfelt Latin ballads into a powerful musical journey. At 10:30 PM, DJ Miro, straight from Cali, Colombia, will take over with a fiery mix of Colombian beats. Later, resident DJ Alex King will close out the night, turning up the heat with Latin hits and ending strong with the latest reggaetón summer vibes. At midnight, enjoy a special folkloric performance by Danza Colombia, followed by a unifying moment as we wave our flag souvenirs and sing the national anthem together. Savor delicious cocktails, soak in vibrant downtown vibes, and enjoy a night filled with alegría, culture, and  Colombian vibes! Get your tickets NOW! First-tier: $20 | Second-tier: $25 Limited tickets available at the door for $27 - Act fast before they are sold out! Party ends at 2:00 AM Each ticket includes a Colombian flag souvenir. Take a piece of the celebration home with you! See less Victoria, British Columbia The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C820" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1132427048350776/</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com or 15$ cash/e-transfer at the door. Formed in the heart of Chinatown, Rosebuds is a dynamic ensemble that brings the vibrant sounds of jazz, blues &amp; swing to life.  The group plays a mixture of originals and jazz standards, and is influenced by artists like Louis Armstrong, Billie Holiday, Lester Young, and Lionel Hampton. Featuring Rebecca Wells (vocals/guitar), Alex Moore (guitar/keys) Bryden Amos (guitar/keys), Matisse Gubby-Hurtig (bass), Owen Chow (trumpet), and Andrew Greenwood (tenor saxophone). Samba e Sol is a newly formed Brazilian bossa nova jazz trio featuring Andrew Greenwood (flute), Alex Moore (guitar), and Matisse Gubby-Hurtig (bass), playing music by artists like Antonio Carlos Jobim, Marcos Valle, Luiz Bonfa, and more. Instagram: https://www.instagram.com/rosebudsband/ See less Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C821" s="3" t="n">
+        <v>45835.46464241899</v>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1293301738436581/</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Sunday 6 April 2025 at 17:00 Kizomba Sundown Party: Free of charge Method Studio - Victoria BC David Lamine Victoria invited you About Discussion More About Discussion Kizomba Sundown Party: Free of charge Details 58 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Method Studio - Victoria BC Public · Anyone on or off Facebook Free Pre-VIKFest party. Bring snack and drink. Expect great music, great energy, great atmosphere. "Dance with your heart. your feet will follow" Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C822" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1029869435768837/</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Saturday 22 March 2025 at 20:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC This event has been cancelled. You cannot share this event, but you can still post. About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 14 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C823" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1179097320623502/</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 37 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C824" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1459643825205914/</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Tomorrow from 10:00-12:00 KIZOMBA NA RUA – AfriCa Fest Victoria 2025 Centennial Square About Discussion More About Discussion KIZOMBA NA RUA – AfriCa Fest Victoria 2025 Interested Going Invite Details 10 people responded Event by African Arts &amp; Cultural Society - Centre Issamba Centre and Pulchérie N. Mboussi Centennial Square Duration: 2 hr Public · Anyone on or off Facebook KIZOMBA NA RUA – AfriCa Fest Victoria 2025 Date: Saturday, June 28, 2025 Time: 10:00 AM – 12:00 PM Location: Centennial Square, Victoria, BC Free &amp; open to the public! We’re inviting all Kizomba dancers to join us for a special Kizomba Na Rua moment at AfriCa Fest Victoria 2025! Dance under the morning sun and feel the rhythm of Afro-Lusophone vibes in the city's heart. This open-air morning dance club moment is for dancers of all levels — whether you're dancing or just enjoying the vibe, the energy will be electric! Let’s connect, move, and celebrate community, culture, and rhythm together. Don’t forget to bring your smiles and dancing shoes — it's going to be unforgettable! #KizombaNaRua #AfriCaFest2025 #DanceInTheSquare #VictoriaBC #AfroLusophoneVibes #AfriCaFestVictoria See less Dance Victoria, British Columbia Centennial Square 10 Centennial Sq, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C825" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1794066937801722/</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Saturday 8 March 2025 from 20:30-23:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 26 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C826" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1079226067560481/</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 57 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 6, 2025 | Lesson:  Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C827" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1861230087752141/</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 6 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 31, 2025 | Lesson:  Intro to Salsa with Adam &amp; Alicia Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C828" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3006474846197996/</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 45 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 27, 2025 | Lesson:  Intro class TBD Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro class TBD • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C829" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2637194793152555/</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 133 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 29, 2025 | Lesson:  Intro to Salsa Rueda with Sam and Katie Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa Rueda • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C830" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/960236445839425/</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Saturday 22 June 2024 from 18:00-21:00 Kizomba/UrbanKiz at Clover Clover Pt, Victoria, BC V8S, Canada About Discussion More About Discussion Kizomba/UrbanKiz at Clover Interested Details 56 people responded Event by Becky Mowat Clover Pt, Victoria, BC V8S, Canada Duration: 3 hr Public · Anyone on or off Facebook Come join us for our first time dancing at Clover Point! There will be no lesson beforehand and this is super casual. Just a bunch of friends hanging out and dancing. Bring snacks, something to drink, blankets, warm clothes (as it is typically cooler by the ocean). There isn't a lot of parking at Clover Point but you can park along Dallas Rd and just walk down. Feel free to invite friends and family. Hope to see you all there! See less Victoria, British Columbia Clover Pt, Victoria, BC V8S, Canada 1301 Clover Pt, Victoria, BC V8S, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C831" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1743571267040445/</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Ali Jorgensen invited you About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Details 55 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 8, 2025 | Lesson: Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C832" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/947213690692385/</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C833" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1337760257449745/</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 6 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 10, 2025 | Lesson:   Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C834" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1060779176049104/</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Thursday 3 October 2024 from 19:30-22:30 Kizomba Practica Thursdays: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Kizomba Practica Thursdays: Fall Series Details 20 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Join us every Thursday for Kizomba/Urbankiz classes. Intermediate 7:30PM-8:15pm Beginner 8:15pm-9:00pm Practica until 10:30pm Class only: $10 Class &amp; Practica: $15 or $10 for university students w/ID Practice only $10 Classes will be provided by your local Instructor (David Lamine) and assistants (Robyn, Becky) and occasionally by some out of town and International Instructors. Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C835" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1152065639712042/</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 20 20 Feb at 19:30 – 23 Feb at 23:00 Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urbankiz &amp; Tarraxo Workshops with Mike Ahombi Details 49 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 days Public · Anyone on or off Facebook Join us for our special edition Urbankiz &amp; Tarraxo workshops with Mike Ahombi Mike has been a big supporter of our VIKF and bringing his talent and low key vibe to the west coast. He is based out of Ottawa but you will find him at many different festivals and cities teaching Kizomba, Urbakiz and Tarraxo. We cannot wait for you all to have the opportunity to learn from such an incredible person and instructor. Details: Feb 20th Urbankiz Workshop 7:30pm-9:30pm Practica 9:30pm-11:00pm Feb 22nd Tarraxo Workshop 8:00pm-10:00pm Practica 10:00-11:30pm Price $90 Workshops only $70 Practica only $20 *** please e transfer to becksmith@hotmail.com *** Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C836" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1184791909680061/</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Thursday 13 March 2025 from 19:30-23:00 Urban Kiz Workshop with Mannie Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 50 people responded Event by Becky Mowat and David Lamine Victoria Ukrainian Cultural Centre Duration: 3 hr 30 min Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C837" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3185065321631809/</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Saturday 15 March 2025 from 20:00-00:00 Urban Kiz Workshop with Mannie Method Studio - Victoria BC Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 48 people responded Event by Becky Mowat and David Lamine Victoria Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C838" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1334757257408713/</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Saturday 25 January 2025 from 19:00-23:30 Special Edition Urbankiz Workshop w/ Kenny Odumosu Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Special Edition Urbankiz Workshop w/ Kenny Odumosu Details 50 people responded Event by Becky Mowat , David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 4 hr 30 min Public · Anyone on or off Facebook SPECIAL EDITION WORKSHOP Join us Saturday January 25th for a 2hr Urbankiz workshop. Joining us from Calgary to share his knowledge and love for Urbankiz. Kenny finished first for the Kizomba/Semba category at the North American Olympiads. With his background in Kizomba/Semba Kenny will help you incorporate techniques and smoothness into your Urbankiz. We are really looking forward to having him here! Schedule 7:00pm-9:00pm (workshop) 9:00pm-11:30pm (social) Price: $40 (includes workshop &amp; social dance) e-transfer to:  becksmith@hotmail.com please include the name you go by if different from your e-transfer account. Thanks See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C839" s="3" t="n">
+        <v>45835.47163334491</v>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1388695712154512/</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Ali Jorgensen invited you About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Details 121 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation June 22, 2025 | Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C840" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/717475250956404/</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Friday 30 May 2025 at 18:00 FREE Beginner Bachata Class 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 About Discussion More About Discussion FREE Beginner Bachata Class Details 65 people responded Event by Mayfair Shopping Centre and Victoria Latin Dance Association 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 Public · Anyone on or off Facebook Ready to get your groove on? We’re teaming up with the Victoria Latin Dance Association  for a FREE Beginner Bachata Class right here at Centre Court! Join us on Friday, May 30 at 6:00 PM for an evening of fun and dancing. FREE Beginner Bachata Class May 30th, Friday at 6PM NO partner or experience necessary! Bachata is a beautiful and easy-to-learn dance that’s great for meeting new people, getting active, and connecting with an amazing community. See less Dance Victoria, British Columbia 221- 3147 Douglas Street, Victoria, BC, Canada, British Columbia V8Z 6E3 3147 Douglas St, Victoria, BC V8Z 3K3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C841" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1350929566137538/</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 7 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation August 10, 2025 | Lesson: Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C842" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/729183856154450/</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Today from 20:00-00:00 Bachata Night Method Studio - Victoria BC About Discussion More About Discussion Bachata Night Interested Going Invite Details 32 people responded Event by Bachata Nights Victoria BC and Alysha Kopala Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights June 27 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance @yourgirlalysha  and @davidch_78 will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C843" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3975145332748137/</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Friday 13 June 2025 from 20:00-00:00 Bachata Night Method Studio - Victoria BC About Discussion More About Discussion Bachata Night Details 77 people responded Event by Bachata Nights Victoria BC , Sebastian Carmona and Alysha Kopala Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights June 13 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C844" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1057471579628015/</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Friday 16 May 2025 at 17:00 Bachata Nights Victoria Bc Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Victoria Bc Details 9 people responded Event by Bachata Nights Victoria BC and Sebastian Carmona Method Studio - Victoria BC Public · Anyone on or off Facebook Join us on our next Bachata Nights May 23 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @sebastianyhannah will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C845" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/601131956358678/</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Thursday 3 July 2025 at 20:00 Bachata &amp; Merengue- All Levels- July Series Studio 4 Athletics About Discussion More About Discussion Bachata &amp; Merengue- All Levels- July Series Interested Going Invite Details 3 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Bachata &amp; Merengue are both dances from the Dominican Republic. Bachata can be anywhere from slow and romantic with lots of dips, sway and body movement to more upbeat and percussive with lots of musical footwork. Merengue is carefree, flirtatious and fun! Classes are registered on a monthly basis and take place every Thursday from 8:00- 9:00pm, July 3,10,17,24,31 No experience required.  No partner is necessary as we rotate partners throughout the lesson.  Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot!d See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C846" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1300938064467261/</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Thursday 20 March 2025 from 20:00-22:00 Intermediate Sensual Bachata Workshop Method Studio - Victoria BC About Discussion More About Discussion Intermediate Sensual Bachata Workshop Details 24 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 2 hr Public · Anyone on or off Facebook Sensual Bachata Workshop in March! Intermediate workshop - March 20 Time: 8:00-9:30 PM + Practice 9:30-10:00 PM Location: Method Studio, 841 Fisgard St. Cost: $30 per workshop (includes 2 hours!) Intermediate workshop: Take your skills to a higher level! Master the advanced variations of the Madrid pass, smooth transitions and musicality. No partner needed, just bring your energy and comfortable shoes! Register at: maximumotion@gmail.com #BachataWorkshop #VictoriaBC #LearnToDance #BachataLovers See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C847" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1901245437276872/</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Friday 9 May 2025 from 20:00-00:00 Bachata Nights Method Studio - Victoria BC About Discussion More About Discussion Bachata Nights Details 40 people responded Event by Bachata Nights Victoria BC , Alysha Kopala and Sebastian Carmona Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us on our next Bachata Nights May 09 at Method Studio (841 Fisgard St) for a night of music, dancing, and fun!Don’t miss it! Schedule: 8:00 PM – Doors open 8:15 PM – All Levels Bachata Lesson 9:00 PM - 12:00 AM – Social Dance This Friday @yourgirlalysha  and @davidch_78  will teach an amazing open level bachata class! Don’t miss it Dance to the perfect 3:1 mix of Bachata &amp; Salsa! Location: Method Studio, 841 Fisgard St Cost: $10 cash per person The evening starts with an Open-level Bachata lesson from 8:15 PM to 9:00 PM—great for all skill levels! Follow @BachataVictoria for updates. Let’s dance, sparkle, and celebrate together! See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C848" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1730246844256904/</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre About Discussion More About Discussion Saturday Salsa/Bachata Social June 28th Interested Going Invite Details 47 people responded Event by Latin Dance Canada Ukrainian Cultural Centre Duration: 3 hr 59 min Public · Anyone on or off Facebook Saturday Salsa/Bachata Social June 28th 3277 Douglas st, Victoria BC Cost? $15 CASH ONLY PLEASE! When? Saturday, June 28th 8:00 pm - 8:30 pm beginner dance lesson 8:30 pm - 12 am Social dancing What? We will be playing a mix of salsa, bachata and more. Where? Ukrainian Cultural Centre 3277 Douglas Street, Victoria See less Dance Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C849" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/9677364319006080/</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Bachata Temptation, Salsa Sensation Interested Going Invite Details 61 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Bachata Temptation, Salsa Sensation July 20, 2025 | Lesson:  Intro to Bachata with Sebastian &amp; Hannah Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Bachata • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C850" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1813229489279716/</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Thursday 29 May 2025 from 19:55-21:00 Sensual Bachata 4 Week Series Method Studio - Victoria BC Thu, 15 May Thu, 22 May Thu, 29 May +1 About Discussion More About Discussion Sensual Bachata 4 Week Series Details 6 people responded Event by Victoria Latin Dance Association Method Studio - Victoria BC Duration: 1 hr 5 min Public · Anyone on or off Facebook Ready to level up your Sensual Bachata? May 8, 15, 22, 29 Method Studio | 7:55–9:00 PM | $80 for all 4 classes Join us for an exciting and dynamic Bachata Sensual class designed for experienced beginners and intermediate dancers! We’re blending solid fundamentals with fresh, fun, and sensual combos to help you grow, challenge yourself, and have an amazing time on the dance floor. No partner needed — just bring yourself and your love for dance! Spots are limited — don’t miss out! Register by e-transferring $80 to maximumotion@gmail.com and mentioning “Bachata Sensual” in the notes. Get ready to connect, move, and elevate your dancing! P.S. All fees are non-refundable as they go directly toward securing the studio space and running the class. See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C851" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/10048344358532607/</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- May series Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. May 6, 13, 20, 27 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C852" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/669591372187091/</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 10:00-11:00 Salsa &amp; ChaCha Solo Westshore Dance Studios Sat, 17 May Sat, 24 May Sat, 31 May +7 About Discussion More About Discussion Salsa &amp; ChaCha Solo Details 2 people responded Event by Dance Praktika Westshore Dance Studios Duration: 1 hr Public · Anyone on or off Facebook Elevate your dance journey with our Ladies Solo Class. Join our exciting series and learn the basics of Salsa and Cha Cha. Perfect for beginners looking to spice up their dance skills! Class Highlights: - Learn exciting dance moves tailored for solo dancers; - Fun and welcoming environment; - Suitable for absolute beginners. Come dance with us and let the rhythm guide you! To register to April classes please use links at "Tickets". See less Langford, British Columbia Westshore Dance Studios 109-2675 Wilfert Road, Victoria www.westshoredance.com 2years+ Competitive&amp;Production a space for everyone with a love of dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C853" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/966455485665576/</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Thursday 3 April 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- April series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. Apr 1, 8, 15, 22, 29 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C854" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/679241811720932/</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Tuesday 6 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Fundamentals- May Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- May Series Details 7 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, May 6, 13, 20, 27 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C855" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2214494908966327/</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Monday 5 May 2025 at 21:00 Salsa &amp; Cha Cha Cha- Int/ Adv- May series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- May series Details 8 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, May 5, 12, 26 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C856" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/745466751313624/</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Tuesday 8 July 2025 at 20:00 Salsa &amp; Cha Cha Cha- Fundamentals- July Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- July Series Interested Going Invite Details 5 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, July 8,15,22,29 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C857" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2579272439096564/</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Tuesday 8 July 2025 at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- July series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Beg/ Int- July series Interested Going Invite Details 4 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is dancers that have completed the Fundamentals course and want to continue to improve their social dancing using the techniques they  have learned. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor.  Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place every Tuesday from 9:00- 10:00pm. July 8,15,22,29 No partner is necessary as we rotate partners throughout the lesson.  Must have completed Fundamentals or have instructor permission to attend. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C858" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342792743590871/</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Monday 7 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/ Adv- April series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/ Adv- April series Details 6 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, April 7, 14, 28. Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C859" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1382188962971661/</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Tuesday 1 April 2025 at 20:00 Salsa &amp; Cha Cha Cha- Fundamentals- April Series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Fundamentals- April Series Details 9 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Contact us to register today! Class Description This class is perfect for brand new beginners, dancers of other styles, or more experienced dancers that want to continue to improve technique. NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Tuesdays, Apr 1, 8, 15, 22, 29 No experience required.  No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C860" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/727053470038104/</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Monday 7 July 2025 at 20:00 Salsa &amp; Cha Cha Cha- Int/Adv- July series Studio 4 Athletics About Discussion More About Discussion Salsa &amp; Cha Cha Cha- Int/Adv- July series Interested Going Invite Details 4 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook NY Style Salsa (Mambo) is danced to the rhythm of the congas and the techniques used allow for quick turns and direction changes, complex partner patterns and more body movement while dancing on a crowded dance floor. Cha Cha Cha is a fun dance with a playful energy that uses a very similar step to Salsa and learning them together will help you understand and be better at both. Classes are registered on a monthly basis and take place from 8:00- 9:00pm, Mondays, July 7,14,21,28 Must be a competent On 2 dancer and have instructor permission to attend. No partner is necessary as we rotate partners throughout the lesson. Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C861" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1342233713680795/</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Thursday 1 May 2025 at 21:00 Bachata &amp; Merengue- All Levels- May Series Studio 4 Athletics About Discussion More About Discussion Bachata &amp; Merengue- All Levels- May Series Details 3 people responded Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Bachata &amp; Merengue are both dances from the Dominican Republic. Bachata can be anywhere from slow and romantic with lots of dips, sway and body movement to more upbeat and percussive with lots of musical footwork. Merengue is carefree, flirtatious and fun! Classes are registered on a monthly basis and take place every Thursday from 8:00- 9:00pm, May 1, 8, 15, 22, 29. No experience required.  No partner is necessary as we rotate partners throughout the lesson.  Call 250-881-6141 or email info@calientedance.com for more details. No drop ins permitted so please contact us to reserve your spot! See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C862" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1636237610432412/</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Saturday 16 August 2025 from 20:00-23:59 Salsa Sunset Latin Party – August 16th! Latin Dance Canada About Discussion More About Discussion 🌅🔥 Salsa Sunset Latin Party – August 16th! 🔥🌅 Interested Going Invite Details 29 people responded Event by Latin Dance Canada Latin Dance Canada Duration: 3 hr 59 min Public · Anyone on or off Facebook Salsa Sunset Latin Party – August 16th! Get ready for a magical summer night filled with Latin rhythms, sunset vibes, and non-stop dancing! Join us for the Salsa Sunset Latin Party, where the Salsa, Bachata, and Merengue beats will keep you moving all night long under the stunning sunset sky! Dress Code: Wear your best sunset-inspired outfit – think bright, tropical colors, and beach party vibes! Dance to the best Salsa, Bachata, Merengue &amp; Latin hits all night! No partner? No problem! Join our fun intro class at 8:00 PM! Location: Ukrainian Cultural Centre, 3277 Douglas St., Victoria, BC Date: Saturday, August 16, 2025 Intro Class: 8:00 PM | Social Dance: 8:30 PM - Late Entry: $15 at the door – Bring cash, please! What to Expect: Vibrant salsa rhythms &amp; tropical vibes! Tropical-themed decorations &amp; stunning sunset views! A welcoming dance community &amp; unforgettable fun! Let’s dance as the sun sets and make it a night to remember! Tag your friends and let’s create memories under the summer sky! #SalsaSunsetLatinParty #SalsaBachata #LatinDanceParty #VictoriaBC #LatinDanceCanada See less Dance Guests See All</t>
+        </is>
+      </c>
+      <c r="C863" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/884101187183426/</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 2 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Saturday 12 July 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Tickets · CA$17.31 www.eventbrite.com/e/caliente-salsa-saturdays-tickets-1415724884239 Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in June. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Tickets Find Tickets Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 5 Jul at 19:00 Josh Warren Presents: The Path (LIVE @ Hermann's!) Hermann's Jazz Club 23 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1509 people interested Interested Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested 32 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C864" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3899920353641309/</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 2 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 9 Saturday 9 August 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in July. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Fri, 11 Jul at 21:00 Locarno at The Coda The Coda Nadia is interested 43 people interested Interested Sat, 5 Jul at 19:00 Josh Warren Presents: The Path (LIVE @ Hermann's!) Hermann's Jazz Club 23 people interested Interested Mon, 30 Jun at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Lorne, Ali and Almeda 51 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C865" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1618420955545842/</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 2 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 30 Friday 30 May 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing at an all ages venue with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 4 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Ali 14 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested Sun, 17 Aug at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Ali is going 2 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C866" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1479111682798589/</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 2 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 13 Saturday 13 September 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in August. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1509 people interested Interested Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested 32 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 57 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C867" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2251848171850840/</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 2 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 Saturday 10 May 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in April. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Fri, 11 Jul at 21:00 Locarno at The Coda The Coda Nadia is interested 43 people interested Interested Sat, 5 Jul at 19:00 Josh Warren Presents: The Path (LIVE @ Hermann's!) Hermann's Jazz Club 23 people interested Interested Sun, 17 Aug at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Ali is going 2 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C868" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1059622278965884/</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>(20+) Caliente Salsa Saturdays  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 2 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 8 Saturday 8 November 2025 at 20:15 Caliente Salsa Saturdays Studio 4 Athletics About Discussion More About Discussion Caliente Salsa Saturdays Interested Going Invite Details Event by Salsa Caliente Studio 4 Athletics Public · Anyone on or off Facebook Join us for Caliente Salsa Saturdays! 8:15pm Doors open 8:30pm Beginner Salsa Lesson No partner or experience required.  Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing for all levels to Salsa, Bachata, Merengue &amp; Cha Cha Cha. Ages 16+ welcome. $15.00 per person CASH ONLY at the door.  Tickets also available on Eventbrite in October. There will be a small non-alcoholic concession available as a fundraiser for the teams. *Limited capacity. First come first served. We reserve the right to refuse entrance at the door. The venue is only accessible via stairs.* See less Dance Victoria, British Columbia Studio 4 Athletics 709 Yates St, Victoria, BC V8W 1L6, Canada Meet your host Salsa Caliente 1923 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1509 people interested Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends 184 people interested Interested Sat, 18 Oct at 20:00 ✨ White and Gold Latin Night – October 18th! ✨ Latin Dance Canada Carmie is interested 33 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C869" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1411005319893067/</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Monday 28 April 2025 from 18:30-22:30 Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Mon, 14 Apr Mon, 21 Apr Mon, 28 Apr +1 About Discussion More About Discussion 🔥Bachata &amp; Brazilian Zouk 🌊 dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard Details 7 people responded Event by Bachata and Zouk with Javi in Victoria 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Duration: 4 hr Public · Anyone on or off Facebook Bachata &amp; Brazilian Zouk dance classes | Mondays April 7 - 28th | 6:30-10:30pm | 1709 Blanshard street | Victoria Join us for a 4 week course exploring the joy and magic of Brazilian Zouk &amp; Bachata dancing! Discover your new passion! Latin Dancing! Experience a new level of joy and connection by learning two popular dance styles focusing on enhancing body awareness, building confidence in dance vocabulary with lead and follow techniques, exploring musicality, and loving yourself deeper with styling! Be prepared to have lots of fun dancing with new friends! Register today! Schedule: Monday April 7 - 28th 6:30-7:25pm | Brazilian Zouk - Level 2 (ask Javi for permission) 7:30-8:25pm | Brazilian Zouk - Level 1 8:30-9:25pm | Sensual Bachata - Beginner Foundations 9:30-10:30pm | Sensual Bachata - Intermediate "Trending Moves" Tuition: $20 | 1 Class $35 | 2 Classes (Brazilian Zouk 1&amp;2, or Brazilian Zouk 1 &amp; Bachata, Bachata 1&amp;2) $50| 3 Classes (3 classes, BEST value) 1709 Blanshard St, Victoria, BC Registration: E-transfer to: danceinflow@gmail.com or send us a message on Whatsapp: 7785877665 (Also accepting credit card/cash at the door) Please add a note if you're registering as a "Leader", "Follower", or "Open to both" Space is limited. Register in advance to reserve your spot! Looking fwd to dancing and flowing with you, Warmly, Javi See less Victoria, British Columbia 1709 Blanshard St, Victoria, BC V8W 2J8, Canada 1709 Blanshard St, Victoria, BC V8W 2J8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C870" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1106484714432492/</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Wednesday 2 July 2025 from 18:30-21:00 Zouk practica and social White Eagle Hall, 90 Dock St, Victoria BC Wed, 4 Jun Wed, 25 Jun Wed, 2 Jul Wed, 9 Jul +40 About Discussion More About Discussion Zouk practica and social Interested Going Invite Details 1 person responded Event by Victoria Zouk Collective and Victoria Zouk Collective Group White Eagle Hall, 90 Dock St, Victoria BC Duration: 2 hr 30 min Public · Anyone on or off Facebook Drop-in zouk practica by donation - everyone welcome! White Eagle Polish Hall every Wednesday 6:30-9 pm Shared warm up, free dance time, review material from lessons and congresses, connect and share knowledge! Help is always available. Minimum $5 donation. Cash at the door, or etransfer to oceanzouk@gmail.com Enter the lower hall by the side door on Niagara Street just beside the Polka food truck. Also available in Victoria are zouk lessons with Javi, an amazing instructor from Vancouver! More info at https://www.facebook.com/Sabor.Asi.Dance.Salsa.Victoria or email danceinflow@gmail.com See you there! See less Victoria, British Columbia White Eagle Hall, 90 Dock St, Victoria BC 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C871" s="3" t="n">
+        <v>45835.4821869213</v>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/544121845403419/</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Saturday 31 May 2025 from 13:00-23:55 Swing Session: Balboa with Yoshi and Etsuko Solwood Studio About Discussion More About Discussion Swing Session: Balboa with Yoshi and Etsuko Details 108 people responded Event by Swing Dance Association of Victoria , Dave Henderson and 2 others Solwood Studio Duration: 10 hr 55 min Public · Anyone on or off Facebook Lace up your shoes on May 31, 2025 for an afternoon of Balboa Classes and an evening of Social Dancing with Yoshi and Etsuko Uemura. 4 Classes for everyone &amp; 1 Social Dance! Passes go on sale April 19 at noon at our SDAV Square Shop! You must know and be comfortable with Balboa basics for all of these classes - they won't be covered at this workshop. All the specifics are available at swingvictoria.net , but here are the notes: May 31st, at Solwood Studio, with doors at 12:30pm . Bring indoor shoes, please! 4 classes for everyone and there's a dance from 9-12am. Passes go on sale April 19th at noon. See less Victoria, British Columbia Solwood Studio 1303 Broad St, Victoria, BC V8W 2A8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C872" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1786895135557126/</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Monday 26 May 2025 at 19:00 The Jive Big Band and The Blue Bosses Hermann's Jazz Club About Discussion More About Discussion The Jive Big Band and The Blue Bosses Details 9 people responded Event by The Jive Big Band Hermann's Jazz Club Public · Anyone on or off Facebook Join the Jive Big Band for a fun night of music featuring big band classics, rock, funk, and the unexpected. Directed by Nick La Riviere, this band is always a good time! Joining them is the fantastic Blue Bosses jazz combo directed by Ashley Wey. Entry by donation to Arts on View, keeping music at Hermann’s alive and strong! See less Victoria, British Columbia Hermann's Jazz Club 753 View Street, Victoria Hermann's Jazz Club is the best place to visit for live jazz and blues in Victoria, BC. On July 15, Guests See All</t>
+        </is>
+      </c>
+      <c r="C873" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663756533046485/</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Friday 11 April 2025 at 21:30 Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 About Discussion More About Discussion Miguelito Valdes presents Contodo- Blues, rock, swing, funk and soul...Havana style. Details 36 people responded Event by The Coda 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 Public · Anyone on or off Facebook Miguelito Valdes presents Contodo What happens when you bring together three Cuban and two Canadian musicians, with a deep love of all music and a wide range of musical experiences?  A joyful mix of party and deep groove, that's what! Guaranteed to make you want to dance, these brothers from other mothers bring it all. Con Todo! Featuring: Miguelito Valdes – brass/vocals/percussion Jose Sanchez – drumset/timbales Hector Ramos – congas/percussion Peter Dowse - bass Brooke Maxwell – keys/vocals See less Victoria, British Columbia 751 View St, Victoria, BC, Canada, British Columbia V8W 1J9 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C874" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/373500473108499/</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Sunday Swing at Logan's Logan's Pub 10 Dec 2017 Debi Wong invited you About Discussion More About Discussion Sunday Swing at Logan's Details Event by Swing X Logan's Pub Duration: 3 hr 30 min Public · Anyone on or off Facebook Sunday Swing at Logan's is BACK! Come join us for some great tunes and we'll party like it's 1939. Bring your dancing shoes, sweet moves, and a few dollars for our fabulous DJ (and gracious bartenders). Feel free to come early to hang out and grab a bite to eat. 19+. NEW: Crash course 15min swing lesson at 8:30pm! This is intended to be the bare minimum for someone to show up and know the basics of swing dancing, nothing fancy! DETAILS: * 8:30pm Quickie 15min beginner lesson! * 8:45pm social dancing until as late as midnight (maybe!) * Usually gets bluesy after 11pm See less Victoria, British Columbia Logan's Pub 1821 Cook Street, Victoria Original - Authentic - Unique Guests See All</t>
+        </is>
+      </c>
+      <c r="C875" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2441697862726705/</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Sunday 30 June 2019 at 19:00 Journey’s 50th Birthday!!  A West Coast Swing dance party!! Eastern Star Hall Chapters No 5 &amp; No 17 Journeey Song invited you About Discussion More About Discussion Journey’s 50th Birthday!!  A West Coast Swing dance party!! Details 13 people responded Event by Journeey Song Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook 3281 Harriet Road, Victoria,BC Bring your own alcohol-free beverage... Bring a gluten-free appie if you’d like. Dance West Coast Swing until 10 pm to Blues, Pop, RnB, Swing, and a wee bit of Ballroom Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C876" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/634773653668605/</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Saturday Night West Coast Swing BC Swing Dance Club Victoria 15 Jun 2019 22 Jun 2019 29 Jun 2019 +2 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night West Coast Swing Details 9 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook June means summertime and sunny days! Along with the weather, things for BC Swing Dance Cub Victoria will be changing too. Here's what is happening this month: 7 - 8pm 1st Saturday of the Month: Lesson with Meaghan, plus an assistant from our dance community 7 - 8pm Remaining Saturdays each month: TBD (stay tuned for workshops, activities or practices - updates will be posted on each event page) Note:  The 7 - 8pm weekly timeslot is included in the dance entrance price. -------------------------------------------------- Come join us every Saturday all year long for a fabulous WCS social dance from 8 - 11pm. Just $10 for the ($5 for students). Meaghan Efford and Bob Gebbie 's lesson on June 1st (starting PROMPTLY at 7pm) will be the only lesson in June, and it will be a great way to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity.  The lesson is included in the dance entrance price.  No experience or partner is required. -------------------------------------------------- • 6:45 pm - Doors open • 7:00 pm - TBD each week* • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *lesson with Meaghan and Bob on June 1st Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C877" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/663135653237580/</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:30-23:00 WACK! Another West Coast Swing Social Dance Method Studio - Victoria BC Canice Ma invited you About Discussion More About Discussion WACK! Another West Coast Swing Social Dance Details 40 people responded Event by Canice Ma and Wyatt Ritchie Method Studio - Victoria BC Duration: 3 hr 30 min Public · Anyone on or off Facebook Guess who's back, it's WACK! (please ignore the fact that it's been 2 years...) The schmucks are back with another spontaneous west coast swing social dance, featuring music by DJs Topknot and Amandance from Vancouver! DETAILS: • Friday, June 20th, 2025 • Method Studio, 841 Fisgard St, Victoria, BC • 7:30-8:30 pm: "Shake That" line dance lesson featuring Kaitlyn • 8:30-11 pm: social dancing with 100% west coast swing • Admission: $10 • Water and AC on us (and maybe some bonus chocolate) • Please keep in mind that parking is limited at the venue GENERAL SOCIAL DANCE ETIQUETTE: • Consent is cool- don't be creepy. • Shake off any shyness and get out there! Ask people to dance regardless if you’re a lead or follow, dancing for 10 years or started yesterday- it's more fun that way! • No teaching or unsolicited feedback on the dance floor. Good vibes only! • If you would like to partake in a steal dance, try to remain with that group for the whole song. • Bring a water bottle! The studio is known to get warm with more bodies in the space so we want you to stay healthy and hydrated. • Personal hygiene is important! Consider bringing a towel and/or a spare shirt to change into if you sweat easily. Our studio has a bathroom and change rooms available for all to use. • We recommend wearing clothes that are easy to move in, especially pants given the nature of the dance. • Clean, comfortable shoes (ideally dance shoes) on the dance floor only! See less Victoria, British Columbia Method Studio - Victoria BC 833 Fisgard St, Victoria, BC V8W 1R9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C878" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1035925295253912/</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Friday 18 April 2025 at 18:30 Swing out with the ATOMIC COCKTAILS 751 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Swing out with the ATOMIC COCKTAILS Details 64 people responded Event by Peter Sandmark 751 View St, Victoria, BC V8W 1J9, Canada Public · Anyone on or off Facebook Join the ATOMIC COCKTAILS as they swing out for their pre-Japan Tour dance party on April 18 at the Coda, 751 View Street.  Doors open 6 pn, show from 6:30-8:30 pm!  Tickets $20.  With songs from their new album BLUE LIGHT BOOGIE! See less Victoria, British Columbia 751 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C879" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/402729737034904/</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Thursday 5 September 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - Thurs Sept 5! Details 123 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for our second fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C880" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/302778660295534/</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Sunday 19 August 2018 from 18:00-21:00 West Coast Swing in the Park! Cameron Bandshell @ Beacon Hill Park Carolyn Gebbie invited you About Discussion More About Discussion West Coast Swing in the Park! Details 58 people responded Event by Carolyn Gebbie Cameron Bandshell @ Beacon Hill Park Duration: 3 hr Public · Anyone on or off Facebook Come join us for another evening of fun and WCS dancing in Beacon Hill Park! WCS music will be provided by DJ Carolyn. For those who are familiar with the routine, the 2018 WCS Rally Song will be played at 6:30, 7:30 and 8:30pm. Sam Jackson and Meaghan Efford, from wcsmovementmethods.com will be on hand to answer questions about WCS or how to improve your WCS dancing. They will also demo some incredible WCS dancing at 7pm. Please invite your WCS dance friends by sharing this event! See less Victoria, British Columbia Cameron Bandshell @ Beacon Hill Park Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C881" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/717783180949020/</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>FRIDAY ! Fort Tectoria About Discussion More About Discussion THIS FRIDAY 🌹🌹ROSEBUDS //swing band -&amp;- MISHA MANOUCHE //gypsy jazz @ Fort Techtoria THIS FRIDAY ! Interested Going Invite Details 34 people responded Event by Rebecca Rose , Bryden Amos and Alex Q Moore Fort Tectoria Public · Anyone on or off Facebook Bring your dancing shoes, we have a whole floor to boogie on this Friday!  We are taking it back to the 30's and 40's with a night of gypsy jazz, swing and blues for you. ROSEBUDS 8pm Victoria's hot new Swing Band, formed in the heart of China Town. Playing old time swing jazz classics and original tunes with bluesy grit.  Rebecca Wells//lead singer, Alex Quincy Moore &amp; Bryden Amos// guitar + keys, Andrew Greenwood//tenor sax, Owen Chow// trumpet, Matisse Gubby-Hurtig//upright bass. We invite you to rock the night away with us, swinging our way into summer. **MISHA MANOUCHE **7pm Kicking off the night, gypsy jazz duo Misha Manouche will be bringing us velvety melodies and the spirit of Django Reinhardt to the room. Adam Paquette &amp; Alex Gnaedinger// Guitar and vocals. Catch us Fort Techtoria this Friday! 777 Fort Street Victoria BC June 27th 6:30pm Doors open Buy Pre sale ticket at 15$ by e transfering rosebudsband@gmail.com Or 20$ tickets at door See you folks there See less Victoria, British Columbia Fort Tectoria 777 Fort Street, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C882" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1594011994641933/</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Tuesday 22 April 2025 from 19:45-21:45 Victoria West Coast Swing Collective social dance Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria West Coast Swing Collective social dance Details 9 people responded Event by Amanda Healey and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 2 hr Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. No street shoes. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C883" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/417338985546213/</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Thursday 29 August 2019 from 18:00-21:00 Free EVENT - West Coast Swing in the Square - August 29! Centennial Square Carolyn Gebbie invited you About Discussion More About Discussion Free EVENT - West Coast Swing in the Square - August 29! Details 109 people responded Event by BC Swing Dance Club Victoria Centennial Square Duration: 3 hr Public · Anyone on or off Facebook Come join BC Swing Victoria for a fabulous (and FREE) evening of fun and West Coast Swing dancing at Centennial Square! The schedule for the night will be: 6pm (sharp) there will be an intro lesson to West Coast Swing. 7 - 9pm WCS music will be provided by DJ Carolyn Gebbie. Note: For those who are familiar with the 2019 WCS Rally routine, and would like to practice performing it live prior to Sept 7, the "Hands Up” song will be played at 7:30 and 8:30pm. There will be WCS instructors on hand to answer questions about WCS or how to improve your WCS dancing. Please invite your dance friends by sharing this event! See less Victoria, British Columbia Centennial Square Victoria Centennial Square is a plaza in Victoria, British Columbia, Canada. It was built to celebrate the 100th anniversary of the incorporation of the City of Victoria. The Victoria Police Station, city hall and McPherson Playhouse are adjacent to the square. There is a fountain in the square.In the summer, the city hires musicians to perform every weekday, charging no admission fee. For the British Columbia Day holiday, Centennial Square is one of the venues for the Victoria Electronic Music Festival, where musicians and DJs play for free.In the winter, the Downtown Victoria Business Association has temporarily set up Christmas lights, a Ferris wheel, and an ice skating rink in the square.In 2011, Occupy Victoria protesters camped in the square until a court, at the behest of the city, ordered them to leave. Guests See All</t>
+        </is>
+      </c>
+      <c r="C884" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1776457206589544/</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Friday 21 March 2025 from 18:30-20:30 Slim Sandy's Atomic Cocktails swing speakeasy party! The Coda About Discussion More About Discussion Slim Sandy's Atomic Cocktails swing speakeasy party! Details 72 people responded Event by Peter Sandmark and Trace Nelson The Coda Duration: 2 hr Public · Anyone on or off Facebook Join Slim Sandy's Atomic Cocktails and dance as they play 2 sets of swing jazz, jive and rhythm and blues from the 20’s to the 40’s. Slim, on guitar and harmonica, is joined by Willa Mae on vocals, “Big Daddy Bo” on bass, and Bryn Bad on trumpet.  Slim Sandy has been playing music for over 40 years with acts such as Ray Condo and the Crazy Rhythm Daddies.  In 2012, he and Willa Mae co-created the Slim Sandy band in Victoria!  They have played music festivals in Canada, France, Spain, Germany, Belgium, and the Netherlands.  In May they will be touring in Japan! See less Victoria, British Columbia The Coda 749 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C885" s="3" t="n">
+        <v>45835.48792023148</v>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1766891834185825/</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam and Alive Tango Victoria Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends SAVE THE DATE! The next Sunday afternoon Milonga is on 8 June 2025 1-4pm. The Coda Club (formerly Hermanns Upstairs) is a beautiful newly renovated venue with awesome ambience, nice wood floor and great sound system. Come join us for a wonderful afternoon of warm hugs and close embrace. Sunday 8June 2025 1-4pm The Coda, 751 View Street, Victoria Admission: $15 (plus tax) Special Guest DJ: Francis Nowaczynski (from Vancouver) Free parking at View Street Parkade (next door) or Broughton Parkade. Cash bar is open for drinks. See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C886" s="3" t="n">
+        <v>45835.49039851852</v>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/754259983939888/</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Sunday 20 July 2025 from 12:00-17:00 Anniversary Milonga Alive Tango Victoria About Discussion More About Discussion Anniversary Milonga Interested Going Invite Details 22 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 5 hr Public · Anyone on or off Facebook 10 years of Alive Tango in Victoria! 10 years of friendships, events and exploring the music, the movement, the possibilities. 10 years of mutual support in tango and life. So many people came and moved on  but everyone left something behind, built a small piece of Alive. So many of you came but stayed building, creating and shaping us. It takes a village and we all are part of it!!! Afternoon Anniversary Milonga ! Cake (made by Danusia!!)and bubbly ( we encourage you to bring your own water bottle or a cup .. we might run out of the ones in the studio ). Let us know if you can come 12pm-5pm $10 Two amazing DJs : Carol Horowitz ( Montreal) and Dan Boccia ( Anchorage) ( the artwork by Rasanga Weerasinghe) See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C887" s="3" t="n">
+        <v>45835.49039851852</v>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1864555154338100/</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 21 21 Jun at 17:00 – 22 Jun at 13:30 Weekend with Tango Alive Tango Victoria About Discussion More About Discussion Weekend with Tango Details 18 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 21st 5pm-6pm solo technique all levels. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) We will continue from May with the musicality for phrase change but this time we will add “double time” to help us with it, using examples of different orchestras. We will work with a “rebound” and half giros to change the direction within the phrase. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 22nd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are September 20th &amp; 21st. Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C888" s="3" t="n">
+        <v>45835.49039851852</v>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1318668532737609/</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 16 16 Apr at 18:30 – 18 Apr at 21:00 Tango week with Lya Alive Tango Victoria About Discussion More About Discussion Tango week with Lya Details 36 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 3 days Public · Anyone on or off Facebook Ignite Your Tango 16th of April, Wednesday 6:30-8:00 On &amp; Off Acis for social dance 18th of April, Friday 6:00 - 7:30 Follower technique 7:45 - 9:00 Switch role / connection Search - Grow &amp; Transform! Seminar series for Tango Dancers that want to transform their way of moving and connecting! We will travel through the Essentials of Tango in order to look for new answers and deeper understanding. What makes tango truly captivating? It’s the embrace, the connection, and the walk. These three fundamental elements are the heartbeat of tango, and mastering them is essential for creating an unforgettable dance experience. You will learn how to condition your body to move with control, fluidity, and elegance. You’ll discover how to find and perfect your axis, which is essential for maintaining balance and stability in every step. We will also explore dissociation, a technique that allows you to move the upper and lower body independently but associated. This workshop series will show you how to apply these principles in both the leader and follower roles, improving connection and response in every moment of the dance. We will apply all this to: The secrets to generating power for boleos effortlessly off and on axis special follower technique class Pro tips to dance with ease and confidence 90 min class - $30 All 3 classes - $80 To register email grazs@shaw.ca or pm me, or talk to me . See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C889" s="3" t="n">
+        <v>45835.49039851852</v>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3637725693193744/</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 22 Mar at 17:00 – 23 Mar at 13:30 Weekend with Tango with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Weekend with Tango with Jorge Olguín Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 22nd 5pm-6pm solo technique all levels. Balance and weight transfer while walking, change of dynamics to create a better connection with your body. ( no partner required) 6.30pm-7.30pm for couples only ( need some experience) Marathon is just around the corner so this month we continue with comfortable close embrace! We continue with dancing in small spaces!! Let’s move gracefully without affecting the partner's axis in elastic hugs of closed embrace. 8pm milonga !!! Join us even if you didn’t take the classes. Free for people registered for the workshops. $10 for drop-ins. Sunday, 23rd 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available only on Saturday. Sunday - sold out Next workshop dates are the May 17th &amp;18th Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C890" s="3" t="n">
+        <v>45835.49039851852</v>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1009684807956058/</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 17 17 May at 17:00 – 18 May at 13:30 Tango weekend with Jorge Olguín Alive Tango Victoria About Discussion More About Discussion Tango weekend with Jorge Olguín Details 28 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Duration: 20 hr 30 min Public · Anyone on or off Facebook Saturday, 17th 5pm-6pm solo technique all levels. ( no partner required) Please bring elastic bands!! 6.30pm-7.30pm for couples only ( need some experience) Sacadas, barridas and colgadas in an elastic embrace in order to create a circular movement. We will work with different orchestras to study the changes we need to do to introduce different tempos and rhythms. Get ready for a workout with musicality! 8pm milonga !!! Join us even if you didn’t take the classes. DJ Ingrid !! Free for people registered for the workshops. $10 for drop-ins. Sunday, 18th 11am-12pm solo technique all levels ( no partner required) 12.30pm-1.30pm for couples only ( need some experience ). We will continue with Saturday topic. We will push for more , go deeper , laugh more . Per person: $20 / technique class $25/ partnered workshop $80 entire weekend To register please contact Grazyna ( grazs@shaw.ca or text me or just talk to me ) Private lessons available- register with Grazyna Next workshop dates are June 21st &amp; 22nd Thank you See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C891" s="3" t="n">
+        <v>45835.49039851852</v>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1225266505917189/</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Saturday Beginner Lesson and Social Dancing Dance Victoria Sat, 14 Jun Sat, 21 Jun Sat, 28 Jun Sat, 12 Jul +3 About Discussion More About Discussion Victoria WCS Collective hosts Saturday Beginner Lesson and Social Dancing Interested Going Invite Details 8 people responded Event by Donna Forsyth Dance Victoria Duration: 3 hr 30 min Public · Anyone on or off Facebook Back to AIR CONDITIONED comfort at Dance Victoria Studios Beginner lesson from 7 to 8 pm Social dancing  from 8 to 10:15 pm Cost $15/$12 for students No need to register and no need for previous dance experience or a partner. Please bring scuff-free inside low-heeled dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C892" s="3" t="n">
+        <v>45835.49294594907</v>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3963074663954670/</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Tuesday dances Eastern Star Hall Chapters No 5 &amp; No 17 Tue, 15 Jul Tue, 22 Jul Tue, 29 Jul About Discussion More About Discussion VIctoria WCS Collective Tuesday dances Interested Going Invite Details 1 person responded Event by Donna Forsyth and Victoria West Coast Swing Collective Eastern Star Hall Chapters No 5 &amp; No 17 Duration: 6 hr 45 min Public · Anyone on or off Facebook $7 at the door - cash or etransfer. Free for dancers registered in a series of WCS lessons. Door opens at 7:30pm. DJ's in the comments. Beginners are welcome. No partner is required. There will NOT be a beginner lesson, but if you're brand new, let the person at the door know and they'll find someone to teach you the starter steps. Dance shoes or socks on the dance floor only. Bring your own water. No food or drink (except water) in the dance area by request of the hall. If you bring a snack to keep your energy up, please enjoy it in the foyer. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Saanich, BC V8Z 3S3, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C893" s="3" t="n">
+        <v>45835.49294594907</v>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/516994561244886/</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:45 Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING White Eagle Polish Association About Discussion More About Discussion Victoria WCS Collective hosts Chantelle for Sat April 5th LESSON  PLUS 3 HOURS  SOCIAL DANCING Details 15 people responded Event by Donna Forsyth , Andre Russo and Victoria West Coast Swing Collective White Eagle Polish Association Public · Anyone on or off Facebook Doors open at 6:45pm at this fabulous new venue! Advanced beginner/intermediate lesson by Chantelle Pianetta from 7 to 8 pm Social dancing for 3 HOURS from 8 to 11 pm DJs Donna and Andre Cost $15 /$12 for students ALL at the spacious White Eagle Hall No need to register and you do not need a dance partner. Please bring scuff-free dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia White Eagle Polish Association 90 Dock St, Victoria, BC V8V 2A1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C894" s="3" t="n">
+        <v>45835.49294594907</v>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2162855673833831/</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Saturday Night WCS Intro Lesson and Social Dance BC Swing Dance Club Victoria 11 May 2019 18 May 2019 25 May 2019 +1 Carolyn Gebbie invited you About Discussion More About Discussion Victoria Saturday Night WCS Intro Lesson and Social Dance Details 8 people responded Event by BC Swing Dance Club Victoria BC Swing Dance Club Victoria Duration: 4 hr 15 min Public · Anyone on or off Facebook Wow! April went by so quickly, which means it must've been super fun, which it definitely was.  Everyone at BC Swing Dance Club Victoria is so pleased with the way the first month of social dances went, and we hope to generate the same amount of enthusiasm in May. Let's make this month just as much fun! Come join us on May 4th for the first intro lesson and social dance of the month (plus every Saturday night after that). Just $10 for the lesson and/or social dance ($5 for students). No experience or partner required. • 6:45 pm - Doors open • 7:00 pm - Intro lesson with Sam Jackson and Meaghan Efford * • 8:00 - 11:00 pm - Social dance with DJ Carolyn Gebbie *PLEASE NOTE that the weekly lessons will start PROMPTLY at 7pm.  It is disruptive to the flow of the lesson if participants arrive late. For anyone who's interested in building their West Coast Swing fundamentals quickly, note that May will be the last month we'll be offering weekly classes with both Sam and Meaghan. With summer approaching it's a great time to build, refresh or accelerate your skills in the dance, so please be sure to take advantage of this opportunity. Please SHARE and INVITE your Westie friends to these events - THANKS! See less Child-friendly Guests See All</t>
+        </is>
+      </c>
+      <c r="C895" s="3" t="n">
+        <v>45835.49294594907</v>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1366072544640156/</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Saturday 17 May 2025 at 18:45 Victoria WCS Collective Beginner Lesson and Social Dancing Dance Victoria About Discussion More About Discussion Victoria WCS Collective Beginner Lesson and Social Dancing Details 9 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson from 7 to 8 pm by John de Pfyffer Social dancing from 8 to 10:15pm DJg by Donna and Nel Cost $15/ $12 for students No need to register and no need for dance experience.. Also, no partner necessary, we got you! Please bring indoor scuff-free dance shoes or socks to dance in. See less Victoria, British Columbia Dance Victoria 2750 Quadra St # 111, Victoria Dance Victoria brings the "World's Best Dance" to the Royal Theatre and supports new dance creation for the international stage from its studios. Guests See All</t>
+        </is>
+      </c>
+      <c r="C896" s="3" t="n">
+        <v>45835.49294594907</v>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/967438905456066/</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Wednesday 26 March 2025 at 10:00 Victoria WCS Lesson and Dance at Eastern Star Hall Eastern Star Hall Chapters No 5 &amp; No 17 About Discussion More About Discussion Victoria WCS Lesson and Dance at Eastern Star Hall Details 1 person responded Event by Donna Forsyth Eastern Star Hall Chapters No 5 &amp; No 17 Public · Anyone on or off Facebook Doors open at 6:45pm Beginner lesson by John de Pyffer from 7 to 8 pm Social dancing from 8 to 10:15pm Djs Amanda and Nel Cost $12 No need to register and no partner required. Please bring scuff-free indoor shoes or socks to dance in  and a water bottle. See less Victoria, British Columbia Eastern Star Hall Chapters No 5 &amp; No 17 3281 Harriet Rd, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C897" s="3" t="n">
+        <v>45835.49294594907</v>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1024182725709172/</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Saturday April 19th Lesson and Social Dance Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 19th Lesson and Social Dance Details 4 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginner plus lesson with Pamela Podmoroff from 8 to 10:15 pm Social dancing from 8 to 10:15 pm DJs Donna and Amanda Cost $15/ $12 for students No need to register and no partner required. Please bring scuff-free indoor dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C898" s="3" t="n">
+        <v>45835.49294594907</v>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/641769172035949/</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Saturday April 12 Beginner lesson and social dance at Dance Victoria Dance Victoria About Discussion More About Discussion Victoria WCS Collective Saturday April 12 Beginner lesson and social dance at Dance Victoria Details 5 people responded Event by Donna Forsyth and Victoria West Coast Swing Collective Dance Victoria Public · Anyone on or off Facebook Doors open at 6:45 pm Beginners lesson by Donna from 7 to 8 pm Social dancing from 8 to 10:15 pm DJs Andre and Nel Cost $15 /$12 for Students No need to register and no partner required. Please bring scuff-free inside dance shoes or socks to dance in and a water bottle. See less Victoria, British Columbia Dance Victoria 2740 Quadra St, Victoria, BC V8T 4E8, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C899" s="3" t="n">
+        <v>45835.49294594907</v>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1022330066692643/</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Wednesday 2 July 2025 at 18:30 Technique and Milonga with Monica Parra Alive Tango Victoria About Discussion More About Discussion Technique and Milonga with Monica Parra Interested Going Invite Details 26 people responded Event by Grazyna Sommerfeld and Alive Tango Victoria Alive Tango Victoria Public · Anyone on or off Facebook 2nd of July , Wednesday 6.30-8pm Follower’s technique: Pivots and turns • Dissociation technique and axis control. • Free leg preparation before the turn. • Turns in tight spaces (useful in a close embrace!!) 90 minutes, $30 9th of July , Wednesday 6.30-8pm Couple workshop: Milonga Lisa and Milonga with traspie using different tempo. 90 minutes, $30 Both workshops (July 2nd and 9th)$50 Register with Grazyna (grazs@shaw.ca, Messenger or simply talk to me) Contact me personally for privates with Monica. See less Victoria, British Columbia Alive Tango Victoria 1303 Broad St. , Victoria Alive Tango offers practicas, milongas, and classes, special events, and workshops with guest instructors in Victoria BC. Guests See All</t>
+        </is>
+      </c>
+      <c r="C900" s="3" t="n">
+        <v>45835.49444399306</v>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/644050564927019/</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Sunday Afternoon Milonga Downtown Victoria, Victoria About Discussion More About Discussion Sunday Afternoon Milonga Details 42 people responded Event by Jeannie Kam Downtown Victoria, Victoria Duration: 3 hr Public · Anyone on or off Facebook Hello Tango Friends! A NEW SUNDAY AFTERNOON MILONGA! This is the first of a regular monthly milonga at a beautiful new venue…The Coda Club (formerly Hermann’s Upstairs) at 751 View Street, Victoria. Great ambience, nice wood floor, good sound system. So come join us for the warm hugs and close embrace and dance to the beautiful music of our very own DJ John Dewhirst. Sunday, 6 April 2025 2.00pm-5.00pm The Coda Club, 751 View Street, Victoria Admission $15 DJ: John Dewhirst Cash Bar is open for drinks Free Parking at View Street Parkade just next door Come celebrate this exciting day with us! See less Victoria, British Columbia Downtown Victoria Downtown Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C901" s="3" t="n">
+        <v>45835.49444399306</v>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/713923214640962/</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Sunday 4 May 2025 from 13:00-16:00 May 4th Afternoon Milonga Solwood Studio About Discussion More About Discussion May 4th Afternoon Milonga Details 45 people responded Event by Ingrid Love and Kathryn Stone Solwood Studio Duration: 3 hr Public · Anyone on or off Facebook A one-time special afternoon milonga! Join us in celebrating the warmth of Spring and return to sunshine. Or, star wars, if you like. Featuring special guests Kimberly and Khang performing live music (violin/guitar) DJ Ingrid Hosts: Kathryn &amp; Ingrid $15 entry (cash only) 1:00pm-4:00pm Solwood Studio 1303 Broad St Victoria, BC See less Victoria, British Columbia Solwood Studio Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C902" s="3" t="n">
+        <v>45835.49444399306</v>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1093118172681618/</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>(20+) The Joan Bessie Cabaret: a celebration of original  live music and dance | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 2 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 29 Sunday from 19:00-22:00 The Joan Bessie Cabaret: a celebration of original  live music and dance Metro Studio Theatre About Discussion More About Discussion The Joan Bessie Cabaret: a celebration of original  live music and dance Interested Going Invite Details Event by Joan Bessie Metro Studio Theatre Tickets · CA$5-CA$35 www.eventbrite.ca/e/joan-bessie-cabaret-tickets-1248762816199 Public · Anyone on or off Facebook Get ready to experience a night of songs and choreography at this one-of-a-kind indie cabaret. Licensed all ages event. Music and audio Victoria, British Columbia Tickets Find Tickets Metro Studio Theatre 1411 Quadra Street at Johnson Street, Victoria Meet your host Joan Bessie 13 past events · Page · Musician/band Joan Bessie is a chart topping Canadian artist. This page shares releases &amp; live tour information Message Suggested events This Sunday at 19:00 GROOVE KITCHEN'S JUNEFEST DANCE!! Hermann's Jazz Club Carmie is interested 98 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1509 people interested Interested Sat, 5 Jul at 12:00 Victoria, BC - Victoria Folk Music Festival, Royal Athletic Park Royal Athletic Park Debi and Carmie are interested 1298 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C903" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1137992241425588/</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Today from 13:00-15:00 Music in Abkhazi Garden Abkhazi Garden Fri, 27 Jun Fri, 4 Jul Fri, 11 Jul +5 About Discussion More About Discussion Music in Abkhazi Garden Interested Going Invite Details 14 people responded Event by Victoria Conservatory of Music Abkhazi Garden Duration: 2 hr Public · Anyone on or off Facebook Abkhazi Garden hosts Victoria Conservatory of Music students and faculty for a season of live outdoor performances from June 13 to August 15, every Friday from 1:00pm to 3:00pm. Admission is by donation. The address of Abkhazi Garden is 1964 Fairfield Road, Victoria, BC V8S 1H4 See less Victoria, British Columbia Abkhazi Garden 1964 Fairfield Road, Victoria Explore a one-of-a-kind west coast, heritage garden in a quiet Victoria neighborhood on Vancouver Island. Open seven days a week 11 am – 5 pm. Last entrance, 4:00pm. Entrance by donation. We suggest $10/person. Guests See All</t>
+        </is>
+      </c>
+      <c r="C904" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1239927167616785/</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Thursday 11 September 2025 at 19:00 Rest and Resonate - Restorative Yoga ft. cozy Live Music Fernwood Community and Arts Association About Discussion More About Discussion Rest and Resonate - Restorative Yoga ft. cozy Live Music Interested Going Invite Details 9 people responded Event by Across the Water Fernwood Community and Arts Association Tickets www.annabiglandpritchard.com/event-details/rest-resonate-restorative-yoga-ft-cozy-live-music-1-1 Public · Anyone on or off Facebook A dreamy and nourishing evening retreat offering restorative yoga, live music, and guided journalling. Still warm with the energy of the September full moon in Pisces (the Corn Moon) - this is a great time to celebrate and embrace life, nourishing our bodies so they can carry out our most impactful dreams. Facilitated by: Roxie Fehr of Across the Water | Yoga, Meditation, and Indian Head Massage &amp; Anna Bigland-Pritchard of Rose House | Music (harp, vocal looping, singing) and poetry reading What to bring: Yoga mat Journal &amp; pen/pencil Yoga bolster Yoga blocks Blanket Any other props you'd like to use Yourself as you are Details: Thursday September 11th, 7-8:30pm at Little Fernwood If cost is a barrier, please contact us directly as we have a limited number of discount codes available Come as you are, leave nourished by your dreams See less Victoria, British Columbia Tickets Find Tickets Fernwood Community and Arts Association 1923 Fernwood Rd., Victoria Welcome to the Fernwood Community and Arts Association FB page. This site is used to distribute updates on FCAA meetings, initiatives and events. Join or renew your membership at www.thefca.ca or our office 1923 Fernwood Rd. Guests See All</t>
+        </is>
+      </c>
+      <c r="C905" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2579625309035667/</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Sunday 18 May 2025 from 12:00-18:00 Live Music @ Junction (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Live Music @ Junction (RAIN OR SHINE) Details 125 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Here we go again, its a long weekend so let's get our Sunday Funday on. First Live Music of the year at Junction Up first is-  Emergency Exit  are playing from 1230-230pm To take us home is - An &amp; Ben are playing from 3-5pm Tasting Room and Picnic Area are open 12-6pm Oh and if you haven't heard me say it before ITS RAIN OR SHINE. Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Cider ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀⠀⠀⠀⠀⠀ Mini Market and a Beautiful location ⠀⠀⠀⠀⠀⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your well behaved two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C906" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1482463219409922/</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Wednesday 2 July 2025 from 19:30-19:31 Live Music Sessions at Crafthouse Vic West #100 - 184 Wilson Street, Victoria, BC, Canada About Discussion More About Discussion Live Music Sessions at Crafthouse Vic West Interested Going Invite Details 2 people responded Event by Browns Crafthouse Vic West #100 - 184 Wilson Street, Victoria, BC, Canada Duration: 1 min Public · Anyone on or off Facebook Join us every Wednesday night for local live music starting at 730pm. 1/2 wings &amp; 1/2 bottles of wine. Victoria, British Columbia #100 - 184 Wilson Street, Victoria, BC, Canada 184 Wilson St, Victoria, BC V9A 7N6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C907" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/650159601522409/</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>(20+) Rest and Resonate - Restorative Yoga ft. cozy Live Music  | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 2 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 9 Saturday 9 August 2025 at 19:30 Rest and Resonate - Restorative Yoga ft. cozy Live Music Fernwood Community and Arts Association About Discussion More About Discussion Rest and Resonate - Restorative Yoga ft. cozy Live Music Interested Going Invite Details Event by Across the Water Fernwood Community and Arts Association Tickets www.annabiglandpritchard.com/event-details/rest-resonate-restorative-yoga-ft-cozy-live-music-1 Public · Anyone on or off Facebook A dreamy and nourishing evening retreat offering restorative yoga, live music, and guided journalling. Fresh on the heels of the August full moon in Aquarius - this is a great time to charge up your batteries and dream up visionary ways to improve the state of world together. Facilitated by: Roxie Fehr of Across the Water Yoga and Wellness | Yoga, guided meditation, and Indian Head Massage  &amp; Anna Bigland-Pritchard of Rose House | Music (harp, vocal looping, singing) &amp; poetry reading What to bring: Yoga mat Journal &amp; pen/pencil Yoga bolster Yoga blocks Blanket Any other props you'd like to use Yourself as you are Details August 19, 7-8:30pm at Little Fernwood If cost is a barrier, please contact us directly as we have a limited number of discount codes available Come as you are, leave nourished by your dreams See less Music and audio Victoria, British Columbia Tickets Find Tickets Fernwood Community and Arts Association 1923 Fernwood Rd., Victoria Welcome to the Fernwood Community and Arts Association FB page. This site is used to distribute updates on FCAA meetings, initiatives and events. Join or renew your membership at www.thefca.ca or our office 1923 Fernwood Rd. Meet your host Across the Water 2 past events · Page · Fitness trainer Across the Water facilitates Yoga and Group Fitness in Victoria, BC. We value community and connection and just love to have fun while moving ou… Contact Us Suggested events Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested 32 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1509 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 58 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C908" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1975172826621817/</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>(20+) Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 2 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 12 Thursday 12 June 2025 from 19:00-20:30 Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Little Fernwood Gallery. About Discussion More About Discussion Rest&amp;Resonate: an Evening of Restorative Yoga and Live Music Details Event by Across the Water and Anna Bigland-Pritchard Little Fernwood Gallery. Duration: 1 hr 30 min Public · Anyone on or off Facebook Do you need some R&amp;R? Join Anna &amp; Roxie for a dreamy candlelit evening of restorative yoga, live music, and guided journalling. Facilitated by Roxie Fehr of Across the Water | Yoga Anna Bigland-Pritchard of ABP Music Studio | Music As experienced, intuitive space-holders, our goal to support your Nervous System and capacity for hope with a feast of restful offerings. We know life is stressful and we want to help you feel more connected to your intuition so you can not only survive, but also have the capacity to take the next right step in your life in a way that positively impacts the world. The space will be dreamy, there will be tea, guided journalling, poetry, restorative yoga shapes that can be adapted for any body, and LIVE MUSIC! Anna will be playing guitar, creating dreamy sound worlds with vocal looping, and singing you lullabies all evening. What to bring Yoga mat (We'll have a few available to borrow) Journal &amp; pen/pencil (We'll also have some spare paper and writing/drawing utensils) Yourself in your comfy cozies Details June 12, 7-8:30pm at Little Fernwood $42 Accessibility This event is on the ground floor There is a unisex/non-gendered bathroom on the same level We care about making this event accessible, so please let us know if you have any questions or accessibility needs. This will be a VERY gentle practice, and modifications will be offered. Happy pride! As members of and allies of the 2SLGBTQIA community, we (Anna &amp; Roxie) will create a supportive, inclusive, affirming environment and expect all participants to do the same. If cost is a barrier, please contact us directly as we have a limited number of discount codes available This is our first time offering this class, and we hope it will be a hit so we can make it a regular thing. Come as you are, leave nourished by your dreams See less Victoria, British Columbia Little Fernwood Gallery. 1923 Fernwood Ave., Victoria Meet your hosts Across the Water 2 past events · Page · Fitness trainer Across the Water facilitates Yoga and Group Fitness in Victoria, BC. We value community and connection and just love to have fun while moving ou… Contact Us Anna Bigland-Pritchard 6 past events · Page · Musician/band Based in Lekwungen territory (Victoria, BC), Anna Bigland-Pritchard is a: -Soprano -Voice teacher… Follow Suggested events Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested 32 people interested Interested Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1509 people interested Interested Sun, 6 Jul at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 58 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C909" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1399479741193649/</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Saxe Point Public House About Discussion More About Discussion TUESDAY NIGHT • LIVE MUSIC with VINYL WAVE! Details 4 people responded Event by Tom Watson Saxe Point Public House Public · Anyone on or off Facebook Join Vinyl Wave at the lovely Saxe Point Pub for a couple of hours of smooth tunes that'll help ease you into the week! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C910" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1085685423617722/</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Thursday 25 September 2025 at 10:00 The Men in Black: A Tribute to the Music of Johnny Cash Mcpherson Playhouse About Discussion More About Discussion The Men in Black: A Tribute to the Music of Johnny Cash Interested Going Invite Details 3 people responded Event by Jeff Scott and Victoria Live Music - @BarsnbandsYYJ Mcpherson Playhouse Public · Anyone on or off Facebook The Men in Black: The Songs and stories of Johnny Cash, presented Live onstage in this Multimedia production. Featuring special guest Tracee Rees singing the parts of June Carter Cash. Tickets on sale from the McPherson Box Office: https://www.rmts.bc.ca/.../2025.../the-men-in-black/ See less Victoria, British Columbia Mcpherson Playhouse 48.428809, -123.366838 Guests See All</t>
+        </is>
+      </c>
+      <c r="C911" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/665127126496204/</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Tuesday 27 May 2025 at 19:30 Live Music at the Saxe Point Public House Saxe Point Public House About Discussion More About Discussion Live Music at the Saxe Point Public House Details 9 people responded Event by VINYL WAVE Saxe Point Public House Public · Anyone on or off Facebook Live Music every other Tuesday starting May 27th! Victoria, British Columbia Saxe Point Public House 101-505 Park Place, Victoria The New Pub Of Esquimalt! A haven for those who appreciate the art of good company and brews. Guests See All</t>
+        </is>
+      </c>
+      <c r="C912" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1142760357225336/</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 26 26 Jul at 10:00 – 27 Jul at 17:00 ArtisTREE Festival 1401 rockland ave, Victoria, BC, Canada About Discussion More About Discussion ArtisTREE Festival Interested Going Invite Details 1.3K people responded Event by Artistree Festival , MORENA CLOTHING and Cory Judge 1401 rockland ave, Victoria, BC, Canada Duration: 2 days Public · Anyone on or off Facebook Saturday July 26 10-7pm Sunday July 27 10-5pm Government House of BC 1402 Rockland Ave Celebration of Creativity profiling 130 Juried Artisans, Live Music, Installation and Performance Art, Indigenous Makers and Traditions, Kids section, Live Painters, Delicious Food and Ice cream. See less Shopping Victoria, British Columbia 1401 rockland ave, Victoria, BC, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C913" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/711942901691957/</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 27 Jun at 18:30 – 29 Jun at 22:00 TD International Jazz Festival Bullen Park Esquimalt About Discussion More About Discussion TD International Jazz Festival Interested Going Invite Details 1 person responded Event by Dig BC Bullen Park Esquimalt Duration: 3 days Public · Anyone on or off Facebook Live music, amazing food, and a great community vibe. We’ll be serving up the best fresh-pressed lemonade on the planet (so I’ve heard), Iced Chai, Cold Brew Coffee, Ice Tea, hot chicken wraps (with a super sauce made from the finest ESB from Milezerobrewing) Veg wraps and a few Jazz Fest specials you won’t want to miss. And look at all that in the forecast! My Go Power  panels will be soaking it all up! Join us Friday through Sunday and make it a weekend to remember. June 28–30 Bullen Park, Esquimalt Tag us in your photos @digbc1979 Victoria Jazz Society See less Victoria, British Columbia Bullen Park Esquimalt 1150 Lyall St, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C914" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/686146924271113/</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>(20+) Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Thursday 3 July 2025 from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 2 friends Recommended events See all Today from 20:00-00:00 Bachata Night Lorne and 4 friends Sunday from 15:45-19:30 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Lorne and 6 friends Tomorrow from 20:00-23:59 Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 5 Thursday 5 June 2025 from 19:00-22:00 Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz 753 View St, Victoria, BC V8W 1J9, Canada About Discussion More About Discussion Adonis Puentes &amp; The Jazz Bohemians - Live at Hermann's Jazz Details Event by Adonis Puentes and Brent Jarvis 753 View St, Victoria, BC V8W 1J9, Canada Duration: 3 hr Public · Anyone on or off Facebook An evening of Jazzy Cuban Fusion Music; traditional, contemporary, romance and dance. Juno &amp; Grammy Nominated vocalist, Adonis Puentes, will be joined by the Jazz Bohemians, featuring Brent Jarvis (piano), Ken Lister (bass), Nicholas Marquez (percussion) and Brooke Maxwell (Sax). Adonis Puentes opens up the marvelous world of Cuban music to his audience the second they hear his rich voice. When the other players kick in with their tight, multi-layered arrangements, it becomes clear that Adonis is a powerful bandleader. Fronting an acoustic band, Adonis' vocals are surrounded by piano, bass, strings, and percussion. Music reflects the present and Adonis Puentes is a Cuban Sonero for our times. Adonis thrives on the growth and acclaim for his original sonero sound. As he puts it, "I feel like a messenger of my roots and tradition, blessed that with me I have taken my music and heritage to many different places in the world; from Cuba, to Canada, USA, Mexico, Europe and Asia. My mission is to make you dance and enjoy my melodies and rhythms." Musician Line-Up: Adonis Puentes - Vocals Brent Jarvis - Piano Ken Lister - Bass Nicolas Marquez - Percussion Brooke Maxwell - Sax See less Music and audio Victoria, British Columbia 753 View St, Victoria, BC V8W 1J9, Canada 751 View St, Victoria, BC V8W 1J9, Canada Meet your hosts Adonis Puentes 34 past events · Page · Musician/band Adonis Puentes is a great singer and an elegant composer and lyricist grounded and nourished by his Cuban roots and worldly experience. Message Brent Jarvis 37 past events · Profile · Musician Message Suggested events Sat, 2 Aug-3 Aug 7th Annual ViVa! Victoria Latin Fest 2025 Centennial Square, Victoria, BC, Canada, British Columbia Lorne, Roy and 10 friends 1509 people interested Interested Fri, 29 Aug at 19:00 GLOW • i-Land Fest Kick-Off Fete Ambrosia Banquet Nadia is interested 131 people interested Interested Thu, 18 Sep at 18:00 THE WAILERS NATURAL MYSTIC 30TH ANNIVERSARY TOUR - THUR. SEPT 18 AT ROYAL ATHLETIC PARK IN VICTORIA! Royal Athletic Park Linda is interested 581 people interested Interested Popular with friends Today at 20:00 Bachata Night Method Studio - Victoria BC Lorne, Roy and 3 friends are interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and 5 friends Interested Tomorrow at 20:00 Saturday Salsa/Bachata Social June 28th Ukrainian Cultural Centre Lorne, Roy and 3 friends Interested Sat, 5 Jul at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Roy and 7 friends Interested Fri, 27 Jun-29 Jun FUNK 'N SOUL IN THE TOWNSHIP: TD JazzFest 2025 Bullen Park Esquimalt Lorne, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C915" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1050242777151793/</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 10 10 Jun at 09:00 – 15 Jun at 19:00 KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Victoria ,BC About Discussion More About Discussion KLEZCADIA Festival--A Safer Shtetl for Klezmer Music &amp; Yiddish Culture Details 46 people responded Event by Congregation Emanu-El, Victoria, British Columbia Victoria ,BC Duration: 6 days Public · Anyone on or off Facebook Registration required for both in person and virtual attendance. https://klezcadia.org https://congregationemanuelnews.wordpress.com/.../klezca.../ Locations of performances and workshops provided upon registration. See less Victoria, British Columbia Victoria ,BC 528 Broughton St, Victoria, BC V8W 1C6, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C916" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1225611168970110/</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Saturday Salsa/Bachata Social June 28th Lorne and 4 friends Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 25 25 Jul at 17:30 – 26 Jul at 20:00 Indigenous Music Festival Hampton Park About Discussion More About Discussion Indigenous Music Festival Interested Going Invite Details 687 people responded Event by Saanich Parks, Recreation &amp; Community Services Hampton Park Duration: 2 days Public · Anyone on or off Facebook Celebrate the 5th Annual Indigenous Music Festival at Hampton Park! A free two-night celebration of Indigenous performers from across Vancouver Island. Craft market and food vendors on site as well. Friday, July 25, 2025, from 5:30 to 8:00pm -Esquimalt Drummers and Dancers -OTR (Off the Reservation) -James Vickers Band Saturday, July 26, 2025, from  5:00 to 8:00pm -Lekwungen Traditional Dancers -Killed Instantly -Yellow Wolf w/ Benny the Jet -Nate Harris - Nate Harris Band featuring Madison Olsen Learn more at saanich.ca/indigenousmusicfestival See less Music and audio Victoria, British Columbia Hampton Park 224 Hampton Rd, Saanich Guests See All</t>
+        </is>
+      </c>
+      <c r="C917" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1451663826076478/</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Sunday 6 July 2025 from 11:00-16:00 Saanich Strawberry Festival Beaver Lake Regional Park, 728 Beaver Lake Rd. About Discussion More About Discussion Saanich Strawberry Festival Interested Going Invite Details 1K people responded Event by Saanich Parks, Recreation &amp; Community Services Beaver Lake Regional Park, 728 Beaver Lake Rd. Duration: 5 hr Public · Anyone on or off Facebook Join Saanich in celebrating the 58th annual Strawberry Festival. This family-friendly, fun, free event features live music, kids' activities, bouncy castles, information booths, arts and craft stations and, of course, the traditional servings of strawberries and ice cream. Strawberries and ice cream sales and service will be from 2 to 4pm, or until sold out. $2/serving. For more details, including vendors, activities and performances, visit saanich.ca/strawberryfestival See less Foods Victoria, British Columbia Beaver Lake Regional Park, 728 Beaver Lake Rd. 728 Beaver Lake Rd, Saanich, BC V8Z 6K2, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C918" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1110747367748372/</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Saturday 5 July 2025 at 12:00 Victoria Folk Music Festival Royal Athletic Park About Discussion More About Discussion Victoria Folk Music Festival Interested Going Invite Details 983 people responded Event by Victoria Folk Music Festival and Cascadia Concerts Royal Athletic Park Tickets · Free-CA$86.53 vicfolkfest.eventbrite.ca Public · Anyone on or off Facebook Date: July 5, 2025 Location: Royal Athletic Park, Victoria, BC Tickets: Available now at vicfolkfest.eventbrite.ca Gates Open: 12:00 PM Victoria Folk Music Festival Join us for a joyful weekend of music, community, and celebration at Victoria Folk Music Festival, on July 5th set in beautiful Royal Athletic Park . Featuring a world-class lineup including Frazey Ford, Joel Plaskett, Kacy &amp; Clayton, Harry Manx, Ferron, Old Man Luedecke, Vince Vaccaro, Canadian Beauty, Daneil Lapp's BC Fiddle Orchestra and more, this family-friendly event brings together the best in folk, roots, and Americana music. With two stages of live performances, the Victoria Folk Music Festival offers a full day of entertainment and community celebration. Explore the ReLove Vintage Pop-Up Market, showcasing top local vendors with the best in thrift, retro, and vintage wear. Enjoy a variety of Artisan goods and vendors, delicious food from Fresh Coast, Deadbeetz, Taco Revolution, and more. Families will love the vibrant children’s area—complete with a jumping castle! Dance in the grass to local Bluegrass groups and explore vendor booth from local music groups &amp; organizations. A community-driven atmosphere with world-class music at its heart, this festival is set to be a summer highlight for music lovers of all ages. Whether you're dancing barefoot in the grass, discovering your new favorite artist, or relaxing in the shade with friends, the Victoria Folk Music Festival is more than a concert — it’s a celebration of sound, soul, and connection. Don’t miss the unforgettable music and summer moments —July 5th at Royal Athletic Park! See less Music and audio Victoria, British Columbia Tickets Find Tickets Royal Athletic Park 1014 Caledonia Ave, Victoria Royal Athletic Park is a multi-purpose, fully lit stadium in Victoria, British Columbia. It is primarily used for baseball, soccer, softball and football, but also hosts special events, such as the annual Great Canadian Beer Festival and Rifflandia Music Festival. It is approximately a ten-minute walk from the city centre.HistoryIn 1907 the burgeoning summer athletic teams did not have enough facilities for senior teams with paid attendances. Baseball in particular was challenged to find available dates at Oak Bay Grounds to operate due to a preference for lacrosse.Subsequently, the supporters of Canada's national summer sport lacrosse, at a meeting chaired by BC Premier McBride formed the Royal Victoria Athletic Association on March 26, 1908, and a senior lacrosse team was founded to enable the best intermediate (Under 21) players to play in the British Columbia Amateur Lacrosse Association (BCALA) League. The Oak Bay Grounds were put under the management of the senior baseball team and then later the Rugby Football Club. The lacrosse group, later shortened to the Royal Athletic Association, issued shares at $25 each with deposits of 10% and biannual calls of 10% to raise $25,000 for improvements to the grounds. The lease was signed for 5 acres at the corner of Cook and Pembroke Streets for the grounds.Contracts had been let by May 12, 1908 and $4,000 from the share offering and gate receipts was spent by June on the construction of a perimeter fence, 2 ticket offices, an inner fence, grandstand, and carriage parking area. The inner fence enclosed the 500 ft x 285 ft (152m x 87m) playing field. The grandstand on the south side of the playing field was 150 ft long x 25 ft deep with 10 rows of seats for more than 1000 spectators. Beneath the grandstand were dressing rooms and concessions. The original layout of the field and grandstand was essentially the same as today's; however based on maps used in advertising the original field also included half of the city block to the west between Quadra and Vancouver Streets. The carriage parking was on the east side off Cook Street. Guests See All</t>
+        </is>
+      </c>
+      <c r="C919" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/651664851189740/</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 12:00-18:00 Music in the Orchard (RAIN OR SHINE) Junction Orchard &amp; Cidery About Discussion More About Discussion Music in the Orchard (RAIN OR SHINE) Details 330 people responded Event by Junction Orchard &amp; Cidery Junction Orchard &amp; Cidery Duration: 6 hr Public · Anyone on or off Facebook Come enjoy the start of the summer in the orchard. We have two amazing artists for you, some delicious fun summer ciders for you to try and amazing food to enjoy to complete the experience. Delicious Cider Live Music ⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀⠀ Bicycle Pizza ⠀⠀⠀⠀ Beautiful location ⠀⠀⠀⠀ Dog Friendly ⠀⠀ ⠀⠀⠀⠀ ⠀⠀⠀⠀⠀⠀⠀⠀⠀ This is an outdoor event so bring your WELL BEHAVED two legged and 4 legged babies and dress appropriately coz we are going ahead RAIN OR SHINE! See less Music and audio Victoria, British Columbia Junction Orchard &amp; Cidery 284 Prospect Lake Rd, Saanich, BC V9E 1J7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C920" s="3" t="n">
+        <v>45835.50200586332</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1514674672845802/</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Saturday 5 July 2025 at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park About Discussion More About Discussion Oak Bay Summer Concerts in the Park: Family Show Interested Going Invite Details 767 people responded Event by Oak Bay Parks, Recreation and Culture Willows Park Public · Anyone on or off Facebook Oak Bay Summer Concerts in the Park: Family Show With a stunning backdrop of Willows Beach, these outdoor concerts gather the community to celebrate music and the arts.  Presented by Oak Bay Parks, Recreation and Culture. Location: Willows Beach Park, Oak Bay Date: Saturday, July 5, 2025 Time: 2:00 p.m. Admission: Free Family Concert: lək̓ʷəŋən Traditional Dancers, Pacific Opera Victoria, STAGES Dance Company, and Marimba Mufaro. More information: https://www.oakbay.ca/.../oak-bay-summer-concerts-in-the.../ See less Victoria, British Columbia Willows Park 2778 Dalhousie St, Oak Bay, BC V8R, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C921" s="3" t="n">
+        <v>45835.50200586332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor bug in defup_llm.py. Incorrect number of calling arguments for handle_long_event_name().
</commit_message>
<xml_diff>
--- a/checkpoint/extracted_text.xlsx
+++ b/checkpoint/extracted_text.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C921"/>
+  <dimension ref="A1:C1033"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13999,7 +13999,7 @@
         </is>
       </c>
       <c r="C903" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="904">
@@ -14014,7 +14014,7 @@
         </is>
       </c>
       <c r="C904" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="905">
@@ -14029,7 +14029,7 @@
         </is>
       </c>
       <c r="C905" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="906">
@@ -14044,7 +14044,7 @@
         </is>
       </c>
       <c r="C906" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="907">
@@ -14059,7 +14059,7 @@
         </is>
       </c>
       <c r="C907" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="908">
@@ -14074,7 +14074,7 @@
         </is>
       </c>
       <c r="C908" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="909">
@@ -14089,7 +14089,7 @@
         </is>
       </c>
       <c r="C909" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="910">
@@ -14104,7 +14104,7 @@
         </is>
       </c>
       <c r="C910" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="911">
@@ -14119,7 +14119,7 @@
         </is>
       </c>
       <c r="C911" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="912">
@@ -14134,7 +14134,7 @@
         </is>
       </c>
       <c r="C912" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="913">
@@ -14149,7 +14149,7 @@
         </is>
       </c>
       <c r="C913" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="914">
@@ -14164,7 +14164,7 @@
         </is>
       </c>
       <c r="C914" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="915">
@@ -14179,7 +14179,7 @@
         </is>
       </c>
       <c r="C915" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="916">
@@ -14194,7 +14194,7 @@
         </is>
       </c>
       <c r="C916" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="917">
@@ -14209,7 +14209,7 @@
         </is>
       </c>
       <c r="C917" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="918">
@@ -14224,7 +14224,7 @@
         </is>
       </c>
       <c r="C918" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="919">
@@ -14239,7 +14239,7 @@
         </is>
       </c>
       <c r="C919" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="920">
@@ -14254,7 +14254,7 @@
         </is>
       </c>
       <c r="C920" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
       </c>
     </row>
     <row r="921">
@@ -14269,7 +14269,1687 @@
         </is>
       </c>
       <c r="C921" s="3" t="n">
-        <v>45835.50200586332</v>
+        <v>45835.50200586805</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/734261429120710/</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Friday 6 June 2025 from 19:30-22:30 Dance City 108 Niagara St, Victoria, BC V8V 1E9, Canada About Discussion More About Discussion Dance City Details 9 people responded Event by Andrew Sanderson 108 Niagara St, Victoria, BC V8V 1E9, Canada Duration: 3 hr Public · Anyone on or off Facebook Beginner Cha Cha workshop with Jane and Andrew at 7:30pm Multi genres dance including Standard, Latin,  West Coast Swing, and more starting at 8:30pm dj Andrew Sanderson Cash Admission: $12/$10 Members See less Victoria, British Columbia 108 Niagara St, Victoria, BC V8V 1E9, Canada 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C922" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1682353965754886/</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Saturday 14 June 2025 from 18:00-20:30 Mamas' Dance Party! 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Sat, 5 Apr Sat, 10 May Sat, 14 Jun About Discussion More About Discussion Mamas' Dance Party! Details 32 people responded Event by Fairfield Gonzales Community Association 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 Duration: 2 hr 30 min Public · Anyone on or off Facebook Calling all mamas, grand-mamas, aunties &amp; mamas-to-be! Join us for a night curated for all mamas (in any season of their motherhood or reproductive journey) to connect through creative expression, freedom of movement and community building! There will be an opening &amp; closing circle and time to connect over light refreshments as the night concludes. Feel free to come for it all, or leave when needed. We can't wait to dance, groove, and connect with you all soon. This is an inclusive space for ALL those who mother. Admission by-donation: suggested donation $5 This event is presented by the FGCA's Neighbourhood Improvement Committee See less Victoria, British Columbia 1330 Fairfield Rd., Victoria, BC, Canada, British Columbia V8S 5J1 1330 Fairfield Rd, Victoria, BC V8S 5J1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C923" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1326132745826079/</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Sunday from 11:00-12:30 Dance Temple w/ guest DJ Efrévescent Edelweiss Club, 108 Niagara Street About Discussion More About Discussion Dance Temple w/ guest DJ Efrévescent Interested Going Invite Details 19 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, July 6th features Efrévescent as our guest facilitator/dj. Details for Sunday, July 6th: Facilitation and music set by Efrévescent: "Skilled in the art of somatic attunement and healing through relational ways of being, Efrévescent (Efré Divina) weaves together luscious soundscapes that open the heart, deepen the breath, and return the body to centre. Inspired by a wide array of musical influences from dancehall to disco, groove to global underground, and hip-hop to house, the Efrévescent experience aims to leave everyone feeling like they have something to dance to, weaved in an arching progression. Expect intelligent lyrics, intentional rhythms, live saxophone, and a soul-clapping good time.” Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C924" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1800174300532918/</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Friday from 19:30-22:30 Dance City 108 Niagara St, Victoria, BC V8V 1E9, Canada About Discussion More About Discussion Dance City Interested Going Invite Details 4 people responded Event by Andrew Sanderson 108 Niagara St, Victoria, BC V8V 1E9, Canada Duration: 3 hr Public · Anyone on or off Facebook Beginner Jive/Swing workshop with Jane and Andrew at 7:30pm Multi genres dance including Standard, Latin,  West Coast Swing, and more starting at 8:30pm dj Andrew Sanderson Cash Admission: $12/$10 Members See less Victoria, British Columbia 108 Niagara St, Victoria, BC V8V 1E9, Canada 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C925" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1363696181561219/</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Friday 20 June 2025 from 19:00-22:00 Pride Contra Dance Fairfield United About Discussion More About Discussion Pride Contra Dance Details 90 people responded Event by Victoria Contra Dance , Code Tron and Rose Jackson Fairfield United Duration: 3 hr Public · Anyone on or off Facebook 𝕍𝕀ℂ𝕋𝕆ℝ𝕀𝔸 ℂ𝕆ℕ𝕋ℝ𝔸 𝔻𝔸ℕℂ𝔼 𝕊𝕆ℂ𝕀𝔼𝕋𝕐 ℙℝ𝔼𝕊𝔼ℕ𝕋𝕊: The return of our ℚ𝕌𝔼𝔼ℝ Contra Dance to celebrate the month of Pride! All Dancers welcome! Join us Friday, June 20th at the United Commons Fellowship Hall to do-si-do the night away to sprightly fiddle tunes and stellar performances from our two favorite drag performers! We'll have more capacity than our previous Valentines Day Dance, but we still might sell out, so grab your tickets online here! https://clannamorna.ca/.../ticket-victoria-pride-contra.../ ......................................................................................................... 𝕄𝕦𝕤𝕚𝕔 𝔹𝕪: 𝐑𝐨𝐬𝐞 𝐉𝐚𝐜𝐤𝐬𝐨𝐧: she/her Coming up in the rich folk scene of western Massachusetts, Rose is based in Montague, MA, where she studied under fiddler Becky Tracy from whom she inherited a wide repertoire of music from Quebec, New England, Ireland, and France, a deep love for old tunes, and the intuitive sense of rhythm and danceability which infuses her playing. Equally at home in the concert hall and on the dance stage, she’s taught fiddle, song, and dance at camps and festivals around New England, toured nationally with her band Polaris and now tours with her quartet Stove Dragon and duo Helen &amp; Rose. https://www.rose-jackson.com/ 𝐇𝐞𝐥𝐞𝐧 𝐊𝐮𝐡𝐚𝐫: they/them Hailing from Seattle, Washington, Helen currently resides in Cambridge, MA. Helen began exploring their connection to folk and Celtic music in 2020 while studying with renowned contra guitarist Alex Sturbaum. Upon moving to Cambridge in 2022, Helen dove into the thriving celtic music scene, playing contra dances, Irish sessions, and concerts around New England and the Pacific Northwest. Since then, Helen has developed their style as a contra accompanist, Irish session backer, and vocalist. https://www.helenkuharmusic.com/ 𝐅𝐢𝐝𝐝𝐥𝐢𝐧' 𝐅𝐢𝐧𝐧: they/them A professional fiddler, singer and banjo player living on the territories of the lekwungen and W̱SÁNEĆ people, colonially known as Victoria BC. Finn has a passion for Irish, Scottish, English, North American and Eastern European folk music, and are known for their dynamic fiddling and soulful voice. They delve into traditional material - bringing a fresh interpretation of songs and tunes from many different places, as well as writing their own material. From the Appalachian mountains to Quebec, to melodic Irish and Scottish tunes, they cover wide musical ground with articulate playing. Finn also performs frequently in Canada and the U.S. with their bands Clanna Morna and Ghostly Hounds. https://finnletourneau.com/ ℂ𝕒𝕝𝕝𝕚𝕟𝕘 𝔹𝕪: 𝐕𝐢𝐜𝐭𝐨𝐫𝐢𝐚 𝐁𝐞𝐚𝐮𝐜𝐡𝐞𝐬𝐧𝐞 One of our local communities up and coming callers! 𝔻𝕣𝕒𝕘 𝕡𝕖𝕣𝕗𝕠𝕣𝕞𝕒𝕟𝕔𝕖𝕤 𝕓𝕪: Aries Moon: Making country gay one song at a time Leo Moon: The island's premiere tap dancing drag thing ......................................................................................................... 6:30 - doors open 7:00 - dancing starts with a beginner friendly dance lesson Everyone welcome, no experience necessary. $12 - Youth $20 - Everyone who is willing and able to NOTAFLOF Poster Art by Sonya Chwyl See less Victoria, British Columbia Fairfield United 925 Balmoral Rd, Victoria, BC V8T 1A7, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C926" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/939376108286434/</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 3 friends Recommended events See all Today at 18:30 Technique and Milonga with Monica Parra Janine Saturday at 14:00 Oak Bay Summer Concerts in the Park: Family Show Lorne and 4 friends Tomorrow from 19:00-21:30 Swingin' in the Shell Robin Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 27 Friday 27 June 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1924 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events Mon, 18 Aug at 17:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour Roy, Ali and Jon 28 people interested Interested This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 63 people interested Interested Tue, 8 Jul at 21:00 Salsa &amp; Cha Cha Cha- Beg/ Int- July series Studio 4 Athletics 1 people interested Interested Popular with friends Happening now Technique and Milonga with Monica Parra Alive Tango Victoria Janine is going Interested Sun, 20 Jul at 12:00 Anniversary Milonga Alive Tango Victoria Janine is going Interested Tomorrow at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested This Saturday at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Amanda and 7 friends Interested Thu, 10 Jul at 18:00 Oak Bay Summer Concerts in the Park: Soul Intention Willows Park Roy, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C927" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2576922459305643/</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Sunday 15 June 2025 from 11:00-12:30 Dance Temple w/ Cedar Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Cedar Details 51 people responded Event by Dance Temple Victoria and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 15th features Cedar Mathias as our facilitator/dj! Details for Sunday, June 15th: Facilitation and music set by Cedar Mathias Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C928" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/719816763903682/</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Monday 28 July 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 63 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Kizomba with Aaron and Fernanda— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C929" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1408949946810887/</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Sunday 8 June 2025 from 11:00-12:30 Dance Temple w/ Lila Edelweiss Club, 108 Niagara Street, Victoria, BC About Discussion More About Discussion Dance Temple w/ Lila Details 32 people responded Event by Dance Temple Victoria , Lyndsay Lila and Jazmin Love Edelweiss Club, 108 Niagara Street, Victoria, BC Duration: 1 hr 30 min Public · Anyone on or off Facebook Welcome to Dance Temple! Conscious dance and community connection in sacred space. Join us at Edelweiss Club for an ecstatic dance journey ~ Sunday, June 8th features Lila Spencer as our facilitator/dj! Details for Sunday, June 8th: Facilitation and music set by Lila Doors open at 10:45am Dance from 11am to 12:30pm (guided opening at 11) Sliding scale: $20-$40 (no charge for kids under 12); $15-$20 low income Cash at the door or reserve your place with an etransfer to dancetempleinfo@gmail.com Dance Temple is a weekly Sunday offering. Newcomers welcome! No experience necessary. Please attend only if you feel 100% well. Regular Temple Guidelines (please read through, especially if you're new to Dance Temple): **SHIRTS ON PLEASE** Please keep your shirt on, regardless of your gender (we've decided out of fairness to ask everyone, regardless of gender, to keep their shirts on). ** IF YOU INTEND TO SWEAT ** Please care for yourself and others by: 1) Taking a shower before you arrive 2) Bringing a towel to wipe up any wake you leave behind **SCENT-FREE SPACE** Please refrain from wearing anything scented in the space (including essential oils, lotions or liniments). ** CELL PHONE USE ** By popular request we have a 'no cell phone use' policy in the dance space. Please silence your phone or turn it off altogether. No cameras in the space either! If you need to use your device, please do so in the foyer or outside. As you can imagine, it's distracting otherwise. ** DANCING &amp; CONSENT ** Enjoy your own personal dance or spark up creative movement with others, if there is mutual agreement . If you wish to dance with another, look for eye contact or the body language of an invitation (if that isn't there then it's a "no"). Remember that a person's willingness to dance can change from moment to moment or week to week. At any time you, or the person you are dancing with, may choose to end the encounter by moving away, or bowing with hands in prayer. ** TALKING ** The dance space is a no-talking zone. This is again done to remove any distractions and to allow for dropping in more fully. If you need to have a conversation, however brief, please step out into the foyer or go outside. If you witness a conversation happening, you are welcome to gently remind people of this request (with a gesture). ** KIDS ** Parents are asked to kindly monitor their kids and keep them close. Please do not permit your kids to run freely through the dance space - this is risky for kids and for dancers. If it's quiet (especially at the beginning and ending), and your kids aren't - please see that they are guided into relative silence. Otherwise we will ask you to take them outside so as not to distract others from the proceedings. **FOOTWEAR** Please wear socks or indoor shoes/sneakers in the dance space. HERE'S MORE OF WHAT DANCE TEMPLE OFFERS: • Practice freedom of expression through movement, while respecting and being aware of those around you. • Tune into an eclectic selection of musical flavors from a revolving lineup of experienced facilitators. • Inspire and explore new ways to move your body. • Explore the altar space for contemplation, reflection and intention setting. • Learn to enter into a state of trance without the use of substances (no drugs or alcohol please). • Non denominational opening and closing (can be in the form of an embodiment practice, prayer or meditation) • Minimal facilitation. You are free to move as you wish. Dance Temple is an inclusive community that celebrates gender diversity and authentic expression. In Closing: Please arrive early or on time so that we may all journey together. Bring a water bottle. Breathe. Take care of yourself, others and the space. Wear comfortable clothing for movement. Be prepared to sweat. We acknowledge with deep respect and gratitude that we gather on unceded Lekwungen Territory, home of the Esquimalt and Songhees First Nations. We honour the long-time, ongoing indigenous stewardship of this land. See less Dance Victoria, British Columbia Edelweiss Club, 108 Niagara Street, Victoria, BC 108 Niagara St, Victoria, BC V8V 1E9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C930" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/556816543734629/</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Monday 7 July 2025 from 17:30-19:30 Free Outdoor Intro Dance Class + Social | Summer Series Ship's Point Inner Harbour About Discussion More About Discussion Free Outdoor Intro Dance Class + Social | Summer Series Interested Going Invite Details 50 people responded Event by Victoria Latin Dance Association Ship's Point Inner Harbour Duration: 2 hr Public · Anyone on or off Facebook Free Outdoor Intro Dance Class + Social | Summer Series Join us for an introduction to Merengue with Sebastian and Hannah— part of our summer series, proudly sponsored by the City of Victoria! Every Monday | June–August 5:30–7:30 PM 1.5-hour dance class followed by a 30-minute outdoor social Dance style rotates monthly — check our content calendar on our website for full details! This free outdoor event is open to everyone — no partner or dance experience needed. All ages, bodies, and abilities are warmly welcomed! Whether you’re dancing the night away or soaking in the summer vibes, come be part of this vibrant community celebration. Don’t forget to bring a water bottle and come ready to move! See less Victoria, British Columbia Ship's Point Inner Harbour Big Blue Sailing, Victoria, BC V8W, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C931" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1187402793186660/</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Saturday 21 June 2025 from 08:00-12:00 Global Underscore Solstice Dance Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada About Discussion More About Discussion Global Underscore Solstice Dance Details 62 people responded Event by Arunimá McNeish , Michael McAmmond and Victoria Contact Improv Jam Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada Duration: 4 hr Public · Anyone on or off Facebook Sweet dancers, This summer solstice we extend a warm invitation to join us in expanding and deepening our practice of Contact Improvisation with participation in The Global Underscore. Please arrive at 8am to join a 40 minute talk-through, introducing the concepts of the Underscore. This is mandatory if you have never attended an Underscore before. The Underscore will begin promptly at 8:45am. If you have attended a talk-through before you're welcome to arrive at this time. We will all start and end together. This is a closed container and we will not be allowing late-comers. TIMELINE: 8am-8:40am Underscore Talk-Through with Arunima 8:45am-11:30am Underscore 11:30am-11:50am Closing Circle COST: $15-$20  etransfer or pay cash at the door if pre-registered (if money is a barrier please reach out to discuss options). Please contact Arunima at ode.to.thylacine@gmail.com for registration, etransfer, questions, etc. VENUE: Centennial United Church (612 David St, Victoria, BC). MORE INFO: The Underscore, which has been evolving since 1990, is a vehicle for incorporating Contact Improvisation into the broader arena of improvisational dance practice; developing greater ease dancing in spherical space—alone and with others; and for integrating kinesthetic and compositional aspects while improvising. It allows for a full spectrum of energetic and physical expressions, embodying a range of forms and changing states. Its practice is familiar yet unpredictable. The practice progresses through a broad range of dynamic states, including long periods of very small, private, and quiet internal activity and other times of higher energy and interactive dancing. There are 20+ phases, 12+ connections, and 7 aspects of the Underscore—each with a name and a graphic symbol—which create a general map for the dancers. Within that frame, dancers are free to create their own movements, dynamics, and relationships—with themselves, each other, the group, and the environment. Each Underscore is unique, providing rich and often inspiring experiences of the human and artistic phenomena of dance improvisation. https://globalunderscore.com/ https://nancystarksmith.com/underscore/ See less Victoria, British Columbia Centennial United Church 612 David St, Victoria, BC V8T 2E1, Canada 612 David St, Victoria, BC V8T 2E1, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C932" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/909522138040202/</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 3 friends Recommended events See all Today at 18:30 Technique and Milonga with Monica Parra Janine Saturday at 14:00 Oak Bay Summer Concerts in the Park: Family Show Lorne and 4 friends Tomorrow from 19:00-21:30 Swingin' in the Shell Robin Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 28 Friday 28 November 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1924 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 63 people interested Interested Sun, 20 Jul at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Lorne, Roy and 2 friends 63 people interested Interested Sun, 20 Jul at 12:00 Anniversary Milonga Alive Tango Victoria Janine is going 27 people interested Interested Popular with friends Happening now Technique and Milonga with Monica Parra Alive Tango Victoria Janine is going Interested Sun, 20 Jul at 12:00 Anniversary Milonga Alive Tango Victoria Janine is going Interested Tomorrow at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested This Saturday at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Amanda and 7 friends Interested This Saturday at 14:00 Oak Bay Summer Concerts in the Park: Family Show Willows Park Lorne, Debi and 3 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C933" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1185783966345055/</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Sunday 25 May 2025 from 10:00-13:00 Shuffle Dance Workshop Victoria, BC About Discussion More About Discussion Shuffle Dance Workshop Details 12 people responded Event by Adelène Buchanan Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another SHUFFLE WORKSHOP coming your way!! Join our Shuffle Dance Workshop and learn a full shuffle choreography set to an energetic electronic track. We’ll guide you through each step, focusing on key shuffle movements, while incorporating them into a dynamic routine. Perfect for ALL LEVELS! This workshop will help you improve your footwork, coordination, and cardiovascular stamina as you master a complete choreography. Here’s what you need to know: DATE: Sunday, May 25th TIME: 10am - 1pm PLACE: The Beat Clinic (1303 Broad Street) Sign-up link here https://www.thebeatclinic.ca/ See less Victoria, British Columbia Victoria, BC Guests See All</t>
+        </is>
+      </c>
+      <c r="C934" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1031573525615192/</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Sunday 29 June 2025 at 19:00 GROOVE KITCHEN'S JUNEFEST DANCE!! Hermann's Jazz Club About Discussion More About Discussion GROOVE KITCHEN'S JUNEFEST DANCE!! Details 103 people responded Event by Groove Kitchen and Hermann's Jazz Club Hermann's Jazz Club Public · Anyone on or off Facebook The festival is over and it seems you still wanna celebrate music, but also... wanna get down and boogie?? You're our kind of people!! Observe the top of Summer with song and funky steps as the kitchen's groove moves your body like they've done before at spots like the Butchart Gardens, The Esquimalt Ribfest, The Osbourne Bay Pub, or the hottest rooms in and outta town. The Chefs are ready to serve their mouthwatering melange of funk, pop, soul, Latin, and flavours to party to the end!! Join us... Doors 5:30 PM / 7:00 PM Show, Sunday June 29th Hermann's Jazz Club 753 View Street Victoria, BC V8W 1J9 https://hermannsjazz.com/show/737557/view See less Victoria, British Columbia Hermann's Jazz Club 751 View St, Victoria, BC V8W 1J9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C935" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/624858640069610/</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>(20+) Salsa Night @ Dance City | Facebook Number of unread notifications 20+ Events Home Your events Notifications Create New Event Your upcoming events See all Tomorrow from 19:30-22:30 Thursdays Practica: Summer Series Lorne and 2 friends Saturday 12 July 2025 from 20:00-23:59 Special Edition Konpa Workshop with Stophy Lorne and 4 friends 10 Sep at 17:00 – 19 Sep at 17:00 Ashby Laine Residency Program Lorne and 3 friends Recommended events See all Today at 18:30 Technique and Milonga with Monica Parra Janine Saturday at 14:00 Oak Bay Summer Concerts in the Park: Family Show Lorne and 4 friends Tomorrow from 19:00-21:30 Swingin' in the Shell Robin Categories Classics Comedy Crafts Dance Drinks Fitness &amp; workouts Foods Games Gardening Health &amp; medical Healthy living and self-care Home and garden Music and audio Parties Professional networking Religions Shopping Social issues Sports Theatre TV and films Visual arts 22 Friday 22 August 2025 at 19:45 Salsa Night @ Dance City Edelweiss Club About Discussion More About Discussion Salsa Night @ Dance City Interested Going Invite Details Event by Salsa Caliente Edelweiss Club Public · Anyone on or off Facebook We are excited to bring you dancing the 4th Friday of every month at an all ages venue right in the heart of downtown, with a wood dance floor!!!!! 7:45pm Doors open Salsa Caliente’s team will be there to greet you. 8:00pm Salsa lesson Taught by World Salsa University certified instructor, Christina Morrison. No experience or partner is necessary as we rotate partners throughout the lesson so you will already know a LOT of people by the time the dancing begins. 9:00pm- midnight Dancing to Salsa, Bachata, Merengue, Cha Cha Cha, Bolero &amp; Latin Hustle. All ages welcome. $15.00 per person + service fee on Eventbrite or cash only at the door. $13 cash for Edelweiss Club members at the door only. *Limited capacity.  First come first served. We reserve the right to refuse entrance at the door. See less Dance Victoria, British Columbia Edelweiss Club 117 St Lawrence St, Victoria, BC V8V 1X7, Canada Meet your host Salsa Caliente 1924 past events · Page · Dance studio Salsa Caliente is an internationally touring dance group from Victoria, Canada. www.CalienteDance.com Message Suggested events This Sunday at 15:45 Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Lorne, Roy and Ali 63 people interested Interested Sun, 20 Jul at 15:45 Sunday Sundown Social: Bachata Temptation, Salsa Sensation Songhees Walkway Lorne, Roy and 2 friends 63 people interested Interested Sun, 20 Jul at 12:00 Anniversary Milonga Alive Tango Victoria Janine is going 27 people interested Interested Popular with friends Happening now Technique and Milonga with Monica Parra Alive Tango Victoria Janine is going Interested Sun, 20 Jul at 12:00 Anniversary Milonga Alive Tango Victoria Janine is going Interested Tomorrow at 19:00 Swingin' in the Shell Cameron Bandshell @ Beacon Hill Park Robin is interested Interested This Saturday at 20:00 🎆🔥 Canada Day Latin Party – July 5th! 🔥🎆 Latin Dance Canada Lorne, Amanda and 7 friends Interested Thu, 10 Jul at 18:00 Oak Bay Summer Concerts in the Park: Soul Intention Willows Park Roy, Debi and 2 friends are interested Interested Privacy · Terms · Advertising · Ad choices · Cookies · More · Meta © 2025</t>
+        </is>
+      </c>
+      <c r="C936" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/650657144184821/</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Saturday 19 July 2025 from 21:00-02:00 COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY The Coda About Discussion More About Discussion COLOMBIAN SUMMER RUMBA “TIERRA QUERIDA” PARTY Interested Going Invite Details 79 people responded Event by Victoria Viva la Fiesta , The Coda and Victoria LATIN Community Society The Coda Tickets gotothecoda.com/show/09235565-4349-4afe-b996-6cff0adb3a6b Public · Anyone on or off Facebook Colombian Summer Rumba: “Tierra Querida” Party Saturday, July 19th Doors: 9:00 PM | Show: 9:30 PM 19+ | ID Required Grab your tickets now! The Victoria Viva la Fiesta Summer Party Has Arrived! Turn up the heat, grab your crew, and get ready for a night of explosive music, non-stop dancing, tropical cocktails, and pure rumba madness! This is Tierra Querida — and It’s gonna be legendary. Start the night with a live tribute to Colombian music by the talented Daniel Sar &amp; Sofia Leonne. Their performance will honor legendary Colombian artists such as Juanes, Maluma, Fonseca, Rodolfo Aicardi, Herencia de Timbiquí, Mon Laferte, and more—blending pop, tropical rhythms, and heartfelt Latin ballads into a powerful musical journey. At 10:30 PM, DJ Miro, straight from Cali, Colombia, will take over with a fiery mix of Colombian beats. Later, resident DJ Alex King will close out the night, turning up the heat with Latin hits and ending strong with the latest reggaetón summer vibes. At midnight, enjoy a special folkloric performance by Danza Colombia as we wave our flag souvenirs to commemorate July 20th. Savor delicious cocktails, soak in vibrant downtown vibes, and enjoy a night filled with alegría, culture, and unforgettable Colombian energy! Get your tickets NOW! First-tier: $20 | Second-tier: $25 Limited tickets available at the door for $27 - Act fast before they are sold out! Party ends at 2:00 AM Each ticket includes a Colombian flag souvenir. Take a piece of the celebration home with you! Click the link and get $20 early bird tickets! Hurry up! limited Capacity! See less Victoria, British Columbia Tickets Find Tickets The Coda 751 View St, Victoria Victoria's Live Music Venue Guests See All</t>
+        </is>
+      </c>
+      <c r="C937" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1132427048350776/</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Saturday 5 April 2025 at 18:30 A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Caffè Fantastico Specialty Coffees About Discussion More About Discussion A Night of Classic Swing and Brazilian Jazz with The RoseBuds  &amp;  Samba E Sol Details 98 people responded Event by Rebecca Rose , Alex Q Moore and Andrew Greenwood Caffè Fantastico Specialty Coffees Public · Anyone on or off Facebook A Night of Classic Swing and Brazilian Jazz with Rosebuds and Samba e Sol Time: Doors at 6:30pm Music at 7-9pm Cover: $12 Presale - E-transfer almix12@gmail.com or 15$ cash/e-transfer at the door. Formed in the heart of Chinatown, Rosebuds is a dynamic ensemble that brings the vibrant sounds of jazz, blues &amp; swing to life.  The group plays a mixture of originals and jazz standards, and is influenced by artists like Louis Armstrong, Billie Holiday, Lester Young, and Lionel Hampton. Featuring Rebecca Wells (vocals/guitar), Alex Moore (guitar/keys) Bryden Amos (guitar/keys), Matisse Gubby-Hurtig (bass), Owen Chow (trumpet), and Andrew Greenwood (tenor saxophone). Samba e Sol is a newly formed Brazilian bossa nova jazz trio featuring Andrew Greenwood (flute), Alex Moore (guitar), and Matisse Gubby-Hurtig (bass), playing music by artists like Antonio Carlos Jobim, Marcos Valle, Luiz Bonfa, and more. Instagram: https://www.instagram.com/rosebudsband/ See less Victoria, British Columbia Caffè Fantastico Specialty Coffees 965 Kings Road, Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C938" s="3" t="n">
+        <v>45840.8461158912</v>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/372311028526699/</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Saturday 9 December 2023 from 20:30-23:30 Victoria Kizomba Social: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Social: Fall Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C939" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/2637194793152555/</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Details 151 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 29, 2025 | Lesson:  Intro to Salsa Rueda with Sam and Katie Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa Rueda • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C940" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1029869435768837/</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Saturday 22 March 2025 at 20:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC This event has been cancelled. You cannot share this event, but you can still post. About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 14 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C941" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1743571267040445/</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway Ali Jorgensen invited you About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Details 55 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire June 8, 2025 | Lesson: Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway Victoria Guests See All</t>
+        </is>
+      </c>
+      <c r="C942" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1337760257449745/</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 6 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 10, 2025 | Lesson:   Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C943" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3006474846197996/</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 48 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 27, 2025 | Lesson:  Intro class TBD Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro class TBD • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C944" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1179097320623502/</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Saturday 10 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 37 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C945" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1060779176049104/</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Thursday 3 October 2024 from 19:30-22:30 Kizomba Practica Thursdays: Fall Series Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Kizomba Practica Thursdays: Fall Series Details 20 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre Duration: 3 hr Public · Anyone on or off Facebook Join us every Thursday for Kizomba/Urbankiz classes. Intermediate 7:30PM-8:15pm Beginner 8:15pm-9:00pm Practica until 10:30pm Class only: $10 Class &amp; Practica: $15 or $10 for university students w/ID Practice only $10 Classes will be provided by your local Instructor (David Lamine) and assistants (Robyn, Becky) and occasionally by some out of town and International Instructors. Please help to spread the word and let’s continue to build this beautiful community See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C946" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1794066937801722/</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Saturday 8 March 2025 from 20:30-23:30 Victoria Kizomba Socials: Winter Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Winter Series Details 26 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C947" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1293301738436581/</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Sunday 6 April 2025 at 17:00 Kizomba Sundown Party: Free of charge Method Studio - Victoria BC David Lamine Victoria invited you About Discussion More About Discussion Kizomba Sundown Party: Free of charge Details 58 people responded Event by David Lamine Victoria and Victoria Kizomba Lovers Group Method Studio - Victoria BC Public · Anyone on or off Facebook Free Pre-VIKFest party. Bring snack and drink. Expect great music, great energy, great atmosphere. "Dance with your heart. your feet will follow" Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C948" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/960236445839425/</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Saturday 22 June 2024 from 18:00-21:00 Kizomba/UrbanKiz at Clover Clover Pt, Victoria, BC V8S, Canada About Discussion More About Discussion Kizomba/UrbanKiz at Clover Interested Details 56 people responded Event by Becky Mowat Clover Pt, Victoria, BC V8S, Canada Duration: 3 hr Public · Anyone on or off Facebook Come join us for our first time dancing at Clover Point! There will be no lesson beforehand and this is super casual. Just a bunch of friends hanging out and dancing. Bring snacks, something to drink, blankets, warm clothes (as it is typically cooler by the ocean). There isn't a lot of parking at Clover Point but you can park along Dallas Rd and just walk down. Feel free to invite friends and family. Hope to see you all there! See less Victoria, British Columbia Clover Pt, Victoria, BC V8S, Canada 1301 Clover Pt, Victoria, BC V8S, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C949" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1079226067560481/</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 63 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire July 6, 2025 | Lesson:  Intro to Kizomba with Alicia &amp; Aaron Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Kizomba • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C950" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/947213690692385/</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Saturday 24 May 2025 from 20:30-23:30 Victoria Kizomba Socials: Spring Series Ukrainian Cultural Centre - Victoria, BC Becky Mowat invited you About Discussion More About Discussion Victoria Kizomba Socials: Spring Series Details 32 people responded Event by Becky Mowat and Victoria Kizomba Lovers Group Ukrainian Cultural Centre - Victoria, BC Duration: 3 hr Public · Anyone on or off Facebook Another Season, another series of kizomba events coming up. Join the island vibe this Saturday. Great music, great energy, great atmosphere. Urban Kiz class starts at 8:30pm, followed by the night social. Cover: $10, cash only. "Dance with your heart. your feet will follow" See less Victoria, British Columbia Ukrainian Cultural Centre - Victoria, BC 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C951" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1861230087752141/</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Songhees Walkway About Discussion More About Discussion Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire Interested Going Invite Details 6 people responded Event by Victoria Latin Dance Association Songhees Walkway Duration: 3 hr 45 min Public · Anyone on or off Facebook Sunday Sundown Social: Salsa Fire, Bachata Desire, Kizomba Inspire August 31, 2025 | Lesson:  Intro to Salsa with Adam &amp; Alicia Join us for a vibrant late afternoon of Latin dancing by the ocean! We’ll begin with a beginner-friendly lesson— no partner or experience needed. After the class, enjoy an open-air social featuring a dynamic blend of Salsa, Bachata, and Kizomba, with just a light touch of Merengue to round out the evening. Whether you want to: • Learn something new in the lesson • Dance your heart out at the social • Or simply enjoy the music, connect with others, and soak in the atmosphere — You’re warmly welcomed. This is a beautiful, inclusive, and supportive community where new friendships are made and everyone belongs. Location: Songhees Plaza (near the Johnson Street Bridge) Schedule: • 3:45 PM – Doors Open (This is a controlled area under our permit) • 4:00 – 4:30 PM – Intro to Salsa • 4:30 – 7:30 PM – Social Dancing Cover: • $5 for students (with valid ID) • $10 general admission • Cash only What to Bring: • Water bottle (we also have water available for purchase if you forget) • A hat or sun umbrella • Sunglasses and sunscreen • Comfortable shoes for dancing on cement This year, we’re excited to offer a 10 x 17.6 ft sun tent to provide shade and help keep you cool while you relax between dances. Why We Charge: We’re still in the process of applying for government funding and, unfortunately, didn’t raise enough through our indoor socials to fully cover summer costs. Your support helps with essentials like permits, insurance, equipment, venue fees, and more (approx. $3500–$4000 annually). Thank you for your understanding and continued support. If you have grant writing experience or would like to volunteer, we’d love to hear from you! Note: Photos and videos may be taken during the event for social media and future promotions. Thank you for your understanding. See less Victoria, British Columbia Songhees Walkway TLC the LND Cnsrvncy of British, 30 Esquimalt Rd, Victoria, BC V9A, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C952" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1184791909680061/</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Thursday 13 March 2025 from 19:30-23:00 Urban Kiz Workshop with Mannie Ukrainian Cultural Centre Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 50 people responded Event by Becky Mowat and David Lamine Victoria Ukrainian Cultural Centre Duration: 3 hr 30 min Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Ukrainian Cultural Centre 3277 Douglas St, Saanich, BC V8Z 3K9, Canada Guests See All</t>
+        </is>
+      </c>
+      <c r="C953" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/3185065321631809/</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Saturday 15 March 2025 from 20:00-00:00 Urban Kiz Workshop with Mannie Method Studio - Victoria BC Becky Mowat invited you About Discussion More About Discussion Urban Kiz Workshop with Mannie Details 48 people responded Event by Becky Mowat and David Lamine Victoria Method Studio - Victoria BC Duration: 4 hr Public · Anyone on or off Facebook Join us in welcoming Mannie for his first time to Victoria! Mannie was born in Zimbabwe and has lived in Manchester, London, San Francisco, NYC and currently in Dallas, Texas. He has a passion for music, dance and performance. He has won both dance and music contests, which is a testament to his technical skill, musicality, and performance artistry. His classes emphasize in precision, fluidity, and personal expression, ensuring that students not only master choreography but also understand the artistry behind it. Whether teaching beginners or advanced dancers, Mannie’s goals are to inspire confidence, discipline, and joy through movement, helping each student discover their unique dance voice. Details We will create two events as they are at separate locations on two different dates. The first one will be held at the Ukrainian Cultural Centre and the second at Medicine Moves Studio. There will be 4 hours of workshops in total. Mannie will be focusing on musicality, expression, connection and communication with your partner. March 13th Workshop: 7:30pm-9:30pm Social Dancing: 9:30-11:00pm Location: Ukrainian Cultural Centre 3277 Douglas St. Victoria, BC March 15th Workshop: 8:00pm-10:00pm Social Dancing: 10:00pm-12:00am Location: Medicine Moves Studio 841 Fisgard St. Victoria, BC Price: $80 (includes both Thursday &amp; Saturday) Please e transfer to becksmith@hotmail.com See less Victoria, British Columbia Method Studio - Victoria BC 841 Fisgard Street, Victoria Beautiful 900+sq feet. cushioned hardwood floor, located in the heart of downtown Victoria. Ideal for dance, yoga, and martial arts classes. Guests See All</t>
+        </is>
+      </c>
+      <c r="C954" s="3" t="n">
+        <v>45840.85424663194</v>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/events/1152065639712042/</t>
+        </is>
+  